<commit_message>
adicionados todos os pokemon de Hoenn no SQLite
</commit_message>
<xml_diff>
--- a/pokemonv2/pokemons.xlsx
+++ b/pokemonv2/pokemons.xlsx
@@ -8405,7 +8405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -8413,6 +8413,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8715,8 +8716,8 @@
   <dimension ref="A1:G1026"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A260" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B273" sqref="B273"/>
+      <pane ySplit="1" topLeftCell="A265" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A273" sqref="A273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14692,2476 +14693,2533 @@
       </c>
     </row>
     <row r="273" spans="1:7">
-      <c r="A273" t="s">
+      <c r="A273" s="5" t="s">
         <v>867</v>
       </c>
-      <c r="B273" t="s">
+      <c r="B273" s="5" t="s">
         <v>868</v>
       </c>
-      <c r="C273" t="s">
+      <c r="C273" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D273" t="s">
+      <c r="D273" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="E273" t="s">
+      <c r="E273" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="F273" t="s">
-        <v>8</v>
-      </c>
-      <c r="G273" t="s">
+      <c r="F273" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G273" s="5" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="274" spans="1:7">
-      <c r="A274" t="s">
+      <c r="A274" s="5" t="s">
         <v>869</v>
       </c>
-      <c r="B274" t="s">
+      <c r="B274" s="5" t="s">
         <v>870</v>
       </c>
-      <c r="C274" t="s">
+      <c r="C274" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="E274" t="s">
+      <c r="D274" s="5"/>
+      <c r="E274" s="5" t="s">
         <v>590</v>
       </c>
-      <c r="F274" t="s">
+      <c r="F274" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G274" t="s">
+      <c r="G274" s="5" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="275" spans="1:7">
-      <c r="A275" t="s">
+      <c r="A275" s="5" t="s">
         <v>871</v>
       </c>
-      <c r="B275" t="s">
+      <c r="B275" s="5" t="s">
         <v>872</v>
       </c>
-      <c r="C275" t="s">
+      <c r="C275" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="D275" t="s">
+      <c r="D275" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="E275" t="s">
+      <c r="E275" s="5" t="s">
         <v>638</v>
       </c>
-      <c r="F275" t="s">
+      <c r="F275" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G275" t="s">
+      <c r="G275" s="5" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="276" spans="1:7">
-      <c r="A276" t="s">
+      <c r="A276" s="5" t="s">
         <v>873</v>
       </c>
-      <c r="B276" t="s">
+      <c r="B276" s="5" t="s">
         <v>874</v>
       </c>
-      <c r="C276" t="s">
+      <c r="C276" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="D276" t="s">
+      <c r="D276" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="E276" t="s">
+      <c r="E276" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="F276" t="s">
-        <v>8</v>
-      </c>
-      <c r="G276" t="s">
+      <c r="F276" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G276" s="5" t="s">
         <v>875</v>
       </c>
     </row>
     <row r="277" spans="1:7">
-      <c r="A277" t="s">
+      <c r="A277" s="5" t="s">
         <v>876</v>
       </c>
-      <c r="B277" t="s">
+      <c r="B277" s="5" t="s">
         <v>877</v>
       </c>
-      <c r="C277" t="s">
+      <c r="C277" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D277" t="s">
+      <c r="D277" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E277" t="s">
+      <c r="E277" s="5" t="s">
         <v>878</v>
       </c>
-      <c r="F277" t="s">
+      <c r="F277" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="G277" t="s">
+      <c r="G277" s="5" t="s">
         <v>879</v>
       </c>
     </row>
     <row r="278" spans="1:7">
-      <c r="A278" t="s">
+      <c r="A278" s="5" t="s">
         <v>880</v>
       </c>
-      <c r="B278" t="s">
+      <c r="B278" s="5" t="s">
         <v>881</v>
       </c>
-      <c r="C278" t="s">
+      <c r="C278" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D278" t="s">
+      <c r="D278" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E278" t="s">
+      <c r="E278" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="F278" t="s">
-        <v>8</v>
-      </c>
-      <c r="G278" t="s">
+      <c r="F278" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G278" s="5" t="s">
         <v>882</v>
       </c>
     </row>
     <row r="279" spans="1:7">
-      <c r="A279" t="s">
+      <c r="A279" s="5" t="s">
         <v>883</v>
       </c>
-      <c r="B279" t="s">
+      <c r="B279" s="5" t="s">
         <v>884</v>
       </c>
-      <c r="C279" t="s">
+      <c r="C279" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D279" t="s">
+      <c r="D279" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E279" t="s">
+      <c r="E279" s="5" t="s">
         <v>878</v>
       </c>
-      <c r="F279" t="s">
+      <c r="F279" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G279" t="s">
+      <c r="G279" s="5" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="280" spans="1:7">
-      <c r="A280" t="s">
+      <c r="A280" s="5" t="s">
         <v>885</v>
       </c>
-      <c r="B280" t="s">
+      <c r="B280" s="5" t="s">
         <v>886</v>
       </c>
-      <c r="C280" t="s">
+      <c r="C280" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D280" t="s">
+      <c r="D280" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E280" t="s">
+      <c r="E280" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="F280" t="s">
-        <v>8</v>
-      </c>
-      <c r="G280" t="s">
+      <c r="F280" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G280" s="5" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="281" spans="1:7">
-      <c r="A281" t="s">
+      <c r="A281" s="5" t="s">
         <v>887</v>
       </c>
-      <c r="B281" t="s">
+      <c r="B281" s="5" t="s">
         <v>888</v>
       </c>
-      <c r="C281" t="s">
+      <c r="C281" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="D281" t="s">
+      <c r="D281" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E281" t="s">
+      <c r="E281" s="5" t="s">
         <v>461</v>
       </c>
-      <c r="F281" t="s">
+      <c r="F281" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="G281" t="s">
+      <c r="G281" s="5" t="s">
         <v>889</v>
       </c>
     </row>
     <row r="282" spans="1:7">
-      <c r="A282" t="s">
+      <c r="A282" s="5" t="s">
         <v>890</v>
       </c>
-      <c r="B282" t="s">
+      <c r="B282" s="5" t="s">
         <v>891</v>
       </c>
-      <c r="C282" t="s">
+      <c r="C282" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="D282" t="s">
+      <c r="D282" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E282" t="s">
+      <c r="E282" s="5" t="s">
         <v>892</v>
       </c>
-      <c r="F282" t="s">
+      <c r="F282" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G282" t="s">
+      <c r="G282" s="5" t="s">
         <v>893</v>
       </c>
     </row>
     <row r="283" spans="1:7">
-      <c r="A283" t="s">
+      <c r="A283" s="5" t="s">
         <v>894</v>
       </c>
-      <c r="B283" t="s">
+      <c r="B283" s="5" t="s">
         <v>895</v>
       </c>
-      <c r="C283" t="s">
+      <c r="C283" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="D283" t="s">
+      <c r="D283" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E283" t="s">
+      <c r="E283" s="5" t="s">
         <v>896</v>
       </c>
-      <c r="F283" t="s">
-        <v>8</v>
-      </c>
-      <c r="G283" t="s">
+      <c r="F283" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G283" s="5" t="s">
         <v>897</v>
       </c>
     </row>
     <row r="284" spans="1:7">
-      <c r="A284" t="s">
+      <c r="A284" s="5" t="s">
         <v>898</v>
       </c>
-      <c r="B284" t="s">
+      <c r="B284" s="5" t="s">
         <v>899</v>
       </c>
-      <c r="C284" t="s">
+      <c r="C284" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D284" t="s">
+      <c r="D284" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E284" t="s">
+      <c r="E284" s="5" t="s">
         <v>878</v>
       </c>
-      <c r="F284" t="s">
+      <c r="F284" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="G284" t="s">
+      <c r="G284" s="5" t="s">
         <v>900</v>
       </c>
     </row>
     <row r="285" spans="1:7">
-      <c r="A285" t="s">
+      <c r="A285" s="5" t="s">
         <v>901</v>
       </c>
-      <c r="B285" t="s">
+      <c r="B285" s="5" t="s">
         <v>902</v>
       </c>
-      <c r="C285" t="s">
+      <c r="C285" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D285" t="s">
+      <c r="D285" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E285" t="s">
+      <c r="E285" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="F285" t="s">
+      <c r="F285" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G285" t="s">
+      <c r="G285" s="5" t="s">
         <v>851</v>
       </c>
     </row>
     <row r="286" spans="1:7">
-      <c r="A286" t="s">
+      <c r="A286" s="5" t="s">
         <v>903</v>
       </c>
-      <c r="B286" t="s">
+      <c r="B286" s="5" t="s">
         <v>904</v>
       </c>
-      <c r="C286" t="s">
+      <c r="C286" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="E286" t="s">
+      <c r="D286" s="5"/>
+      <c r="E286" s="5" t="s">
         <v>420</v>
       </c>
-      <c r="F286" t="s">
+      <c r="F286" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G286" t="s">
+      <c r="G286" s="5" t="s">
         <v>905</v>
       </c>
     </row>
     <row r="287" spans="1:7">
-      <c r="A287" t="s">
+      <c r="A287" s="5" t="s">
         <v>906</v>
       </c>
-      <c r="B287" t="s">
+      <c r="B287" s="5" t="s">
         <v>907</v>
       </c>
-      <c r="C287" t="s">
+      <c r="C287" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="D287" t="s">
+      <c r="D287" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="E287" t="s">
+      <c r="E287" s="5" t="s">
         <v>438</v>
       </c>
-      <c r="F287" t="s">
+      <c r="F287" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="G287" t="s">
+      <c r="G287" s="5" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="288" spans="1:7">
-      <c r="A288" t="s">
+      <c r="A288" s="5" t="s">
         <v>908</v>
       </c>
-      <c r="B288" t="s">
+      <c r="B288" s="5" t="s">
         <v>909</v>
       </c>
-      <c r="C288" t="s">
+      <c r="C288" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="E288" t="s">
+      <c r="D288" s="5"/>
+      <c r="E288" s="5" t="s">
         <v>606</v>
       </c>
-      <c r="F288" t="s">
+      <c r="F288" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G288" t="s">
+      <c r="G288" s="5" t="s">
         <v>910</v>
       </c>
     </row>
     <row r="289" spans="1:7">
-      <c r="A289" t="s">
+      <c r="A289" s="5" t="s">
         <v>911</v>
       </c>
-      <c r="B289" t="s">
+      <c r="B289" s="5" t="s">
         <v>912</v>
       </c>
-      <c r="C289" t="s">
+      <c r="C289" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="E289" t="s">
+      <c r="D289" s="5"/>
+      <c r="E289" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="F289" t="s">
+      <c r="F289" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G289" t="s">
+      <c r="G289" s="5" t="s">
         <v>913</v>
       </c>
     </row>
     <row r="290" spans="1:7">
-      <c r="A290" t="s">
+      <c r="A290" s="5" t="s">
         <v>914</v>
       </c>
-      <c r="B290" t="s">
+      <c r="B290" s="5" t="s">
         <v>915</v>
       </c>
-      <c r="C290" t="s">
+      <c r="C290" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="E290" t="s">
+      <c r="D290" s="5"/>
+      <c r="E290" s="5" t="s">
         <v>916</v>
       </c>
-      <c r="F290" t="s">
-        <v>8</v>
-      </c>
-      <c r="G290" t="s">
+      <c r="F290" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G290" s="5" t="s">
         <v>917</v>
       </c>
     </row>
     <row r="291" spans="1:7">
-      <c r="A291" t="s">
+      <c r="A291" s="5" t="s">
         <v>918</v>
       </c>
-      <c r="B291" t="s">
+      <c r="B291" s="5" t="s">
         <v>919</v>
       </c>
-      <c r="C291" t="s">
+      <c r="C291" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D291" t="s">
+      <c r="D291" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="E291" t="s">
+      <c r="E291" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="F291" t="s">
+      <c r="F291" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G291" t="s">
+      <c r="G291" s="5" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="292" spans="1:7">
-      <c r="A292" t="s">
+      <c r="A292" s="5" t="s">
         <v>920</v>
       </c>
-      <c r="B292" t="s">
+      <c r="B292" s="5" t="s">
         <v>921</v>
       </c>
-      <c r="C292" t="s">
+      <c r="C292" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D292" t="s">
+      <c r="D292" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E292" t="s">
+      <c r="E292" s="5" t="s">
         <v>922</v>
       </c>
-      <c r="F292" t="s">
+      <c r="F292" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G292" t="s">
+      <c r="G292" s="5" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="293" spans="1:7">
-      <c r="A293" t="s">
+      <c r="A293" s="5" t="s">
         <v>923</v>
       </c>
-      <c r="B293" t="s">
+      <c r="B293" s="5" t="s">
         <v>924</v>
       </c>
-      <c r="C293" t="s">
+      <c r="C293" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D293" t="s">
+      <c r="D293" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="E293" t="s">
+      <c r="E293" s="5" t="s">
         <v>925</v>
       </c>
-      <c r="F293" t="s">
-        <v>8</v>
-      </c>
-      <c r="G293" t="s">
+      <c r="F293" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G293" s="5" t="s">
         <v>926</v>
       </c>
     </row>
     <row r="294" spans="1:7">
-      <c r="A294" t="s">
+      <c r="A294" s="5" t="s">
         <v>927</v>
       </c>
-      <c r="B294" t="s">
+      <c r="B294" s="5" t="s">
         <v>928</v>
       </c>
-      <c r="C294" t="s">
+      <c r="C294" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="E294" t="s">
+      <c r="D294" s="5"/>
+      <c r="E294" s="5" t="s">
         <v>929</v>
       </c>
-      <c r="F294" t="s">
+      <c r="F294" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G294" t="s">
+      <c r="G294" s="5" t="s">
         <v>930</v>
       </c>
     </row>
     <row r="295" spans="1:7">
-      <c r="A295" t="s">
+      <c r="A295" s="5" t="s">
         <v>931</v>
       </c>
-      <c r="B295" t="s">
+      <c r="B295" s="5" t="s">
         <v>932</v>
       </c>
-      <c r="C295" t="s">
+      <c r="C295" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="E295" t="s">
+      <c r="D295" s="5"/>
+      <c r="E295" s="5" t="s">
         <v>933</v>
       </c>
-      <c r="F295" t="s">
+      <c r="F295" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G295" t="s">
+      <c r="G295" s="5" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="296" spans="1:7">
-      <c r="A296" t="s">
+      <c r="A296" s="5" t="s">
         <v>934</v>
       </c>
-      <c r="B296" t="s">
+      <c r="B296" s="5" t="s">
         <v>935</v>
       </c>
-      <c r="C296" t="s">
+      <c r="C296" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="E296" t="s">
+      <c r="D296" s="5"/>
+      <c r="E296" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="F296" t="s">
-        <v>8</v>
-      </c>
-      <c r="G296" t="s">
+      <c r="F296" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G296" s="5" t="s">
         <v>936</v>
       </c>
     </row>
     <row r="297" spans="1:7">
-      <c r="A297" t="s">
+      <c r="A297" s="5" t="s">
         <v>937</v>
       </c>
-      <c r="B297" t="s">
+      <c r="B297" s="5" t="s">
         <v>938</v>
       </c>
-      <c r="C297" t="s">
+      <c r="C297" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="E297" t="s">
+      <c r="D297" s="5"/>
+      <c r="E297" s="5" t="s">
         <v>939</v>
       </c>
-      <c r="F297" t="s">
+      <c r="F297" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="G297" t="s">
+      <c r="G297" s="5" t="s">
         <v>940</v>
       </c>
     </row>
     <row r="298" spans="1:7">
-      <c r="A298" t="s">
+      <c r="A298" s="5" t="s">
         <v>941</v>
       </c>
-      <c r="B298" t="s">
+      <c r="B298" s="5" t="s">
         <v>942</v>
       </c>
-      <c r="C298" t="s">
+      <c r="C298" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="E298" t="s">
+      <c r="D298" s="5"/>
+      <c r="E298" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="F298" t="s">
+      <c r="F298" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="G298" t="s">
+      <c r="G298" s="5" t="s">
         <v>943</v>
       </c>
     </row>
     <row r="299" spans="1:7">
-      <c r="A299" t="s">
+      <c r="A299" s="5" t="s">
         <v>944</v>
       </c>
-      <c r="B299" t="s">
+      <c r="B299" s="5" t="s">
         <v>945</v>
       </c>
-      <c r="C299" t="s">
+      <c r="C299" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D299" t="s">
+      <c r="D299" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E299" t="s">
+      <c r="E299" s="5" t="s">
         <v>946</v>
       </c>
-      <c r="F299" t="s">
+      <c r="F299" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="G299" t="s">
+      <c r="G299" s="5" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="300" spans="1:7">
-      <c r="A300" t="s">
+      <c r="A300" s="5" t="s">
         <v>947</v>
       </c>
-      <c r="B300" t="s">
+      <c r="B300" s="5" t="s">
         <v>948</v>
       </c>
-      <c r="C300" t="s">
+      <c r="C300" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="E300" t="s">
+      <c r="D300" s="5"/>
+      <c r="E300" s="5" t="s">
         <v>949</v>
       </c>
-      <c r="F300" t="s">
+      <c r="F300" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G300" t="s">
+      <c r="G300" s="5" t="s">
         <v>950</v>
       </c>
     </row>
     <row r="301" spans="1:7">
-      <c r="A301" t="s">
+      <c r="A301" s="5" t="s">
         <v>951</v>
       </c>
-      <c r="B301" t="s">
+      <c r="B301" s="5" t="s">
         <v>952</v>
       </c>
-      <c r="C301" t="s">
+      <c r="C301" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="E301" t="s">
+      <c r="D301" s="5"/>
+      <c r="E301" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="F301" t="s">
+      <c r="F301" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G301" t="s">
+      <c r="G301" s="5" t="s">
         <v>953</v>
       </c>
     </row>
     <row r="302" spans="1:7">
-      <c r="A302" t="s">
+      <c r="A302" s="5" t="s">
         <v>954</v>
       </c>
-      <c r="B302" t="s">
+      <c r="B302" s="5" t="s">
         <v>955</v>
       </c>
-      <c r="C302" t="s">
+      <c r="C302" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="E302" t="s">
+      <c r="D302" s="5"/>
+      <c r="E302" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="F302" t="s">
+      <c r="F302" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="G302" t="s">
+      <c r="G302" s="5" t="s">
         <v>956</v>
       </c>
     </row>
     <row r="303" spans="1:7">
-      <c r="A303" t="s">
+      <c r="A303" s="5" t="s">
         <v>957</v>
       </c>
-      <c r="B303" t="s">
+      <c r="B303" s="5" t="s">
         <v>958</v>
       </c>
-      <c r="C303" t="s">
+      <c r="C303" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="D303" t="s">
+      <c r="D303" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="E303" t="s">
+      <c r="E303" s="5" t="s">
         <v>959</v>
       </c>
-      <c r="F303" t="s">
-        <v>8</v>
-      </c>
-      <c r="G303" t="s">
+      <c r="F303" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G303" s="5" t="s">
         <v>953</v>
       </c>
     </row>
     <row r="304" spans="1:7">
-      <c r="A304" t="s">
+      <c r="A304" s="5" t="s">
         <v>960</v>
       </c>
-      <c r="B304" t="s">
+      <c r="B304" s="5" t="s">
         <v>961</v>
       </c>
-      <c r="C304" t="s">
+      <c r="C304" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="D304" t="s">
+      <c r="D304" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E304" t="s">
+      <c r="E304" s="5" t="s">
         <v>959</v>
       </c>
-      <c r="F304" t="s">
-        <v>8</v>
-      </c>
-      <c r="G304" t="s">
+      <c r="F304" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G304" s="5" t="s">
         <v>495</v>
       </c>
     </row>
     <row r="305" spans="1:7">
-      <c r="A305" t="s">
+      <c r="A305" s="5" t="s">
         <v>962</v>
       </c>
-      <c r="B305" t="s">
+      <c r="B305" s="5" t="s">
         <v>963</v>
       </c>
-      <c r="C305" t="s">
+      <c r="C305" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="D305" t="s">
+      <c r="D305" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="E305" t="s">
+      <c r="E305" s="5" t="s">
         <v>351</v>
       </c>
-      <c r="F305" t="s">
+      <c r="F305" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="G305" t="s">
+      <c r="G305" s="5" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="306" spans="1:7">
-      <c r="A306" t="s">
+      <c r="A306" s="5" t="s">
         <v>964</v>
       </c>
-      <c r="B306" t="s">
+      <c r="B306" s="5" t="s">
         <v>965</v>
       </c>
-      <c r="C306" t="s">
+      <c r="C306" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="D306" t="s">
+      <c r="D306" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="E306" t="s">
+      <c r="E306" s="5" t="s">
         <v>655</v>
       </c>
-      <c r="F306" t="s">
+      <c r="F306" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="G306" t="s">
+      <c r="G306" s="5" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="307" spans="1:7">
-      <c r="A307" t="s">
+      <c r="A307" s="5" t="s">
         <v>966</v>
       </c>
-      <c r="B307" t="s">
+      <c r="B307" s="5" t="s">
         <v>967</v>
       </c>
-      <c r="C307" t="s">
+      <c r="C307" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="D307" t="s">
+      <c r="D307" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="E307" t="s">
+      <c r="E307" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F307" t="s">
-        <v>8</v>
-      </c>
-      <c r="G307" t="s">
+      <c r="F307" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G307" s="5" t="s">
         <v>968</v>
       </c>
     </row>
     <row r="308" spans="1:7">
-      <c r="A308" t="s">
+      <c r="A308" s="5" t="s">
         <v>969</v>
       </c>
-      <c r="B308" t="s">
+      <c r="B308" s="5" t="s">
         <v>970</v>
       </c>
-      <c r="C308" t="s">
+      <c r="C308" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="D308" t="s">
+      <c r="D308" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E308" t="s">
+      <c r="E308" s="5" t="s">
         <v>606</v>
       </c>
-      <c r="F308" t="s">
+      <c r="F308" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="G308" t="s">
+      <c r="G308" s="5" t="s">
         <v>971</v>
       </c>
     </row>
     <row r="309" spans="1:7">
-      <c r="A309" t="s">
+      <c r="A309" s="5" t="s">
         <v>972</v>
       </c>
-      <c r="B309" t="s">
+      <c r="B309" s="5" t="s">
         <v>973</v>
       </c>
-      <c r="C309" t="s">
+      <c r="C309" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="D309" t="s">
+      <c r="D309" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E309" t="s">
+      <c r="E309" s="5" t="s">
         <v>628</v>
       </c>
-      <c r="F309" t="s">
+      <c r="F309" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="G309" t="s">
+      <c r="G309" s="5" t="s">
         <v>974</v>
       </c>
     </row>
     <row r="310" spans="1:7">
-      <c r="A310" t="s">
+      <c r="A310" s="5" t="s">
         <v>975</v>
       </c>
-      <c r="B310" t="s">
+      <c r="B310" s="5" t="s">
         <v>976</v>
       </c>
-      <c r="C310" t="s">
+      <c r="C310" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="E310" t="s">
+      <c r="D310" s="5"/>
+      <c r="E310" s="5" t="s">
         <v>420</v>
       </c>
-      <c r="F310" t="s">
+      <c r="F310" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G310" t="s">
+      <c r="G310" s="5" t="s">
         <v>977</v>
       </c>
     </row>
     <row r="311" spans="1:7">
-      <c r="A311" t="s">
+      <c r="A311" s="5" t="s">
         <v>978</v>
       </c>
-      <c r="B311" t="s">
+      <c r="B311" s="5" t="s">
         <v>979</v>
       </c>
-      <c r="C311" t="s">
+      <c r="C311" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="E311" t="s">
+      <c r="D311" s="5"/>
+      <c r="E311" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="F311" t="s">
-        <v>8</v>
-      </c>
-      <c r="G311" t="s">
+      <c r="F311" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G311" s="5" t="s">
         <v>980</v>
       </c>
     </row>
     <row r="312" spans="1:7">
-      <c r="A312" t="s">
+      <c r="A312" s="5" t="s">
         <v>981</v>
       </c>
-      <c r="B312" t="s">
+      <c r="B312" s="5" t="s">
         <v>982</v>
       </c>
-      <c r="C312" t="s">
+      <c r="C312" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="E312" t="s">
+      <c r="D312" s="5"/>
+      <c r="E312" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F312" t="s">
+      <c r="F312" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="G312" t="s">
+      <c r="G312" s="5" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="313" spans="1:7">
-      <c r="A313" t="s">
+      <c r="A313" s="5" t="s">
         <v>983</v>
       </c>
-      <c r="B313" t="s">
+      <c r="B313" s="5" t="s">
         <v>984</v>
       </c>
-      <c r="C313" t="s">
+      <c r="C313" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="E313" t="s">
+      <c r="D313" s="5"/>
+      <c r="E313" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F313" t="s">
+      <c r="F313" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="G313" t="s">
+      <c r="G313" s="5" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="314" spans="1:7">
-      <c r="A314" t="s">
+      <c r="A314" s="5" t="s">
         <v>985</v>
       </c>
-      <c r="B314" t="s">
+      <c r="B314" s="5" t="s">
         <v>986</v>
       </c>
-      <c r="C314" t="s">
+      <c r="C314" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E314" t="s">
+      <c r="D314" s="5"/>
+      <c r="E314" s="5" t="s">
         <v>655</v>
       </c>
-      <c r="F314" t="s">
+      <c r="F314" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="G314" t="s">
+      <c r="G314" s="5" t="s">
         <v>987</v>
       </c>
     </row>
     <row r="315" spans="1:7">
-      <c r="A315" t="s">
+      <c r="A315" s="5" t="s">
         <v>988</v>
       </c>
-      <c r="B315" t="s">
+      <c r="B315" s="5" t="s">
         <v>989</v>
       </c>
-      <c r="C315" t="s">
+      <c r="C315" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E315" t="s">
+      <c r="D315" s="5"/>
+      <c r="E315" s="5" t="s">
         <v>655</v>
       </c>
-      <c r="F315" t="s">
+      <c r="F315" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="G315" t="s">
+      <c r="G315" s="5" t="s">
         <v>987</v>
       </c>
     </row>
     <row r="316" spans="1:7">
-      <c r="A316" t="s">
+      <c r="A316" s="5" t="s">
         <v>990</v>
       </c>
-      <c r="B316" t="s">
+      <c r="B316" s="5" t="s">
         <v>991</v>
       </c>
-      <c r="C316" t="s">
+      <c r="C316" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="D316" t="s">
+      <c r="D316" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="E316" t="s">
+      <c r="E316" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="F316" t="s">
+      <c r="F316" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="G316" t="s">
+      <c r="G316" s="5" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="317" spans="1:7">
-      <c r="A317" t="s">
+      <c r="A317" s="5" t="s">
         <v>992</v>
       </c>
-      <c r="B317" t="s">
+      <c r="B317" s="5" t="s">
         <v>993</v>
       </c>
-      <c r="C317" t="s">
+      <c r="C317" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="E317" t="s">
+      <c r="D317" s="5"/>
+      <c r="E317" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="F317" t="s">
+      <c r="F317" s="5" t="s">
         <v>359</v>
       </c>
-      <c r="G317" t="s">
+      <c r="G317" s="5" t="s">
         <v>994</v>
       </c>
     </row>
     <row r="318" spans="1:7">
-      <c r="A318" t="s">
+      <c r="A318" s="5" t="s">
         <v>995</v>
       </c>
-      <c r="B318" t="s">
+      <c r="B318" s="5" t="s">
         <v>996</v>
       </c>
-      <c r="C318" t="s">
+      <c r="C318" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="E318" t="s">
+      <c r="D318" s="5"/>
+      <c r="E318" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="F318" t="s">
+      <c r="F318" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G318" t="s">
+      <c r="G318" s="5" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="319" spans="1:7">
-      <c r="A319" t="s">
+      <c r="A319" s="5" t="s">
         <v>997</v>
       </c>
-      <c r="B319" t="s">
+      <c r="B319" s="5" t="s">
         <v>998</v>
       </c>
-      <c r="C319" t="s">
+      <c r="C319" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D319" t="s">
+      <c r="D319" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="E319" t="s">
+      <c r="E319" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="F319" t="s">
+      <c r="F319" s="5" t="s">
         <v>359</v>
       </c>
-      <c r="G319" t="s">
+      <c r="G319" s="5" t="s">
         <v>999</v>
       </c>
     </row>
     <row r="320" spans="1:7">
-      <c r="A320" t="s">
+      <c r="A320" s="5" t="s">
         <v>1000</v>
       </c>
-      <c r="B320" t="s">
+      <c r="B320" s="5" t="s">
         <v>1001</v>
       </c>
-      <c r="C320" t="s">
+      <c r="C320" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D320" t="s">
+      <c r="D320" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="E320" t="s">
+      <c r="E320" s="5" t="s">
         <v>438</v>
       </c>
-      <c r="F320" t="s">
+      <c r="F320" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="G320" t="s">
+      <c r="G320" s="5" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="321" spans="1:7">
-      <c r="A321" t="s">
+      <c r="A321" s="5" t="s">
         <v>1002</v>
       </c>
-      <c r="B321" t="s">
+      <c r="B321" s="5" t="s">
         <v>1003</v>
       </c>
-      <c r="C321" t="s">
+      <c r="C321" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E321" t="s">
+      <c r="D321" s="5"/>
+      <c r="E321" s="5" t="s">
         <v>1004</v>
       </c>
-      <c r="F321" t="s">
+      <c r="F321" s="5" t="s">
         <v>1005</v>
       </c>
-      <c r="G321" t="s">
+      <c r="G321" s="5" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="322" spans="1:7">
-      <c r="A322" t="s">
+      <c r="A322" s="5" t="s">
         <v>1006</v>
       </c>
-      <c r="B322" t="s">
+      <c r="B322" s="5" t="s">
         <v>1007</v>
       </c>
-      <c r="C322" t="s">
+      <c r="C322" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E322" t="s">
+      <c r="D322" s="5"/>
+      <c r="E322" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F322" t="s">
+      <c r="F322" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="G322" t="s">
+      <c r="G322" s="5" t="s">
         <v>1008</v>
       </c>
     </row>
     <row r="323" spans="1:7">
-      <c r="A323" t="s">
+      <c r="A323" s="5" t="s">
         <v>1009</v>
       </c>
-      <c r="B323" t="s">
+      <c r="B323" s="5" t="s">
         <v>1010</v>
       </c>
-      <c r="C323" t="s">
+      <c r="C323" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D323" t="s">
+      <c r="D323" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="E323" t="s">
+      <c r="E323" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="F323" t="s">
+      <c r="F323" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G323" t="s">
+      <c r="G323" s="5" t="s">
         <v>910</v>
       </c>
     </row>
     <row r="324" spans="1:7">
-      <c r="A324" t="s">
+      <c r="A324" s="5" t="s">
         <v>1011</v>
       </c>
-      <c r="B324" t="s">
+      <c r="B324" s="5" t="s">
         <v>1012</v>
       </c>
-      <c r="C324" t="s">
+      <c r="C324" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D324" t="s">
+      <c r="D324" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="E324" t="s">
+      <c r="E324" s="5" t="s">
         <v>438</v>
       </c>
-      <c r="F324" t="s">
+      <c r="F324" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="G324" t="s">
+      <c r="G324" s="5" t="s">
         <v>469</v>
       </c>
     </row>
     <row r="325" spans="1:7">
-      <c r="A325" t="s">
+      <c r="A325" s="5" t="s">
         <v>1013</v>
       </c>
-      <c r="B325" t="s">
+      <c r="B325" s="5" t="s">
         <v>1014</v>
       </c>
-      <c r="C325" t="s">
+      <c r="C325" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E325" t="s">
+      <c r="D325" s="5"/>
+      <c r="E325" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="F325" t="s">
+      <c r="F325" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="G325" t="s">
+      <c r="G325" s="5" t="s">
         <v>1015</v>
       </c>
     </row>
     <row r="326" spans="1:7">
-      <c r="A326" t="s">
+      <c r="A326" s="5" t="s">
         <v>1016</v>
       </c>
-      <c r="B326" t="s">
+      <c r="B326" s="5" t="s">
         <v>1017</v>
       </c>
-      <c r="C326" t="s">
+      <c r="C326" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E326" t="s">
+      <c r="D326" s="5"/>
+      <c r="E326" s="5" t="s">
         <v>351</v>
       </c>
-      <c r="F326" t="s">
+      <c r="F326" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G326" t="s">
+      <c r="G326" s="5" t="s">
         <v>1018</v>
       </c>
     </row>
     <row r="327" spans="1:7">
-      <c r="A327" t="s">
+      <c r="A327" s="5" t="s">
         <v>1019</v>
       </c>
-      <c r="B327" t="s">
+      <c r="B327" s="5" t="s">
         <v>1020</v>
       </c>
-      <c r="C327" t="s">
+      <c r="C327" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E327" t="s">
+      <c r="D327" s="5"/>
+      <c r="E327" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="F327" t="s">
+      <c r="F327" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="G327" t="s">
+      <c r="G327" s="5" t="s">
         <v>1021</v>
       </c>
     </row>
     <row r="328" spans="1:7">
-      <c r="A328" t="s">
+      <c r="A328" s="5" t="s">
         <v>1022</v>
       </c>
-      <c r="B328" t="s">
+      <c r="B328" s="5" t="s">
         <v>1023</v>
       </c>
-      <c r="C328" t="s">
+      <c r="C328" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="E328" t="s">
+      <c r="D328" s="5"/>
+      <c r="E328" s="5" t="s">
         <v>933</v>
       </c>
-      <c r="F328" t="s">
+      <c r="F328" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G328" t="s">
+      <c r="G328" s="5" t="s">
         <v>676</v>
       </c>
     </row>
     <row r="329" spans="1:7">
-      <c r="A329" t="s">
+      <c r="A329" s="5" t="s">
         <v>1024</v>
       </c>
-      <c r="B329" t="s">
+      <c r="B329" s="5" t="s">
         <v>1025</v>
       </c>
-      <c r="C329" t="s">
+      <c r="C329" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="E329" t="s">
+      <c r="D329" s="5"/>
+      <c r="E329" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="F329" t="s">
+      <c r="F329" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G329" t="s">
+      <c r="G329" s="5" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="330" spans="1:7">
-      <c r="A330" t="s">
+      <c r="A330" s="5" t="s">
         <v>1026</v>
       </c>
-      <c r="B330" t="s">
+      <c r="B330" s="5" t="s">
         <v>1027</v>
       </c>
-      <c r="C330" t="s">
+      <c r="C330" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="D330" t="s">
+      <c r="D330" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="E330" t="s">
+      <c r="E330" s="5" t="s">
         <v>638</v>
       </c>
-      <c r="F330" t="s">
+      <c r="F330" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G330" t="s">
+      <c r="G330" s="5" t="s">
         <v>1028</v>
       </c>
     </row>
     <row r="331" spans="1:7">
-      <c r="A331" t="s">
+      <c r="A331" s="5" t="s">
         <v>1029</v>
       </c>
-      <c r="B331" t="s">
+      <c r="B331" s="5" t="s">
         <v>1030</v>
       </c>
-      <c r="C331" t="s">
+      <c r="C331" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="D331" t="s">
+      <c r="D331" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="E331" t="s">
+      <c r="E331" s="5" t="s">
         <v>1031</v>
       </c>
-      <c r="F331" t="s">
-        <v>8</v>
-      </c>
-      <c r="G331" t="s">
+      <c r="F331" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G331" s="5" t="s">
         <v>1032</v>
       </c>
     </row>
     <row r="332" spans="1:7">
-      <c r="A332" t="s">
+      <c r="A332" s="5" t="s">
         <v>1033</v>
       </c>
-      <c r="B332" t="s">
+      <c r="B332" s="5" t="s">
         <v>1034</v>
       </c>
-      <c r="C332" t="s">
+      <c r="C332" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="E332" t="s">
+      <c r="D332" s="5"/>
+      <c r="E332" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="F332" t="s">
+      <c r="F332" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G332" t="s">
+      <c r="G332" s="5" t="s">
         <v>1035</v>
       </c>
     </row>
     <row r="333" spans="1:7">
-      <c r="A333" t="s">
+      <c r="A333" s="5" t="s">
         <v>1036</v>
       </c>
-      <c r="B333" t="s">
+      <c r="B333" s="5" t="s">
         <v>1037</v>
       </c>
-      <c r="C333" t="s">
+      <c r="C333" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="D333" t="s">
+      <c r="D333" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="E333" t="s">
+      <c r="E333" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="F333" t="s">
+      <c r="F333" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="G333" t="s">
+      <c r="G333" s="5" t="s">
         <v>1038</v>
       </c>
     </row>
     <row r="334" spans="1:7">
-      <c r="A334" t="s">
+      <c r="A334" s="5" t="s">
         <v>1039</v>
       </c>
-      <c r="B334" t="s">
+      <c r="B334" s="5" t="s">
         <v>1040</v>
       </c>
-      <c r="C334" t="s">
+      <c r="C334" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D334" t="s">
+      <c r="D334" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E334" t="s">
+      <c r="E334" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F334" t="s">
+      <c r="F334" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G334" t="s">
+      <c r="G334" s="5" t="s">
         <v>926</v>
       </c>
     </row>
     <row r="335" spans="1:7">
-      <c r="A335" t="s">
+      <c r="A335" s="5" t="s">
         <v>1041</v>
       </c>
-      <c r="B335" t="s">
+      <c r="B335" s="5" t="s">
         <v>1042</v>
       </c>
-      <c r="C335" t="s">
+      <c r="C335" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="D335" t="s">
+      <c r="D335" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E335" t="s">
+      <c r="E335" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="F335" t="s">
-        <v>8</v>
-      </c>
-      <c r="G335" t="s">
+      <c r="F335" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G335" s="5" t="s">
         <v>1043</v>
       </c>
     </row>
     <row r="336" spans="1:7">
-      <c r="A336" t="s">
+      <c r="A336" s="5" t="s">
         <v>1044</v>
       </c>
-      <c r="B336" t="s">
+      <c r="B336" s="5" t="s">
         <v>1045</v>
       </c>
-      <c r="C336" t="s">
+      <c r="C336" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="E336" t="s">
+      <c r="D336" s="5"/>
+      <c r="E336" s="5" t="s">
         <v>922</v>
       </c>
-      <c r="F336" t="s">
+      <c r="F336" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="G336" t="s">
+      <c r="G336" s="5" t="s">
         <v>1046</v>
       </c>
     </row>
     <row r="337" spans="1:7">
-      <c r="A337" t="s">
+      <c r="A337" s="5" t="s">
         <v>1047</v>
       </c>
-      <c r="B337" t="s">
+      <c r="B337" s="5" t="s">
         <v>1048</v>
       </c>
-      <c r="C337" t="s">
+      <c r="C337" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="E337" t="s">
+      <c r="D337" s="5"/>
+      <c r="E337" s="5" t="s">
         <v>922</v>
       </c>
-      <c r="F337" t="s">
+      <c r="F337" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="G337" t="s">
+      <c r="G337" s="5" t="s">
         <v>1049</v>
       </c>
     </row>
     <row r="338" spans="1:7">
-      <c r="A338" t="s">
+      <c r="A338" s="5" t="s">
         <v>1050</v>
       </c>
-      <c r="B338" t="s">
+      <c r="B338" s="5" t="s">
         <v>1051</v>
       </c>
-      <c r="C338" t="s">
+      <c r="C338" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="D338" t="s">
+      <c r="D338" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E338" t="s">
+      <c r="E338" s="5" t="s">
         <v>438</v>
       </c>
-      <c r="F338" t="s">
-        <v>8</v>
-      </c>
-      <c r="G338" t="s">
+      <c r="F338" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G338" s="5" t="s">
         <v>1052</v>
       </c>
     </row>
     <row r="339" spans="1:7">
-      <c r="A339" t="s">
+      <c r="A339" s="5" t="s">
         <v>1053</v>
       </c>
-      <c r="B339" t="s">
+      <c r="B339" s="5" t="s">
         <v>1054</v>
       </c>
-      <c r="C339" t="s">
+      <c r="C339" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="D339" t="s">
+      <c r="D339" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E339" t="s">
+      <c r="E339" s="5" t="s">
         <v>438</v>
       </c>
-      <c r="F339" t="s">
-        <v>8</v>
-      </c>
-      <c r="G339" t="s">
+      <c r="F339" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G339" s="5" t="s">
         <v>1055</v>
       </c>
     </row>
     <row r="340" spans="1:7">
-      <c r="A340" t="s">
+      <c r="A340" s="5" t="s">
         <v>1056</v>
       </c>
-      <c r="B340" t="s">
+      <c r="B340" s="5" t="s">
         <v>1057</v>
       </c>
-      <c r="C340" t="s">
+      <c r="C340" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D340" t="s">
+      <c r="D340" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="E340" t="s">
+      <c r="E340" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="F340" t="s">
+      <c r="F340" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G340" t="s">
+      <c r="G340" s="5" t="s">
         <v>1058</v>
       </c>
     </row>
     <row r="341" spans="1:7">
-      <c r="A341" t="s">
+      <c r="A341" s="5" t="s">
         <v>1059</v>
       </c>
-      <c r="B341" t="s">
+      <c r="B341" s="5" t="s">
         <v>1060</v>
       </c>
-      <c r="C341" t="s">
+      <c r="C341" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D341" t="s">
+      <c r="D341" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="E341" t="s">
+      <c r="E341" s="5" t="s">
         <v>1061</v>
       </c>
-      <c r="F341" t="s">
+      <c r="F341" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G341" t="s">
+      <c r="G341" s="5" t="s">
         <v>1062</v>
       </c>
     </row>
     <row r="342" spans="1:7">
-      <c r="A342" t="s">
+      <c r="A342" s="5" t="s">
         <v>1063</v>
       </c>
-      <c r="B342" t="s">
+      <c r="B342" s="5" t="s">
         <v>1064</v>
       </c>
-      <c r="C342" t="s">
+      <c r="C342" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E342" t="s">
+      <c r="D342" s="5"/>
+      <c r="E342" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F342" t="s">
+      <c r="F342" s="5" t="s">
         <v>1065</v>
       </c>
-      <c r="G342" t="s">
+      <c r="G342" s="5" t="s">
         <v>495</v>
       </c>
     </row>
     <row r="343" spans="1:7">
-      <c r="A343" t="s">
+      <c r="A343" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B343" t="s">
+      <c r="B343" s="5" t="s">
         <v>1067</v>
       </c>
-      <c r="C343" t="s">
+      <c r="C343" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D343" t="s">
+      <c r="D343" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="E343" t="s">
+      <c r="E343" s="5" t="s">
         <v>1061</v>
       </c>
-      <c r="F343" t="s">
+      <c r="F343" s="5" t="s">
         <v>1068</v>
       </c>
-      <c r="G343" t="s">
+      <c r="G343" s="5" t="s">
         <v>1069</v>
       </c>
     </row>
     <row r="344" spans="1:7">
-      <c r="A344" t="s">
+      <c r="A344" s="5" t="s">
         <v>1070</v>
       </c>
-      <c r="B344" t="s">
+      <c r="B344" s="5" t="s">
         <v>1071</v>
       </c>
-      <c r="C344" t="s">
+      <c r="C344" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="D344" t="s">
+      <c r="D344" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E344" t="s">
+      <c r="E344" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="F344" t="s">
+      <c r="F344" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G344" t="s">
+      <c r="G344" s="5" t="s">
         <v>1072</v>
       </c>
     </row>
     <row r="345" spans="1:7">
-      <c r="A345" t="s">
+      <c r="A345" s="5" t="s">
         <v>1073</v>
       </c>
-      <c r="B345" t="s">
+      <c r="B345" s="5" t="s">
         <v>1074</v>
       </c>
-      <c r="C345" t="s">
+      <c r="C345" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="D345" t="s">
+      <c r="D345" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E345" t="s">
+      <c r="E345" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F345" t="s">
+      <c r="F345" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="G345" t="s">
+      <c r="G345" s="5" t="s">
         <v>1075</v>
       </c>
     </row>
     <row r="346" spans="1:7">
-      <c r="A346" t="s">
+      <c r="A346" s="5" t="s">
         <v>1076</v>
       </c>
-      <c r="B346" t="s">
+      <c r="B346" s="5" t="s">
         <v>1077</v>
       </c>
-      <c r="C346" t="s">
+      <c r="C346" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="D346" t="s">
+      <c r="D346" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="E346" t="s">
+      <c r="E346" s="5" t="s">
         <v>490</v>
       </c>
-      <c r="F346" t="s">
-        <v>8</v>
-      </c>
-      <c r="G346" t="s">
+      <c r="F346" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G346" s="5" t="s">
         <v>1078</v>
       </c>
     </row>
     <row r="347" spans="1:7">
-      <c r="A347" t="s">
+      <c r="A347" s="5" t="s">
         <v>1079</v>
       </c>
-      <c r="B347" t="s">
+      <c r="B347" s="5" t="s">
         <v>1080</v>
       </c>
-      <c r="C347" t="s">
+      <c r="C347" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="D347" t="s">
+      <c r="D347" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="E347" t="s">
+      <c r="E347" s="5" t="s">
         <v>452</v>
       </c>
-      <c r="F347" t="s">
-        <v>8</v>
-      </c>
-      <c r="G347" t="s">
+      <c r="F347" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G347" s="5" t="s">
         <v>1081</v>
       </c>
     </row>
     <row r="348" spans="1:7">
-      <c r="A348" t="s">
+      <c r="A348" s="5" t="s">
         <v>1082</v>
       </c>
-      <c r="B348" t="s">
+      <c r="B348" s="5" t="s">
         <v>1083</v>
       </c>
-      <c r="C348" t="s">
+      <c r="C348" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="D348" t="s">
+      <c r="D348" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E348" t="s">
+      <c r="E348" s="5" t="s">
         <v>490</v>
       </c>
-      <c r="F348" t="s">
-        <v>8</v>
-      </c>
-      <c r="G348" t="s">
+      <c r="F348" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G348" s="5" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="349" spans="1:7">
-      <c r="A349" t="s">
+      <c r="A349" s="5" t="s">
         <v>1084</v>
       </c>
-      <c r="B349" t="s">
+      <c r="B349" s="5" t="s">
         <v>1085</v>
       </c>
-      <c r="C349" t="s">
+      <c r="C349" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="D349" t="s">
+      <c r="D349" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E349" t="s">
+      <c r="E349" s="5" t="s">
         <v>452</v>
       </c>
-      <c r="F349" t="s">
-        <v>8</v>
-      </c>
-      <c r="G349" t="s">
+      <c r="F349" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G349" s="5" t="s">
         <v>1086</v>
       </c>
     </row>
     <row r="350" spans="1:7">
-      <c r="A350" t="s">
+      <c r="A350" s="5" t="s">
         <v>1087</v>
       </c>
-      <c r="B350" t="s">
+      <c r="B350" s="5" t="s">
         <v>1088</v>
       </c>
-      <c r="C350" t="s">
+      <c r="C350" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E350" t="s">
+      <c r="D350" s="5"/>
+      <c r="E350" s="5" t="s">
         <v>461</v>
       </c>
-      <c r="F350" t="s">
+      <c r="F350" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G350" t="s">
+      <c r="G350" s="5" t="s">
         <v>1089</v>
       </c>
     </row>
     <row r="351" spans="1:7">
-      <c r="A351" t="s">
+      <c r="A351" s="5" t="s">
         <v>1090</v>
       </c>
-      <c r="B351" t="s">
+      <c r="B351" s="5" t="s">
         <v>1091</v>
       </c>
-      <c r="C351" t="s">
+      <c r="C351" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E351" t="s">
+      <c r="D351" s="5"/>
+      <c r="E351" s="5" t="s">
         <v>464</v>
       </c>
-      <c r="F351" t="s">
+      <c r="F351" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="G351" t="s">
+      <c r="G351" s="5" t="s">
         <v>1092</v>
       </c>
     </row>
     <row r="352" spans="1:7">
-      <c r="A352" t="s">
+      <c r="A352" s="5" t="s">
         <v>1093</v>
       </c>
-      <c r="B352" t="s">
+      <c r="B352" s="5" t="s">
         <v>1094</v>
       </c>
-      <c r="C352" t="s">
+      <c r="C352" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="E352" t="s">
+      <c r="D352" s="5"/>
+      <c r="E352" s="5" t="s">
         <v>520</v>
       </c>
-      <c r="F352" t="s">
-        <v>8</v>
-      </c>
-      <c r="G352" t="s">
+      <c r="F352" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G352" s="5" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="353" spans="1:7">
-      <c r="A353" t="s">
+      <c r="A353" s="5" t="s">
         <v>1095</v>
       </c>
-      <c r="B353" t="s">
+      <c r="B353" s="5" t="s">
         <v>1096</v>
       </c>
-      <c r="C353" t="s">
+      <c r="C353" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="E353" t="s">
+      <c r="D353" s="5"/>
+      <c r="E353" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="F353" t="s">
+      <c r="F353" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="G353" t="s">
+      <c r="G353" s="5" t="s">
         <v>1097</v>
       </c>
     </row>
     <row r="354" spans="1:7">
-      <c r="A354" t="s">
+      <c r="A354" s="5" t="s">
         <v>1098</v>
       </c>
-      <c r="B354" t="s">
+      <c r="B354" s="5" t="s">
         <v>1099</v>
       </c>
-      <c r="C354" t="s">
+      <c r="C354" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="E354" t="s">
+      <c r="D354" s="5"/>
+      <c r="E354" s="5" t="s">
         <v>420</v>
       </c>
-      <c r="F354" t="s">
+      <c r="F354" s="5" t="s">
         <v>359</v>
       </c>
-      <c r="G354" t="s">
+      <c r="G354" s="5" t="s">
         <v>879</v>
       </c>
     </row>
     <row r="355" spans="1:7">
-      <c r="A355" t="s">
+      <c r="A355" s="5" t="s">
         <v>1100</v>
       </c>
-      <c r="B355" t="s">
+      <c r="B355" s="5" t="s">
         <v>1101</v>
       </c>
-      <c r="C355" t="s">
+      <c r="C355" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="E355" t="s">
+      <c r="D355" s="5"/>
+      <c r="E355" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="F355" t="s">
-        <v>8</v>
-      </c>
-      <c r="G355" t="s">
+      <c r="F355" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G355" s="5" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="356" spans="1:7">
-      <c r="A356" t="s">
+      <c r="A356" s="5" t="s">
         <v>1102</v>
       </c>
-      <c r="B356" t="s">
+      <c r="B356" s="5" t="s">
         <v>1103</v>
       </c>
-      <c r="C356" t="s">
+      <c r="C356" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="E356" t="s">
+      <c r="D356" s="5"/>
+      <c r="E356" s="5" t="s">
         <v>420</v>
       </c>
-      <c r="F356" t="s">
+      <c r="F356" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G356" t="s">
+      <c r="G356" s="5" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="357" spans="1:7">
-      <c r="A357" t="s">
+      <c r="A357" s="5" t="s">
         <v>1104</v>
       </c>
-      <c r="B357" t="s">
+      <c r="B357" s="5" t="s">
         <v>1105</v>
       </c>
-      <c r="C357" t="s">
+      <c r="C357" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="E357" t="s">
+      <c r="D357" s="5"/>
+      <c r="E357" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="F357" t="s">
+      <c r="F357" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="G357" t="s">
+      <c r="G357" s="5" t="s">
         <v>1018</v>
       </c>
     </row>
     <row r="358" spans="1:7">
-      <c r="A358" t="s">
+      <c r="A358" s="5" t="s">
         <v>1106</v>
       </c>
-      <c r="B358" t="s">
+      <c r="B358" s="5" t="s">
         <v>1107</v>
       </c>
-      <c r="C358" t="s">
+      <c r="C358" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="D358" t="s">
+      <c r="D358" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E358" t="s">
+      <c r="E358" s="5" t="s">
         <v>438</v>
       </c>
-      <c r="F358" t="s">
+      <c r="F358" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="G358" t="s">
+      <c r="G358" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="359" spans="1:7">
-      <c r="A359" t="s">
+      <c r="A359" s="5" t="s">
         <v>1108</v>
       </c>
-      <c r="B359" t="s">
+      <c r="B359" s="5" t="s">
         <v>1109</v>
       </c>
-      <c r="C359" t="s">
+      <c r="C359" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E359" t="s">
+      <c r="D359" s="5"/>
+      <c r="E359" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="F359" t="s">
-        <v>8</v>
-      </c>
-      <c r="G359" t="s">
+      <c r="F359" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G359" s="5" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="360" spans="1:7">
-      <c r="A360" t="s">
+      <c r="A360" s="5" t="s">
         <v>1110</v>
       </c>
-      <c r="B360" t="s">
+      <c r="B360" s="5" t="s">
         <v>1111</v>
       </c>
-      <c r="C360" t="s">
+      <c r="C360" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="E360" t="s">
+      <c r="D360" s="5"/>
+      <c r="E360" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="F360" t="s">
+      <c r="F360" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="G360" t="s">
+      <c r="G360" s="5" t="s">
         <v>1112</v>
       </c>
     </row>
     <row r="361" spans="1:7">
-      <c r="A361" t="s">
+      <c r="A361" s="5" t="s">
         <v>1113</v>
       </c>
-      <c r="B361" t="s">
+      <c r="B361" s="5" t="s">
         <v>1114</v>
       </c>
-      <c r="C361" t="s">
+      <c r="C361" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E361" t="s">
+      <c r="D361" s="5"/>
+      <c r="E361" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="F361" t="s">
+      <c r="F361" s="5" t="s">
         <v>1005</v>
       </c>
-      <c r="G361" t="s">
+      <c r="G361" s="5" t="s">
         <v>690</v>
       </c>
     </row>
     <row r="362" spans="1:7">
-      <c r="A362" t="s">
+      <c r="A362" s="5" t="s">
         <v>1115</v>
       </c>
-      <c r="B362" t="s">
+      <c r="B362" s="5" t="s">
         <v>1116</v>
       </c>
-      <c r="C362" t="s">
+      <c r="C362" s="5" t="s">
         <v>1117</v>
       </c>
-      <c r="E362" t="s">
+      <c r="D362" s="5"/>
+      <c r="E362" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="F362" t="s">
+      <c r="F362" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G362" t="s">
+      <c r="G362" s="5" t="s">
         <v>1118</v>
       </c>
     </row>
     <row r="363" spans="1:7">
-      <c r="A363" t="s">
+      <c r="A363" s="5" t="s">
         <v>1119</v>
       </c>
-      <c r="B363" t="s">
+      <c r="B363" s="5" t="s">
         <v>1120</v>
       </c>
-      <c r="C363" t="s">
+      <c r="C363" s="5" t="s">
         <v>1117</v>
       </c>
-      <c r="E363" t="s">
+      <c r="D363" s="5"/>
+      <c r="E363" s="5" t="s">
         <v>737</v>
       </c>
-      <c r="F363" t="s">
+      <c r="F363" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G363" t="s">
+      <c r="G363" s="5" t="s">
         <v>1121</v>
       </c>
     </row>
     <row r="364" spans="1:7">
-      <c r="A364" t="s">
+      <c r="A364" s="5" t="s">
         <v>1122</v>
       </c>
-      <c r="B364" t="s">
+      <c r="B364" s="5" t="s">
         <v>1123</v>
       </c>
-      <c r="C364" t="s">
+      <c r="C364" s="5" t="s">
         <v>1117</v>
       </c>
-      <c r="D364" t="s">
+      <c r="D364" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E364" t="s">
+      <c r="E364" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="F364" t="s">
+      <c r="F364" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G364" t="s">
+      <c r="G364" s="5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="365" spans="1:7">
-      <c r="A365" t="s">
+      <c r="A365" s="5" t="s">
         <v>1124</v>
       </c>
-      <c r="B365" t="s">
+      <c r="B365" s="5" t="s">
         <v>1125</v>
       </c>
-      <c r="C365" t="s">
+      <c r="C365" s="5" t="s">
         <v>1117</v>
       </c>
-      <c r="D365" t="s">
+      <c r="D365" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E365" t="s">
+      <c r="E365" s="5" t="s">
         <v>628</v>
       </c>
-      <c r="F365" t="s">
+      <c r="F365" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G365" t="s">
+      <c r="G365" s="5" t="s">
         <v>1126</v>
       </c>
     </row>
     <row r="366" spans="1:7">
-      <c r="A366" t="s">
+      <c r="A366" s="5" t="s">
         <v>1127</v>
       </c>
-      <c r="B366" t="s">
+      <c r="B366" s="5" t="s">
         <v>1128</v>
       </c>
-      <c r="C366" t="s">
+      <c r="C366" s="5" t="s">
         <v>1117</v>
       </c>
-      <c r="D366" t="s">
+      <c r="D366" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E366" t="s">
+      <c r="E366" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F366" t="s">
-        <v>8</v>
-      </c>
-      <c r="G366" t="s">
+      <c r="F366" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G366" s="5" t="s">
         <v>1129</v>
       </c>
     </row>
     <row r="367" spans="1:7">
-      <c r="A367" t="s">
+      <c r="A367" s="5" t="s">
         <v>1130</v>
       </c>
-      <c r="B367" t="s">
+      <c r="B367" s="5" t="s">
         <v>1131</v>
       </c>
-      <c r="C367" t="s">
+      <c r="C367" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E367" t="s">
+      <c r="D367" s="5"/>
+      <c r="E367" s="5" t="s">
         <v>400</v>
       </c>
-      <c r="F367" t="s">
+      <c r="F367" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G367" t="s">
+      <c r="G367" s="5" t="s">
         <v>1049</v>
       </c>
     </row>
     <row r="368" spans="1:7">
-      <c r="A368" t="s">
+      <c r="A368" s="5" t="s">
         <v>1132</v>
       </c>
-      <c r="B368" t="s">
+      <c r="B368" s="5" t="s">
         <v>1133</v>
       </c>
-      <c r="C368" t="s">
+      <c r="C368" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E368" t="s">
+      <c r="D368" s="5"/>
+      <c r="E368" s="5" t="s">
         <v>404</v>
       </c>
-      <c r="F368" t="s">
+      <c r="F368" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="G368" t="s">
+      <c r="G368" s="5" t="s">
         <v>662</v>
       </c>
     </row>
     <row r="369" spans="1:7">
-      <c r="A369" t="s">
+      <c r="A369" s="5" t="s">
         <v>1134</v>
       </c>
-      <c r="B369" t="s">
+      <c r="B369" s="5" t="s">
         <v>1135</v>
       </c>
-      <c r="C369" t="s">
+      <c r="C369" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E369" t="s">
+      <c r="D369" s="5"/>
+      <c r="E369" s="5" t="s">
         <v>404</v>
       </c>
-      <c r="F369" t="s">
+      <c r="F369" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="G369" t="s">
+      <c r="G369" s="5" t="s">
         <v>1136</v>
       </c>
     </row>
     <row r="370" spans="1:7">
-      <c r="A370" t="s">
+      <c r="A370" s="5" t="s">
         <v>1137</v>
       </c>
-      <c r="B370" t="s">
+      <c r="B370" s="5" t="s">
         <v>1138</v>
       </c>
-      <c r="C370" t="s">
+      <c r="C370" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D370" t="s">
+      <c r="D370" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="E370" t="s">
+      <c r="E370" s="5" t="s">
         <v>404</v>
       </c>
-      <c r="F370" t="s">
+      <c r="F370" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="G370" t="s">
+      <c r="G370" s="5" t="s">
         <v>1139</v>
       </c>
     </row>
     <row r="371" spans="1:7">
-      <c r="A371" t="s">
+      <c r="A371" s="5" t="s">
         <v>1140</v>
       </c>
-      <c r="B371" t="s">
+      <c r="B371" s="5" t="s">
         <v>1141</v>
       </c>
-      <c r="C371" t="s">
+      <c r="C371" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E371" t="s">
+      <c r="D371" s="5"/>
+      <c r="E371" s="5" t="s">
         <v>740</v>
       </c>
-      <c r="F371" t="s">
+      <c r="F371" s="5" t="s">
         <v>359</v>
       </c>
-      <c r="G371" t="s">
+      <c r="G371" s="5" t="s">
         <v>1142</v>
       </c>
     </row>
     <row r="372" spans="1:7">
-      <c r="A372" t="s">
+      <c r="A372" s="5" t="s">
         <v>1143</v>
       </c>
-      <c r="B372" t="s">
+      <c r="B372" s="5" t="s">
         <v>1144</v>
       </c>
-      <c r="C372" t="s">
+      <c r="C372" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="E372" t="s">
+      <c r="D372" s="5"/>
+      <c r="E372" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="F372" t="s">
-        <v>8</v>
-      </c>
-      <c r="G372" t="s">
+      <c r="F372" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G372" s="5" t="s">
         <v>1145</v>
       </c>
     </row>
     <row r="373" spans="1:7">
-      <c r="A373" t="s">
+      <c r="A373" s="5" t="s">
         <v>1146</v>
       </c>
-      <c r="B373" t="s">
+      <c r="B373" s="5" t="s">
         <v>1147</v>
       </c>
-      <c r="C373" t="s">
+      <c r="C373" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="E373" t="s">
+      <c r="D373" s="5"/>
+      <c r="E373" s="5" t="s">
         <v>520</v>
       </c>
-      <c r="F373" t="s">
-        <v>8</v>
-      </c>
-      <c r="G373" t="s">
+      <c r="F373" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G373" s="5" t="s">
         <v>1148</v>
       </c>
     </row>
     <row r="374" spans="1:7">
-      <c r="A374" t="s">
+      <c r="A374" s="5" t="s">
         <v>1149</v>
       </c>
-      <c r="B374" t="s">
+      <c r="B374" s="5" t="s">
         <v>1150</v>
       </c>
-      <c r="C374" t="s">
+      <c r="C374" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="D374" t="s">
+      <c r="D374" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E374" t="s">
+      <c r="E374" s="5" t="s">
         <v>524</v>
       </c>
-      <c r="F374" t="s">
-        <v>8</v>
-      </c>
-      <c r="G374" t="s">
+      <c r="F374" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G374" s="5" t="s">
         <v>1151</v>
       </c>
     </row>
     <row r="375" spans="1:7">
-      <c r="A375" t="s">
+      <c r="A375" s="5" t="s">
         <v>1152</v>
       </c>
-      <c r="B375" t="s">
+      <c r="B375" s="5" t="s">
         <v>1153</v>
       </c>
-      <c r="C375" t="s">
+      <c r="C375" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="D375" t="s">
+      <c r="D375" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E375" t="s">
+      <c r="E375" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="F375" t="s">
+      <c r="F375" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G375" t="s">
+      <c r="G375" s="5" t="s">
         <v>1154</v>
       </c>
     </row>
     <row r="376" spans="1:7">
-      <c r="A376" t="s">
+      <c r="A376" s="5" t="s">
         <v>1155</v>
       </c>
-      <c r="B376" t="s">
+      <c r="B376" s="5" t="s">
         <v>1156</v>
       </c>
-      <c r="C376" t="s">
+      <c r="C376" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="D376" t="s">
+      <c r="D376" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E376" t="s">
+      <c r="E376" s="5" t="s">
         <v>520</v>
       </c>
-      <c r="F376" t="s">
+      <c r="F376" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G376" t="s">
+      <c r="G376" s="5" t="s">
         <v>1157</v>
       </c>
     </row>
     <row r="377" spans="1:7">
-      <c r="A377" t="s">
+      <c r="A377" s="5" t="s">
         <v>1158</v>
       </c>
-      <c r="B377" t="s">
+      <c r="B377" s="5" t="s">
         <v>1159</v>
       </c>
-      <c r="C377" t="s">
+      <c r="C377" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="D377" t="s">
+      <c r="D377" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E377" t="s">
+      <c r="E377" s="5" t="s">
         <v>814</v>
       </c>
-      <c r="F377" t="s">
+      <c r="F377" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G377" t="s">
+      <c r="G377" s="5" t="s">
         <v>1160</v>
       </c>
     </row>
     <row r="378" spans="1:7">
-      <c r="A378" t="s">
+      <c r="A378" s="5" t="s">
         <v>1161</v>
       </c>
-      <c r="B378" t="s">
+      <c r="B378" s="5" t="s">
         <v>1162</v>
       </c>
-      <c r="C378" t="s">
+      <c r="C378" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="E378" t="s">
+      <c r="D378" s="5"/>
+      <c r="E378" s="5" t="s">
         <v>789</v>
       </c>
-      <c r="F378" t="s">
+      <c r="F378" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G378" t="s">
+      <c r="G378" s="5" t="s">
         <v>1163</v>
       </c>
     </row>
     <row r="379" spans="1:7">
-      <c r="A379" t="s">
+      <c r="A379" s="5" t="s">
         <v>1164</v>
       </c>
-      <c r="B379" t="s">
+      <c r="B379" s="5" t="s">
         <v>1165</v>
       </c>
-      <c r="C379" t="s">
+      <c r="C379" s="5" t="s">
         <v>1117</v>
       </c>
-      <c r="E379" t="s">
+      <c r="D379" s="5"/>
+      <c r="E379" s="5" t="s">
         <v>789</v>
       </c>
-      <c r="F379" t="s">
+      <c r="F379" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G379" t="s">
+      <c r="G379" s="5" t="s">
         <v>1166</v>
       </c>
     </row>
     <row r="380" spans="1:7">
-      <c r="A380" t="s">
+      <c r="A380" s="5" t="s">
         <v>1167</v>
       </c>
-      <c r="B380" t="s">
+      <c r="B380" s="5" t="s">
         <v>1168</v>
       </c>
-      <c r="C380" t="s">
+      <c r="C380" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="E380" t="s">
+      <c r="D380" s="5"/>
+      <c r="E380" s="5" t="s">
         <v>789</v>
       </c>
-      <c r="F380" t="s">
+      <c r="F380" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G380" t="s">
+      <c r="G380" s="5" t="s">
         <v>1170</v>
       </c>
     </row>
     <row r="381" spans="1:7">
-      <c r="A381" t="s">
+      <c r="A381" s="5" t="s">
         <v>1171</v>
       </c>
-      <c r="B381" t="s">
+      <c r="B381" s="5" t="s">
         <v>1172</v>
       </c>
-      <c r="C381" t="s">
+      <c r="C381" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="D381" t="s">
+      <c r="D381" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E381" t="s">
+      <c r="E381" s="5" t="s">
         <v>814</v>
       </c>
-      <c r="F381" t="s">
+      <c r="F381" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G381" t="s">
+      <c r="G381" s="5" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="382" spans="1:7">
-      <c r="A382" t="s">
+      <c r="A382" s="5" t="s">
         <v>1173</v>
       </c>
-      <c r="B382" t="s">
+      <c r="B382" s="5" t="s">
         <v>1174</v>
       </c>
-      <c r="C382" t="s">
+      <c r="C382" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="D382" t="s">
+      <c r="D382" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E382" t="s">
+      <c r="E382" s="5" t="s">
         <v>814</v>
       </c>
-      <c r="F382" t="s">
+      <c r="F382" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G382" t="s">
+      <c r="G382" s="5" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="383" spans="1:7">
-      <c r="A383" t="s">
+      <c r="A383" s="5" t="s">
         <v>1175</v>
       </c>
-      <c r="B383" t="s">
+      <c r="B383" s="5" t="s">
         <v>1176</v>
       </c>
-      <c r="C383" t="s">
+      <c r="C383" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E383" t="s">
+      <c r="D383" s="5"/>
+      <c r="E383" s="5" t="s">
         <v>1177</v>
       </c>
-      <c r="F383" t="s">
+      <c r="F383" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G383" t="s">
+      <c r="G383" s="5" t="s">
         <v>1178</v>
       </c>
     </row>
     <row r="384" spans="1:7">
-      <c r="A384" t="s">
+      <c r="A384" s="5" t="s">
         <v>1179</v>
       </c>
-      <c r="B384" t="s">
+      <c r="B384" s="5" t="s">
         <v>1180</v>
       </c>
-      <c r="C384" t="s">
+      <c r="C384" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="E384" t="s">
+      <c r="D384" s="5"/>
+      <c r="E384" s="5" t="s">
         <v>1177</v>
       </c>
-      <c r="F384" t="s">
+      <c r="F384" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G384" t="s">
+      <c r="G384" s="5" t="s">
         <v>1181</v>
       </c>
     </row>
     <row r="385" spans="1:7">
-      <c r="A385" t="s">
+      <c r="A385" s="5" t="s">
         <v>1182</v>
       </c>
-      <c r="B385" t="s">
+      <c r="B385" s="5" t="s">
         <v>1183</v>
       </c>
-      <c r="C385" t="s">
+      <c r="C385" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="D385" t="s">
+      <c r="D385" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E385" t="s">
+      <c r="E385" s="5" t="s">
         <v>527</v>
       </c>
-      <c r="F385" t="s">
-        <v>8</v>
-      </c>
-      <c r="G385" t="s">
+      <c r="F385" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G385" s="5" t="s">
         <v>1184</v>
       </c>
     </row>
     <row r="386" spans="1:7">
-      <c r="A386" t="s">
+      <c r="A386" s="5" t="s">
         <v>1185</v>
       </c>
-      <c r="B386" t="s">
+      <c r="B386" s="5" t="s">
         <v>1186</v>
       </c>
-      <c r="C386" t="s">
+      <c r="C386" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="D386" t="s">
+      <c r="D386" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E386" t="s">
+      <c r="E386" s="5" t="s">
         <v>814</v>
       </c>
-      <c r="F386" t="s">
+      <c r="F386" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G386" t="s">
+      <c r="G386" s="5" t="s">
         <v>1187</v>
       </c>
     </row>
     <row r="387" spans="1:7">
-      <c r="A387" t="s">
+      <c r="A387" s="5" t="s">
         <v>1188</v>
       </c>
-      <c r="B387" t="s">
+      <c r="B387" s="5" t="s">
         <v>1189</v>
       </c>
-      <c r="C387" t="s">
+      <c r="C387" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E387" t="s">
+      <c r="D387" s="5"/>
+      <c r="E387" s="5" t="s">
         <v>814</v>
       </c>
-      <c r="F387" t="s">
+      <c r="F387" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G387" t="s">
+      <c r="G387" s="5" t="s">
         <v>1190</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adcionado +59 Pokémon da 3ª Geração
</commit_message>
<xml_diff>
--- a/pokemonv2/pokemons.xlsx
+++ b/pokemonv2/pokemons.xlsx
@@ -8713,11 +8713,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1026"/>
+  <dimension ref="A1:H1026"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A265" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A273" sqref="A273"/>
+      <pane ySplit="1" topLeftCell="A323" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C331" sqref="C331"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14693,1303 +14693,1304 @@
       </c>
     </row>
     <row r="273" spans="1:7">
-      <c r="A273" s="5" t="s">
+      <c r="A273" s="2" t="s">
         <v>867</v>
       </c>
-      <c r="B273" s="5" t="s">
+      <c r="B273" s="2" t="s">
         <v>868</v>
       </c>
-      <c r="C273" s="5" t="s">
+      <c r="C273" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D273" s="5" t="s">
+      <c r="D273" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="E273" s="5" t="s">
+      <c r="E273" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F273" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G273" s="5" t="s">
+      <c r="F273" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G273" s="2" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="274" spans="1:7">
-      <c r="A274" s="5" t="s">
+      <c r="A274" s="2" t="s">
         <v>869</v>
       </c>
-      <c r="B274" s="5" t="s">
+      <c r="B274" s="2" t="s">
         <v>870</v>
       </c>
-      <c r="C274" s="5" t="s">
+      <c r="C274" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D274" s="5"/>
-      <c r="E274" s="5" t="s">
+      <c r="D274" s="2"/>
+      <c r="E274" s="2" t="s">
         <v>590</v>
       </c>
-      <c r="F274" s="5" t="s">
+      <c r="F274" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G274" s="5" t="s">
+      <c r="G274" s="2" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="275" spans="1:7">
-      <c r="A275" s="5" t="s">
+      <c r="A275" s="2" t="s">
         <v>871</v>
       </c>
-      <c r="B275" s="5" t="s">
+      <c r="B275" s="2" t="s">
         <v>872</v>
       </c>
-      <c r="C275" s="5" t="s">
+      <c r="C275" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D275" s="5" t="s">
+      <c r="D275" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="E275" s="5" t="s">
+      <c r="E275" s="2" t="s">
         <v>638</v>
       </c>
-      <c r="F275" s="5" t="s">
+      <c r="F275" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G275" s="5" t="s">
+      <c r="G275" s="2" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="276" spans="1:7">
-      <c r="A276" s="5" t="s">
+      <c r="A276" s="2" t="s">
         <v>873</v>
       </c>
-      <c r="B276" s="5" t="s">
+      <c r="B276" s="2" t="s">
         <v>874</v>
       </c>
-      <c r="C276" s="5" t="s">
+      <c r="C276" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D276" s="5" t="s">
+      <c r="D276" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="E276" s="5" t="s">
+      <c r="E276" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F276" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G276" s="5" t="s">
+      <c r="F276" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G276" s="2" t="s">
         <v>875</v>
       </c>
     </row>
     <row r="277" spans="1:7">
-      <c r="A277" s="5" t="s">
+      <c r="A277" s="2" t="s">
         <v>876</v>
       </c>
-      <c r="B277" s="5" t="s">
+      <c r="B277" s="2" t="s">
         <v>877</v>
       </c>
-      <c r="C277" s="5" t="s">
+      <c r="C277" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D277" s="5" t="s">
+      <c r="D277" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E277" s="5" t="s">
+      <c r="E277" s="2" t="s">
         <v>878</v>
       </c>
-      <c r="F277" s="5" t="s">
+      <c r="F277" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="G277" s="5" t="s">
+      <c r="G277" s="2" t="s">
         <v>879</v>
       </c>
     </row>
     <row r="278" spans="1:7">
-      <c r="A278" s="5" t="s">
+      <c r="A278" s="2" t="s">
         <v>880</v>
       </c>
-      <c r="B278" s="5" t="s">
+      <c r="B278" s="2" t="s">
         <v>881</v>
       </c>
-      <c r="C278" s="5" t="s">
+      <c r="C278" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D278" s="5" t="s">
+      <c r="D278" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E278" s="5" t="s">
+      <c r="E278" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="F278" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G278" s="5" t="s">
+      <c r="F278" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G278" s="2" t="s">
         <v>882</v>
       </c>
     </row>
     <row r="279" spans="1:7">
-      <c r="A279" s="5" t="s">
+      <c r="A279" s="2" t="s">
         <v>883</v>
       </c>
-      <c r="B279" s="5" t="s">
+      <c r="B279" s="2" t="s">
         <v>884</v>
       </c>
-      <c r="C279" s="5" t="s">
+      <c r="C279" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D279" s="5" t="s">
+      <c r="D279" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E279" s="5" t="s">
+      <c r="E279" s="2" t="s">
         <v>878</v>
       </c>
-      <c r="F279" s="5" t="s">
+      <c r="F279" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G279" s="5" t="s">
+      <c r="G279" s="2" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="280" spans="1:7">
-      <c r="A280" s="5" t="s">
+      <c r="A280" s="2" t="s">
         <v>885</v>
       </c>
-      <c r="B280" s="5" t="s">
+      <c r="B280" s="2" t="s">
         <v>886</v>
       </c>
-      <c r="C280" s="5" t="s">
+      <c r="C280" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D280" s="5" t="s">
+      <c r="D280" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E280" s="5" t="s">
+      <c r="E280" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="F280" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G280" s="5" t="s">
+      <c r="F280" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G280" s="2" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="281" spans="1:7">
-      <c r="A281" s="5" t="s">
+      <c r="A281" s="2" t="s">
         <v>887</v>
       </c>
-      <c r="B281" s="5" t="s">
+      <c r="B281" s="2" t="s">
         <v>888</v>
       </c>
-      <c r="C281" s="5" t="s">
+      <c r="C281" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D281" s="5" t="s">
+      <c r="D281" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E281" s="5" t="s">
+      <c r="E281" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="F281" s="5" t="s">
+      <c r="F281" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="G281" s="5" t="s">
+      <c r="G281" s="2" t="s">
         <v>889</v>
       </c>
     </row>
     <row r="282" spans="1:7">
-      <c r="A282" s="5" t="s">
+      <c r="A282" s="2" t="s">
         <v>890</v>
       </c>
-      <c r="B282" s="5" t="s">
+      <c r="B282" s="2" t="s">
         <v>891</v>
       </c>
-      <c r="C282" s="5" t="s">
+      <c r="C282" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D282" s="5" t="s">
+      <c r="D282" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E282" s="5" t="s">
+      <c r="E282" s="2" t="s">
         <v>892</v>
       </c>
-      <c r="F282" s="5" t="s">
+      <c r="F282" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G282" s="5" t="s">
+      <c r="G282" s="2" t="s">
         <v>893</v>
       </c>
     </row>
     <row r="283" spans="1:7">
-      <c r="A283" s="5" t="s">
+      <c r="A283" s="2" t="s">
         <v>894</v>
       </c>
-      <c r="B283" s="5" t="s">
+      <c r="B283" s="2" t="s">
         <v>895</v>
       </c>
-      <c r="C283" s="5" t="s">
+      <c r="C283" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D283" s="5" t="s">
+      <c r="D283" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E283" s="5" t="s">
+      <c r="E283" s="2" t="s">
         <v>896</v>
       </c>
-      <c r="F283" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G283" s="5" t="s">
+      <c r="F283" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G283" s="2" t="s">
         <v>897</v>
       </c>
     </row>
     <row r="284" spans="1:7">
-      <c r="A284" s="5" t="s">
+      <c r="A284" s="2" t="s">
         <v>898</v>
       </c>
-      <c r="B284" s="5" t="s">
+      <c r="B284" s="2" t="s">
         <v>899</v>
       </c>
-      <c r="C284" s="5" t="s">
+      <c r="C284" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D284" s="5" t="s">
+      <c r="D284" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E284" s="5" t="s">
+      <c r="E284" s="2" t="s">
         <v>878</v>
       </c>
-      <c r="F284" s="5" t="s">
+      <c r="F284" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="G284" s="5" t="s">
+      <c r="G284" s="2" t="s">
         <v>900</v>
       </c>
     </row>
     <row r="285" spans="1:7">
-      <c r="A285" s="5" t="s">
+      <c r="A285" s="2" t="s">
         <v>901</v>
       </c>
-      <c r="B285" s="5" t="s">
+      <c r="B285" s="2" t="s">
         <v>902</v>
       </c>
-      <c r="C285" s="5" t="s">
+      <c r="C285" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D285" s="5" t="s">
+      <c r="D285" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E285" s="5" t="s">
+      <c r="E285" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="F285" s="5" t="s">
+      <c r="F285" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G285" s="5" t="s">
+      <c r="G285" s="2" t="s">
         <v>851</v>
       </c>
     </row>
     <row r="286" spans="1:7">
-      <c r="A286" s="5" t="s">
+      <c r="A286" s="2" t="s">
         <v>903</v>
       </c>
-      <c r="B286" s="5" t="s">
+      <c r="B286" s="2" t="s">
         <v>904</v>
       </c>
-      <c r="C286" s="5" t="s">
+      <c r="C286" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D286" s="5"/>
-      <c r="E286" s="5" t="s">
+      <c r="D286" s="2"/>
+      <c r="E286" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="F286" s="5" t="s">
+      <c r="F286" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G286" s="5" t="s">
+      <c r="G286" s="2" t="s">
         <v>905</v>
       </c>
     </row>
     <row r="287" spans="1:7">
-      <c r="A287" s="5" t="s">
+      <c r="A287" s="2" t="s">
         <v>906</v>
       </c>
-      <c r="B287" s="5" t="s">
+      <c r="B287" s="2" t="s">
         <v>907</v>
       </c>
-      <c r="C287" s="5" t="s">
+      <c r="C287" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D287" s="5" t="s">
+      <c r="D287" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="E287" s="5" t="s">
+      <c r="E287" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="F287" s="5" t="s">
+      <c r="F287" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G287" s="5" t="s">
+      <c r="G287" s="2" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="288" spans="1:7">
-      <c r="A288" s="5" t="s">
+      <c r="A288" s="2" t="s">
         <v>908</v>
       </c>
-      <c r="B288" s="5" t="s">
+      <c r="B288" s="2" t="s">
         <v>909</v>
       </c>
-      <c r="C288" s="5" t="s">
+      <c r="C288" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D288" s="5"/>
-      <c r="E288" s="5" t="s">
+      <c r="D288" s="2"/>
+      <c r="E288" s="2" t="s">
         <v>606</v>
       </c>
-      <c r="F288" s="5" t="s">
+      <c r="F288" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G288" s="5" t="s">
+      <c r="G288" s="2" t="s">
         <v>910</v>
       </c>
     </row>
-    <row r="289" spans="1:7">
-      <c r="A289" s="5" t="s">
+    <row r="289" spans="1:8">
+      <c r="A289" s="2" t="s">
         <v>911</v>
       </c>
-      <c r="B289" s="5" t="s">
+      <c r="B289" s="2" t="s">
         <v>912</v>
       </c>
-      <c r="C289" s="5" t="s">
+      <c r="C289" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D289" s="5"/>
-      <c r="E289" s="5" t="s">
+      <c r="D289" s="2"/>
+      <c r="E289" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="F289" s="5" t="s">
+      <c r="F289" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G289" s="5" t="s">
+      <c r="G289" s="2" t="s">
         <v>913</v>
       </c>
     </row>
-    <row r="290" spans="1:7">
-      <c r="A290" s="5" t="s">
+    <row r="290" spans="1:8">
+      <c r="A290" s="2" t="s">
         <v>914</v>
       </c>
-      <c r="B290" s="5" t="s">
+      <c r="B290" s="2" t="s">
         <v>915</v>
       </c>
-      <c r="C290" s="5" t="s">
+      <c r="C290" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D290" s="5"/>
-      <c r="E290" s="5" t="s">
+      <c r="D290" s="2"/>
+      <c r="E290" s="2" t="s">
         <v>916</v>
       </c>
-      <c r="F290" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G290" s="5" t="s">
+      <c r="F290" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G290" s="2" t="s">
         <v>917</v>
       </c>
     </row>
-    <row r="291" spans="1:7">
-      <c r="A291" s="5" t="s">
+    <row r="291" spans="1:8">
+      <c r="A291" s="2" t="s">
         <v>918</v>
       </c>
-      <c r="B291" s="5" t="s">
+      <c r="B291" s="2" t="s">
         <v>919</v>
       </c>
-      <c r="C291" s="5" t="s">
+      <c r="C291" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D291" s="5" t="s">
+      <c r="D291" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="E291" s="5" t="s">
+      <c r="E291" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="F291" s="5" t="s">
+      <c r="F291" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G291" s="5" t="s">
+      <c r="G291" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="292" spans="1:7">
-      <c r="A292" s="5" t="s">
+    <row r="292" spans="1:8">
+      <c r="A292" s="2" t="s">
         <v>920</v>
       </c>
-      <c r="B292" s="5" t="s">
+      <c r="B292" s="2" t="s">
         <v>921</v>
       </c>
-      <c r="C292" s="5" t="s">
+      <c r="C292" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D292" s="5" t="s">
+      <c r="D292" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E292" s="5" t="s">
+      <c r="E292" s="2" t="s">
         <v>922</v>
       </c>
-      <c r="F292" s="5" t="s">
+      <c r="F292" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G292" s="5" t="s">
+      <c r="G292" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="293" spans="1:7">
-      <c r="A293" s="5" t="s">
+      <c r="H292" s="2"/>
+    </row>
+    <row r="293" spans="1:8">
+      <c r="A293" s="2" t="s">
         <v>923</v>
       </c>
-      <c r="B293" s="5" t="s">
+      <c r="B293" s="2" t="s">
         <v>924</v>
       </c>
-      <c r="C293" s="5" t="s">
+      <c r="C293" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D293" s="5" t="s">
+      <c r="D293" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="E293" s="5" t="s">
+      <c r="E293" s="2" t="s">
         <v>925</v>
       </c>
-      <c r="F293" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G293" s="5" t="s">
+      <c r="F293" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G293" s="2" t="s">
         <v>926</v>
       </c>
     </row>
-    <row r="294" spans="1:7">
-      <c r="A294" s="5" t="s">
+    <row r="294" spans="1:8">
+      <c r="A294" s="2" t="s">
         <v>927</v>
       </c>
-      <c r="B294" s="5" t="s">
+      <c r="B294" s="2" t="s">
         <v>928</v>
       </c>
-      <c r="C294" s="5" t="s">
+      <c r="C294" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D294" s="5"/>
-      <c r="E294" s="5" t="s">
+      <c r="D294" s="2"/>
+      <c r="E294" s="2" t="s">
         <v>929</v>
       </c>
-      <c r="F294" s="5" t="s">
+      <c r="F294" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G294" s="5" t="s">
+      <c r="G294" s="2" t="s">
         <v>930</v>
       </c>
     </row>
-    <row r="295" spans="1:7">
-      <c r="A295" s="5" t="s">
+    <row r="295" spans="1:8">
+      <c r="A295" s="2" t="s">
         <v>931</v>
       </c>
-      <c r="B295" s="5" t="s">
+      <c r="B295" s="2" t="s">
         <v>932</v>
       </c>
-      <c r="C295" s="5" t="s">
+      <c r="C295" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D295" s="5"/>
-      <c r="E295" s="5" t="s">
+      <c r="D295" s="2"/>
+      <c r="E295" s="2" t="s">
         <v>933</v>
       </c>
-      <c r="F295" s="5" t="s">
+      <c r="F295" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G295" s="5" t="s">
+      <c r="G295" s="2" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="296" spans="1:7">
-      <c r="A296" s="5" t="s">
+    <row r="296" spans="1:8">
+      <c r="A296" s="2" t="s">
         <v>934</v>
       </c>
-      <c r="B296" s="5" t="s">
+      <c r="B296" s="2" t="s">
         <v>935</v>
       </c>
-      <c r="C296" s="5" t="s">
+      <c r="C296" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D296" s="5"/>
-      <c r="E296" s="5" t="s">
+      <c r="D296" s="2"/>
+      <c r="E296" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="F296" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G296" s="5" t="s">
+      <c r="F296" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G296" s="2" t="s">
         <v>936</v>
       </c>
     </row>
-    <row r="297" spans="1:7">
-      <c r="A297" s="5" t="s">
+    <row r="297" spans="1:8">
+      <c r="A297" s="2" t="s">
         <v>937</v>
       </c>
-      <c r="B297" s="5" t="s">
+      <c r="B297" s="2" t="s">
         <v>938</v>
       </c>
-      <c r="C297" s="5" t="s">
+      <c r="C297" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="D297" s="5"/>
-      <c r="E297" s="5" t="s">
+      <c r="D297" s="2"/>
+      <c r="E297" s="2" t="s">
         <v>939</v>
       </c>
-      <c r="F297" s="5" t="s">
+      <c r="F297" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="G297" s="5" t="s">
+      <c r="G297" s="2" t="s">
         <v>940</v>
       </c>
     </row>
-    <row r="298" spans="1:7">
-      <c r="A298" s="5" t="s">
+    <row r="298" spans="1:8">
+      <c r="A298" s="2" t="s">
         <v>941</v>
       </c>
-      <c r="B298" s="5" t="s">
+      <c r="B298" s="2" t="s">
         <v>942</v>
       </c>
-      <c r="C298" s="5" t="s">
+      <c r="C298" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="D298" s="5"/>
-      <c r="E298" s="5" t="s">
+      <c r="D298" s="2"/>
+      <c r="E298" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="F298" s="5" t="s">
+      <c r="F298" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="G298" s="5" t="s">
+      <c r="G298" s="2" t="s">
         <v>943</v>
       </c>
     </row>
-    <row r="299" spans="1:7">
-      <c r="A299" s="5" t="s">
+    <row r="299" spans="1:8">
+      <c r="A299" s="2" t="s">
         <v>944</v>
       </c>
-      <c r="B299" s="5" t="s">
+      <c r="B299" s="2" t="s">
         <v>945</v>
       </c>
-      <c r="C299" s="5" t="s">
+      <c r="C299" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D299" s="5" t="s">
+      <c r="D299" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E299" s="5" t="s">
+      <c r="E299" s="2" t="s">
         <v>946</v>
       </c>
-      <c r="F299" s="5" t="s">
+      <c r="F299" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="G299" s="5" t="s">
+      <c r="G299" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="300" spans="1:7">
-      <c r="A300" s="5" t="s">
+    <row r="300" spans="1:8">
+      <c r="A300" s="2" t="s">
         <v>947</v>
       </c>
-      <c r="B300" s="5" t="s">
+      <c r="B300" s="2" t="s">
         <v>948</v>
       </c>
-      <c r="C300" s="5" t="s">
+      <c r="C300" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="D300" s="5"/>
-      <c r="E300" s="5" t="s">
+      <c r="D300" s="2"/>
+      <c r="E300" s="2" t="s">
         <v>949</v>
       </c>
-      <c r="F300" s="5" t="s">
+      <c r="F300" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G300" s="5" t="s">
+      <c r="G300" s="2" t="s">
         <v>950</v>
       </c>
     </row>
-    <row r="301" spans="1:7">
-      <c r="A301" s="5" t="s">
+    <row r="301" spans="1:8">
+      <c r="A301" s="2" t="s">
         <v>951</v>
       </c>
-      <c r="B301" s="5" t="s">
+      <c r="B301" s="2" t="s">
         <v>952</v>
       </c>
-      <c r="C301" s="5" t="s">
+      <c r="C301" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D301" s="5"/>
-      <c r="E301" s="5" t="s">
+      <c r="D301" s="2"/>
+      <c r="E301" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F301" s="5" t="s">
+      <c r="F301" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G301" s="5" t="s">
+      <c r="G301" s="2" t="s">
         <v>953</v>
       </c>
     </row>
-    <row r="302" spans="1:7">
-      <c r="A302" s="5" t="s">
+    <row r="302" spans="1:8">
+      <c r="A302" s="2" t="s">
         <v>954</v>
       </c>
-      <c r="B302" s="5" t="s">
+      <c r="B302" s="2" t="s">
         <v>955</v>
       </c>
-      <c r="C302" s="5" t="s">
+      <c r="C302" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D302" s="5"/>
-      <c r="E302" s="5" t="s">
+      <c r="D302" s="2"/>
+      <c r="E302" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="F302" s="5" t="s">
+      <c r="F302" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="G302" s="5" t="s">
+      <c r="G302" s="2" t="s">
         <v>956</v>
       </c>
     </row>
-    <row r="303" spans="1:7">
-      <c r="A303" s="5" t="s">
+    <row r="303" spans="1:8">
+      <c r="A303" s="2" t="s">
         <v>957</v>
       </c>
-      <c r="B303" s="5" t="s">
+      <c r="B303" s="2" t="s">
         <v>958</v>
       </c>
-      <c r="C303" s="5" t="s">
+      <c r="C303" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="D303" s="5" t="s">
+      <c r="D303" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="E303" s="5" t="s">
+      <c r="E303" s="2" t="s">
         <v>959</v>
       </c>
-      <c r="F303" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G303" s="5" t="s">
+      <c r="F303" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G303" s="2" t="s">
         <v>953</v>
       </c>
     </row>
-    <row r="304" spans="1:7">
-      <c r="A304" s="5" t="s">
+    <row r="304" spans="1:8">
+      <c r="A304" s="2" t="s">
         <v>960</v>
       </c>
-      <c r="B304" s="5" t="s">
+      <c r="B304" s="2" t="s">
         <v>961</v>
       </c>
-      <c r="C304" s="5" t="s">
+      <c r="C304" s="2" t="s">
         <v>1169</v>
       </c>
-      <c r="D304" s="5" t="s">
+      <c r="D304" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E304" s="5" t="s">
+      <c r="E304" s="2" t="s">
         <v>959</v>
       </c>
-      <c r="F304" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G304" s="5" t="s">
+      <c r="F304" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G304" s="2" t="s">
         <v>495</v>
       </c>
     </row>
     <row r="305" spans="1:7">
-      <c r="A305" s="5" t="s">
+      <c r="A305" s="2" t="s">
         <v>962</v>
       </c>
-      <c r="B305" s="5" t="s">
+      <c r="B305" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="C305" s="5" t="s">
+      <c r="C305" s="2" t="s">
         <v>1169</v>
       </c>
-      <c r="D305" s="5" t="s">
+      <c r="D305" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="E305" s="5" t="s">
+      <c r="E305" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="F305" s="5" t="s">
+      <c r="F305" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="G305" s="5" t="s">
+      <c r="G305" s="2" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="306" spans="1:7">
-      <c r="A306" s="5" t="s">
+      <c r="A306" s="2" t="s">
         <v>964</v>
       </c>
-      <c r="B306" s="5" t="s">
+      <c r="B306" s="2" t="s">
         <v>965</v>
       </c>
-      <c r="C306" s="5" t="s">
+      <c r="C306" s="2" t="s">
         <v>1169</v>
       </c>
-      <c r="D306" s="5" t="s">
+      <c r="D306" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="E306" s="5" t="s">
+      <c r="E306" s="2" t="s">
         <v>655</v>
       </c>
-      <c r="F306" s="5" t="s">
+      <c r="F306" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G306" s="5" t="s">
+      <c r="G306" s="2" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="307" spans="1:7">
-      <c r="A307" s="5" t="s">
+      <c r="A307" s="2" t="s">
         <v>966</v>
       </c>
-      <c r="B307" s="5" t="s">
+      <c r="B307" s="2" t="s">
         <v>967</v>
       </c>
-      <c r="C307" s="5" t="s">
+      <c r="C307" s="2" t="s">
         <v>1169</v>
       </c>
-      <c r="D307" s="5" t="s">
+      <c r="D307" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="E307" s="5" t="s">
+      <c r="E307" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F307" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G307" s="5" t="s">
+      <c r="F307" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G307" s="2" t="s">
         <v>968</v>
       </c>
     </row>
     <row r="308" spans="1:7">
-      <c r="A308" s="5" t="s">
+      <c r="A308" s="2" t="s">
         <v>969</v>
       </c>
-      <c r="B308" s="5" t="s">
+      <c r="B308" s="2" t="s">
         <v>970</v>
       </c>
-      <c r="C308" s="5" t="s">
+      <c r="C308" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="D308" s="5" t="s">
+      <c r="D308" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="E308" s="5" t="s">
+      <c r="E308" s="2" t="s">
         <v>606</v>
       </c>
-      <c r="F308" s="5" t="s">
+      <c r="F308" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="G308" s="5" t="s">
+      <c r="G308" s="2" t="s">
         <v>971</v>
       </c>
     </row>
     <row r="309" spans="1:7">
-      <c r="A309" s="5" t="s">
+      <c r="A309" s="2" t="s">
         <v>972</v>
       </c>
-      <c r="B309" s="5" t="s">
+      <c r="B309" s="2" t="s">
         <v>973</v>
       </c>
-      <c r="C309" s="5" t="s">
+      <c r="C309" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="D309" s="5" t="s">
+      <c r="D309" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="E309" s="5" t="s">
+      <c r="E309" s="2" t="s">
         <v>628</v>
       </c>
-      <c r="F309" s="5" t="s">
+      <c r="F309" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G309" s="5" t="s">
+      <c r="G309" s="2" t="s">
         <v>974</v>
       </c>
     </row>
     <row r="310" spans="1:7">
-      <c r="A310" s="5" t="s">
+      <c r="A310" s="2" t="s">
         <v>975</v>
       </c>
-      <c r="B310" s="5" t="s">
+      <c r="B310" s="2" t="s">
         <v>976</v>
       </c>
-      <c r="C310" s="5" t="s">
+      <c r="C310" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="D310" s="5"/>
-      <c r="E310" s="5" t="s">
+      <c r="D310" s="2"/>
+      <c r="E310" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="F310" s="5" t="s">
+      <c r="F310" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G310" s="5" t="s">
+      <c r="G310" s="2" t="s">
         <v>977</v>
       </c>
     </row>
     <row r="311" spans="1:7">
-      <c r="A311" s="5" t="s">
+      <c r="A311" s="2" t="s">
         <v>978</v>
       </c>
-      <c r="B311" s="5" t="s">
+      <c r="B311" s="2" t="s">
         <v>979</v>
       </c>
-      <c r="C311" s="5" t="s">
+      <c r="C311" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="D311" s="5"/>
-      <c r="E311" s="5" t="s">
+      <c r="D311" s="2"/>
+      <c r="E311" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="F311" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G311" s="5" t="s">
+      <c r="F311" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G311" s="2" t="s">
         <v>980</v>
       </c>
     </row>
     <row r="312" spans="1:7">
-      <c r="A312" s="5" t="s">
+      <c r="A312" s="2" t="s">
         <v>981</v>
       </c>
-      <c r="B312" s="5" t="s">
+      <c r="B312" s="2" t="s">
         <v>982</v>
       </c>
-      <c r="C312" s="5" t="s">
+      <c r="C312" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="D312" s="5"/>
-      <c r="E312" s="5" t="s">
+      <c r="D312" s="2"/>
+      <c r="E312" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F312" s="5" t="s">
+      <c r="F312" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="G312" s="5" t="s">
+      <c r="G312" s="2" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="313" spans="1:7">
-      <c r="A313" s="5" t="s">
+      <c r="A313" s="2" t="s">
         <v>983</v>
       </c>
-      <c r="B313" s="5" t="s">
+      <c r="B313" s="2" t="s">
         <v>984</v>
       </c>
-      <c r="C313" s="5" t="s">
+      <c r="C313" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="D313" s="5"/>
-      <c r="E313" s="5" t="s">
+      <c r="D313" s="2"/>
+      <c r="E313" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F313" s="5" t="s">
+      <c r="F313" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="G313" s="5" t="s">
+      <c r="G313" s="2" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="314" spans="1:7">
-      <c r="A314" s="5" t="s">
+      <c r="A314" s="2" t="s">
         <v>985</v>
       </c>
-      <c r="B314" s="5" t="s">
+      <c r="B314" s="2" t="s">
         <v>986</v>
       </c>
-      <c r="C314" s="5" t="s">
+      <c r="C314" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D314" s="5"/>
-      <c r="E314" s="5" t="s">
+      <c r="D314" s="2"/>
+      <c r="E314" s="2" t="s">
         <v>655</v>
       </c>
-      <c r="F314" s="5" t="s">
+      <c r="F314" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="G314" s="5" t="s">
+      <c r="G314" s="2" t="s">
         <v>987</v>
       </c>
     </row>
     <row r="315" spans="1:7">
-      <c r="A315" s="5" t="s">
+      <c r="A315" s="2" t="s">
         <v>988</v>
       </c>
-      <c r="B315" s="5" t="s">
+      <c r="B315" s="2" t="s">
         <v>989</v>
       </c>
-      <c r="C315" s="5" t="s">
+      <c r="C315" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D315" s="5"/>
-      <c r="E315" s="5" t="s">
+      <c r="D315" s="2"/>
+      <c r="E315" s="2" t="s">
         <v>655</v>
       </c>
-      <c r="F315" s="5" t="s">
+      <c r="F315" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="G315" s="5" t="s">
+      <c r="G315" s="2" t="s">
         <v>987</v>
       </c>
     </row>
     <row r="316" spans="1:7">
-      <c r="A316" s="5" t="s">
+      <c r="A316" s="2" t="s">
         <v>990</v>
       </c>
-      <c r="B316" s="5" t="s">
+      <c r="B316" s="2" t="s">
         <v>991</v>
       </c>
-      <c r="C316" s="5" t="s">
+      <c r="C316" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D316" s="5" t="s">
+      <c r="D316" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E316" s="5" t="s">
+      <c r="E316" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="F316" s="5" t="s">
+      <c r="F316" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="G316" s="5" t="s">
+      <c r="G316" s="2" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="317" spans="1:7">
-      <c r="A317" s="5" t="s">
+      <c r="A317" s="2" t="s">
         <v>992</v>
       </c>
-      <c r="B317" s="5" t="s">
+      <c r="B317" s="2" t="s">
         <v>993</v>
       </c>
-      <c r="C317" s="5" t="s">
+      <c r="C317" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D317" s="5"/>
-      <c r="E317" s="5" t="s">
+      <c r="D317" s="2"/>
+      <c r="E317" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F317" s="5" t="s">
+      <c r="F317" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="G317" s="5" t="s">
+      <c r="G317" s="2" t="s">
         <v>994</v>
       </c>
     </row>
     <row r="318" spans="1:7">
-      <c r="A318" s="5" t="s">
+      <c r="A318" s="2" t="s">
         <v>995</v>
       </c>
-      <c r="B318" s="5" t="s">
+      <c r="B318" s="2" t="s">
         <v>996</v>
       </c>
-      <c r="C318" s="5" t="s">
+      <c r="C318" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D318" s="5"/>
-      <c r="E318" s="5" t="s">
+      <c r="D318" s="2"/>
+      <c r="E318" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="F318" s="5" t="s">
+      <c r="F318" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G318" s="5" t="s">
+      <c r="G318" s="2" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="319" spans="1:7">
-      <c r="A319" s="5" t="s">
+      <c r="A319" s="2" t="s">
         <v>997</v>
       </c>
-      <c r="B319" s="5" t="s">
+      <c r="B319" s="2" t="s">
         <v>998</v>
       </c>
-      <c r="C319" s="5" t="s">
+      <c r="C319" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D319" s="5" t="s">
+      <c r="D319" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="E319" s="5" t="s">
+      <c r="E319" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="F319" s="5" t="s">
+      <c r="F319" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="G319" s="5" t="s">
+      <c r="G319" s="2" t="s">
         <v>999</v>
       </c>
     </row>
     <row r="320" spans="1:7">
-      <c r="A320" s="5" t="s">
+      <c r="A320" s="2" t="s">
         <v>1000</v>
       </c>
-      <c r="B320" s="5" t="s">
+      <c r="B320" s="2" t="s">
         <v>1001</v>
       </c>
-      <c r="C320" s="5" t="s">
+      <c r="C320" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D320" s="5" t="s">
+      <c r="D320" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="E320" s="5" t="s">
+      <c r="E320" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="F320" s="5" t="s">
+      <c r="F320" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="G320" s="5" t="s">
+      <c r="G320" s="2" t="s">
         <v>553</v>
       </c>
     </row>
     <row r="321" spans="1:7">
-      <c r="A321" s="5" t="s">
+      <c r="A321" s="2" t="s">
         <v>1002</v>
       </c>
-      <c r="B321" s="5" t="s">
+      <c r="B321" s="2" t="s">
         <v>1003</v>
       </c>
-      <c r="C321" s="5" t="s">
+      <c r="C321" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D321" s="5"/>
-      <c r="E321" s="5" t="s">
+      <c r="D321" s="2"/>
+      <c r="E321" s="2" t="s">
         <v>1004</v>
       </c>
-      <c r="F321" s="5" t="s">
+      <c r="F321" s="2" t="s">
         <v>1005</v>
       </c>
-      <c r="G321" s="5" t="s">
+      <c r="G321" s="2" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="322" spans="1:7">
-      <c r="A322" s="5" t="s">
+      <c r="A322" s="2" t="s">
         <v>1006</v>
       </c>
-      <c r="B322" s="5" t="s">
+      <c r="B322" s="2" t="s">
         <v>1007</v>
       </c>
-      <c r="C322" s="5" t="s">
+      <c r="C322" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D322" s="5"/>
-      <c r="E322" s="5" t="s">
+      <c r="D322" s="2"/>
+      <c r="E322" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="F322" s="5" t="s">
+      <c r="F322" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="G322" s="5" t="s">
+      <c r="G322" s="2" t="s">
         <v>1008</v>
       </c>
     </row>
     <row r="323" spans="1:7">
-      <c r="A323" s="5" t="s">
+      <c r="A323" s="2" t="s">
         <v>1009</v>
       </c>
-      <c r="B323" s="5" t="s">
+      <c r="B323" s="2" t="s">
         <v>1010</v>
       </c>
-      <c r="C323" s="5" t="s">
+      <c r="C323" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D323" s="5" t="s">
+      <c r="D323" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="E323" s="5" t="s">
+      <c r="E323" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="F323" s="5" t="s">
+      <c r="F323" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G323" s="5" t="s">
+      <c r="G323" s="2" t="s">
         <v>910</v>
       </c>
     </row>
     <row r="324" spans="1:7">
-      <c r="A324" s="5" t="s">
+      <c r="A324" s="2" t="s">
         <v>1011</v>
       </c>
-      <c r="B324" s="5" t="s">
+      <c r="B324" s="2" t="s">
         <v>1012</v>
       </c>
-      <c r="C324" s="5" t="s">
+      <c r="C324" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D324" s="5" t="s">
+      <c r="D324" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="E324" s="5" t="s">
+      <c r="E324" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="F324" s="5" t="s">
+      <c r="F324" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="G324" s="5" t="s">
+      <c r="G324" s="2" t="s">
         <v>469</v>
       </c>
     </row>
     <row r="325" spans="1:7">
-      <c r="A325" s="5" t="s">
+      <c r="A325" s="2" t="s">
         <v>1013</v>
       </c>
-      <c r="B325" s="5" t="s">
+      <c r="B325" s="2" t="s">
         <v>1014</v>
       </c>
-      <c r="C325" s="5" t="s">
+      <c r="C325" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D325" s="5"/>
-      <c r="E325" s="5" t="s">
+      <c r="D325" s="2"/>
+      <c r="E325" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="F325" s="5" t="s">
+      <c r="F325" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G325" s="5" t="s">
+      <c r="G325" s="2" t="s">
         <v>1015</v>
       </c>
     </row>
     <row r="326" spans="1:7">
-      <c r="A326" s="5" t="s">
+      <c r="A326" s="2" t="s">
         <v>1016</v>
       </c>
-      <c r="B326" s="5" t="s">
+      <c r="B326" s="2" t="s">
         <v>1017</v>
       </c>
-      <c r="C326" s="5" t="s">
+      <c r="C326" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D326" s="5"/>
-      <c r="E326" s="5" t="s">
+      <c r="D326" s="2"/>
+      <c r="E326" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="F326" s="5" t="s">
+      <c r="F326" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G326" s="5" t="s">
+      <c r="G326" s="2" t="s">
         <v>1018</v>
       </c>
     </row>
     <row r="327" spans="1:7">
-      <c r="A327" s="5" t="s">
+      <c r="A327" s="2" t="s">
         <v>1019</v>
       </c>
-      <c r="B327" s="5" t="s">
+      <c r="B327" s="2" t="s">
         <v>1020</v>
       </c>
-      <c r="C327" s="5" t="s">
+      <c r="C327" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D327" s="5"/>
-      <c r="E327" s="5" t="s">
+      <c r="D327" s="2"/>
+      <c r="E327" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="F327" s="5" t="s">
+      <c r="F327" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="G327" s="5" t="s">
+      <c r="G327" s="2" t="s">
         <v>1021</v>
       </c>
     </row>
     <row r="328" spans="1:7">
-      <c r="A328" s="5" t="s">
+      <c r="A328" s="2" t="s">
         <v>1022</v>
       </c>
-      <c r="B328" s="5" t="s">
+      <c r="B328" s="2" t="s">
         <v>1023</v>
       </c>
-      <c r="C328" s="5" t="s">
+      <c r="C328" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D328" s="5"/>
-      <c r="E328" s="5" t="s">
+      <c r="D328" s="2"/>
+      <c r="E328" s="2" t="s">
         <v>933</v>
       </c>
-      <c r="F328" s="5" t="s">
+      <c r="F328" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G328" s="5" t="s">
+      <c r="G328" s="2" t="s">
         <v>676</v>
       </c>
     </row>
     <row r="329" spans="1:7">
-      <c r="A329" s="5" t="s">
+      <c r="A329" s="2" t="s">
         <v>1024</v>
       </c>
-      <c r="B329" s="5" t="s">
+      <c r="B329" s="2" t="s">
         <v>1025</v>
       </c>
-      <c r="C329" s="5" t="s">
+      <c r="C329" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="D329" s="5"/>
-      <c r="E329" s="5" t="s">
+      <c r="D329" s="2"/>
+      <c r="E329" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F329" s="5" t="s">
+      <c r="F329" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G329" s="5" t="s">
+      <c r="G329" s="2" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="330" spans="1:7">
-      <c r="A330" s="5" t="s">
+      <c r="A330" s="2" t="s">
         <v>1026</v>
       </c>
-      <c r="B330" s="5" t="s">
+      <c r="B330" s="2" t="s">
         <v>1027</v>
       </c>
-      <c r="C330" s="5" t="s">
+      <c r="C330" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="D330" s="5" t="s">
+      <c r="D330" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="E330" s="5" t="s">
+      <c r="E330" s="2" t="s">
         <v>638</v>
       </c>
-      <c r="F330" s="5" t="s">
+      <c r="F330" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G330" s="5" t="s">
+      <c r="G330" s="2" t="s">
         <v>1028</v>
       </c>
     </row>
     <row r="331" spans="1:7">
-      <c r="A331" s="5" t="s">
+      <c r="A331" s="2" t="s">
         <v>1029</v>
       </c>
-      <c r="B331" s="5" t="s">
+      <c r="B331" s="2" t="s">
         <v>1030</v>
       </c>
-      <c r="C331" s="5" t="s">
+      <c r="C331" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="D331" s="5" t="s">
+      <c r="D331" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="E331" s="5" t="s">
+      <c r="E331" s="2" t="s">
         <v>1031</v>
       </c>
-      <c r="F331" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G331" s="5" t="s">
+      <c r="F331" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G331" s="2" t="s">
         <v>1032</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adicionado +20 Pokémon da 4ª geração
</commit_message>
<xml_diff>
--- a/pokemonv2/pokemons.xlsx
+++ b/pokemonv2/pokemons.xlsx
@@ -8364,7 +8364,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -8374,6 +8374,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8405,7 +8411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -8413,6 +8419,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8715,8 +8722,8 @@
   <dimension ref="A1:H1026"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <pane ySplit="1" topLeftCell="A397" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B406" sqref="B406"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17224,2301 +17231,2355 @@
       </c>
     </row>
     <row r="388" spans="1:7">
-      <c r="A388" t="s">
+      <c r="A388" s="2" t="s">
         <v>1191</v>
       </c>
-      <c r="B388" t="s">
+      <c r="B388" s="2" t="s">
         <v>1192</v>
       </c>
-      <c r="C388" t="s">
+      <c r="C388" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="E388" t="s">
+      <c r="D388" s="2"/>
+      <c r="E388" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F388" t="s">
-        <v>8</v>
-      </c>
-      <c r="G388" t="s">
+      <c r="F388" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G388" s="2" t="s">
         <v>1193</v>
       </c>
     </row>
     <row r="389" spans="1:7">
-      <c r="A389" t="s">
+      <c r="A389" s="2" t="s">
         <v>1194</v>
       </c>
-      <c r="B389" t="s">
+      <c r="B389" s="2" t="s">
         <v>1195</v>
       </c>
-      <c r="C389" t="s">
+      <c r="C389" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="E389" t="s">
+      <c r="D389" s="2"/>
+      <c r="E389" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F389" t="s">
-        <v>8</v>
-      </c>
-      <c r="G389" t="s">
+      <c r="F389" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G389" s="2" t="s">
         <v>950</v>
       </c>
     </row>
     <row r="390" spans="1:7">
-      <c r="A390" t="s">
+      <c r="A390" s="2" t="s">
         <v>1196</v>
       </c>
-      <c r="B390" t="s">
+      <c r="B390" s="2" t="s">
         <v>1197</v>
       </c>
-      <c r="C390" t="s">
+      <c r="C390" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D390" t="s">
+      <c r="D390" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="E390" t="s">
+      <c r="E390" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F390" t="s">
-        <v>8</v>
-      </c>
-      <c r="G390" t="s">
+      <c r="F390" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G390" s="2" t="s">
         <v>1198</v>
       </c>
     </row>
     <row r="391" spans="1:7">
-      <c r="A391" t="s">
+      <c r="A391" s="2" t="s">
         <v>1199</v>
       </c>
-      <c r="B391" t="s">
+      <c r="B391" s="2" t="s">
         <v>1200</v>
       </c>
-      <c r="C391" t="s">
+      <c r="C391" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E391" t="s">
+      <c r="D391" s="2"/>
+      <c r="E391" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F391" t="s">
-        <v>8</v>
-      </c>
-      <c r="G391" t="s">
+      <c r="F391" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G391" s="2" t="s">
         <v>1201</v>
       </c>
     </row>
     <row r="392" spans="1:7">
-      <c r="A392" t="s">
+      <c r="A392" s="2" t="s">
         <v>1202</v>
       </c>
-      <c r="B392" t="s">
+      <c r="B392" s="2" t="s">
         <v>1203</v>
       </c>
-      <c r="C392" t="s">
+      <c r="C392" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D392" t="s">
+      <c r="D392" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="E392" t="s">
+      <c r="E392" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F392" t="s">
-        <v>8</v>
-      </c>
-      <c r="G392" t="s">
+      <c r="F392" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G392" s="2" t="s">
         <v>1097</v>
       </c>
     </row>
     <row r="393" spans="1:7">
-      <c r="A393" t="s">
+      <c r="A393" s="2" t="s">
         <v>1204</v>
       </c>
-      <c r="B393" t="s">
+      <c r="B393" s="2" t="s">
         <v>1205</v>
       </c>
-      <c r="C393" t="s">
+      <c r="C393" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D393" t="s">
+      <c r="D393" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="E393" t="s">
+      <c r="E393" s="2" t="s">
         <v>1206</v>
       </c>
-      <c r="F393" t="s">
-        <v>8</v>
-      </c>
-      <c r="G393" t="s">
+      <c r="F393" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G393" s="2" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="394" spans="1:7">
-      <c r="A394" t="s">
+      <c r="A394" s="2" t="s">
         <v>1207</v>
       </c>
-      <c r="B394" t="s">
+      <c r="B394" s="2" t="s">
         <v>1208</v>
       </c>
-      <c r="C394" t="s">
+      <c r="C394" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E394" t="s">
+      <c r="D394" s="2"/>
+      <c r="E394" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F394" t="s">
-        <v>8</v>
-      </c>
-      <c r="G394" t="s">
+      <c r="F394" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G394" s="2" t="s">
         <v>1209</v>
       </c>
     </row>
     <row r="395" spans="1:7">
-      <c r="A395" t="s">
+      <c r="A395" s="2" t="s">
         <v>1210</v>
       </c>
-      <c r="B395" t="s">
+      <c r="B395" s="2" t="s">
         <v>1211</v>
       </c>
-      <c r="C395" t="s">
+      <c r="C395" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E395" t="s">
+      <c r="D395" s="2"/>
+      <c r="E395" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F395" t="s">
-        <v>8</v>
-      </c>
-      <c r="G395" t="s">
+      <c r="F395" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G395" s="2" t="s">
         <v>1212</v>
       </c>
     </row>
     <row r="396" spans="1:7">
-      <c r="A396" t="s">
+      <c r="A396" s="2" t="s">
         <v>1213</v>
       </c>
-      <c r="B396" t="s">
+      <c r="B396" s="2" t="s">
         <v>1214</v>
       </c>
-      <c r="C396" t="s">
+      <c r="C396" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D396" t="s">
+      <c r="D396" s="2" t="s">
         <v>1169</v>
       </c>
-      <c r="E396" t="s">
+      <c r="E396" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F396" t="s">
-        <v>8</v>
-      </c>
-      <c r="G396" t="s">
+      <c r="F396" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G396" s="2" t="s">
         <v>1215</v>
       </c>
     </row>
     <row r="397" spans="1:7">
-      <c r="A397" t="s">
+      <c r="A397" s="2" t="s">
         <v>1216</v>
       </c>
-      <c r="B397" t="s">
+      <c r="B397" s="2" t="s">
         <v>1217</v>
       </c>
-      <c r="C397" t="s">
+      <c r="C397" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D397" t="s">
+      <c r="D397" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E397" t="s">
+      <c r="E397" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="F397" t="s">
+      <c r="F397" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G397" t="s">
+      <c r="G397" s="2" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="398" spans="1:7">
-      <c r="A398" t="s">
+      <c r="A398" s="2" t="s">
         <v>1218</v>
       </c>
-      <c r="B398" t="s">
+      <c r="B398" s="2" t="s">
         <v>1219</v>
       </c>
-      <c r="C398" t="s">
+      <c r="C398" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D398" t="s">
+      <c r="D398" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E398" t="s">
+      <c r="E398" s="2" t="s">
         <v>638</v>
       </c>
-      <c r="F398" t="s">
+      <c r="F398" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G398" t="s">
+      <c r="G398" s="2" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="399" spans="1:7">
-      <c r="A399" t="s">
+      <c r="A399" s="2" t="s">
         <v>1220</v>
       </c>
-      <c r="B399" t="s">
+      <c r="B399" s="2" t="s">
         <v>1221</v>
       </c>
-      <c r="C399" t="s">
+      <c r="C399" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D399" t="s">
+      <c r="D399" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E399" t="s">
+      <c r="E399" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F399" t="s">
-        <v>8</v>
-      </c>
-      <c r="G399" t="s">
+      <c r="F399" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G399" s="2" t="s">
         <v>1222</v>
       </c>
     </row>
     <row r="400" spans="1:7">
-      <c r="A400" t="s">
+      <c r="A400" s="2" t="s">
         <v>1223</v>
       </c>
-      <c r="B400" t="s">
+      <c r="B400" s="2" t="s">
         <v>1224</v>
       </c>
-      <c r="C400" t="s">
+      <c r="C400" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="E400" t="s">
+      <c r="D400" s="2"/>
+      <c r="E400" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F400" t="s">
+      <c r="F400" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G400" t="s">
+      <c r="G400" s="2" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="401" spans="1:7">
-      <c r="A401" t="s">
+      <c r="A401" s="2" t="s">
         <v>1225</v>
       </c>
-      <c r="B401" t="s">
+      <c r="B401" s="2" t="s">
         <v>1226</v>
       </c>
-      <c r="C401" t="s">
+      <c r="C401" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D401" t="s">
+      <c r="D401" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E401" t="s">
+      <c r="E401" s="2" t="s">
         <v>628</v>
       </c>
-      <c r="F401" t="s">
+      <c r="F401" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G401" t="s">
+      <c r="G401" s="2" t="s">
         <v>974</v>
       </c>
     </row>
     <row r="402" spans="1:7">
-      <c r="A402" t="s">
+      <c r="A402" s="2" t="s">
         <v>1227</v>
       </c>
-      <c r="B402" t="s">
+      <c r="B402" s="2" t="s">
         <v>1228</v>
       </c>
-      <c r="C402" t="s">
+      <c r="C402" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E402" t="s">
+      <c r="D402" s="2"/>
+      <c r="E402" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F402" t="s">
+      <c r="F402" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G402" t="s">
+      <c r="G402" s="2" t="s">
         <v>1229</v>
       </c>
     </row>
     <row r="403" spans="1:7">
-      <c r="A403" t="s">
+      <c r="A403" s="2" t="s">
         <v>1230</v>
       </c>
-      <c r="B403" t="s">
+      <c r="B403" s="2" t="s">
         <v>1231</v>
       </c>
-      <c r="C403" t="s">
+      <c r="C403" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E403" t="s">
+      <c r="D403" s="2"/>
+      <c r="E403" s="2" t="s">
         <v>1232</v>
       </c>
-      <c r="F403" t="s">
-        <v>8</v>
-      </c>
-      <c r="G403" t="s">
+      <c r="F403" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G403" s="2" t="s">
         <v>1233</v>
       </c>
     </row>
     <row r="404" spans="1:7">
-      <c r="A404" t="s">
+      <c r="A404" s="2" t="s">
         <v>1234</v>
       </c>
-      <c r="B404" t="s">
+      <c r="B404" s="2" t="s">
         <v>1235</v>
       </c>
-      <c r="C404" t="s">
+      <c r="C404" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="E404" t="s">
+      <c r="D404" s="2"/>
+      <c r="E404" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="F404" t="s">
+      <c r="F404" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="G404" t="s">
+      <c r="G404" s="2" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="405" spans="1:7">
-      <c r="A405" t="s">
+      <c r="A405" s="2" t="s">
         <v>1236</v>
       </c>
-      <c r="B405" t="s">
+      <c r="B405" s="2" t="s">
         <v>1237</v>
       </c>
-      <c r="C405" t="s">
+      <c r="C405" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="E405" t="s">
+      <c r="D405" s="2"/>
+      <c r="E405" s="2" t="s">
         <v>1238</v>
       </c>
-      <c r="F405" t="s">
+      <c r="F405" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G405" t="s">
+      <c r="G405" s="2" t="s">
         <v>1239</v>
       </c>
     </row>
     <row r="406" spans="1:7">
-      <c r="A406" t="s">
+      <c r="A406" s="2" t="s">
         <v>1240</v>
       </c>
-      <c r="B406" t="s">
+      <c r="B406" s="2" t="s">
         <v>1241</v>
       </c>
-      <c r="C406" t="s">
+      <c r="C406" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="E406" t="s">
+      <c r="D406" s="2"/>
+      <c r="E406" s="2" t="s">
         <v>1242</v>
       </c>
-      <c r="F406" t="s">
-        <v>8</v>
-      </c>
-      <c r="G406" t="s">
+      <c r="F406" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G406" s="2" t="s">
         <v>1243</v>
       </c>
     </row>
     <row r="407" spans="1:7">
-      <c r="A407" t="s">
+      <c r="A407" s="2" t="s">
         <v>1244</v>
       </c>
-      <c r="B407" t="s">
+      <c r="B407" s="2" t="s">
         <v>1245</v>
       </c>
-      <c r="C407" t="s">
+      <c r="C407" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D407" t="s">
+      <c r="D407" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E407" t="s">
+      <c r="E407" s="2" t="s">
         <v>606</v>
       </c>
-      <c r="F407" t="s">
+      <c r="F407" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G407" t="s">
+      <c r="G407" s="2" t="s">
         <v>926</v>
       </c>
     </row>
     <row r="408" spans="1:7">
-      <c r="A408" t="s">
+      <c r="A408" s="5" t="s">
         <v>1246</v>
       </c>
-      <c r="B408" t="s">
+      <c r="B408" s="5" t="s">
         <v>1247</v>
       </c>
-      <c r="C408" t="s">
+      <c r="C408" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="D408" t="s">
+      <c r="D408" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="E408" t="s">
+      <c r="E408" s="5" t="s">
         <v>1248</v>
       </c>
-      <c r="F408" t="s">
+      <c r="F408" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G408" t="s">
+      <c r="G408" s="5" t="s">
         <v>1249</v>
       </c>
     </row>
     <row r="409" spans="1:7">
-      <c r="A409" t="s">
+      <c r="A409" s="5" t="s">
         <v>1250</v>
       </c>
-      <c r="B409" t="s">
+      <c r="B409" s="5" t="s">
         <v>1251</v>
       </c>
-      <c r="C409" t="s">
+      <c r="C409" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="E409" t="s">
+      <c r="D409" s="5"/>
+      <c r="E409" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="F409" t="s">
-        <v>8</v>
-      </c>
-      <c r="G409" t="s">
+      <c r="F409" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G409" s="5" t="s">
         <v>974</v>
       </c>
     </row>
     <row r="410" spans="1:7">
-      <c r="A410" t="s">
+      <c r="A410" s="5" t="s">
         <v>1252</v>
       </c>
-      <c r="B410" t="s">
+      <c r="B410" s="5" t="s">
         <v>1253</v>
       </c>
-      <c r="C410" t="s">
+      <c r="C410" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="E410" t="s">
+      <c r="D410" s="5"/>
+      <c r="E410" s="5" t="s">
         <v>452</v>
       </c>
-      <c r="F410" t="s">
-        <v>8</v>
-      </c>
-      <c r="G410" t="s">
+      <c r="F410" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G410" s="5" t="s">
         <v>1254</v>
       </c>
     </row>
     <row r="411" spans="1:7">
-      <c r="A411" t="s">
+      <c r="A411" s="5" t="s">
         <v>1255</v>
       </c>
-      <c r="B411" t="s">
+      <c r="B411" s="5" t="s">
         <v>1256</v>
       </c>
-      <c r="C411" t="s">
+      <c r="C411" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="D411" t="s">
+      <c r="D411" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="E411" t="s">
+      <c r="E411" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="F411" t="s">
-        <v>8</v>
-      </c>
-      <c r="G411" t="s">
+      <c r="F411" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G411" s="5" t="s">
         <v>1257</v>
       </c>
     </row>
     <row r="412" spans="1:7">
-      <c r="A412" t="s">
+      <c r="A412" s="5" t="s">
         <v>1258</v>
       </c>
-      <c r="B412" t="s">
+      <c r="B412" s="5" t="s">
         <v>1259</v>
       </c>
-      <c r="C412" t="s">
+      <c r="C412" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="D412" t="s">
+      <c r="D412" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="E412" t="s">
+      <c r="E412" s="5" t="s">
         <v>452</v>
       </c>
-      <c r="F412" t="s">
-        <v>8</v>
-      </c>
-      <c r="G412" t="s">
+      <c r="F412" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G412" s="5" t="s">
         <v>1260</v>
       </c>
     </row>
     <row r="413" spans="1:7">
-      <c r="A413" t="s">
+      <c r="A413" s="5" t="s">
         <v>1261</v>
       </c>
-      <c r="B413" t="s">
+      <c r="B413" s="5" t="s">
         <v>1262</v>
       </c>
-      <c r="C413" t="s">
+      <c r="C413" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E413" t="s">
+      <c r="D413" s="5"/>
+      <c r="E413" s="5" t="s">
         <v>1263</v>
       </c>
-      <c r="F413" t="s">
+      <c r="F413" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G413" t="s">
+      <c r="G413" s="5" t="s">
         <v>1264</v>
       </c>
     </row>
     <row r="414" spans="1:7">
-      <c r="A414" t="s">
+      <c r="A414" s="5" t="s">
         <v>1265</v>
       </c>
-      <c r="B414" t="s">
+      <c r="B414" s="5" t="s">
         <v>1266</v>
       </c>
-      <c r="C414" t="s">
+      <c r="C414" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D414" t="s">
+      <c r="D414" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="E414" t="s">
+      <c r="E414" s="5" t="s">
         <v>1267</v>
       </c>
-      <c r="F414" t="s">
-        <v>8</v>
-      </c>
-      <c r="G414" t="s">
+      <c r="F414" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G414" s="5" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="415" spans="1:7">
-      <c r="A415" t="s">
+      <c r="A415" s="5" t="s">
         <v>1268</v>
       </c>
-      <c r="B415" t="s">
+      <c r="B415" s="5" t="s">
         <v>1269</v>
       </c>
-      <c r="C415" t="s">
+      <c r="C415" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D415" t="s">
+      <c r="D415" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E415" t="s">
+      <c r="E415" s="5" t="s">
         <v>1267</v>
       </c>
-      <c r="F415" t="s">
-        <v>8</v>
-      </c>
-      <c r="G415" t="s">
+      <c r="F415" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G415" s="5" t="s">
         <v>1270</v>
       </c>
     </row>
     <row r="416" spans="1:7">
-      <c r="A416" t="s">
+      <c r="A416" s="5" t="s">
         <v>1271</v>
       </c>
-      <c r="B416" t="s">
+      <c r="B416" s="5" t="s">
         <v>1272</v>
       </c>
-      <c r="C416" t="s">
+      <c r="C416" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D416" t="s">
+      <c r="D416" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E416" t="s">
+      <c r="E416" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="F416" t="s">
+      <c r="F416" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G416" t="s">
+      <c r="G416" s="5" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="417" spans="1:7">
-      <c r="A417" t="s">
+      <c r="A417" s="5" t="s">
         <v>1273</v>
       </c>
-      <c r="B417" t="s">
+      <c r="B417" s="5" t="s">
         <v>1274</v>
       </c>
-      <c r="C417" t="s">
+      <c r="C417" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D417" t="s">
+      <c r="D417" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E417" t="s">
+      <c r="E417" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="F417" t="s">
-        <v>8</v>
-      </c>
-      <c r="G417" t="s">
+      <c r="F417" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G417" s="5" t="s">
         <v>1275</v>
       </c>
     </row>
     <row r="418" spans="1:7">
-      <c r="A418" t="s">
+      <c r="A418" s="5" t="s">
         <v>1276</v>
       </c>
-      <c r="B418" t="s">
+      <c r="B418" s="5" t="s">
         <v>1277</v>
       </c>
-      <c r="C418" t="s">
+      <c r="C418" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="E418" t="s">
+      <c r="D418" s="5"/>
+      <c r="E418" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F418" t="s">
+      <c r="F418" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="G418" t="s">
+      <c r="G418" s="5" t="s">
         <v>706</v>
       </c>
     </row>
     <row r="419" spans="1:7">
-      <c r="A419" t="s">
+      <c r="A419" s="5" t="s">
         <v>1278</v>
       </c>
-      <c r="B419" t="s">
+      <c r="B419" s="5" t="s">
         <v>1279</v>
       </c>
-      <c r="C419" t="s">
+      <c r="C419" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E419" t="s">
+      <c r="D419" s="5"/>
+      <c r="E419" s="5" t="s">
         <v>351</v>
       </c>
-      <c r="F419" t="s">
+      <c r="F419" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G419" t="s">
+      <c r="G419" s="5" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="420" spans="1:7">
-      <c r="A420" t="s">
+      <c r="A420" s="5" t="s">
         <v>1280</v>
       </c>
-      <c r="B420" t="s">
+      <c r="B420" s="5" t="s">
         <v>1281</v>
       </c>
-      <c r="C420" t="s">
+      <c r="C420" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E420" t="s">
+      <c r="D420" s="5"/>
+      <c r="E420" s="5" t="s">
         <v>452</v>
       </c>
-      <c r="F420" t="s">
+      <c r="F420" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G420" t="s">
+      <c r="G420" s="5" t="s">
         <v>576</v>
       </c>
     </row>
     <row r="421" spans="1:7">
-      <c r="A421" t="s">
+      <c r="A421" s="5" t="s">
         <v>1282</v>
       </c>
-      <c r="B421" t="s">
+      <c r="B421" s="5" t="s">
         <v>1283</v>
       </c>
-      <c r="C421" t="s">
+      <c r="C421" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="E421" t="s">
+      <c r="D421" s="5"/>
+      <c r="E421" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F421" t="s">
+      <c r="F421" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G421" t="s">
+      <c r="G421" s="5" t="s">
         <v>517</v>
       </c>
     </row>
     <row r="422" spans="1:7">
-      <c r="A422" t="s">
+      <c r="A422" s="5" t="s">
         <v>1284</v>
       </c>
-      <c r="B422" t="s">
+      <c r="B422" s="5" t="s">
         <v>1285</v>
       </c>
-      <c r="C422" t="s">
+      <c r="C422" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="E422" t="s">
+      <c r="D422" s="5"/>
+      <c r="E422" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="F422" t="s">
+      <c r="F422" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G422" t="s">
+      <c r="G422" s="5" t="s">
         <v>1286</v>
       </c>
     </row>
     <row r="423" spans="1:7">
-      <c r="A423" t="s">
+      <c r="A423" s="5" t="s">
         <v>1287</v>
       </c>
-      <c r="B423" t="s">
+      <c r="B423" s="5" t="s">
         <v>1288</v>
       </c>
-      <c r="C423" t="s">
+      <c r="C423" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E423" t="s">
+      <c r="D423" s="5"/>
+      <c r="E423" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="F423" t="s">
+      <c r="F423" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G423" t="s">
+      <c r="G423" s="5" t="s">
         <v>1289</v>
       </c>
     </row>
     <row r="424" spans="1:7">
-      <c r="A424" t="s">
+      <c r="A424" s="5" t="s">
         <v>1290</v>
       </c>
-      <c r="B424" t="s">
+      <c r="B424" s="5" t="s">
         <v>1291</v>
       </c>
-      <c r="C424" t="s">
+      <c r="C424" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D424" t="s">
+      <c r="D424" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="E424" t="s">
+      <c r="E424" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="F424" t="s">
+      <c r="F424" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G424" t="s">
+      <c r="G424" s="5" t="s">
         <v>1292</v>
       </c>
     </row>
     <row r="425" spans="1:7">
-      <c r="A425" t="s">
+      <c r="A425" s="5" t="s">
         <v>1293</v>
       </c>
-      <c r="B425" t="s">
+      <c r="B425" s="5" t="s">
         <v>1294</v>
       </c>
-      <c r="C425" t="s">
+      <c r="C425" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="E425" t="s">
+      <c r="D425" s="5"/>
+      <c r="E425" s="5" t="s">
         <v>355</v>
       </c>
-      <c r="F425" t="s">
-        <v>8</v>
-      </c>
-      <c r="G425" t="s">
+      <c r="F425" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G425" s="5" t="s">
         <v>1295</v>
       </c>
     </row>
     <row r="426" spans="1:7">
-      <c r="A426" t="s">
+      <c r="A426" s="5" t="s">
         <v>1296</v>
       </c>
-      <c r="B426" t="s">
+      <c r="B426" s="5" t="s">
         <v>1297</v>
       </c>
-      <c r="C426" t="s">
+      <c r="C426" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="D426" t="s">
+      <c r="D426" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E426" t="s">
+      <c r="E426" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="F426" t="s">
+      <c r="F426" s="5" t="s">
         <v>1005</v>
       </c>
-      <c r="G426" t="s">
+      <c r="G426" s="5" t="s">
         <v>926</v>
       </c>
     </row>
     <row r="427" spans="1:7">
-      <c r="A427" t="s">
+      <c r="A427" s="5" t="s">
         <v>1298</v>
       </c>
-      <c r="B427" t="s">
+      <c r="B427" s="5" t="s">
         <v>1299</v>
       </c>
-      <c r="C427" t="s">
+      <c r="C427" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="D427" t="s">
+      <c r="D427" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E427" t="s">
+      <c r="E427" s="5" t="s">
         <v>1300</v>
       </c>
-      <c r="F427" t="s">
+      <c r="F427" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="G427" t="s">
+      <c r="G427" s="5" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="428" spans="1:7">
-      <c r="A428" t="s">
+      <c r="A428" s="5" t="s">
         <v>1301</v>
       </c>
-      <c r="B428" t="s">
+      <c r="B428" s="5" t="s">
         <v>1302</v>
       </c>
-      <c r="C428" t="s">
+      <c r="C428" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="E428" t="s">
+      <c r="D428" s="5"/>
+      <c r="E428" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="F428" t="s">
+      <c r="F428" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G428" t="s">
+      <c r="G428" s="5" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="429" spans="1:7">
-      <c r="A429" t="s">
+      <c r="A429" s="5" t="s">
         <v>1303</v>
       </c>
-      <c r="B429" t="s">
+      <c r="B429" s="5" t="s">
         <v>1304</v>
       </c>
-      <c r="C429" t="s">
+      <c r="C429" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="E429" t="s">
+      <c r="D429" s="5"/>
+      <c r="E429" s="5" t="s">
         <v>737</v>
       </c>
-      <c r="F429" t="s">
+      <c r="F429" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="G429" t="s">
+      <c r="G429" s="5" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="430" spans="1:7">
-      <c r="A430" t="s">
+      <c r="A430" s="5" t="s">
         <v>1305</v>
       </c>
-      <c r="B430" t="s">
+      <c r="B430" s="5" t="s">
         <v>1306</v>
       </c>
-      <c r="C430" t="s">
+      <c r="C430" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="E430" t="s">
+      <c r="D430" s="5"/>
+      <c r="E430" s="5" t="s">
         <v>452</v>
       </c>
-      <c r="F430" t="s">
-        <v>8</v>
-      </c>
-      <c r="G430" t="s">
+      <c r="F430" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G430" s="5" t="s">
         <v>1307</v>
       </c>
     </row>
     <row r="431" spans="1:7">
-      <c r="A431" t="s">
+      <c r="A431" s="5" t="s">
         <v>1308</v>
       </c>
-      <c r="B431" t="s">
+      <c r="B431" s="5" t="s">
         <v>1309</v>
       </c>
-      <c r="C431" t="s">
+      <c r="C431" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="D431" t="s">
+      <c r="D431" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E431" t="s">
+      <c r="E431" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="F431" t="s">
+      <c r="F431" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="G431" t="s">
+      <c r="G431" s="5" t="s">
         <v>1310</v>
       </c>
     </row>
     <row r="432" spans="1:7">
-      <c r="A432" t="s">
+      <c r="A432" s="5" t="s">
         <v>1311</v>
       </c>
-      <c r="B432" t="s">
+      <c r="B432" s="5" t="s">
         <v>1312</v>
       </c>
-      <c r="C432" t="s">
+      <c r="C432" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="E432" t="s">
+      <c r="D432" s="5"/>
+      <c r="E432" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F432" t="s">
+      <c r="F432" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G432" t="s">
+      <c r="G432" s="5" t="s">
         <v>706</v>
       </c>
     </row>
     <row r="433" spans="1:7">
-      <c r="A433" t="s">
+      <c r="A433" s="5" t="s">
         <v>1313</v>
       </c>
-      <c r="B433" t="s">
+      <c r="B433" s="5" t="s">
         <v>1314</v>
       </c>
-      <c r="C433" t="s">
+      <c r="C433" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="E433" t="s">
+      <c r="D433" s="5"/>
+      <c r="E433" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="F433" t="s">
+      <c r="F433" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G433" t="s">
+      <c r="G433" s="5" t="s">
         <v>1315</v>
       </c>
     </row>
     <row r="434" spans="1:7">
-      <c r="A434" t="s">
+      <c r="A434" s="5" t="s">
         <v>1316</v>
       </c>
-      <c r="B434" t="s">
+      <c r="B434" s="5" t="s">
         <v>1317</v>
       </c>
-      <c r="C434" t="s">
+      <c r="C434" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E434" t="s">
+      <c r="D434" s="5"/>
+      <c r="E434" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="F434" t="s">
+      <c r="F434" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G434" t="s">
+      <c r="G434" s="5" t="s">
         <v>1318</v>
       </c>
     </row>
     <row r="435" spans="1:7">
-      <c r="A435" t="s">
+      <c r="A435" s="5" t="s">
         <v>1319</v>
       </c>
-      <c r="B435" t="s">
+      <c r="B435" s="5" t="s">
         <v>1320</v>
       </c>
-      <c r="C435" t="s">
+      <c r="C435" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D435" t="s">
+      <c r="D435" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="E435" t="s">
+      <c r="E435" s="5" t="s">
         <v>351</v>
       </c>
-      <c r="F435" t="s">
+      <c r="F435" s="5" t="s">
         <v>359</v>
       </c>
-      <c r="G435" t="s">
+      <c r="G435" s="5" t="s">
         <v>1321</v>
       </c>
     </row>
     <row r="436" spans="1:7">
-      <c r="A436" t="s">
+      <c r="A436" s="5" t="s">
         <v>1322</v>
       </c>
-      <c r="B436" t="s">
+      <c r="B436" s="5" t="s">
         <v>1323</v>
       </c>
-      <c r="C436" t="s">
+      <c r="C436" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D436" t="s">
+      <c r="D436" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="E436" t="s">
+      <c r="E436" s="5" t="s">
         <v>737</v>
       </c>
-      <c r="F436" t="s">
+      <c r="F436" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="G436" t="s">
+      <c r="G436" s="5" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="437" spans="1:7">
-      <c r="A437" t="s">
+      <c r="A437" s="5" t="s">
         <v>1324</v>
       </c>
-      <c r="B437" t="s">
+      <c r="B437" s="5" t="s">
         <v>1325</v>
       </c>
-      <c r="C437" t="s">
+      <c r="C437" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="D437" t="s">
+      <c r="D437" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E437" t="s">
+      <c r="E437" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="F437" t="s">
+      <c r="F437" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G437" t="s">
+      <c r="G437" s="5" t="s">
         <v>1326</v>
       </c>
     </row>
     <row r="438" spans="1:7">
-      <c r="A438" t="s">
+      <c r="A438" s="5" t="s">
         <v>1327</v>
       </c>
-      <c r="B438" t="s">
+      <c r="B438" s="5" t="s">
         <v>1328</v>
       </c>
-      <c r="C438" t="s">
+      <c r="C438" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="D438" t="s">
+      <c r="D438" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E438" t="s">
+      <c r="E438" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F438" t="s">
+      <c r="F438" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="G438" t="s">
+      <c r="G438" s="5" t="s">
         <v>796</v>
       </c>
     </row>
     <row r="439" spans="1:7">
-      <c r="A439" t="s">
+      <c r="A439" s="5" t="s">
         <v>1329</v>
       </c>
-      <c r="B439" t="s">
+      <c r="B439" s="5" t="s">
         <v>1330</v>
       </c>
-      <c r="C439" t="s">
+      <c r="C439" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="E439" t="s">
+      <c r="D439" s="5"/>
+      <c r="E439" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="F439" t="s">
+      <c r="F439" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G439" t="s">
+      <c r="G439" s="5" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="440" spans="1:7">
-      <c r="A440" t="s">
+      <c r="A440" s="5" t="s">
         <v>1331</v>
       </c>
-      <c r="B440" t="s">
+      <c r="B440" s="5" t="s">
         <v>1332</v>
       </c>
-      <c r="C440" t="s">
+      <c r="C440" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="D440" t="s">
+      <c r="D440" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E440" t="s">
+      <c r="E440" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F440" t="s">
+      <c r="F440" s="5" t="s">
         <v>1333</v>
       </c>
-      <c r="G440" t="s">
+      <c r="G440" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="441" spans="1:7">
-      <c r="A441" t="s">
+      <c r="A441" s="5" t="s">
         <v>1334</v>
       </c>
-      <c r="B441" t="s">
+      <c r="B441" s="5" t="s">
         <v>1335</v>
       </c>
-      <c r="C441" t="s">
+      <c r="C441" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="E441" t="s">
+      <c r="D441" s="5"/>
+      <c r="E441" s="5" t="s">
         <v>1336</v>
       </c>
-      <c r="F441" t="s">
+      <c r="F441" s="5" t="s">
         <v>1337</v>
       </c>
-      <c r="G441" t="s">
+      <c r="G441" s="5" t="s">
         <v>1338</v>
       </c>
     </row>
     <row r="442" spans="1:7">
-      <c r="A442" t="s">
+      <c r="A442" s="5" t="s">
         <v>1339</v>
       </c>
-      <c r="B442" t="s">
+      <c r="B442" s="5" t="s">
         <v>1340</v>
       </c>
-      <c r="C442" t="s">
+      <c r="C442" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D442" t="s">
+      <c r="D442" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E442" t="s">
+      <c r="E442" s="5" t="s">
         <v>628</v>
       </c>
-      <c r="F442" t="s">
+      <c r="F442" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="G442" t="s">
+      <c r="G442" s="5" t="s">
         <v>1058</v>
       </c>
     </row>
     <row r="443" spans="1:7">
-      <c r="A443" t="s">
+      <c r="A443" s="5" t="s">
         <v>1341</v>
       </c>
-      <c r="B443" t="s">
+      <c r="B443" s="5" t="s">
         <v>1342</v>
       </c>
-      <c r="C443" t="s">
+      <c r="C443" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="D443" t="s">
+      <c r="D443" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="E443" t="s">
+      <c r="E443" s="5" t="s">
         <v>404</v>
       </c>
-      <c r="F443" t="s">
+      <c r="F443" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="G443" t="s">
+      <c r="G443" s="5" t="s">
         <v>1075</v>
       </c>
     </row>
     <row r="444" spans="1:7">
-      <c r="A444" t="s">
+      <c r="A444" s="5" t="s">
         <v>1343</v>
       </c>
-      <c r="B444" t="s">
+      <c r="B444" s="5" t="s">
         <v>1344</v>
       </c>
-      <c r="C444" t="s">
+      <c r="C444" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="D444" t="s">
+      <c r="D444" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="E444" t="s">
+      <c r="E444" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="F444" t="s">
-        <v>8</v>
-      </c>
-      <c r="G444" t="s">
+      <c r="F444" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G444" s="5" t="s">
         <v>712</v>
       </c>
     </row>
     <row r="445" spans="1:7">
-      <c r="A445" t="s">
+      <c r="A445" s="5" t="s">
         <v>1345</v>
       </c>
-      <c r="B445" t="s">
+      <c r="B445" s="5" t="s">
         <v>1346</v>
       </c>
-      <c r="C445" t="s">
+      <c r="C445" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="D445" t="s">
+      <c r="D445" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="E445" t="s">
+      <c r="E445" s="5" t="s">
         <v>628</v>
       </c>
-      <c r="F445" t="s">
-        <v>8</v>
-      </c>
-      <c r="G445" t="s">
+      <c r="F445" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G445" s="5" t="s">
         <v>443</v>
       </c>
     </row>
     <row r="446" spans="1:7">
-      <c r="A446" t="s">
+      <c r="A446" s="5" t="s">
         <v>1347</v>
       </c>
-      <c r="B446" t="s">
+      <c r="B446" s="5" t="s">
         <v>1348</v>
       </c>
-      <c r="C446" t="s">
+      <c r="C446" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="D446" t="s">
+      <c r="D446" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="E446" t="s">
+      <c r="E446" s="5" t="s">
         <v>524</v>
       </c>
-      <c r="F446" t="s">
-        <v>8</v>
-      </c>
-      <c r="G446" t="s">
+      <c r="F446" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G446" s="5" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="447" spans="1:7">
-      <c r="A447" t="s">
+      <c r="A447" s="5" t="s">
         <v>1349</v>
       </c>
-      <c r="B447" t="s">
+      <c r="B447" s="5" t="s">
         <v>1350</v>
       </c>
-      <c r="C447" t="s">
+      <c r="C447" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="E447" t="s">
+      <c r="D447" s="5"/>
+      <c r="E447" s="5" t="s">
         <v>650</v>
       </c>
-      <c r="F447" t="s">
+      <c r="F447" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="G447" t="s">
+      <c r="G447" s="5" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="448" spans="1:7">
-      <c r="A448" t="s">
+      <c r="A448" s="5" t="s">
         <v>1351</v>
       </c>
-      <c r="B448" t="s">
+      <c r="B448" s="5" t="s">
         <v>1352</v>
       </c>
-      <c r="C448" t="s">
+      <c r="C448" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="E448" t="s">
+      <c r="D448" s="5"/>
+      <c r="E448" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="F448" t="s">
+      <c r="F448" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G448" t="s">
+      <c r="G448" s="5" t="s">
         <v>893</v>
       </c>
     </row>
     <row r="449" spans="1:7">
-      <c r="A449" t="s">
+      <c r="A449" s="5" t="s">
         <v>1353</v>
       </c>
-      <c r="B449" t="s">
+      <c r="B449" s="5" t="s">
         <v>1354</v>
       </c>
-      <c r="C449" t="s">
+      <c r="C449" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="D449" t="s">
+      <c r="D449" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="E449" t="s">
+      <c r="E449" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="F449" t="s">
-        <v>8</v>
-      </c>
-      <c r="G449" t="s">
+      <c r="F449" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G449" s="5" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="450" spans="1:7">
-      <c r="A450" t="s">
+      <c r="A450" s="5" t="s">
         <v>1355</v>
       </c>
-      <c r="B450" t="s">
+      <c r="B450" s="5" t="s">
         <v>1356</v>
       </c>
-      <c r="C450" t="s">
+      <c r="C450" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="E450" t="s">
+      <c r="D450" s="5"/>
+      <c r="E450" s="5" t="s">
         <v>351</v>
       </c>
-      <c r="F450" t="s">
+      <c r="F450" s="5" t="s">
         <v>1357</v>
       </c>
-      <c r="G450" t="s">
+      <c r="G450" s="5" t="s">
         <v>1358</v>
       </c>
     </row>
     <row r="451" spans="1:7">
-      <c r="A451" t="s">
+      <c r="A451" s="5" t="s">
         <v>1359</v>
       </c>
-      <c r="B451" t="s">
+      <c r="B451" s="5" t="s">
         <v>1360</v>
       </c>
-      <c r="C451" t="s">
+      <c r="C451" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="E451" t="s">
+      <c r="D451" s="5"/>
+      <c r="E451" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="F451" t="s">
+      <c r="F451" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="G451" t="s">
+      <c r="G451" s="5" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="452" spans="1:7">
-      <c r="A452" t="s">
+      <c r="A452" s="5" t="s">
         <v>1361</v>
       </c>
-      <c r="B452" t="s">
+      <c r="B452" s="5" t="s">
         <v>1362</v>
       </c>
-      <c r="C452" t="s">
+      <c r="C452" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D452" t="s">
+      <c r="D452" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E452" t="s">
+      <c r="E452" s="5" t="s">
         <v>351</v>
       </c>
-      <c r="F452" t="s">
+      <c r="F452" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G452" t="s">
+      <c r="G452" s="5" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="453" spans="1:7">
-      <c r="A453" t="s">
+      <c r="A453" s="5" t="s">
         <v>1363</v>
       </c>
-      <c r="B453" t="s">
+      <c r="B453" s="5" t="s">
         <v>1364</v>
       </c>
-      <c r="C453" t="s">
+      <c r="C453" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D453" t="s">
+      <c r="D453" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="E453" t="s">
+      <c r="E453" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F453" t="s">
-        <v>8</v>
-      </c>
-      <c r="G453" t="s">
+      <c r="F453" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G453" s="5" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="454" spans="1:7">
-      <c r="A454" t="s">
+      <c r="A454" s="5" t="s">
         <v>1365</v>
       </c>
-      <c r="B454" t="s">
+      <c r="B454" s="5" t="s">
         <v>1366</v>
       </c>
-      <c r="C454" t="s">
+      <c r="C454" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D454" t="s">
+      <c r="D454" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="E454" t="s">
+      <c r="E454" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="F454" t="s">
+      <c r="F454" s="5" t="s">
         <v>1357</v>
       </c>
-      <c r="G454" t="s">
+      <c r="G454" s="5" t="s">
         <v>1212</v>
       </c>
     </row>
     <row r="455" spans="1:7">
-      <c r="A455" t="s">
+      <c r="A455" s="5" t="s">
         <v>1367</v>
       </c>
-      <c r="B455" t="s">
+      <c r="B455" s="5" t="s">
         <v>1368</v>
       </c>
-      <c r="C455" t="s">
+      <c r="C455" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D455" t="s">
+      <c r="D455" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="E455" t="s">
+      <c r="E455" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="F455" t="s">
+      <c r="F455" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G455" t="s">
+      <c r="G455" s="5" t="s">
         <v>1369</v>
       </c>
     </row>
     <row r="456" spans="1:7">
-      <c r="A456" t="s">
+      <c r="A456" s="5" t="s">
         <v>1370</v>
       </c>
-      <c r="B456" t="s">
+      <c r="B456" s="5" t="s">
         <v>1371</v>
       </c>
-      <c r="C456" t="s">
+      <c r="C456" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="E456" t="s">
+      <c r="D456" s="5"/>
+      <c r="E456" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="F456" t="s">
+      <c r="F456" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="G456" t="s">
+      <c r="G456" s="5" t="s">
         <v>662</v>
       </c>
     </row>
     <row r="457" spans="1:7">
-      <c r="A457" t="s">
+      <c r="A457" s="5" t="s">
         <v>1372</v>
       </c>
-      <c r="B457" t="s">
+      <c r="B457" s="5" t="s">
         <v>1373</v>
       </c>
-      <c r="C457" t="s">
+      <c r="C457" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E457" t="s">
+      <c r="D457" s="5"/>
+      <c r="E457" s="5" t="s">
         <v>351</v>
       </c>
-      <c r="F457" t="s">
+      <c r="F457" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G457" t="s">
+      <c r="G457" s="5" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="458" spans="1:7">
-      <c r="A458" t="s">
+      <c r="A458" s="5" t="s">
         <v>1374</v>
       </c>
-      <c r="B458" t="s">
+      <c r="B458" s="5" t="s">
         <v>1375</v>
       </c>
-      <c r="C458" t="s">
+      <c r="C458" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E458" t="s">
+      <c r="D458" s="5"/>
+      <c r="E458" s="5" t="s">
         <v>438</v>
       </c>
-      <c r="F458" t="s">
+      <c r="F458" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G458" t="s">
+      <c r="G458" s="5" t="s">
         <v>910</v>
       </c>
     </row>
     <row r="459" spans="1:7">
-      <c r="A459" t="s">
+      <c r="A459" s="5" t="s">
         <v>1376</v>
       </c>
-      <c r="B459" t="s">
+      <c r="B459" s="5" t="s">
         <v>1377</v>
       </c>
-      <c r="C459" t="s">
+      <c r="C459" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D459" t="s">
+      <c r="D459" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E459" t="s">
+      <c r="E459" s="5" t="s">
         <v>400</v>
       </c>
-      <c r="F459" t="s">
+      <c r="F459" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="G459" t="s">
+      <c r="G459" s="5" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="460" spans="1:7">
-      <c r="A460" t="s">
+      <c r="A460" s="5" t="s">
         <v>1378</v>
       </c>
-      <c r="B460" t="s">
+      <c r="B460" s="5" t="s">
         <v>1379</v>
       </c>
-      <c r="C460" t="s">
+      <c r="C460" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="D460" t="s">
+      <c r="D460" s="5" t="s">
         <v>1117</v>
       </c>
-      <c r="E460" t="s">
+      <c r="E460" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="F460" t="s">
+      <c r="F460" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G460" t="s">
+      <c r="G460" s="5" t="s">
         <v>746</v>
       </c>
     </row>
     <row r="461" spans="1:7">
-      <c r="A461" t="s">
+      <c r="A461" s="5" t="s">
         <v>1380</v>
       </c>
-      <c r="B461" t="s">
+      <c r="B461" s="5" t="s">
         <v>1381</v>
       </c>
-      <c r="C461" t="s">
+      <c r="C461" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="D461" t="s">
+      <c r="D461" s="5" t="s">
         <v>1117</v>
       </c>
-      <c r="E461" t="s">
+      <c r="E461" s="5" t="s">
         <v>452</v>
       </c>
-      <c r="F461" t="s">
+      <c r="F461" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="G461" t="s">
+      <c r="G461" s="5" t="s">
         <v>1382</v>
       </c>
     </row>
     <row r="462" spans="1:7">
-      <c r="A462" t="s">
+      <c r="A462" s="5" t="s">
         <v>1383</v>
       </c>
-      <c r="B462" t="s">
+      <c r="B462" s="5" t="s">
         <v>1384</v>
       </c>
-      <c r="C462" t="s">
+      <c r="C462" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="D462" t="s">
+      <c r="D462" s="5" t="s">
         <v>1117</v>
       </c>
-      <c r="E462" t="s">
+      <c r="E462" s="5" t="s">
         <v>697</v>
       </c>
-      <c r="F462" t="s">
-        <v>8</v>
-      </c>
-      <c r="G462" t="s">
+      <c r="F462" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G462" s="5" t="s">
         <v>1385</v>
       </c>
     </row>
     <row r="463" spans="1:7">
-      <c r="A463" t="s">
+      <c r="A463" s="5" t="s">
         <v>1386</v>
       </c>
-      <c r="B463" t="s">
+      <c r="B463" s="5" t="s">
         <v>1387</v>
       </c>
-      <c r="C463" t="s">
+      <c r="C463" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="D463" t="s">
+      <c r="D463" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="E463" t="s">
+      <c r="E463" s="5" t="s">
         <v>1388</v>
       </c>
-      <c r="F463" t="s">
+      <c r="F463" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="G463" t="s">
+      <c r="G463" s="5" t="s">
         <v>1389</v>
       </c>
     </row>
     <row r="464" spans="1:7">
-      <c r="A464" t="s">
+      <c r="A464" s="5" t="s">
         <v>1390</v>
       </c>
-      <c r="B464" t="s">
+      <c r="B464" s="5" t="s">
         <v>1391</v>
       </c>
-      <c r="C464" t="s">
+      <c r="C464" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="E464" t="s">
+      <c r="D464" s="5"/>
+      <c r="E464" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="F464" t="s">
+      <c r="F464" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="G464" t="s">
+      <c r="G464" s="5" t="s">
         <v>1392</v>
       </c>
     </row>
     <row r="465" spans="1:7">
-      <c r="A465" t="s">
+      <c r="A465" s="5" t="s">
         <v>1393</v>
       </c>
-      <c r="B465" t="s">
+      <c r="B465" s="5" t="s">
         <v>1394</v>
       </c>
-      <c r="C465" t="s">
+      <c r="C465" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="D465" t="s">
+      <c r="D465" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="E465" t="s">
+      <c r="E465" s="5" t="s">
         <v>579</v>
       </c>
-      <c r="F465" t="s">
+      <c r="F465" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="G465" t="s">
+      <c r="G465" s="5" t="s">
         <v>1395</v>
       </c>
     </row>
     <row r="466" spans="1:7">
-      <c r="A466" t="s">
+      <c r="A466" s="5" t="s">
         <v>1396</v>
       </c>
-      <c r="B466" t="s">
+      <c r="B466" s="5" t="s">
         <v>1397</v>
       </c>
-      <c r="C466" t="s">
+      <c r="C466" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="E466" t="s">
+      <c r="D466" s="5"/>
+      <c r="E466" s="5" t="s">
         <v>468</v>
       </c>
-      <c r="F466" t="s">
+      <c r="F466" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="G466" t="s">
+      <c r="G466" s="5" t="s">
         <v>1398</v>
       </c>
     </row>
     <row r="467" spans="1:7">
-      <c r="A467" t="s">
+      <c r="A467" s="5" t="s">
         <v>1399</v>
       </c>
-      <c r="B467" t="s">
+      <c r="B467" s="5" t="s">
         <v>1400</v>
       </c>
-      <c r="C467" t="s">
+      <c r="C467" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="E467" t="s">
+      <c r="D467" s="5"/>
+      <c r="E467" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="F467" t="s">
+      <c r="F467" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="G467" t="s">
+      <c r="G467" s="5" t="s">
         <v>1401</v>
       </c>
     </row>
     <row r="468" spans="1:7">
-      <c r="A468" t="s">
+      <c r="A468" s="5" t="s">
         <v>1402</v>
       </c>
-      <c r="B468" t="s">
+      <c r="B468" s="5" t="s">
         <v>1403</v>
       </c>
-      <c r="C468" t="s">
+      <c r="C468" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E468" t="s">
+      <c r="D468" s="5"/>
+      <c r="E468" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="F468" t="s">
+      <c r="F468" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="G468" t="s">
+      <c r="G468" s="5" t="s">
         <v>1404</v>
       </c>
     </row>
     <row r="469" spans="1:7">
-      <c r="A469" t="s">
+      <c r="A469" s="5" t="s">
         <v>1405</v>
       </c>
-      <c r="B469" t="s">
+      <c r="B469" s="5" t="s">
         <v>1406</v>
       </c>
-      <c r="C469" t="s">
+      <c r="C469" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="D469" t="s">
+      <c r="D469" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E469" t="s">
+      <c r="E469" s="5" t="s">
         <v>1407</v>
       </c>
-      <c r="F469" t="s">
+      <c r="F469" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="G469" t="s">
+      <c r="G469" s="5" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="470" spans="1:7">
-      <c r="A470" t="s">
+      <c r="A470" s="5" t="s">
         <v>1408</v>
       </c>
-      <c r="B470" t="s">
+      <c r="B470" s="5" t="s">
         <v>1409</v>
       </c>
-      <c r="C470" t="s">
+      <c r="C470" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D470" t="s">
+      <c r="D470" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E470" t="s">
+      <c r="E470" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="F470" t="s">
+      <c r="F470" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="G470" t="s">
+      <c r="G470" s="5" t="s">
         <v>1410</v>
       </c>
     </row>
     <row r="471" spans="1:7">
-      <c r="A471" t="s">
+      <c r="A471" s="5" t="s">
         <v>1411</v>
       </c>
-      <c r="B471" t="s">
+      <c r="B471" s="5" t="s">
         <v>1412</v>
       </c>
-      <c r="C471" t="s">
+      <c r="C471" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="E471" t="s">
+      <c r="D471" s="5"/>
+      <c r="E471" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="F471" t="s">
-        <v>8</v>
-      </c>
-      <c r="G471" t="s">
+      <c r="F471" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G471" s="5" t="s">
         <v>1233</v>
       </c>
     </row>
     <row r="472" spans="1:7">
-      <c r="A472" t="s">
+      <c r="A472" s="5" t="s">
         <v>1413</v>
       </c>
-      <c r="B472" t="s">
+      <c r="B472" s="5" t="s">
         <v>1414</v>
       </c>
-      <c r="C472" t="s">
+      <c r="C472" s="5" t="s">
         <v>1117</v>
       </c>
-      <c r="E472" t="s">
+      <c r="D472" s="5"/>
+      <c r="E472" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="F472" t="s">
-        <v>8</v>
-      </c>
-      <c r="G472" t="s">
+      <c r="F472" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G472" s="5" t="s">
         <v>1415</v>
       </c>
     </row>
     <row r="473" spans="1:7">
-      <c r="A473" t="s">
+      <c r="A473" s="5" t="s">
         <v>1416</v>
       </c>
-      <c r="B473" t="s">
+      <c r="B473" s="5" t="s">
         <v>1417</v>
       </c>
-      <c r="C473" t="s">
+      <c r="C473" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="D473" t="s">
+      <c r="D473" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E473" t="s">
+      <c r="E473" s="5" t="s">
         <v>697</v>
       </c>
-      <c r="F473" t="s">
+      <c r="F473" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="G473" t="s">
+      <c r="G473" s="5" t="s">
         <v>1418</v>
       </c>
     </row>
     <row r="474" spans="1:7">
-      <c r="A474" t="s">
+      <c r="A474" s="5" t="s">
         <v>1419</v>
       </c>
-      <c r="B474" t="s">
+      <c r="B474" s="5" t="s">
         <v>1420</v>
       </c>
-      <c r="C474" t="s">
+      <c r="C474" s="5" t="s">
         <v>1117</v>
       </c>
-      <c r="D474" t="s">
+      <c r="D474" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="E474" t="s">
+      <c r="E474" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F474" t="s">
+      <c r="F474" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="G474" t="s">
+      <c r="G474" s="5" t="s">
         <v>1421</v>
       </c>
     </row>
     <row r="475" spans="1:7">
-      <c r="A475" t="s">
+      <c r="A475" s="5" t="s">
         <v>1422</v>
       </c>
-      <c r="B475" t="s">
+      <c r="B475" s="5" t="s">
         <v>1423</v>
       </c>
-      <c r="C475" t="s">
+      <c r="C475" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="E475" t="s">
+      <c r="D475" s="5"/>
+      <c r="E475" s="5" t="s">
         <v>579</v>
       </c>
-      <c r="F475" t="s">
+      <c r="F475" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="G475" t="s">
+      <c r="G475" s="5" t="s">
         <v>1385</v>
       </c>
     </row>
     <row r="476" spans="1:7">
-      <c r="A476" t="s">
+      <c r="A476" s="5" t="s">
         <v>1424</v>
       </c>
-      <c r="B476" t="s">
+      <c r="B476" s="5" t="s">
         <v>1425</v>
       </c>
-      <c r="C476" t="s">
+      <c r="C476" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="D476" t="s">
+      <c r="D476" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="E476" t="s">
+      <c r="E476" s="5" t="s">
         <v>896</v>
       </c>
-      <c r="F476" t="s">
-        <v>8</v>
-      </c>
-      <c r="G476" t="s">
+      <c r="F476" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G476" s="5" t="s">
         <v>829</v>
       </c>
     </row>
     <row r="477" spans="1:7">
-      <c r="A477" t="s">
+      <c r="A477" s="5" t="s">
         <v>1426</v>
       </c>
-      <c r="B477" t="s">
+      <c r="B477" s="5" t="s">
         <v>1427</v>
       </c>
-      <c r="C477" t="s">
+      <c r="C477" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="D477" t="s">
+      <c r="D477" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="E477" t="s">
+      <c r="E477" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="F477" t="s">
+      <c r="F477" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="G477" t="s">
+      <c r="G477" s="5" t="s">
         <v>1428</v>
       </c>
     </row>
     <row r="478" spans="1:7">
-      <c r="A478" t="s">
+      <c r="A478" s="5" t="s">
         <v>1429</v>
       </c>
-      <c r="B478" t="s">
+      <c r="B478" s="5" t="s">
         <v>1430</v>
       </c>
-      <c r="C478" t="s">
+      <c r="C478" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="E478" t="s">
+      <c r="D478" s="5"/>
+      <c r="E478" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F478" t="s">
-        <v>8</v>
-      </c>
-      <c r="G478" t="s">
+      <c r="F478" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G478" s="5" t="s">
         <v>1431</v>
       </c>
     </row>
     <row r="479" spans="1:7">
-      <c r="A479" t="s">
+      <c r="A479" s="5" t="s">
         <v>1432</v>
       </c>
-      <c r="B479" t="s">
+      <c r="B479" s="5" t="s">
         <v>1433</v>
       </c>
-      <c r="C479" t="s">
+      <c r="C479" s="5" t="s">
         <v>1117</v>
       </c>
-      <c r="D479" t="s">
+      <c r="D479" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="E479" t="s">
+      <c r="E479" s="5" t="s">
         <v>737</v>
       </c>
-      <c r="F479" t="s">
+      <c r="F479" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G479" t="s">
+      <c r="G479" s="5" t="s">
         <v>1434</v>
       </c>
     </row>
     <row r="480" spans="1:7">
-      <c r="A480" t="s">
+      <c r="A480" s="5" t="s">
         <v>1435</v>
       </c>
-      <c r="B480" t="s">
+      <c r="B480" s="5" t="s">
         <v>1436</v>
       </c>
-      <c r="C480" t="s">
+      <c r="C480" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="D480" t="s">
+      <c r="D480" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="E480" t="s">
+      <c r="E480" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="F480" t="s">
-        <v>8</v>
-      </c>
-      <c r="G480" t="s">
+      <c r="F480" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G480" s="5" t="s">
         <v>1437</v>
       </c>
     </row>
     <row r="481" spans="1:7">
-      <c r="A481" t="s">
+      <c r="A481" s="5" t="s">
         <v>1438</v>
       </c>
-      <c r="B481" t="s">
+      <c r="B481" s="5" t="s">
         <v>1439</v>
       </c>
-      <c r="C481" t="s">
+      <c r="C481" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E481" t="s">
+      <c r="D481" s="5"/>
+      <c r="E481" s="5" t="s">
         <v>506</v>
       </c>
-      <c r="F481" t="s">
+      <c r="F481" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G481" t="s">
+      <c r="G481" s="5" t="s">
         <v>1437</v>
       </c>
     </row>
     <row r="482" spans="1:7">
-      <c r="A482" t="s">
+      <c r="A482" s="5" t="s">
         <v>1440</v>
       </c>
-      <c r="B482" t="s">
+      <c r="B482" s="5" t="s">
         <v>1441</v>
       </c>
-      <c r="C482" t="s">
+      <c r="C482" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E482" t="s">
+      <c r="D482" s="5"/>
+      <c r="E482" s="5" t="s">
         <v>506</v>
       </c>
-      <c r="F482" t="s">
+      <c r="F482" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G482" t="s">
+      <c r="G482" s="5" t="s">
         <v>1437</v>
       </c>
     </row>
     <row r="483" spans="1:7">
-      <c r="A483" t="s">
+      <c r="A483" s="5" t="s">
         <v>1442</v>
       </c>
-      <c r="B483" t="s">
+      <c r="B483" s="5" t="s">
         <v>1443</v>
       </c>
-      <c r="C483" t="s">
+      <c r="C483" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E483" t="s">
+      <c r="D483" s="5"/>
+      <c r="E483" s="5" t="s">
         <v>506</v>
       </c>
-      <c r="F483" t="s">
+      <c r="F483" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G483" t="s">
+      <c r="G483" s="5" t="s">
         <v>1437</v>
       </c>
     </row>
     <row r="484" spans="1:7">
-      <c r="A484" t="s">
+      <c r="A484" s="5" t="s">
         <v>1444</v>
       </c>
-      <c r="B484" t="s">
+      <c r="B484" s="5" t="s">
         <v>1445</v>
       </c>
-      <c r="C484" t="s">
+      <c r="C484" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="D484" t="s">
+      <c r="D484" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="E484" t="s">
+      <c r="E484" s="5" t="s">
         <v>527</v>
       </c>
-      <c r="F484" t="s">
+      <c r="F484" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G484" t="s">
+      <c r="G484" s="5" t="s">
         <v>1446</v>
       </c>
     </row>
     <row r="485" spans="1:7">
-      <c r="A485" t="s">
+      <c r="A485" s="5" t="s">
         <v>1447</v>
       </c>
-      <c r="B485" t="s">
+      <c r="B485" s="5" t="s">
         <v>1448</v>
       </c>
-      <c r="C485" t="s">
+      <c r="C485" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D485" t="s">
+      <c r="D485" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="E485" t="s">
+      <c r="E485" s="5" t="s">
         <v>527</v>
       </c>
-      <c r="F485" t="s">
+      <c r="F485" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G485" t="s">
+      <c r="G485" s="5" t="s">
         <v>1449</v>
       </c>
     </row>
     <row r="486" spans="1:7">
-      <c r="A486" t="s">
+      <c r="A486" s="5" t="s">
         <v>1450</v>
       </c>
-      <c r="B486" t="s">
+      <c r="B486" s="5" t="s">
         <v>1451</v>
       </c>
-      <c r="C486" t="s">
+      <c r="C486" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D486" t="s">
+      <c r="D486" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="E486" t="s">
+      <c r="E486" s="5" t="s">
         <v>524</v>
       </c>
-      <c r="F486" t="s">
+      <c r="F486" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G486" t="s">
+      <c r="G486" s="5" t="s">
         <v>1452</v>
       </c>
     </row>
     <row r="487" spans="1:7">
-      <c r="A487" t="s">
+      <c r="A487" s="5" t="s">
         <v>1453</v>
       </c>
-      <c r="B487" t="s">
+      <c r="B487" s="5" t="s">
         <v>1454</v>
       </c>
-      <c r="C487" t="s">
+      <c r="C487" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="E487" t="s">
+      <c r="D487" s="5"/>
+      <c r="E487" s="5" t="s">
         <v>1455</v>
       </c>
-      <c r="F487" t="s">
+      <c r="F487" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G487" t="s">
+      <c r="G487" s="5" t="s">
         <v>1456</v>
       </c>
     </row>
     <row r="488" spans="1:7">
-      <c r="A488" t="s">
+      <c r="A488" s="5" t="s">
         <v>1457</v>
       </c>
-      <c r="B488" t="s">
+      <c r="B488" s="5" t="s">
         <v>1458</v>
       </c>
-      <c r="C488" t="s">
+      <c r="C488" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="D488" t="s">
+      <c r="D488" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="E488" t="s">
+      <c r="E488" s="5" t="s">
         <v>527</v>
       </c>
-      <c r="F488" t="s">
+      <c r="F488" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G488" t="s">
+      <c r="G488" s="5" t="s">
         <v>1459</v>
       </c>
     </row>
     <row r="489" spans="1:7">
-      <c r="A489" t="s">
+      <c r="A489" s="5" t="s">
         <v>1460</v>
       </c>
-      <c r="B489" t="s">
+      <c r="B489" s="5" t="s">
         <v>1461</v>
       </c>
-      <c r="C489" t="s">
+      <c r="C489" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E489" t="s">
+      <c r="D489" s="5"/>
+      <c r="E489" s="5" t="s">
         <v>506</v>
       </c>
-      <c r="F489" t="s">
+      <c r="F489" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G489" t="s">
+      <c r="G489" s="5" t="s">
         <v>1462</v>
       </c>
     </row>
     <row r="490" spans="1:7">
-      <c r="A490" t="s">
+      <c r="A490" s="5" t="s">
         <v>1463</v>
       </c>
-      <c r="B490" t="s">
+      <c r="B490" s="5" t="s">
         <v>1464</v>
       </c>
-      <c r="C490" t="s">
+      <c r="C490" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E490" t="s">
+      <c r="D490" s="5"/>
+      <c r="E490" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="F490" t="s">
+      <c r="F490" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="G490" t="s">
+      <c r="G490" s="5" t="s">
         <v>1465</v>
       </c>
     </row>
     <row r="491" spans="1:7">
-      <c r="A491" t="s">
+      <c r="A491" s="5" t="s">
         <v>1466</v>
       </c>
-      <c r="B491" t="s">
+      <c r="B491" s="5" t="s">
         <v>1467</v>
       </c>
-      <c r="C491" t="s">
+      <c r="C491" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E491" t="s">
+      <c r="D491" s="5"/>
+      <c r="E491" s="5" t="s">
         <v>814</v>
       </c>
-      <c r="F491" t="s">
+      <c r="F491" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G491" t="s">
+      <c r="G491" s="5" t="s">
         <v>1468</v>
       </c>
     </row>
     <row r="492" spans="1:7">
-      <c r="A492" t="s">
+      <c r="A492" s="5" t="s">
         <v>1469</v>
       </c>
-      <c r="B492" t="s">
+      <c r="B492" s="5" t="s">
         <v>1470</v>
       </c>
-      <c r="C492" t="s">
+      <c r="C492" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="E492" t="s">
+      <c r="D492" s="5"/>
+      <c r="E492" s="5" t="s">
         <v>814</v>
       </c>
-      <c r="F492" t="s">
+      <c r="F492" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G492" t="s">
+      <c r="G492" s="5" t="s">
         <v>746</v>
       </c>
     </row>
     <row r="493" spans="1:7">
-      <c r="A493" t="s">
+      <c r="A493" s="5" t="s">
         <v>1471</v>
       </c>
-      <c r="B493" t="s">
+      <c r="B493" s="5" t="s">
         <v>1472</v>
       </c>
-      <c r="C493" t="s">
+      <c r="C493" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="E493" t="s">
+      <c r="D493" s="5"/>
+      <c r="E493" s="5" t="s">
         <v>814</v>
       </c>
-      <c r="F493" t="s">
-        <v>8</v>
-      </c>
-      <c r="G493" t="s">
+      <c r="F493" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G493" s="5" t="s">
         <v>666</v>
       </c>
     </row>
     <row r="494" spans="1:7">
-      <c r="A494" t="s">
+      <c r="A494" s="5" t="s">
         <v>1473</v>
       </c>
-      <c r="B494" t="s">
+      <c r="B494" s="5" t="s">
         <v>1474</v>
       </c>
-      <c r="C494" t="s">
+      <c r="C494" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="E494" t="s">
+      <c r="D494" s="5"/>
+      <c r="E494" s="5" t="s">
         <v>1475</v>
       </c>
-      <c r="F494" t="s">
+      <c r="F494" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G494" t="s">
+      <c r="G494" s="5" t="s">
         <v>1476</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adicionado +40 pokémon da 4ª geração
</commit_message>
<xml_diff>
--- a/pokemonv2/pokemons.xlsx
+++ b/pokemonv2/pokemons.xlsx
@@ -8722,8 +8722,8 @@
   <dimension ref="A1:H1026"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A397" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B406" sqref="B406"/>
+      <pane ySplit="1" topLeftCell="A431" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B489" sqref="B489"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8732,7 +8732,7 @@
     <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -17669,884 +17669,884 @@
       </c>
     </row>
     <row r="408" spans="1:7">
-      <c r="A408" s="5" t="s">
+      <c r="A408" s="2" t="s">
         <v>1246</v>
       </c>
-      <c r="B408" s="5" t="s">
+      <c r="B408" s="2" t="s">
         <v>1247</v>
       </c>
-      <c r="C408" s="5" t="s">
+      <c r="C408" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D408" s="5" t="s">
+      <c r="D408" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E408" s="5" t="s">
+      <c r="E408" s="2" t="s">
         <v>1248</v>
       </c>
-      <c r="F408" s="5" t="s">
+      <c r="F408" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G408" s="5" t="s">
+      <c r="G408" s="2" t="s">
         <v>1249</v>
       </c>
     </row>
     <row r="409" spans="1:7">
-      <c r="A409" s="5" t="s">
+      <c r="A409" s="2" t="s">
         <v>1250</v>
       </c>
-      <c r="B409" s="5" t="s">
+      <c r="B409" s="2" t="s">
         <v>1251</v>
       </c>
-      <c r="C409" s="5" t="s">
+      <c r="C409" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="D409" s="5"/>
-      <c r="E409" s="5" t="s">
+      <c r="D409" s="2"/>
+      <c r="E409" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="F409" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G409" s="5" t="s">
+      <c r="F409" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G409" s="2" t="s">
         <v>974</v>
       </c>
     </row>
     <row r="410" spans="1:7">
-      <c r="A410" s="5" t="s">
+      <c r="A410" s="2" t="s">
         <v>1252</v>
       </c>
-      <c r="B410" s="5" t="s">
+      <c r="B410" s="2" t="s">
         <v>1253</v>
       </c>
-      <c r="C410" s="5" t="s">
+      <c r="C410" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="D410" s="5"/>
-      <c r="E410" s="5" t="s">
+      <c r="D410" s="2"/>
+      <c r="E410" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="F410" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G410" s="5" t="s">
+      <c r="F410" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G410" s="2" t="s">
         <v>1254</v>
       </c>
     </row>
     <row r="411" spans="1:7">
-      <c r="A411" s="5" t="s">
+      <c r="A411" s="2" t="s">
         <v>1255</v>
       </c>
-      <c r="B411" s="5" t="s">
+      <c r="B411" s="2" t="s">
         <v>1256</v>
       </c>
-      <c r="C411" s="5" t="s">
+      <c r="C411" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="D411" s="5" t="s">
+      <c r="D411" s="2" t="s">
         <v>1169</v>
       </c>
-      <c r="E411" s="5" t="s">
+      <c r="E411" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="F411" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G411" s="5" t="s">
+      <c r="F411" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G411" s="2" t="s">
         <v>1257</v>
       </c>
     </row>
     <row r="412" spans="1:7">
-      <c r="A412" s="5" t="s">
+      <c r="A412" s="2" t="s">
         <v>1258</v>
       </c>
-      <c r="B412" s="5" t="s">
+      <c r="B412" s="2" t="s">
         <v>1259</v>
       </c>
-      <c r="C412" s="5" t="s">
+      <c r="C412" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="D412" s="5" t="s">
+      <c r="D412" s="2" t="s">
         <v>1169</v>
       </c>
-      <c r="E412" s="5" t="s">
+      <c r="E412" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="F412" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G412" s="5" t="s">
+      <c r="F412" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G412" s="2" t="s">
         <v>1260</v>
       </c>
     </row>
     <row r="413" spans="1:7">
-      <c r="A413" s="5" t="s">
+      <c r="A413" s="2" t="s">
         <v>1261</v>
       </c>
-      <c r="B413" s="5" t="s">
+      <c r="B413" s="2" t="s">
         <v>1262</v>
       </c>
-      <c r="C413" s="5" t="s">
+      <c r="C413" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D413" s="5"/>
-      <c r="E413" s="5" t="s">
+      <c r="D413" s="2"/>
+      <c r="E413" s="2" t="s">
         <v>1263</v>
       </c>
-      <c r="F413" s="5" t="s">
+      <c r="F413" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G413" s="5" t="s">
+      <c r="G413" s="2" t="s">
         <v>1264</v>
       </c>
     </row>
     <row r="414" spans="1:7">
-      <c r="A414" s="5" t="s">
+      <c r="A414" s="2" t="s">
         <v>1265</v>
       </c>
-      <c r="B414" s="5" t="s">
+      <c r="B414" s="2" t="s">
         <v>1266</v>
       </c>
-      <c r="C414" s="5" t="s">
+      <c r="C414" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D414" s="5" t="s">
+      <c r="D414" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="E414" s="5" t="s">
+      <c r="E414" s="2" t="s">
         <v>1267</v>
       </c>
-      <c r="F414" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G414" s="5" t="s">
+      <c r="F414" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G414" s="2" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="415" spans="1:7">
-      <c r="A415" s="5" t="s">
+      <c r="A415" s="2" t="s">
         <v>1268</v>
       </c>
-      <c r="B415" s="5" t="s">
+      <c r="B415" s="2" t="s">
         <v>1269</v>
       </c>
-      <c r="C415" s="5" t="s">
+      <c r="C415" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D415" s="5" t="s">
+      <c r="D415" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E415" s="5" t="s">
+      <c r="E415" s="2" t="s">
         <v>1267</v>
       </c>
-      <c r="F415" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G415" s="5" t="s">
+      <c r="F415" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G415" s="2" t="s">
         <v>1270</v>
       </c>
     </row>
     <row r="416" spans="1:7">
-      <c r="A416" s="5" t="s">
+      <c r="A416" s="2" t="s">
         <v>1271</v>
       </c>
-      <c r="B416" s="5" t="s">
+      <c r="B416" s="2" t="s">
         <v>1272</v>
       </c>
-      <c r="C416" s="5" t="s">
+      <c r="C416" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D416" s="5" t="s">
+      <c r="D416" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E416" s="5" t="s">
+      <c r="E416" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="F416" s="5" t="s">
+      <c r="F416" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G416" s="5" t="s">
+      <c r="G416" s="2" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="417" spans="1:7">
-      <c r="A417" s="5" t="s">
+      <c r="A417" s="2" t="s">
         <v>1273</v>
       </c>
-      <c r="B417" s="5" t="s">
+      <c r="B417" s="2" t="s">
         <v>1274</v>
       </c>
-      <c r="C417" s="5" t="s">
+      <c r="C417" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D417" s="5" t="s">
+      <c r="D417" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E417" s="5" t="s">
+      <c r="E417" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="F417" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G417" s="5" t="s">
+      <c r="F417" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G417" s="2" t="s">
         <v>1275</v>
       </c>
     </row>
     <row r="418" spans="1:7">
-      <c r="A418" s="5" t="s">
+      <c r="A418" s="2" t="s">
         <v>1276</v>
       </c>
-      <c r="B418" s="5" t="s">
+      <c r="B418" s="2" t="s">
         <v>1277</v>
       </c>
-      <c r="C418" s="5" t="s">
+      <c r="C418" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="D418" s="5"/>
-      <c r="E418" s="5" t="s">
+      <c r="D418" s="2"/>
+      <c r="E418" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F418" s="5" t="s">
+      <c r="F418" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="G418" s="5" t="s">
+      <c r="G418" s="2" t="s">
         <v>706</v>
       </c>
     </row>
     <row r="419" spans="1:7">
-      <c r="A419" s="5" t="s">
+      <c r="A419" s="2" t="s">
         <v>1278</v>
       </c>
-      <c r="B419" s="5" t="s">
+      <c r="B419" s="2" t="s">
         <v>1279</v>
       </c>
-      <c r="C419" s="5" t="s">
+      <c r="C419" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D419" s="5"/>
-      <c r="E419" s="5" t="s">
+      <c r="D419" s="2"/>
+      <c r="E419" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="F419" s="5" t="s">
+      <c r="F419" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G419" s="5" t="s">
+      <c r="G419" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="420" spans="1:7">
-      <c r="A420" s="5" t="s">
+      <c r="A420" s="2" t="s">
         <v>1280</v>
       </c>
-      <c r="B420" s="5" t="s">
+      <c r="B420" s="2" t="s">
         <v>1281</v>
       </c>
-      <c r="C420" s="5" t="s">
+      <c r="C420" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D420" s="5"/>
-      <c r="E420" s="5" t="s">
+      <c r="D420" s="2"/>
+      <c r="E420" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="F420" s="5" t="s">
+      <c r="F420" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G420" s="5" t="s">
+      <c r="G420" s="2" t="s">
         <v>576</v>
       </c>
     </row>
     <row r="421" spans="1:7">
-      <c r="A421" s="5" t="s">
+      <c r="A421" s="2" t="s">
         <v>1282</v>
       </c>
-      <c r="B421" s="5" t="s">
+      <c r="B421" s="2" t="s">
         <v>1283</v>
       </c>
-      <c r="C421" s="5" t="s">
+      <c r="C421" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D421" s="5"/>
-      <c r="E421" s="5" t="s">
+      <c r="D421" s="2"/>
+      <c r="E421" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F421" s="5" t="s">
+      <c r="F421" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G421" s="5" t="s">
+      <c r="G421" s="2" t="s">
         <v>517</v>
       </c>
     </row>
     <row r="422" spans="1:7">
-      <c r="A422" s="5" t="s">
+      <c r="A422" s="2" t="s">
         <v>1284</v>
       </c>
-      <c r="B422" s="5" t="s">
+      <c r="B422" s="2" t="s">
         <v>1285</v>
       </c>
-      <c r="C422" s="5" t="s">
+      <c r="C422" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D422" s="5"/>
-      <c r="E422" s="5" t="s">
+      <c r="D422" s="2"/>
+      <c r="E422" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F422" s="5" t="s">
+      <c r="F422" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G422" s="5" t="s">
+      <c r="G422" s="2" t="s">
         <v>1286</v>
       </c>
     </row>
     <row r="423" spans="1:7">
-      <c r="A423" s="5" t="s">
+      <c r="A423" s="2" t="s">
         <v>1287</v>
       </c>
-      <c r="B423" s="5" t="s">
+      <c r="B423" s="2" t="s">
         <v>1288</v>
       </c>
-      <c r="C423" s="5" t="s">
+      <c r="C423" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D423" s="5"/>
-      <c r="E423" s="5" t="s">
+      <c r="D423" s="2"/>
+      <c r="E423" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="F423" s="5" t="s">
+      <c r="F423" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G423" s="5" t="s">
+      <c r="G423" s="2" t="s">
         <v>1289</v>
       </c>
     </row>
     <row r="424" spans="1:7">
-      <c r="A424" s="5" t="s">
+      <c r="A424" s="2" t="s">
         <v>1290</v>
       </c>
-      <c r="B424" s="5" t="s">
+      <c r="B424" s="2" t="s">
         <v>1291</v>
       </c>
-      <c r="C424" s="5" t="s">
+      <c r="C424" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D424" s="5" t="s">
+      <c r="D424" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="E424" s="5" t="s">
+      <c r="E424" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="F424" s="5" t="s">
+      <c r="F424" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G424" s="5" t="s">
+      <c r="G424" s="2" t="s">
         <v>1292</v>
       </c>
     </row>
     <row r="425" spans="1:7">
-      <c r="A425" s="5" t="s">
+      <c r="A425" s="2" t="s">
         <v>1293</v>
       </c>
-      <c r="B425" s="5" t="s">
+      <c r="B425" s="2" t="s">
         <v>1294</v>
       </c>
-      <c r="C425" s="5" t="s">
+      <c r="C425" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D425" s="5"/>
-      <c r="E425" s="5" t="s">
+      <c r="D425" s="2"/>
+      <c r="E425" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="F425" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G425" s="5" t="s">
+      <c r="F425" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G425" s="2" t="s">
         <v>1295</v>
       </c>
     </row>
     <row r="426" spans="1:7">
-      <c r="A426" s="5" t="s">
+      <c r="A426" s="2" t="s">
         <v>1296</v>
       </c>
-      <c r="B426" s="5" t="s">
+      <c r="B426" s="2" t="s">
         <v>1297</v>
       </c>
-      <c r="C426" s="5" t="s">
+      <c r="C426" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="D426" s="5" t="s">
+      <c r="D426" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E426" s="5" t="s">
+      <c r="E426" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="F426" s="5" t="s">
+      <c r="F426" s="2" t="s">
         <v>1005</v>
       </c>
-      <c r="G426" s="5" t="s">
+      <c r="G426" s="2" t="s">
         <v>926</v>
       </c>
     </row>
     <row r="427" spans="1:7">
-      <c r="A427" s="5" t="s">
+      <c r="A427" s="2" t="s">
         <v>1298</v>
       </c>
-      <c r="B427" s="5" t="s">
+      <c r="B427" s="2" t="s">
         <v>1299</v>
       </c>
-      <c r="C427" s="5" t="s">
+      <c r="C427" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="D427" s="5" t="s">
+      <c r="D427" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E427" s="5" t="s">
+      <c r="E427" s="2" t="s">
         <v>1300</v>
       </c>
-      <c r="F427" s="5" t="s">
+      <c r="F427" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="G427" s="5" t="s">
+      <c r="G427" s="2" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="428" spans="1:7">
-      <c r="A428" s="5" t="s">
+      <c r="A428" s="2" t="s">
         <v>1301</v>
       </c>
-      <c r="B428" s="5" t="s">
+      <c r="B428" s="2" t="s">
         <v>1302</v>
       </c>
-      <c r="C428" s="5" t="s">
+      <c r="C428" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D428" s="5"/>
-      <c r="E428" s="5" t="s">
+      <c r="D428" s="2"/>
+      <c r="E428" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="F428" s="5" t="s">
+      <c r="F428" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G428" s="5" t="s">
+      <c r="G428" s="2" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="429" spans="1:7">
-      <c r="A429" s="5" t="s">
+      <c r="A429" s="2" t="s">
         <v>1303</v>
       </c>
-      <c r="B429" s="5" t="s">
+      <c r="B429" s="2" t="s">
         <v>1304</v>
       </c>
-      <c r="C429" s="5" t="s">
+      <c r="C429" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D429" s="5"/>
-      <c r="E429" s="5" t="s">
+      <c r="D429" s="2"/>
+      <c r="E429" s="2" t="s">
         <v>737</v>
       </c>
-      <c r="F429" s="5" t="s">
+      <c r="F429" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="G429" s="5" t="s">
+      <c r="G429" s="2" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="430" spans="1:7">
-      <c r="A430" s="5" t="s">
+      <c r="A430" s="2" t="s">
         <v>1305</v>
       </c>
-      <c r="B430" s="5" t="s">
+      <c r="B430" s="2" t="s">
         <v>1306</v>
       </c>
-      <c r="C430" s="5" t="s">
+      <c r="C430" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="D430" s="5"/>
-      <c r="E430" s="5" t="s">
+      <c r="D430" s="2"/>
+      <c r="E430" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="F430" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G430" s="5" t="s">
+      <c r="F430" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G430" s="2" t="s">
         <v>1307</v>
       </c>
     </row>
     <row r="431" spans="1:7">
-      <c r="A431" s="5" t="s">
+      <c r="A431" s="2" t="s">
         <v>1308</v>
       </c>
-      <c r="B431" s="5" t="s">
+      <c r="B431" s="2" t="s">
         <v>1309</v>
       </c>
-      <c r="C431" s="5" t="s">
+      <c r="C431" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="D431" s="5" t="s">
+      <c r="D431" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E431" s="5" t="s">
+      <c r="E431" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="F431" s="5" t="s">
+      <c r="F431" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="G431" s="5" t="s">
+      <c r="G431" s="2" t="s">
         <v>1310</v>
       </c>
     </row>
     <row r="432" spans="1:7">
-      <c r="A432" s="5" t="s">
+      <c r="A432" s="2" t="s">
         <v>1311</v>
       </c>
-      <c r="B432" s="5" t="s">
+      <c r="B432" s="2" t="s">
         <v>1312</v>
       </c>
-      <c r="C432" s="5" t="s">
+      <c r="C432" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D432" s="5"/>
-      <c r="E432" s="5" t="s">
+      <c r="D432" s="2"/>
+      <c r="E432" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F432" s="5" t="s">
+      <c r="F432" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G432" s="5" t="s">
+      <c r="G432" s="2" t="s">
         <v>706</v>
       </c>
     </row>
     <row r="433" spans="1:7">
-      <c r="A433" s="5" t="s">
+      <c r="A433" s="2" t="s">
         <v>1313</v>
       </c>
-      <c r="B433" s="5" t="s">
+      <c r="B433" s="2" t="s">
         <v>1314</v>
       </c>
-      <c r="C433" s="5" t="s">
+      <c r="C433" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D433" s="5"/>
-      <c r="E433" s="5" t="s">
+      <c r="D433" s="2"/>
+      <c r="E433" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F433" s="5" t="s">
+      <c r="F433" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G433" s="5" t="s">
+      <c r="G433" s="2" t="s">
         <v>1315</v>
       </c>
     </row>
     <row r="434" spans="1:7">
-      <c r="A434" s="5" t="s">
+      <c r="A434" s="2" t="s">
         <v>1316</v>
       </c>
-      <c r="B434" s="5" t="s">
+      <c r="B434" s="2" t="s">
         <v>1317</v>
       </c>
-      <c r="C434" s="5" t="s">
+      <c r="C434" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D434" s="5"/>
-      <c r="E434" s="5" t="s">
+      <c r="D434" s="2"/>
+      <c r="E434" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="F434" s="5" t="s">
+      <c r="F434" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G434" s="5" t="s">
+      <c r="G434" s="2" t="s">
         <v>1318</v>
       </c>
     </row>
     <row r="435" spans="1:7">
-      <c r="A435" s="5" t="s">
+      <c r="A435" s="2" t="s">
         <v>1319</v>
       </c>
-      <c r="B435" s="5" t="s">
+      <c r="B435" s="2" t="s">
         <v>1320</v>
       </c>
-      <c r="C435" s="5" t="s">
+      <c r="C435" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D435" s="5" t="s">
+      <c r="D435" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="E435" s="5" t="s">
+      <c r="E435" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="F435" s="5" t="s">
+      <c r="F435" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="G435" s="5" t="s">
+      <c r="G435" s="2" t="s">
         <v>1321</v>
       </c>
     </row>
     <row r="436" spans="1:7">
-      <c r="A436" s="5" t="s">
+      <c r="A436" s="2" t="s">
         <v>1322</v>
       </c>
-      <c r="B436" s="5" t="s">
+      <c r="B436" s="2" t="s">
         <v>1323</v>
       </c>
-      <c r="C436" s="5" t="s">
+      <c r="C436" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D436" s="5" t="s">
+      <c r="D436" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="E436" s="5" t="s">
+      <c r="E436" s="2" t="s">
         <v>737</v>
       </c>
-      <c r="F436" s="5" t="s">
+      <c r="F436" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="G436" s="5" t="s">
+      <c r="G436" s="2" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="437" spans="1:7">
-      <c r="A437" s="5" t="s">
+      <c r="A437" s="2" t="s">
         <v>1324</v>
       </c>
-      <c r="B437" s="5" t="s">
+      <c r="B437" s="2" t="s">
         <v>1325</v>
       </c>
-      <c r="C437" s="5" t="s">
+      <c r="C437" s="2" t="s">
         <v>1169</v>
       </c>
-      <c r="D437" s="5" t="s">
+      <c r="D437" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="E437" s="5" t="s">
+      <c r="E437" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F437" s="5" t="s">
+      <c r="F437" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G437" s="5" t="s">
+      <c r="G437" s="2" t="s">
         <v>1326</v>
       </c>
     </row>
     <row r="438" spans="1:7">
-      <c r="A438" s="5" t="s">
+      <c r="A438" s="2" t="s">
         <v>1327</v>
       </c>
-      <c r="B438" s="5" t="s">
+      <c r="B438" s="2" t="s">
         <v>1328</v>
       </c>
-      <c r="C438" s="5" t="s">
+      <c r="C438" s="2" t="s">
         <v>1169</v>
       </c>
-      <c r="D438" s="5" t="s">
+      <c r="D438" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="E438" s="5" t="s">
+      <c r="E438" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="F438" s="5" t="s">
+      <c r="F438" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G438" s="5" t="s">
+      <c r="G438" s="2" t="s">
         <v>796</v>
       </c>
     </row>
     <row r="439" spans="1:7">
-      <c r="A439" s="5" t="s">
+      <c r="A439" s="2" t="s">
         <v>1329</v>
       </c>
-      <c r="B439" s="5" t="s">
+      <c r="B439" s="2" t="s">
         <v>1330</v>
       </c>
-      <c r="C439" s="5" t="s">
+      <c r="C439" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="D439" s="5"/>
-      <c r="E439" s="5" t="s">
+      <c r="D439" s="2"/>
+      <c r="E439" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F439" s="5" t="s">
+      <c r="F439" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G439" s="5" t="s">
+      <c r="G439" s="2" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="440" spans="1:7">
-      <c r="A440" s="5" t="s">
+      <c r="A440" s="2" t="s">
         <v>1331</v>
       </c>
-      <c r="B440" s="5" t="s">
+      <c r="B440" s="2" t="s">
         <v>1332</v>
       </c>
-      <c r="C440" s="5" t="s">
+      <c r="C440" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D440" s="5" t="s">
+      <c r="D440" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E440" s="5" t="s">
+      <c r="E440" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F440" s="5" t="s">
+      <c r="F440" s="2" t="s">
         <v>1333</v>
       </c>
-      <c r="G440" s="5" t="s">
+      <c r="G440" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="441" spans="1:7">
-      <c r="A441" s="5" t="s">
+      <c r="A441" s="2" t="s">
         <v>1334</v>
       </c>
-      <c r="B441" s="5" t="s">
+      <c r="B441" s="2" t="s">
         <v>1335</v>
       </c>
-      <c r="C441" s="5" t="s">
+      <c r="C441" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D441" s="5"/>
-      <c r="E441" s="5" t="s">
+      <c r="D441" s="2"/>
+      <c r="E441" s="2" t="s">
         <v>1336</v>
       </c>
-      <c r="F441" s="5" t="s">
+      <c r="F441" s="2" t="s">
         <v>1337</v>
       </c>
-      <c r="G441" s="5" t="s">
+      <c r="G441" s="2" t="s">
         <v>1338</v>
       </c>
     </row>
     <row r="442" spans="1:7">
-      <c r="A442" s="5" t="s">
+      <c r="A442" s="2" t="s">
         <v>1339</v>
       </c>
-      <c r="B442" s="5" t="s">
+      <c r="B442" s="2" t="s">
         <v>1340</v>
       </c>
-      <c r="C442" s="5" t="s">
+      <c r="C442" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D442" s="5" t="s">
+      <c r="D442" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E442" s="5" t="s">
+      <c r="E442" s="2" t="s">
         <v>628</v>
       </c>
-      <c r="F442" s="5" t="s">
+      <c r="F442" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="G442" s="5" t="s">
+      <c r="G442" s="2" t="s">
         <v>1058</v>
       </c>
     </row>
     <row r="443" spans="1:7">
-      <c r="A443" s="5" t="s">
+      <c r="A443" s="2" t="s">
         <v>1341</v>
       </c>
-      <c r="B443" s="5" t="s">
+      <c r="B443" s="2" t="s">
         <v>1342</v>
       </c>
-      <c r="C443" s="5" t="s">
+      <c r="C443" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="D443" s="5" t="s">
+      <c r="D443" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="E443" s="5" t="s">
+      <c r="E443" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="F443" s="5" t="s">
+      <c r="F443" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="G443" s="5" t="s">
+      <c r="G443" s="2" t="s">
         <v>1075</v>
       </c>
     </row>
     <row r="444" spans="1:7">
-      <c r="A444" s="5" t="s">
+      <c r="A444" s="2" t="s">
         <v>1343</v>
       </c>
-      <c r="B444" s="5" t="s">
+      <c r="B444" s="2" t="s">
         <v>1344</v>
       </c>
-      <c r="C444" s="5" t="s">
+      <c r="C444" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="D444" s="5" t="s">
+      <c r="D444" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="E444" s="5" t="s">
+      <c r="E444" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F444" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G444" s="5" t="s">
+      <c r="F444" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G444" s="2" t="s">
         <v>712</v>
       </c>
     </row>
     <row r="445" spans="1:7">
-      <c r="A445" s="5" t="s">
+      <c r="A445" s="2" t="s">
         <v>1345</v>
       </c>
-      <c r="B445" s="5" t="s">
+      <c r="B445" s="2" t="s">
         <v>1346</v>
       </c>
-      <c r="C445" s="5" t="s">
+      <c r="C445" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="D445" s="5" t="s">
+      <c r="D445" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="E445" s="5" t="s">
+      <c r="E445" s="2" t="s">
         <v>628</v>
       </c>
-      <c r="F445" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G445" s="5" t="s">
+      <c r="F445" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G445" s="2" t="s">
         <v>443</v>
       </c>
     </row>
     <row r="446" spans="1:7">
-      <c r="A446" s="5" t="s">
+      <c r="A446" s="2" t="s">
         <v>1347</v>
       </c>
-      <c r="B446" s="5" t="s">
+      <c r="B446" s="2" t="s">
         <v>1348</v>
       </c>
-      <c r="C446" s="5" t="s">
+      <c r="C446" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="D446" s="5" t="s">
+      <c r="D446" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="E446" s="5" t="s">
+      <c r="E446" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="F446" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G446" s="5" t="s">
+      <c r="F446" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G446" s="2" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="447" spans="1:7">
-      <c r="A447" s="5" t="s">
+      <c r="A447" s="2" t="s">
         <v>1349</v>
       </c>
-      <c r="B447" s="5" t="s">
+      <c r="B447" s="2" t="s">
         <v>1350</v>
       </c>
-      <c r="C447" s="5" t="s">
+      <c r="C447" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D447" s="5"/>
-      <c r="E447" s="5" t="s">
+      <c r="D447" s="2"/>
+      <c r="E447" s="2" t="s">
         <v>650</v>
       </c>
-      <c r="F447" s="5" t="s">
+      <c r="F447" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="G447" s="5" t="s">
+      <c r="G447" s="2" t="s">
         <v>284</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adicionado +27 pokemon da 4ª geração
</commit_message>
<xml_diff>
--- a/pokemonv2/pokemons.xlsx
+++ b/pokemonv2/pokemons.xlsx
@@ -8722,8 +8722,8 @@
   <dimension ref="A1:H1026"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A431" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B489" sqref="B489"/>
+      <pane ySplit="1" topLeftCell="A461" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C472" sqref="C472"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18551,599 +18551,599 @@
       </c>
     </row>
     <row r="448" spans="1:7">
-      <c r="A448" s="5" t="s">
+      <c r="A448" s="2" t="s">
         <v>1351</v>
       </c>
-      <c r="B448" s="5" t="s">
+      <c r="B448" s="2" t="s">
         <v>1352</v>
       </c>
-      <c r="C448" s="5" t="s">
+      <c r="C448" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="D448" s="5"/>
-      <c r="E448" s="5" t="s">
+      <c r="D448" s="2"/>
+      <c r="E448" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="F448" s="5" t="s">
+      <c r="F448" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G448" s="5" t="s">
+      <c r="G448" s="2" t="s">
         <v>893</v>
       </c>
     </row>
     <row r="449" spans="1:7">
-      <c r="A449" s="5" t="s">
+      <c r="A449" s="2" t="s">
         <v>1353</v>
       </c>
-      <c r="B449" s="5" t="s">
+      <c r="B449" s="2" t="s">
         <v>1354</v>
       </c>
-      <c r="C449" s="5" t="s">
+      <c r="C449" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="D449" s="5" t="s">
+      <c r="D449" s="2" t="s">
         <v>1169</v>
       </c>
-      <c r="E449" s="5" t="s">
+      <c r="E449" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="F449" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G449" s="5" t="s">
+      <c r="F449" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G449" s="2" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="450" spans="1:7">
-      <c r="A450" s="5" t="s">
+      <c r="A450" s="2" t="s">
         <v>1355</v>
       </c>
-      <c r="B450" s="5" t="s">
+      <c r="B450" s="2" t="s">
         <v>1356</v>
       </c>
-      <c r="C450" s="5" t="s">
+      <c r="C450" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="D450" s="5"/>
-      <c r="E450" s="5" t="s">
+      <c r="D450" s="2"/>
+      <c r="E450" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="F450" s="5" t="s">
+      <c r="F450" s="2" t="s">
         <v>1357</v>
       </c>
-      <c r="G450" s="5" t="s">
+      <c r="G450" s="2" t="s">
         <v>1358</v>
       </c>
     </row>
     <row r="451" spans="1:7">
-      <c r="A451" s="5" t="s">
+      <c r="A451" s="2" t="s">
         <v>1359</v>
       </c>
-      <c r="B451" s="5" t="s">
+      <c r="B451" s="2" t="s">
         <v>1360</v>
       </c>
-      <c r="C451" s="5" t="s">
+      <c r="C451" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="D451" s="5"/>
-      <c r="E451" s="5" t="s">
+      <c r="D451" s="2"/>
+      <c r="E451" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="F451" s="5" t="s">
+      <c r="F451" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="G451" s="5" t="s">
+      <c r="G451" s="2" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="452" spans="1:7">
-      <c r="A452" s="5" t="s">
+      <c r="A452" s="2" t="s">
         <v>1361</v>
       </c>
-      <c r="B452" s="5" t="s">
+      <c r="B452" s="2" t="s">
         <v>1362</v>
       </c>
-      <c r="C452" s="5" t="s">
+      <c r="C452" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D452" s="5" t="s">
+      <c r="D452" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E452" s="5" t="s">
+      <c r="E452" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="F452" s="5" t="s">
+      <c r="F452" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G452" s="5" t="s">
+      <c r="G452" s="2" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="453" spans="1:7">
-      <c r="A453" s="5" t="s">
+      <c r="A453" s="2" t="s">
         <v>1363</v>
       </c>
-      <c r="B453" s="5" t="s">
+      <c r="B453" s="2" t="s">
         <v>1364</v>
       </c>
-      <c r="C453" s="5" t="s">
+      <c r="C453" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D453" s="5" t="s">
+      <c r="D453" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="E453" s="5" t="s">
+      <c r="E453" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="F453" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G453" s="5" t="s">
+      <c r="F453" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G453" s="2" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="454" spans="1:7">
-      <c r="A454" s="5" t="s">
+      <c r="A454" s="2" t="s">
         <v>1365</v>
       </c>
-      <c r="B454" s="5" t="s">
+      <c r="B454" s="2" t="s">
         <v>1366</v>
       </c>
-      <c r="C454" s="5" t="s">
+      <c r="C454" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D454" s="5" t="s">
+      <c r="D454" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="E454" s="5" t="s">
+      <c r="E454" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F454" s="5" t="s">
+      <c r="F454" s="2" t="s">
         <v>1357</v>
       </c>
-      <c r="G454" s="5" t="s">
+      <c r="G454" s="2" t="s">
         <v>1212</v>
       </c>
     </row>
     <row r="455" spans="1:7">
-      <c r="A455" s="5" t="s">
+      <c r="A455" s="2" t="s">
         <v>1367</v>
       </c>
-      <c r="B455" s="5" t="s">
+      <c r="B455" s="2" t="s">
         <v>1368</v>
       </c>
-      <c r="C455" s="5" t="s">
+      <c r="C455" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D455" s="5" t="s">
+      <c r="D455" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="E455" s="5" t="s">
+      <c r="E455" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="F455" s="5" t="s">
+      <c r="F455" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G455" s="5" t="s">
+      <c r="G455" s="2" t="s">
         <v>1369</v>
       </c>
     </row>
     <row r="456" spans="1:7">
-      <c r="A456" s="5" t="s">
+      <c r="A456" s="2" t="s">
         <v>1370</v>
       </c>
-      <c r="B456" s="5" t="s">
+      <c r="B456" s="2" t="s">
         <v>1371</v>
       </c>
-      <c r="C456" s="5" t="s">
+      <c r="C456" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D456" s="5"/>
-      <c r="E456" s="5" t="s">
+      <c r="D456" s="2"/>
+      <c r="E456" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="F456" s="5" t="s">
+      <c r="F456" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="G456" s="5" t="s">
+      <c r="G456" s="2" t="s">
         <v>662</v>
       </c>
     </row>
     <row r="457" spans="1:7">
-      <c r="A457" s="5" t="s">
+      <c r="A457" s="2" t="s">
         <v>1372</v>
       </c>
-      <c r="B457" s="5" t="s">
+      <c r="B457" s="2" t="s">
         <v>1373</v>
       </c>
-      <c r="C457" s="5" t="s">
+      <c r="C457" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D457" s="5"/>
-      <c r="E457" s="5" t="s">
+      <c r="D457" s="2"/>
+      <c r="E457" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="F457" s="5" t="s">
+      <c r="F457" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G457" s="5" t="s">
+      <c r="G457" s="2" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="458" spans="1:7">
-      <c r="A458" s="5" t="s">
+      <c r="A458" s="2" t="s">
         <v>1374</v>
       </c>
-      <c r="B458" s="5" t="s">
+      <c r="B458" s="2" t="s">
         <v>1375</v>
       </c>
-      <c r="C458" s="5" t="s">
+      <c r="C458" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D458" s="5"/>
-      <c r="E458" s="5" t="s">
+      <c r="D458" s="2"/>
+      <c r="E458" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="F458" s="5" t="s">
+      <c r="F458" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G458" s="5" t="s">
+      <c r="G458" s="2" t="s">
         <v>910</v>
       </c>
     </row>
     <row r="459" spans="1:7">
-      <c r="A459" s="5" t="s">
+      <c r="A459" s="2" t="s">
         <v>1376</v>
       </c>
-      <c r="B459" s="5" t="s">
+      <c r="B459" s="2" t="s">
         <v>1377</v>
       </c>
-      <c r="C459" s="5" t="s">
+      <c r="C459" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D459" s="5" t="s">
+      <c r="D459" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E459" s="5" t="s">
+      <c r="E459" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="F459" s="5" t="s">
+      <c r="F459" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="G459" s="5" t="s">
+      <c r="G459" s="2" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="460" spans="1:7">
-      <c r="A460" s="5" t="s">
+      <c r="A460" s="2" t="s">
         <v>1378</v>
       </c>
-      <c r="B460" s="5" t="s">
+      <c r="B460" s="2" t="s">
         <v>1379</v>
       </c>
-      <c r="C460" s="5" t="s">
+      <c r="C460" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D460" s="5" t="s">
+      <c r="D460" s="2" t="s">
         <v>1117</v>
       </c>
-      <c r="E460" s="5" t="s">
+      <c r="E460" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="F460" s="5" t="s">
+      <c r="F460" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G460" s="5" t="s">
+      <c r="G460" s="2" t="s">
         <v>746</v>
       </c>
     </row>
     <row r="461" spans="1:7">
-      <c r="A461" s="5" t="s">
+      <c r="A461" s="2" t="s">
         <v>1380</v>
       </c>
-      <c r="B461" s="5" t="s">
+      <c r="B461" s="2" t="s">
         <v>1381</v>
       </c>
-      <c r="C461" s="5" t="s">
+      <c r="C461" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D461" s="5" t="s">
+      <c r="D461" s="2" t="s">
         <v>1117</v>
       </c>
-      <c r="E461" s="5" t="s">
+      <c r="E461" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="F461" s="5" t="s">
+      <c r="F461" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="G461" s="5" t="s">
+      <c r="G461" s="2" t="s">
         <v>1382</v>
       </c>
     </row>
     <row r="462" spans="1:7">
-      <c r="A462" s="5" t="s">
+      <c r="A462" s="2" t="s">
         <v>1383</v>
       </c>
-      <c r="B462" s="5" t="s">
+      <c r="B462" s="2" t="s">
         <v>1384</v>
       </c>
-      <c r="C462" s="5" t="s">
+      <c r="C462" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="D462" s="5" t="s">
+      <c r="D462" s="2" t="s">
         <v>1117</v>
       </c>
-      <c r="E462" s="5" t="s">
+      <c r="E462" s="2" t="s">
         <v>697</v>
       </c>
-      <c r="F462" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G462" s="5" t="s">
+      <c r="F462" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G462" s="2" t="s">
         <v>1385</v>
       </c>
     </row>
     <row r="463" spans="1:7">
-      <c r="A463" s="5" t="s">
+      <c r="A463" s="2" t="s">
         <v>1386</v>
       </c>
-      <c r="B463" s="5" t="s">
+      <c r="B463" s="2" t="s">
         <v>1387</v>
       </c>
-      <c r="C463" s="5" t="s">
+      <c r="C463" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="D463" s="5" t="s">
+      <c r="D463" s="2" t="s">
         <v>1169</v>
       </c>
-      <c r="E463" s="5" t="s">
+      <c r="E463" s="2" t="s">
         <v>1388</v>
       </c>
-      <c r="F463" s="5" t="s">
+      <c r="F463" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="G463" s="5" t="s">
+      <c r="G463" s="2" t="s">
         <v>1389</v>
       </c>
     </row>
     <row r="464" spans="1:7">
-      <c r="A464" s="5" t="s">
+      <c r="A464" s="2" t="s">
         <v>1390</v>
       </c>
-      <c r="B464" s="5" t="s">
+      <c r="B464" s="2" t="s">
         <v>1391</v>
       </c>
-      <c r="C464" s="5" t="s">
+      <c r="C464" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D464" s="5"/>
-      <c r="E464" s="5" t="s">
+      <c r="D464" s="2"/>
+      <c r="E464" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="F464" s="5" t="s">
+      <c r="F464" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="G464" s="5" t="s">
+      <c r="G464" s="2" t="s">
         <v>1392</v>
       </c>
     </row>
     <row r="465" spans="1:7">
-      <c r="A465" s="5" t="s">
+      <c r="A465" s="2" t="s">
         <v>1393</v>
       </c>
-      <c r="B465" s="5" t="s">
+      <c r="B465" s="2" t="s">
         <v>1394</v>
       </c>
-      <c r="C465" s="5" t="s">
+      <c r="C465" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="D465" s="5" t="s">
+      <c r="D465" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="E465" s="5" t="s">
+      <c r="E465" s="2" t="s">
         <v>579</v>
       </c>
-      <c r="F465" s="5" t="s">
+      <c r="F465" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="G465" s="5" t="s">
+      <c r="G465" s="2" t="s">
         <v>1395</v>
       </c>
     </row>
     <row r="466" spans="1:7">
-      <c r="A466" s="5" t="s">
+      <c r="A466" s="2" t="s">
         <v>1396</v>
       </c>
-      <c r="B466" s="5" t="s">
+      <c r="B466" s="2" t="s">
         <v>1397</v>
       </c>
-      <c r="C466" s="5" t="s">
+      <c r="C466" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D466" s="5"/>
-      <c r="E466" s="5" t="s">
+      <c r="D466" s="2"/>
+      <c r="E466" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="F466" s="5" t="s">
+      <c r="F466" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="G466" s="5" t="s">
+      <c r="G466" s="2" t="s">
         <v>1398</v>
       </c>
     </row>
     <row r="467" spans="1:7">
-      <c r="A467" s="5" t="s">
+      <c r="A467" s="2" t="s">
         <v>1399</v>
       </c>
-      <c r="B467" s="5" t="s">
+      <c r="B467" s="2" t="s">
         <v>1400</v>
       </c>
-      <c r="C467" s="5" t="s">
+      <c r="C467" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="D467" s="5"/>
-      <c r="E467" s="5" t="s">
+      <c r="D467" s="2"/>
+      <c r="E467" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F467" s="5" t="s">
+      <c r="F467" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="G467" s="5" t="s">
+      <c r="G467" s="2" t="s">
         <v>1401</v>
       </c>
     </row>
     <row r="468" spans="1:7">
-      <c r="A468" s="5" t="s">
+      <c r="A468" s="2" t="s">
         <v>1402</v>
       </c>
-      <c r="B468" s="5" t="s">
+      <c r="B468" s="2" t="s">
         <v>1403</v>
       </c>
-      <c r="C468" s="5" t="s">
+      <c r="C468" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D468" s="5"/>
-      <c r="E468" s="5" t="s">
+      <c r="D468" s="2"/>
+      <c r="E468" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F468" s="5" t="s">
+      <c r="F468" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="G468" s="5" t="s">
+      <c r="G468" s="2" t="s">
         <v>1404</v>
       </c>
     </row>
     <row r="469" spans="1:7">
-      <c r="A469" s="5" t="s">
+      <c r="A469" s="2" t="s">
         <v>1405</v>
       </c>
-      <c r="B469" s="5" t="s">
+      <c r="B469" s="2" t="s">
         <v>1406</v>
       </c>
-      <c r="C469" s="5" t="s">
+      <c r="C469" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D469" s="5" t="s">
+      <c r="D469" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E469" s="5" t="s">
+      <c r="E469" s="2" t="s">
         <v>1407</v>
       </c>
-      <c r="F469" s="5" t="s">
+      <c r="F469" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="G469" s="5" t="s">
+      <c r="G469" s="2" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="470" spans="1:7">
-      <c r="A470" s="5" t="s">
+      <c r="A470" s="2" t="s">
         <v>1408</v>
       </c>
-      <c r="B470" s="5" t="s">
+      <c r="B470" s="2" t="s">
         <v>1409</v>
       </c>
-      <c r="C470" s="5" t="s">
+      <c r="C470" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D470" s="5" t="s">
+      <c r="D470" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E470" s="5" t="s">
+      <c r="E470" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="F470" s="5" t="s">
+      <c r="F470" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="G470" s="5" t="s">
+      <c r="G470" s="2" t="s">
         <v>1410</v>
       </c>
     </row>
     <row r="471" spans="1:7">
-      <c r="A471" s="5" t="s">
+      <c r="A471" s="2" t="s">
         <v>1411</v>
       </c>
-      <c r="B471" s="5" t="s">
+      <c r="B471" s="2" t="s">
         <v>1412</v>
       </c>
-      <c r="C471" s="5" t="s">
+      <c r="C471" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D471" s="5"/>
-      <c r="E471" s="5" t="s">
+      <c r="D471" s="2"/>
+      <c r="E471" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="F471" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G471" s="5" t="s">
+      <c r="F471" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G471" s="2" t="s">
         <v>1233</v>
       </c>
     </row>
     <row r="472" spans="1:7">
-      <c r="A472" s="5" t="s">
+      <c r="A472" s="2" t="s">
         <v>1413</v>
       </c>
-      <c r="B472" s="5" t="s">
+      <c r="B472" s="2" t="s">
         <v>1414</v>
       </c>
-      <c r="C472" s="5" t="s">
+      <c r="C472" s="2" t="s">
         <v>1117</v>
       </c>
-      <c r="D472" s="5"/>
-      <c r="E472" s="5" t="s">
+      <c r="D472" s="2"/>
+      <c r="E472" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="F472" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G472" s="5" t="s">
+      <c r="F472" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G472" s="2" t="s">
         <v>1415</v>
       </c>
     </row>
     <row r="473" spans="1:7">
-      <c r="A473" s="5" t="s">
+      <c r="A473" s="2" t="s">
         <v>1416</v>
       </c>
-      <c r="B473" s="5" t="s">
+      <c r="B473" s="2" t="s">
         <v>1417</v>
       </c>
-      <c r="C473" s="5" t="s">
+      <c r="C473" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="D473" s="5" t="s">
+      <c r="D473" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E473" s="5" t="s">
+      <c r="E473" s="2" t="s">
         <v>697</v>
       </c>
-      <c r="F473" s="5" t="s">
+      <c r="F473" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="G473" s="5" t="s">
+      <c r="G473" s="2" t="s">
         <v>1418</v>
       </c>
     </row>
     <row r="474" spans="1:7">
-      <c r="A474" s="5" t="s">
+      <c r="A474" s="2" t="s">
         <v>1419</v>
       </c>
-      <c r="B474" s="5" t="s">
+      <c r="B474" s="2" t="s">
         <v>1420</v>
       </c>
-      <c r="C474" s="5" t="s">
+      <c r="C474" s="2" t="s">
         <v>1117</v>
       </c>
-      <c r="D474" s="5" t="s">
+      <c r="D474" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="E474" s="5" t="s">
+      <c r="E474" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F474" s="5" t="s">
+      <c r="F474" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="G474" s="5" t="s">
+      <c r="G474" s="2" t="s">
         <v>1421</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adicionado +20 pokémon da 4ª geração. (finalizado)
</commit_message>
<xml_diff>
--- a/pokemonv2/pokemons.xlsx
+++ b/pokemonv2/pokemons.xlsx
@@ -8364,7 +8364,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -8374,12 +8374,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8411,7 +8405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -8419,7 +8413,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8722,8 +8715,8 @@
   <dimension ref="A1:H1026"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A461" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C472" sqref="C472"/>
+      <pane ySplit="1" topLeftCell="A377" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C386" sqref="C386"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19148,438 +19141,438 @@
       </c>
     </row>
     <row r="475" spans="1:7">
-      <c r="A475" s="5" t="s">
+      <c r="A475" s="2" t="s">
         <v>1422</v>
       </c>
-      <c r="B475" s="5" t="s">
+      <c r="B475" s="2" t="s">
         <v>1423</v>
       </c>
-      <c r="C475" s="5" t="s">
+      <c r="C475" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D475" s="5"/>
-      <c r="E475" s="5" t="s">
+      <c r="D475" s="2"/>
+      <c r="E475" s="2" t="s">
         <v>579</v>
       </c>
-      <c r="F475" s="5" t="s">
+      <c r="F475" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="G475" s="5" t="s">
+      <c r="G475" s="2" t="s">
         <v>1385</v>
       </c>
     </row>
     <row r="476" spans="1:7">
-      <c r="A476" s="5" t="s">
+      <c r="A476" s="2" t="s">
         <v>1424</v>
       </c>
-      <c r="B476" s="5" t="s">
+      <c r="B476" s="2" t="s">
         <v>1425</v>
       </c>
-      <c r="C476" s="5" t="s">
+      <c r="C476" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D476" s="5" t="s">
+      <c r="D476" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="E476" s="5" t="s">
+      <c r="E476" s="2" t="s">
         <v>896</v>
       </c>
-      <c r="F476" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G476" s="5" t="s">
+      <c r="F476" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G476" s="2" t="s">
         <v>829</v>
       </c>
     </row>
     <row r="477" spans="1:7">
-      <c r="A477" s="5" t="s">
+      <c r="A477" s="2" t="s">
         <v>1426</v>
       </c>
-      <c r="B477" s="5" t="s">
+      <c r="B477" s="2" t="s">
         <v>1427</v>
       </c>
-      <c r="C477" s="5" t="s">
+      <c r="C477" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="D477" s="5" t="s">
+      <c r="D477" s="2" t="s">
         <v>1169</v>
       </c>
-      <c r="E477" s="5" t="s">
+      <c r="E477" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="F477" s="5" t="s">
+      <c r="F477" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="G477" s="5" t="s">
+      <c r="G477" s="2" t="s">
         <v>1428</v>
       </c>
     </row>
     <row r="478" spans="1:7">
-      <c r="A478" s="5" t="s">
+      <c r="A478" s="2" t="s">
         <v>1429</v>
       </c>
-      <c r="B478" s="5" t="s">
+      <c r="B478" s="2" t="s">
         <v>1430</v>
       </c>
-      <c r="C478" s="5" t="s">
+      <c r="C478" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="D478" s="5"/>
-      <c r="E478" s="5" t="s">
+      <c r="D478" s="2"/>
+      <c r="E478" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F478" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G478" s="5" t="s">
+      <c r="F478" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G478" s="2" t="s">
         <v>1431</v>
       </c>
     </row>
     <row r="479" spans="1:7">
-      <c r="A479" s="5" t="s">
+      <c r="A479" s="2" t="s">
         <v>1432</v>
       </c>
-      <c r="B479" s="5" t="s">
+      <c r="B479" s="2" t="s">
         <v>1433</v>
       </c>
-      <c r="C479" s="5" t="s">
+      <c r="C479" s="2" t="s">
         <v>1117</v>
       </c>
-      <c r="D479" s="5" t="s">
+      <c r="D479" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="E479" s="5" t="s">
+      <c r="E479" s="2" t="s">
         <v>737</v>
       </c>
-      <c r="F479" s="5" t="s">
+      <c r="F479" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G479" s="5" t="s">
+      <c r="G479" s="2" t="s">
         <v>1434</v>
       </c>
     </row>
     <row r="480" spans="1:7">
-      <c r="A480" s="5" t="s">
+      <c r="A480" s="2" t="s">
         <v>1435</v>
       </c>
-      <c r="B480" s="5" t="s">
+      <c r="B480" s="2" t="s">
         <v>1436</v>
       </c>
-      <c r="C480" s="5" t="s">
+      <c r="C480" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="D480" s="5" t="s">
+      <c r="D480" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="E480" s="5" t="s">
+      <c r="E480" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="F480" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G480" s="5" t="s">
+      <c r="F480" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G480" s="2" t="s">
         <v>1437</v>
       </c>
     </row>
     <row r="481" spans="1:7">
-      <c r="A481" s="5" t="s">
+      <c r="A481" s="2" t="s">
         <v>1438</v>
       </c>
-      <c r="B481" s="5" t="s">
+      <c r="B481" s="2" t="s">
         <v>1439</v>
       </c>
-      <c r="C481" s="5" t="s">
+      <c r="C481" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D481" s="5"/>
-      <c r="E481" s="5" t="s">
+      <c r="D481" s="2"/>
+      <c r="E481" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="F481" s="5" t="s">
+      <c r="F481" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="G481" s="5" t="s">
+      <c r="G481" s="2" t="s">
         <v>1437</v>
       </c>
     </row>
     <row r="482" spans="1:7">
-      <c r="A482" s="5" t="s">
+      <c r="A482" s="2" t="s">
         <v>1440</v>
       </c>
-      <c r="B482" s="5" t="s">
+      <c r="B482" s="2" t="s">
         <v>1441</v>
       </c>
-      <c r="C482" s="5" t="s">
+      <c r="C482" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D482" s="5"/>
-      <c r="E482" s="5" t="s">
+      <c r="D482" s="2"/>
+      <c r="E482" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="F482" s="5" t="s">
+      <c r="F482" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="G482" s="5" t="s">
+      <c r="G482" s="2" t="s">
         <v>1437</v>
       </c>
     </row>
     <row r="483" spans="1:7">
-      <c r="A483" s="5" t="s">
+      <c r="A483" s="2" t="s">
         <v>1442</v>
       </c>
-      <c r="B483" s="5" t="s">
+      <c r="B483" s="2" t="s">
         <v>1443</v>
       </c>
-      <c r="C483" s="5" t="s">
+      <c r="C483" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D483" s="5"/>
-      <c r="E483" s="5" t="s">
+      <c r="D483" s="2"/>
+      <c r="E483" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="F483" s="5" t="s">
+      <c r="F483" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="G483" s="5" t="s">
+      <c r="G483" s="2" t="s">
         <v>1437</v>
       </c>
     </row>
     <row r="484" spans="1:7">
-      <c r="A484" s="5" t="s">
+      <c r="A484" s="2" t="s">
         <v>1444</v>
       </c>
-      <c r="B484" s="5" t="s">
+      <c r="B484" s="2" t="s">
         <v>1445</v>
       </c>
-      <c r="C484" s="5" t="s">
+      <c r="C484" s="2" t="s">
         <v>1169</v>
       </c>
-      <c r="D484" s="5" t="s">
+      <c r="D484" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="E484" s="5" t="s">
+      <c r="E484" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="F484" s="5" t="s">
+      <c r="F484" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="G484" s="5" t="s">
+      <c r="G484" s="2" t="s">
         <v>1446</v>
       </c>
     </row>
     <row r="485" spans="1:7">
-      <c r="A485" s="5" t="s">
+      <c r="A485" s="2" t="s">
         <v>1447</v>
       </c>
-      <c r="B485" s="5" t="s">
+      <c r="B485" s="2" t="s">
         <v>1448</v>
       </c>
-      <c r="C485" s="5" t="s">
+      <c r="C485" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D485" s="5" t="s">
+      <c r="D485" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="E485" s="5" t="s">
+      <c r="E485" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="F485" s="5" t="s">
+      <c r="F485" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="G485" s="5" t="s">
+      <c r="G485" s="2" t="s">
         <v>1449</v>
       </c>
     </row>
     <row r="486" spans="1:7">
-      <c r="A486" s="5" t="s">
+      <c r="A486" s="2" t="s">
         <v>1450</v>
       </c>
-      <c r="B486" s="5" t="s">
+      <c r="B486" s="2" t="s">
         <v>1451</v>
       </c>
-      <c r="C486" s="5" t="s">
+      <c r="C486" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D486" s="5" t="s">
+      <c r="D486" s="2" t="s">
         <v>1169</v>
       </c>
-      <c r="E486" s="5" t="s">
+      <c r="E486" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="F486" s="5" t="s">
+      <c r="F486" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="G486" s="5" t="s">
+      <c r="G486" s="2" t="s">
         <v>1452</v>
       </c>
     </row>
     <row r="487" spans="1:7">
-      <c r="A487" s="5" t="s">
+      <c r="A487" s="2" t="s">
         <v>1453</v>
       </c>
-      <c r="B487" s="5" t="s">
+      <c r="B487" s="2" t="s">
         <v>1454</v>
       </c>
-      <c r="C487" s="5" t="s">
+      <c r="C487" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D487" s="5"/>
-      <c r="E487" s="5" t="s">
+      <c r="D487" s="2"/>
+      <c r="E487" s="2" t="s">
         <v>1455</v>
       </c>
-      <c r="F487" s="5" t="s">
+      <c r="F487" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="G487" s="5" t="s">
+      <c r="G487" s="2" t="s">
         <v>1456</v>
       </c>
     </row>
     <row r="488" spans="1:7">
-      <c r="A488" s="5" t="s">
+      <c r="A488" s="2" t="s">
         <v>1457</v>
       </c>
-      <c r="B488" s="5" t="s">
+      <c r="B488" s="2" t="s">
         <v>1458</v>
       </c>
-      <c r="C488" s="5" t="s">
+      <c r="C488" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="D488" s="5" t="s">
+      <c r="D488" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="E488" s="5" t="s">
+      <c r="E488" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="F488" s="5" t="s">
+      <c r="F488" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="G488" s="5" t="s">
+      <c r="G488" s="2" t="s">
         <v>1459</v>
       </c>
     </row>
     <row r="489" spans="1:7">
-      <c r="A489" s="5" t="s">
+      <c r="A489" s="2" t="s">
         <v>1460</v>
       </c>
-      <c r="B489" s="5" t="s">
+      <c r="B489" s="2" t="s">
         <v>1461</v>
       </c>
-      <c r="C489" s="5" t="s">
+      <c r="C489" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D489" s="5"/>
-      <c r="E489" s="5" t="s">
+      <c r="D489" s="2"/>
+      <c r="E489" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="F489" s="5" t="s">
+      <c r="F489" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="G489" s="5" t="s">
+      <c r="G489" s="2" t="s">
         <v>1462</v>
       </c>
     </row>
     <row r="490" spans="1:7">
-      <c r="A490" s="5" t="s">
+      <c r="A490" s="2" t="s">
         <v>1463</v>
       </c>
-      <c r="B490" s="5" t="s">
+      <c r="B490" s="2" t="s">
         <v>1464</v>
       </c>
-      <c r="C490" s="5" t="s">
+      <c r="C490" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D490" s="5"/>
-      <c r="E490" s="5" t="s">
+      <c r="D490" s="2"/>
+      <c r="E490" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F490" s="5" t="s">
+      <c r="F490" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="G490" s="5" t="s">
+      <c r="G490" s="2" t="s">
         <v>1465</v>
       </c>
     </row>
     <row r="491" spans="1:7">
-      <c r="A491" s="5" t="s">
+      <c r="A491" s="2" t="s">
         <v>1466</v>
       </c>
-      <c r="B491" s="5" t="s">
+      <c r="B491" s="2" t="s">
         <v>1467</v>
       </c>
-      <c r="C491" s="5" t="s">
+      <c r="C491" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D491" s="5"/>
-      <c r="E491" s="5" t="s">
+      <c r="D491" s="2"/>
+      <c r="E491" s="2" t="s">
         <v>814</v>
       </c>
-      <c r="F491" s="5" t="s">
+      <c r="F491" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="G491" s="5" t="s">
+      <c r="G491" s="2" t="s">
         <v>1468</v>
       </c>
     </row>
     <row r="492" spans="1:7">
-      <c r="A492" s="5" t="s">
+      <c r="A492" s="2" t="s">
         <v>1469</v>
       </c>
-      <c r="B492" s="5" t="s">
+      <c r="B492" s="2" t="s">
         <v>1470</v>
       </c>
-      <c r="C492" s="5" t="s">
+      <c r="C492" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="D492" s="5"/>
-      <c r="E492" s="5" t="s">
+      <c r="D492" s="2"/>
+      <c r="E492" s="2" t="s">
         <v>814</v>
       </c>
-      <c r="F492" s="5" t="s">
+      <c r="F492" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="G492" s="5" t="s">
+      <c r="G492" s="2" t="s">
         <v>746</v>
       </c>
     </row>
     <row r="493" spans="1:7">
-      <c r="A493" s="5" t="s">
+      <c r="A493" s="2" t="s">
         <v>1471</v>
       </c>
-      <c r="B493" s="5" t="s">
+      <c r="B493" s="2" t="s">
         <v>1472</v>
       </c>
-      <c r="C493" s="5" t="s">
+      <c r="C493" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D493" s="5"/>
-      <c r="E493" s="5" t="s">
+      <c r="D493" s="2"/>
+      <c r="E493" s="2" t="s">
         <v>814</v>
       </c>
-      <c r="F493" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G493" s="5" t="s">
+      <c r="F493" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G493" s="2" t="s">
         <v>666</v>
       </c>
     </row>
     <row r="494" spans="1:7">
-      <c r="A494" s="5" t="s">
+      <c r="A494" s="2" t="s">
         <v>1473</v>
       </c>
-      <c r="B494" s="5" t="s">
+      <c r="B494" s="2" t="s">
         <v>1474</v>
       </c>
-      <c r="C494" s="5" t="s">
+      <c r="C494" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D494" s="5"/>
-      <c r="E494" s="5" t="s">
+      <c r="D494" s="2"/>
+      <c r="E494" s="2" t="s">
         <v>1475</v>
       </c>
-      <c r="F494" s="5" t="s">
+      <c r="F494" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="G494" s="5" t="s">
+      <c r="G494" s="2" t="s">
         <v>1476</v>
       </c>
     </row>

</xml_diff>

<commit_message>
pokemons da 4ª Geração distribuidos nos mapas e disponiveis para captura
</commit_message>
<xml_diff>
--- a/pokemonv2/pokemons.xlsx
+++ b/pokemonv2/pokemons.xlsx
@@ -8364,7 +8364,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -8374,6 +8374,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8405,7 +8411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -8413,6 +8419,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8715,8 +8722,8 @@
   <dimension ref="A1:H1026"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A377" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C386" sqref="C386"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C206" sqref="C206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17224,2355 +17231,2355 @@
       </c>
     </row>
     <row r="388" spans="1:7">
-      <c r="A388" s="2" t="s">
+      <c r="A388" s="5" t="s">
         <v>1191</v>
       </c>
-      <c r="B388" s="2" t="s">
+      <c r="B388" s="5" t="s">
         <v>1192</v>
       </c>
-      <c r="C388" s="2" t="s">
+      <c r="C388" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="D388" s="2"/>
-      <c r="E388" s="2" t="s">
+      <c r="D388" s="5"/>
+      <c r="E388" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F388" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G388" s="2" t="s">
+      <c r="F388" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G388" s="5" t="s">
         <v>1193</v>
       </c>
     </row>
     <row r="389" spans="1:7">
-      <c r="A389" s="2" t="s">
+      <c r="A389" s="5" t="s">
         <v>1194</v>
       </c>
-      <c r="B389" s="2" t="s">
+      <c r="B389" s="5" t="s">
         <v>1195</v>
       </c>
-      <c r="C389" s="2" t="s">
+      <c r="C389" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="D389" s="2"/>
-      <c r="E389" s="2" t="s">
+      <c r="D389" s="5"/>
+      <c r="E389" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F389" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G389" s="2" t="s">
+      <c r="F389" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G389" s="5" t="s">
         <v>950</v>
       </c>
     </row>
     <row r="390" spans="1:7">
-      <c r="A390" s="2" t="s">
+      <c r="A390" s="5" t="s">
         <v>1196</v>
       </c>
-      <c r="B390" s="2" t="s">
+      <c r="B390" s="5" t="s">
         <v>1197</v>
       </c>
-      <c r="C390" s="2" t="s">
+      <c r="C390" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="D390" s="2" t="s">
+      <c r="D390" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="E390" s="2" t="s">
+      <c r="E390" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F390" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G390" s="2" t="s">
+      <c r="F390" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G390" s="5" t="s">
         <v>1198</v>
       </c>
     </row>
     <row r="391" spans="1:7">
-      <c r="A391" s="2" t="s">
+      <c r="A391" s="5" t="s">
         <v>1199</v>
       </c>
-      <c r="B391" s="2" t="s">
+      <c r="B391" s="5" t="s">
         <v>1200</v>
       </c>
-      <c r="C391" s="2" t="s">
+      <c r="C391" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D391" s="2"/>
-      <c r="E391" s="2" t="s">
+      <c r="D391" s="5"/>
+      <c r="E391" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F391" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G391" s="2" t="s">
+      <c r="F391" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G391" s="5" t="s">
         <v>1201</v>
       </c>
     </row>
     <row r="392" spans="1:7">
-      <c r="A392" s="2" t="s">
+      <c r="A392" s="5" t="s">
         <v>1202</v>
       </c>
-      <c r="B392" s="2" t="s">
+      <c r="B392" s="5" t="s">
         <v>1203</v>
       </c>
-      <c r="C392" s="2" t="s">
+      <c r="C392" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D392" s="2" t="s">
+      <c r="D392" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="E392" s="2" t="s">
+      <c r="E392" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F392" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G392" s="2" t="s">
+      <c r="F392" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G392" s="5" t="s">
         <v>1097</v>
       </c>
     </row>
     <row r="393" spans="1:7">
-      <c r="A393" s="2" t="s">
+      <c r="A393" s="5" t="s">
         <v>1204</v>
       </c>
-      <c r="B393" s="2" t="s">
+      <c r="B393" s="5" t="s">
         <v>1205</v>
       </c>
-      <c r="C393" s="2" t="s">
+      <c r="C393" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D393" s="2" t="s">
+      <c r="D393" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="E393" s="2" t="s">
+      <c r="E393" s="5" t="s">
         <v>1206</v>
       </c>
-      <c r="F393" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G393" s="2" t="s">
+      <c r="F393" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G393" s="5" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="394" spans="1:7">
-      <c r="A394" s="2" t="s">
+      <c r="A394" s="5" t="s">
         <v>1207</v>
       </c>
-      <c r="B394" s="2" t="s">
+      <c r="B394" s="5" t="s">
         <v>1208</v>
       </c>
-      <c r="C394" s="2" t="s">
+      <c r="C394" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D394" s="2"/>
-      <c r="E394" s="2" t="s">
+      <c r="D394" s="5"/>
+      <c r="E394" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F394" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G394" s="2" t="s">
+      <c r="F394" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G394" s="5" t="s">
         <v>1209</v>
       </c>
     </row>
     <row r="395" spans="1:7">
-      <c r="A395" s="2" t="s">
+      <c r="A395" s="5" t="s">
         <v>1210</v>
       </c>
-      <c r="B395" s="2" t="s">
+      <c r="B395" s="5" t="s">
         <v>1211</v>
       </c>
-      <c r="C395" s="2" t="s">
+      <c r="C395" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D395" s="2"/>
-      <c r="E395" s="2" t="s">
+      <c r="D395" s="5"/>
+      <c r="E395" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F395" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G395" s="2" t="s">
+      <c r="F395" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G395" s="5" t="s">
         <v>1212</v>
       </c>
     </row>
     <row r="396" spans="1:7">
-      <c r="A396" s="2" t="s">
+      <c r="A396" s="5" t="s">
         <v>1213</v>
       </c>
-      <c r="B396" s="2" t="s">
+      <c r="B396" s="5" t="s">
         <v>1214</v>
       </c>
-      <c r="C396" s="2" t="s">
+      <c r="C396" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D396" s="2" t="s">
+      <c r="D396" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="E396" s="2" t="s">
+      <c r="E396" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F396" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G396" s="2" t="s">
+      <c r="F396" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G396" s="5" t="s">
         <v>1215</v>
       </c>
     </row>
     <row r="397" spans="1:7">
-      <c r="A397" s="2" t="s">
+      <c r="A397" s="5" t="s">
         <v>1216</v>
       </c>
-      <c r="B397" s="2" t="s">
+      <c r="B397" s="5" t="s">
         <v>1217</v>
       </c>
-      <c r="C397" s="2" t="s">
+      <c r="C397" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D397" s="2" t="s">
+      <c r="D397" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E397" s="2" t="s">
+      <c r="E397" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="F397" s="2" t="s">
+      <c r="F397" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G397" s="2" t="s">
+      <c r="G397" s="5" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="398" spans="1:7">
-      <c r="A398" s="2" t="s">
+      <c r="A398" s="5" t="s">
         <v>1218</v>
       </c>
-      <c r="B398" s="2" t="s">
+      <c r="B398" s="5" t="s">
         <v>1219</v>
       </c>
-      <c r="C398" s="2" t="s">
+      <c r="C398" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D398" s="2" t="s">
+      <c r="D398" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E398" s="2" t="s">
+      <c r="E398" s="5" t="s">
         <v>638</v>
       </c>
-      <c r="F398" s="2" t="s">
+      <c r="F398" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G398" s="2" t="s">
+      <c r="G398" s="5" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="399" spans="1:7">
-      <c r="A399" s="2" t="s">
+      <c r="A399" s="5" t="s">
         <v>1220</v>
       </c>
-      <c r="B399" s="2" t="s">
+      <c r="B399" s="5" t="s">
         <v>1221</v>
       </c>
-      <c r="C399" s="2" t="s">
+      <c r="C399" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D399" s="2" t="s">
+      <c r="D399" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E399" s="2" t="s">
+      <c r="E399" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="F399" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G399" s="2" t="s">
+      <c r="F399" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G399" s="5" t="s">
         <v>1222</v>
       </c>
     </row>
     <row r="400" spans="1:7">
-      <c r="A400" s="2" t="s">
+      <c r="A400" s="5" t="s">
         <v>1223</v>
       </c>
-      <c r="B400" s="2" t="s">
+      <c r="B400" s="5" t="s">
         <v>1224</v>
       </c>
-      <c r="C400" s="2" t="s">
+      <c r="C400" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D400" s="2"/>
-      <c r="E400" s="2" t="s">
+      <c r="D400" s="5"/>
+      <c r="E400" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F400" s="2" t="s">
+      <c r="F400" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G400" s="2" t="s">
+      <c r="G400" s="5" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="401" spans="1:7">
-      <c r="A401" s="2" t="s">
+      <c r="A401" s="5" t="s">
         <v>1225</v>
       </c>
-      <c r="B401" s="2" t="s">
+      <c r="B401" s="5" t="s">
         <v>1226</v>
       </c>
-      <c r="C401" s="2" t="s">
+      <c r="C401" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D401" s="2" t="s">
+      <c r="D401" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E401" s="2" t="s">
+      <c r="E401" s="5" t="s">
         <v>628</v>
       </c>
-      <c r="F401" s="2" t="s">
+      <c r="F401" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="G401" s="2" t="s">
+      <c r="G401" s="5" t="s">
         <v>974</v>
       </c>
     </row>
     <row r="402" spans="1:7">
-      <c r="A402" s="2" t="s">
+      <c r="A402" s="5" t="s">
         <v>1227</v>
       </c>
-      <c r="B402" s="2" t="s">
+      <c r="B402" s="5" t="s">
         <v>1228</v>
       </c>
-      <c r="C402" s="2" t="s">
+      <c r="C402" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D402" s="2"/>
-      <c r="E402" s="2" t="s">
+      <c r="D402" s="5"/>
+      <c r="E402" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F402" s="2" t="s">
+      <c r="F402" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G402" s="2" t="s">
+      <c r="G402" s="5" t="s">
         <v>1229</v>
       </c>
     </row>
     <row r="403" spans="1:7">
-      <c r="A403" s="2" t="s">
+      <c r="A403" s="5" t="s">
         <v>1230</v>
       </c>
-      <c r="B403" s="2" t="s">
+      <c r="B403" s="5" t="s">
         <v>1231</v>
       </c>
-      <c r="C403" s="2" t="s">
+      <c r="C403" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D403" s="2"/>
-      <c r="E403" s="2" t="s">
+      <c r="D403" s="5"/>
+      <c r="E403" s="5" t="s">
         <v>1232</v>
       </c>
-      <c r="F403" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G403" s="2" t="s">
+      <c r="F403" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G403" s="5" t="s">
         <v>1233</v>
       </c>
     </row>
     <row r="404" spans="1:7">
-      <c r="A404" s="2" t="s">
+      <c r="A404" s="5" t="s">
         <v>1234</v>
       </c>
-      <c r="B404" s="2" t="s">
+      <c r="B404" s="5" t="s">
         <v>1235</v>
       </c>
-      <c r="C404" s="2" t="s">
+      <c r="C404" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="D404" s="2"/>
-      <c r="E404" s="2" t="s">
+      <c r="D404" s="5"/>
+      <c r="E404" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="F404" s="2" t="s">
+      <c r="F404" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="G404" s="2" t="s">
+      <c r="G404" s="5" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="405" spans="1:7">
-      <c r="A405" s="2" t="s">
+      <c r="A405" s="5" t="s">
         <v>1236</v>
       </c>
-      <c r="B405" s="2" t="s">
+      <c r="B405" s="5" t="s">
         <v>1237</v>
       </c>
-      <c r="C405" s="2" t="s">
+      <c r="C405" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="D405" s="2"/>
-      <c r="E405" s="2" t="s">
+      <c r="D405" s="5"/>
+      <c r="E405" s="5" t="s">
         <v>1238</v>
       </c>
-      <c r="F405" s="2" t="s">
+      <c r="F405" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G405" s="2" t="s">
+      <c r="G405" s="5" t="s">
         <v>1239</v>
       </c>
     </row>
     <row r="406" spans="1:7">
-      <c r="A406" s="2" t="s">
+      <c r="A406" s="5" t="s">
         <v>1240</v>
       </c>
-      <c r="B406" s="2" t="s">
+      <c r="B406" s="5" t="s">
         <v>1241</v>
       </c>
-      <c r="C406" s="2" t="s">
+      <c r="C406" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="D406" s="2"/>
-      <c r="E406" s="2" t="s">
+      <c r="D406" s="5"/>
+      <c r="E406" s="5" t="s">
         <v>1242</v>
       </c>
-      <c r="F406" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G406" s="2" t="s">
+      <c r="F406" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G406" s="5" t="s">
         <v>1243</v>
       </c>
     </row>
     <row r="407" spans="1:7">
-      <c r="A407" s="2" t="s">
+      <c r="A407" s="5" t="s">
         <v>1244</v>
       </c>
-      <c r="B407" s="2" t="s">
+      <c r="B407" s="5" t="s">
         <v>1245</v>
       </c>
-      <c r="C407" s="2" t="s">
+      <c r="C407" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="D407" s="2" t="s">
+      <c r="D407" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="E407" s="2" t="s">
+      <c r="E407" s="5" t="s">
         <v>606</v>
       </c>
-      <c r="F407" s="2" t="s">
+      <c r="F407" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G407" s="2" t="s">
+      <c r="G407" s="5" t="s">
         <v>926</v>
       </c>
     </row>
     <row r="408" spans="1:7">
-      <c r="A408" s="2" t="s">
+      <c r="A408" s="5" t="s">
         <v>1246</v>
       </c>
-      <c r="B408" s="2" t="s">
+      <c r="B408" s="5" t="s">
         <v>1247</v>
       </c>
-      <c r="C408" s="2" t="s">
+      <c r="C408" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="D408" s="2" t="s">
+      <c r="D408" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="E408" s="2" t="s">
+      <c r="E408" s="5" t="s">
         <v>1248</v>
       </c>
-      <c r="F408" s="2" t="s">
+      <c r="F408" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G408" s="2" t="s">
+      <c r="G408" s="5" t="s">
         <v>1249</v>
       </c>
     </row>
     <row r="409" spans="1:7">
-      <c r="A409" s="2" t="s">
+      <c r="A409" s="5" t="s">
         <v>1250</v>
       </c>
-      <c r="B409" s="2" t="s">
+      <c r="B409" s="5" t="s">
         <v>1251</v>
       </c>
-      <c r="C409" s="2" t="s">
+      <c r="C409" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="D409" s="2"/>
-      <c r="E409" s="2" t="s">
+      <c r="D409" s="5"/>
+      <c r="E409" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="F409" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G409" s="2" t="s">
+      <c r="F409" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G409" s="5" t="s">
         <v>974</v>
       </c>
     </row>
     <row r="410" spans="1:7">
-      <c r="A410" s="2" t="s">
+      <c r="A410" s="5" t="s">
         <v>1252</v>
       </c>
-      <c r="B410" s="2" t="s">
+      <c r="B410" s="5" t="s">
         <v>1253</v>
       </c>
-      <c r="C410" s="2" t="s">
+      <c r="C410" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="D410" s="2"/>
-      <c r="E410" s="2" t="s">
+      <c r="D410" s="5"/>
+      <c r="E410" s="5" t="s">
         <v>452</v>
       </c>
-      <c r="F410" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G410" s="2" t="s">
+      <c r="F410" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G410" s="5" t="s">
         <v>1254</v>
       </c>
     </row>
     <row r="411" spans="1:7">
-      <c r="A411" s="2" t="s">
+      <c r="A411" s="5" t="s">
         <v>1255</v>
       </c>
-      <c r="B411" s="2" t="s">
+      <c r="B411" s="5" t="s">
         <v>1256</v>
       </c>
-      <c r="C411" s="2" t="s">
+      <c r="C411" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="D411" s="2" t="s">
+      <c r="D411" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="E411" s="2" t="s">
+      <c r="E411" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="F411" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G411" s="2" t="s">
+      <c r="F411" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G411" s="5" t="s">
         <v>1257</v>
       </c>
     </row>
     <row r="412" spans="1:7">
-      <c r="A412" s="2" t="s">
+      <c r="A412" s="5" t="s">
         <v>1258</v>
       </c>
-      <c r="B412" s="2" t="s">
+      <c r="B412" s="5" t="s">
         <v>1259</v>
       </c>
-      <c r="C412" s="2" t="s">
+      <c r="C412" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="D412" s="2" t="s">
+      <c r="D412" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="E412" s="2" t="s">
+      <c r="E412" s="5" t="s">
         <v>452</v>
       </c>
-      <c r="F412" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G412" s="2" t="s">
+      <c r="F412" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G412" s="5" t="s">
         <v>1260</v>
       </c>
     </row>
     <row r="413" spans="1:7">
-      <c r="A413" s="2" t="s">
+      <c r="A413" s="5" t="s">
         <v>1261</v>
       </c>
-      <c r="B413" s="2" t="s">
+      <c r="B413" s="5" t="s">
         <v>1262</v>
       </c>
-      <c r="C413" s="2" t="s">
+      <c r="C413" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D413" s="2"/>
-      <c r="E413" s="2" t="s">
+      <c r="D413" s="5"/>
+      <c r="E413" s="5" t="s">
         <v>1263</v>
       </c>
-      <c r="F413" s="2" t="s">
+      <c r="F413" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G413" s="2" t="s">
+      <c r="G413" s="5" t="s">
         <v>1264</v>
       </c>
     </row>
     <row r="414" spans="1:7">
-      <c r="A414" s="2" t="s">
+      <c r="A414" s="5" t="s">
         <v>1265</v>
       </c>
-      <c r="B414" s="2" t="s">
+      <c r="B414" s="5" t="s">
         <v>1266</v>
       </c>
-      <c r="C414" s="2" t="s">
+      <c r="C414" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D414" s="2" t="s">
+      <c r="D414" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="E414" s="2" t="s">
+      <c r="E414" s="5" t="s">
         <v>1267</v>
       </c>
-      <c r="F414" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G414" s="2" t="s">
+      <c r="F414" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G414" s="5" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="415" spans="1:7">
-      <c r="A415" s="2" t="s">
+      <c r="A415" s="5" t="s">
         <v>1268</v>
       </c>
-      <c r="B415" s="2" t="s">
+      <c r="B415" s="5" t="s">
         <v>1269</v>
       </c>
-      <c r="C415" s="2" t="s">
+      <c r="C415" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D415" s="2" t="s">
+      <c r="D415" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E415" s="2" t="s">
+      <c r="E415" s="5" t="s">
         <v>1267</v>
       </c>
-      <c r="F415" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G415" s="2" t="s">
+      <c r="F415" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G415" s="5" t="s">
         <v>1270</v>
       </c>
     </row>
     <row r="416" spans="1:7">
-      <c r="A416" s="2" t="s">
+      <c r="A416" s="5" t="s">
         <v>1271</v>
       </c>
-      <c r="B416" s="2" t="s">
+      <c r="B416" s="5" t="s">
         <v>1272</v>
       </c>
-      <c r="C416" s="2" t="s">
+      <c r="C416" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D416" s="2" t="s">
+      <c r="D416" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E416" s="2" t="s">
+      <c r="E416" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="F416" s="2" t="s">
+      <c r="F416" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G416" s="2" t="s">
+      <c r="G416" s="5" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="417" spans="1:7">
-      <c r="A417" s="2" t="s">
+      <c r="A417" s="5" t="s">
         <v>1273</v>
       </c>
-      <c r="B417" s="2" t="s">
+      <c r="B417" s="5" t="s">
         <v>1274</v>
       </c>
-      <c r="C417" s="2" t="s">
+      <c r="C417" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D417" s="2" t="s">
+      <c r="D417" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E417" s="2" t="s">
+      <c r="E417" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="F417" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G417" s="2" t="s">
+      <c r="F417" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G417" s="5" t="s">
         <v>1275</v>
       </c>
     </row>
     <row r="418" spans="1:7">
-      <c r="A418" s="2" t="s">
+      <c r="A418" s="5" t="s">
         <v>1276</v>
       </c>
-      <c r="B418" s="2" t="s">
+      <c r="B418" s="5" t="s">
         <v>1277</v>
       </c>
-      <c r="C418" s="2" t="s">
+      <c r="C418" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="D418" s="2"/>
-      <c r="E418" s="2" t="s">
+      <c r="D418" s="5"/>
+      <c r="E418" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F418" s="2" t="s">
+      <c r="F418" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="G418" s="2" t="s">
+      <c r="G418" s="5" t="s">
         <v>706</v>
       </c>
     </row>
     <row r="419" spans="1:7">
-      <c r="A419" s="2" t="s">
+      <c r="A419" s="5" t="s">
         <v>1278</v>
       </c>
-      <c r="B419" s="2" t="s">
+      <c r="B419" s="5" t="s">
         <v>1279</v>
       </c>
-      <c r="C419" s="2" t="s">
+      <c r="C419" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D419" s="2"/>
-      <c r="E419" s="2" t="s">
+      <c r="D419" s="5"/>
+      <c r="E419" s="5" t="s">
         <v>351</v>
       </c>
-      <c r="F419" s="2" t="s">
+      <c r="F419" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G419" s="2" t="s">
+      <c r="G419" s="5" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="420" spans="1:7">
-      <c r="A420" s="2" t="s">
+      <c r="A420" s="5" t="s">
         <v>1280</v>
       </c>
-      <c r="B420" s="2" t="s">
+      <c r="B420" s="5" t="s">
         <v>1281</v>
       </c>
-      <c r="C420" s="2" t="s">
+      <c r="C420" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D420" s="2"/>
-      <c r="E420" s="2" t="s">
+      <c r="D420" s="5"/>
+      <c r="E420" s="5" t="s">
         <v>452</v>
       </c>
-      <c r="F420" s="2" t="s">
+      <c r="F420" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G420" s="2" t="s">
+      <c r="G420" s="5" t="s">
         <v>576</v>
       </c>
     </row>
     <row r="421" spans="1:7">
-      <c r="A421" s="2" t="s">
+      <c r="A421" s="5" t="s">
         <v>1282</v>
       </c>
-      <c r="B421" s="2" t="s">
+      <c r="B421" s="5" t="s">
         <v>1283</v>
       </c>
-      <c r="C421" s="2" t="s">
+      <c r="C421" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="D421" s="2"/>
-      <c r="E421" s="2" t="s">
+      <c r="D421" s="5"/>
+      <c r="E421" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F421" s="2" t="s">
+      <c r="F421" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G421" s="2" t="s">
+      <c r="G421" s="5" t="s">
         <v>517</v>
       </c>
     </row>
     <row r="422" spans="1:7">
-      <c r="A422" s="2" t="s">
+      <c r="A422" s="5" t="s">
         <v>1284</v>
       </c>
-      <c r="B422" s="2" t="s">
+      <c r="B422" s="5" t="s">
         <v>1285</v>
       </c>
-      <c r="C422" s="2" t="s">
+      <c r="C422" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="D422" s="2"/>
-      <c r="E422" s="2" t="s">
+      <c r="D422" s="5"/>
+      <c r="E422" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="F422" s="2" t="s">
+      <c r="F422" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G422" s="2" t="s">
+      <c r="G422" s="5" t="s">
         <v>1286</v>
       </c>
     </row>
     <row r="423" spans="1:7">
-      <c r="A423" s="2" t="s">
+      <c r="A423" s="5" t="s">
         <v>1287</v>
       </c>
-      <c r="B423" s="2" t="s">
+      <c r="B423" s="5" t="s">
         <v>1288</v>
       </c>
-      <c r="C423" s="2" t="s">
+      <c r="C423" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D423" s="2"/>
-      <c r="E423" s="2" t="s">
+      <c r="D423" s="5"/>
+      <c r="E423" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="F423" s="2" t="s">
+      <c r="F423" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G423" s="2" t="s">
+      <c r="G423" s="5" t="s">
         <v>1289</v>
       </c>
     </row>
     <row r="424" spans="1:7">
-      <c r="A424" s="2" t="s">
+      <c r="A424" s="5" t="s">
         <v>1290</v>
       </c>
-      <c r="B424" s="2" t="s">
+      <c r="B424" s="5" t="s">
         <v>1291</v>
       </c>
-      <c r="C424" s="2" t="s">
+      <c r="C424" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D424" s="2" t="s">
+      <c r="D424" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="E424" s="2" t="s">
+      <c r="E424" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="F424" s="2" t="s">
+      <c r="F424" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G424" s="2" t="s">
+      <c r="G424" s="5" t="s">
         <v>1292</v>
       </c>
     </row>
     <row r="425" spans="1:7">
-      <c r="A425" s="2" t="s">
+      <c r="A425" s="5" t="s">
         <v>1293</v>
       </c>
-      <c r="B425" s="2" t="s">
+      <c r="B425" s="5" t="s">
         <v>1294</v>
       </c>
-      <c r="C425" s="2" t="s">
+      <c r="C425" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D425" s="2"/>
-      <c r="E425" s="2" t="s">
+      <c r="D425" s="5"/>
+      <c r="E425" s="5" t="s">
         <v>355</v>
       </c>
-      <c r="F425" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G425" s="2" t="s">
+      <c r="F425" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G425" s="5" t="s">
         <v>1295</v>
       </c>
     </row>
     <row r="426" spans="1:7">
-      <c r="A426" s="2" t="s">
+      <c r="A426" s="5" t="s">
         <v>1296</v>
       </c>
-      <c r="B426" s="2" t="s">
+      <c r="B426" s="5" t="s">
         <v>1297</v>
       </c>
-      <c r="C426" s="2" t="s">
+      <c r="C426" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="D426" s="2" t="s">
+      <c r="D426" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E426" s="2" t="s">
+      <c r="E426" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="F426" s="2" t="s">
+      <c r="F426" s="5" t="s">
         <v>1005</v>
       </c>
-      <c r="G426" s="2" t="s">
+      <c r="G426" s="5" t="s">
         <v>926</v>
       </c>
     </row>
     <row r="427" spans="1:7">
-      <c r="A427" s="2" t="s">
+      <c r="A427" s="5" t="s">
         <v>1298</v>
       </c>
-      <c r="B427" s="2" t="s">
+      <c r="B427" s="5" t="s">
         <v>1299</v>
       </c>
-      <c r="C427" s="2" t="s">
+      <c r="C427" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="D427" s="2" t="s">
+      <c r="D427" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E427" s="2" t="s">
+      <c r="E427" s="5" t="s">
         <v>1300</v>
       </c>
-      <c r="F427" s="2" t="s">
+      <c r="F427" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="G427" s="2" t="s">
+      <c r="G427" s="5" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="428" spans="1:7">
-      <c r="A428" s="2" t="s">
+      <c r="A428" s="5" t="s">
         <v>1301</v>
       </c>
-      <c r="B428" s="2" t="s">
+      <c r="B428" s="5" t="s">
         <v>1302</v>
       </c>
-      <c r="C428" s="2" t="s">
+      <c r="C428" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D428" s="2"/>
-      <c r="E428" s="2" t="s">
+      <c r="D428" s="5"/>
+      <c r="E428" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="F428" s="2" t="s">
+      <c r="F428" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G428" s="2" t="s">
+      <c r="G428" s="5" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="429" spans="1:7">
-      <c r="A429" s="2" t="s">
+      <c r="A429" s="5" t="s">
         <v>1303</v>
       </c>
-      <c r="B429" s="2" t="s">
+      <c r="B429" s="5" t="s">
         <v>1304</v>
       </c>
-      <c r="C429" s="2" t="s">
+      <c r="C429" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D429" s="2"/>
-      <c r="E429" s="2" t="s">
+      <c r="D429" s="5"/>
+      <c r="E429" s="5" t="s">
         <v>737</v>
       </c>
-      <c r="F429" s="2" t="s">
+      <c r="F429" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="G429" s="2" t="s">
+      <c r="G429" s="5" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="430" spans="1:7">
-      <c r="A430" s="2" t="s">
+      <c r="A430" s="5" t="s">
         <v>1305</v>
       </c>
-      <c r="B430" s="2" t="s">
+      <c r="B430" s="5" t="s">
         <v>1306</v>
       </c>
-      <c r="C430" s="2" t="s">
+      <c r="C430" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="D430" s="2"/>
-      <c r="E430" s="2" t="s">
+      <c r="D430" s="5"/>
+      <c r="E430" s="5" t="s">
         <v>452</v>
       </c>
-      <c r="F430" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G430" s="2" t="s">
+      <c r="F430" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G430" s="5" t="s">
         <v>1307</v>
       </c>
     </row>
     <row r="431" spans="1:7">
-      <c r="A431" s="2" t="s">
+      <c r="A431" s="5" t="s">
         <v>1308</v>
       </c>
-      <c r="B431" s="2" t="s">
+      <c r="B431" s="5" t="s">
         <v>1309</v>
       </c>
-      <c r="C431" s="2" t="s">
+      <c r="C431" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="D431" s="2" t="s">
+      <c r="D431" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E431" s="2" t="s">
+      <c r="E431" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="F431" s="2" t="s">
+      <c r="F431" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="G431" s="2" t="s">
+      <c r="G431" s="5" t="s">
         <v>1310</v>
       </c>
     </row>
     <row r="432" spans="1:7">
-      <c r="A432" s="2" t="s">
+      <c r="A432" s="5" t="s">
         <v>1311</v>
       </c>
-      <c r="B432" s="2" t="s">
+      <c r="B432" s="5" t="s">
         <v>1312</v>
       </c>
-      <c r="C432" s="2" t="s">
+      <c r="C432" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D432" s="2"/>
-      <c r="E432" s="2" t="s">
+      <c r="D432" s="5"/>
+      <c r="E432" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F432" s="2" t="s">
+      <c r="F432" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G432" s="2" t="s">
+      <c r="G432" s="5" t="s">
         <v>706</v>
       </c>
     </row>
     <row r="433" spans="1:7">
-      <c r="A433" s="2" t="s">
+      <c r="A433" s="5" t="s">
         <v>1313</v>
       </c>
-      <c r="B433" s="2" t="s">
+      <c r="B433" s="5" t="s">
         <v>1314</v>
       </c>
-      <c r="C433" s="2" t="s">
+      <c r="C433" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D433" s="2"/>
-      <c r="E433" s="2" t="s">
+      <c r="D433" s="5"/>
+      <c r="E433" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="F433" s="2" t="s">
+      <c r="F433" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G433" s="2" t="s">
+      <c r="G433" s="5" t="s">
         <v>1315</v>
       </c>
     </row>
     <row r="434" spans="1:7">
-      <c r="A434" s="2" t="s">
+      <c r="A434" s="5" t="s">
         <v>1316</v>
       </c>
-      <c r="B434" s="2" t="s">
+      <c r="B434" s="5" t="s">
         <v>1317</v>
       </c>
-      <c r="C434" s="2" t="s">
+      <c r="C434" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="D434" s="2"/>
-      <c r="E434" s="2" t="s">
+      <c r="D434" s="5"/>
+      <c r="E434" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="F434" s="2" t="s">
+      <c r="F434" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G434" s="2" t="s">
+      <c r="G434" s="5" t="s">
         <v>1318</v>
       </c>
     </row>
     <row r="435" spans="1:7">
-      <c r="A435" s="2" t="s">
+      <c r="A435" s="5" t="s">
         <v>1319</v>
       </c>
-      <c r="B435" s="2" t="s">
+      <c r="B435" s="5" t="s">
         <v>1320</v>
       </c>
-      <c r="C435" s="2" t="s">
+      <c r="C435" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D435" s="2" t="s">
+      <c r="D435" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="E435" s="2" t="s">
+      <c r="E435" s="5" t="s">
         <v>351</v>
       </c>
-      <c r="F435" s="2" t="s">
+      <c r="F435" s="5" t="s">
         <v>359</v>
       </c>
-      <c r="G435" s="2" t="s">
+      <c r="G435" s="5" t="s">
         <v>1321</v>
       </c>
     </row>
     <row r="436" spans="1:7">
-      <c r="A436" s="2" t="s">
+      <c r="A436" s="5" t="s">
         <v>1322</v>
       </c>
-      <c r="B436" s="2" t="s">
+      <c r="B436" s="5" t="s">
         <v>1323</v>
       </c>
-      <c r="C436" s="2" t="s">
+      <c r="C436" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D436" s="2" t="s">
+      <c r="D436" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="E436" s="2" t="s">
+      <c r="E436" s="5" t="s">
         <v>737</v>
       </c>
-      <c r="F436" s="2" t="s">
+      <c r="F436" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="G436" s="2" t="s">
+      <c r="G436" s="5" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="437" spans="1:7">
-      <c r="A437" s="2" t="s">
+      <c r="A437" s="5" t="s">
         <v>1324</v>
       </c>
-      <c r="B437" s="2" t="s">
+      <c r="B437" s="5" t="s">
         <v>1325</v>
       </c>
-      <c r="C437" s="2" t="s">
+      <c r="C437" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="D437" s="2" t="s">
+      <c r="D437" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E437" s="2" t="s">
+      <c r="E437" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="F437" s="2" t="s">
+      <c r="F437" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G437" s="2" t="s">
+      <c r="G437" s="5" t="s">
         <v>1326</v>
       </c>
     </row>
     <row r="438" spans="1:7">
-      <c r="A438" s="2" t="s">
+      <c r="A438" s="5" t="s">
         <v>1327</v>
       </c>
-      <c r="B438" s="2" t="s">
+      <c r="B438" s="5" t="s">
         <v>1328</v>
       </c>
-      <c r="C438" s="2" t="s">
+      <c r="C438" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="D438" s="2" t="s">
+      <c r="D438" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E438" s="2" t="s">
+      <c r="E438" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F438" s="2" t="s">
+      <c r="F438" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="G438" s="2" t="s">
+      <c r="G438" s="5" t="s">
         <v>796</v>
       </c>
     </row>
     <row r="439" spans="1:7">
-      <c r="A439" s="2" t="s">
+      <c r="A439" s="5" t="s">
         <v>1329</v>
       </c>
-      <c r="B439" s="2" t="s">
+      <c r="B439" s="5" t="s">
         <v>1330</v>
       </c>
-      <c r="C439" s="2" t="s">
+      <c r="C439" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="D439" s="2"/>
-      <c r="E439" s="2" t="s">
+      <c r="D439" s="5"/>
+      <c r="E439" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="F439" s="2" t="s">
+      <c r="F439" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G439" s="2" t="s">
+      <c r="G439" s="5" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="440" spans="1:7">
-      <c r="A440" s="2" t="s">
+      <c r="A440" s="5" t="s">
         <v>1331</v>
       </c>
-      <c r="B440" s="2" t="s">
+      <c r="B440" s="5" t="s">
         <v>1332</v>
       </c>
-      <c r="C440" s="2" t="s">
+      <c r="C440" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="D440" s="2" t="s">
+      <c r="D440" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E440" s="2" t="s">
+      <c r="E440" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F440" s="2" t="s">
+      <c r="F440" s="5" t="s">
         <v>1333</v>
       </c>
-      <c r="G440" s="2" t="s">
+      <c r="G440" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="441" spans="1:7">
-      <c r="A441" s="2" t="s">
+      <c r="A441" s="5" t="s">
         <v>1334</v>
       </c>
-      <c r="B441" s="2" t="s">
+      <c r="B441" s="5" t="s">
         <v>1335</v>
       </c>
-      <c r="C441" s="2" t="s">
+      <c r="C441" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D441" s="2"/>
-      <c r="E441" s="2" t="s">
+      <c r="D441" s="5"/>
+      <c r="E441" s="5" t="s">
         <v>1336</v>
       </c>
-      <c r="F441" s="2" t="s">
+      <c r="F441" s="5" t="s">
         <v>1337</v>
       </c>
-      <c r="G441" s="2" t="s">
+      <c r="G441" s="5" t="s">
         <v>1338</v>
       </c>
     </row>
     <row r="442" spans="1:7">
-      <c r="A442" s="2" t="s">
+      <c r="A442" s="5" t="s">
         <v>1339</v>
       </c>
-      <c r="B442" s="2" t="s">
+      <c r="B442" s="5" t="s">
         <v>1340</v>
       </c>
-      <c r="C442" s="2" t="s">
+      <c r="C442" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D442" s="2" t="s">
+      <c r="D442" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E442" s="2" t="s">
+      <c r="E442" s="5" t="s">
         <v>628</v>
       </c>
-      <c r="F442" s="2" t="s">
+      <c r="F442" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="G442" s="2" t="s">
+      <c r="G442" s="5" t="s">
         <v>1058</v>
       </c>
     </row>
     <row r="443" spans="1:7">
-      <c r="A443" s="2" t="s">
+      <c r="A443" s="5" t="s">
         <v>1341</v>
       </c>
-      <c r="B443" s="2" t="s">
+      <c r="B443" s="5" t="s">
         <v>1342</v>
       </c>
-      <c r="C443" s="2" t="s">
+      <c r="C443" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="D443" s="2" t="s">
+      <c r="D443" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="E443" s="2" t="s">
+      <c r="E443" s="5" t="s">
         <v>404</v>
       </c>
-      <c r="F443" s="2" t="s">
+      <c r="F443" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="G443" s="2" t="s">
+      <c r="G443" s="5" t="s">
         <v>1075</v>
       </c>
     </row>
     <row r="444" spans="1:7">
-      <c r="A444" s="2" t="s">
+      <c r="A444" s="5" t="s">
         <v>1343</v>
       </c>
-      <c r="B444" s="2" t="s">
+      <c r="B444" s="5" t="s">
         <v>1344</v>
       </c>
-      <c r="C444" s="2" t="s">
+      <c r="C444" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="D444" s="2" t="s">
+      <c r="D444" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="E444" s="2" t="s">
+      <c r="E444" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="F444" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G444" s="2" t="s">
+      <c r="F444" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G444" s="5" t="s">
         <v>712</v>
       </c>
     </row>
     <row r="445" spans="1:7">
-      <c r="A445" s="2" t="s">
+      <c r="A445" s="5" t="s">
         <v>1345</v>
       </c>
-      <c r="B445" s="2" t="s">
+      <c r="B445" s="5" t="s">
         <v>1346</v>
       </c>
-      <c r="C445" s="2" t="s">
+      <c r="C445" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="D445" s="2" t="s">
+      <c r="D445" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="E445" s="2" t="s">
+      <c r="E445" s="5" t="s">
         <v>628</v>
       </c>
-      <c r="F445" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G445" s="2" t="s">
+      <c r="F445" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G445" s="5" t="s">
         <v>443</v>
       </c>
     </row>
     <row r="446" spans="1:7">
-      <c r="A446" s="2" t="s">
+      <c r="A446" s="5" t="s">
         <v>1347</v>
       </c>
-      <c r="B446" s="2" t="s">
+      <c r="B446" s="5" t="s">
         <v>1348</v>
       </c>
-      <c r="C446" s="2" t="s">
+      <c r="C446" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="D446" s="2" t="s">
+      <c r="D446" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="E446" s="2" t="s">
+      <c r="E446" s="5" t="s">
         <v>524</v>
       </c>
-      <c r="F446" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G446" s="2" t="s">
+      <c r="F446" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G446" s="5" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="447" spans="1:7">
-      <c r="A447" s="2" t="s">
+      <c r="A447" s="5" t="s">
         <v>1349</v>
       </c>
-      <c r="B447" s="2" t="s">
+      <c r="B447" s="5" t="s">
         <v>1350</v>
       </c>
-      <c r="C447" s="2" t="s">
+      <c r="C447" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D447" s="2"/>
-      <c r="E447" s="2" t="s">
+      <c r="D447" s="5"/>
+      <c r="E447" s="5" t="s">
         <v>650</v>
       </c>
-      <c r="F447" s="2" t="s">
+      <c r="F447" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="G447" s="2" t="s">
+      <c r="G447" s="5" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="448" spans="1:7">
-      <c r="A448" s="2" t="s">
+      <c r="A448" s="5" t="s">
         <v>1351</v>
       </c>
-      <c r="B448" s="2" t="s">
+      <c r="B448" s="5" t="s">
         <v>1352</v>
       </c>
-      <c r="C448" s="2" t="s">
+      <c r="C448" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="D448" s="2"/>
-      <c r="E448" s="2" t="s">
+      <c r="D448" s="5"/>
+      <c r="E448" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="F448" s="2" t="s">
+      <c r="F448" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G448" s="2" t="s">
+      <c r="G448" s="5" t="s">
         <v>893</v>
       </c>
     </row>
     <row r="449" spans="1:7">
-      <c r="A449" s="2" t="s">
+      <c r="A449" s="5" t="s">
         <v>1353</v>
       </c>
-      <c r="B449" s="2" t="s">
+      <c r="B449" s="5" t="s">
         <v>1354</v>
       </c>
-      <c r="C449" s="2" t="s">
+      <c r="C449" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="D449" s="2" t="s">
+      <c r="D449" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="E449" s="2" t="s">
+      <c r="E449" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="F449" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G449" s="2" t="s">
+      <c r="F449" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G449" s="5" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="450" spans="1:7">
-      <c r="A450" s="2" t="s">
+      <c r="A450" s="5" t="s">
         <v>1355</v>
       </c>
-      <c r="B450" s="2" t="s">
+      <c r="B450" s="5" t="s">
         <v>1356</v>
       </c>
-      <c r="C450" s="2" t="s">
+      <c r="C450" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="D450" s="2"/>
-      <c r="E450" s="2" t="s">
+      <c r="D450" s="5"/>
+      <c r="E450" s="5" t="s">
         <v>351</v>
       </c>
-      <c r="F450" s="2" t="s">
+      <c r="F450" s="5" t="s">
         <v>1357</v>
       </c>
-      <c r="G450" s="2" t="s">
+      <c r="G450" s="5" t="s">
         <v>1358</v>
       </c>
     </row>
     <row r="451" spans="1:7">
-      <c r="A451" s="2" t="s">
+      <c r="A451" s="5" t="s">
         <v>1359</v>
       </c>
-      <c r="B451" s="2" t="s">
+      <c r="B451" s="5" t="s">
         <v>1360</v>
       </c>
-      <c r="C451" s="2" t="s">
+      <c r="C451" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="D451" s="2"/>
-      <c r="E451" s="2" t="s">
+      <c r="D451" s="5"/>
+      <c r="E451" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="F451" s="2" t="s">
+      <c r="F451" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="G451" s="2" t="s">
+      <c r="G451" s="5" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="452" spans="1:7">
-      <c r="A452" s="2" t="s">
+      <c r="A452" s="5" t="s">
         <v>1361</v>
       </c>
-      <c r="B452" s="2" t="s">
+      <c r="B452" s="5" t="s">
         <v>1362</v>
       </c>
-      <c r="C452" s="2" t="s">
+      <c r="C452" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D452" s="2" t="s">
+      <c r="D452" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E452" s="2" t="s">
+      <c r="E452" s="5" t="s">
         <v>351</v>
       </c>
-      <c r="F452" s="2" t="s">
+      <c r="F452" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G452" s="2" t="s">
+      <c r="G452" s="5" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="453" spans="1:7">
-      <c r="A453" s="2" t="s">
+      <c r="A453" s="5" t="s">
         <v>1363</v>
       </c>
-      <c r="B453" s="2" t="s">
+      <c r="B453" s="5" t="s">
         <v>1364</v>
       </c>
-      <c r="C453" s="2" t="s">
+      <c r="C453" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D453" s="2" t="s">
+      <c r="D453" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="E453" s="2" t="s">
+      <c r="E453" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F453" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G453" s="2" t="s">
+      <c r="F453" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G453" s="5" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="454" spans="1:7">
-      <c r="A454" s="2" t="s">
+      <c r="A454" s="5" t="s">
         <v>1365</v>
       </c>
-      <c r="B454" s="2" t="s">
+      <c r="B454" s="5" t="s">
         <v>1366</v>
       </c>
-      <c r="C454" s="2" t="s">
+      <c r="C454" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D454" s="2" t="s">
+      <c r="D454" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="E454" s="2" t="s">
+      <c r="E454" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="F454" s="2" t="s">
+      <c r="F454" s="5" t="s">
         <v>1357</v>
       </c>
-      <c r="G454" s="2" t="s">
+      <c r="G454" s="5" t="s">
         <v>1212</v>
       </c>
     </row>
     <row r="455" spans="1:7">
-      <c r="A455" s="2" t="s">
+      <c r="A455" s="5" t="s">
         <v>1367</v>
       </c>
-      <c r="B455" s="2" t="s">
+      <c r="B455" s="5" t="s">
         <v>1368</v>
       </c>
-      <c r="C455" s="2" t="s">
+      <c r="C455" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D455" s="2" t="s">
+      <c r="D455" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="E455" s="2" t="s">
+      <c r="E455" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="F455" s="2" t="s">
+      <c r="F455" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G455" s="2" t="s">
+      <c r="G455" s="5" t="s">
         <v>1369</v>
       </c>
     </row>
     <row r="456" spans="1:7">
-      <c r="A456" s="2" t="s">
+      <c r="A456" s="5" t="s">
         <v>1370</v>
       </c>
-      <c r="B456" s="2" t="s">
+      <c r="B456" s="5" t="s">
         <v>1371</v>
       </c>
-      <c r="C456" s="2" t="s">
+      <c r="C456" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="D456" s="2"/>
-      <c r="E456" s="2" t="s">
+      <c r="D456" s="5"/>
+      <c r="E456" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="F456" s="2" t="s">
+      <c r="F456" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="G456" s="2" t="s">
+      <c r="G456" s="5" t="s">
         <v>662</v>
       </c>
     </row>
     <row r="457" spans="1:7">
-      <c r="A457" s="2" t="s">
+      <c r="A457" s="5" t="s">
         <v>1372</v>
       </c>
-      <c r="B457" s="2" t="s">
+      <c r="B457" s="5" t="s">
         <v>1373</v>
       </c>
-      <c r="C457" s="2" t="s">
+      <c r="C457" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D457" s="2"/>
-      <c r="E457" s="2" t="s">
+      <c r="D457" s="5"/>
+      <c r="E457" s="5" t="s">
         <v>351</v>
       </c>
-      <c r="F457" s="2" t="s">
+      <c r="F457" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G457" s="2" t="s">
+      <c r="G457" s="5" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="458" spans="1:7">
-      <c r="A458" s="2" t="s">
+      <c r="A458" s="5" t="s">
         <v>1374</v>
       </c>
-      <c r="B458" s="2" t="s">
+      <c r="B458" s="5" t="s">
         <v>1375</v>
       </c>
-      <c r="C458" s="2" t="s">
+      <c r="C458" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D458" s="2"/>
-      <c r="E458" s="2" t="s">
+      <c r="D458" s="5"/>
+      <c r="E458" s="5" t="s">
         <v>438</v>
       </c>
-      <c r="F458" s="2" t="s">
+      <c r="F458" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G458" s="2" t="s">
+      <c r="G458" s="5" t="s">
         <v>910</v>
       </c>
     </row>
     <row r="459" spans="1:7">
-      <c r="A459" s="2" t="s">
+      <c r="A459" s="5" t="s">
         <v>1376</v>
       </c>
-      <c r="B459" s="2" t="s">
+      <c r="B459" s="5" t="s">
         <v>1377</v>
       </c>
-      <c r="C459" s="2" t="s">
+      <c r="C459" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D459" s="2" t="s">
+      <c r="D459" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E459" s="2" t="s">
+      <c r="E459" s="5" t="s">
         <v>400</v>
       </c>
-      <c r="F459" s="2" t="s">
+      <c r="F459" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="G459" s="2" t="s">
+      <c r="G459" s="5" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="460" spans="1:7">
-      <c r="A460" s="2" t="s">
+      <c r="A460" s="5" t="s">
         <v>1378</v>
       </c>
-      <c r="B460" s="2" t="s">
+      <c r="B460" s="5" t="s">
         <v>1379</v>
       </c>
-      <c r="C460" s="2" t="s">
+      <c r="C460" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="D460" s="2" t="s">
+      <c r="D460" s="5" t="s">
         <v>1117</v>
       </c>
-      <c r="E460" s="2" t="s">
+      <c r="E460" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="F460" s="2" t="s">
+      <c r="F460" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G460" s="2" t="s">
+      <c r="G460" s="5" t="s">
         <v>746</v>
       </c>
     </row>
     <row r="461" spans="1:7">
-      <c r="A461" s="2" t="s">
+      <c r="A461" s="5" t="s">
         <v>1380</v>
       </c>
-      <c r="B461" s="2" t="s">
+      <c r="B461" s="5" t="s">
         <v>1381</v>
       </c>
-      <c r="C461" s="2" t="s">
+      <c r="C461" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="D461" s="2" t="s">
+      <c r="D461" s="5" t="s">
         <v>1117</v>
       </c>
-      <c r="E461" s="2" t="s">
+      <c r="E461" s="5" t="s">
         <v>452</v>
       </c>
-      <c r="F461" s="2" t="s">
+      <c r="F461" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="G461" s="2" t="s">
+      <c r="G461" s="5" t="s">
         <v>1382</v>
       </c>
     </row>
     <row r="462" spans="1:7">
-      <c r="A462" s="2" t="s">
+      <c r="A462" s="5" t="s">
         <v>1383</v>
       </c>
-      <c r="B462" s="2" t="s">
+      <c r="B462" s="5" t="s">
         <v>1384</v>
       </c>
-      <c r="C462" s="2" t="s">
+      <c r="C462" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="D462" s="2" t="s">
+      <c r="D462" s="5" t="s">
         <v>1117</v>
       </c>
-      <c r="E462" s="2" t="s">
+      <c r="E462" s="5" t="s">
         <v>697</v>
       </c>
-      <c r="F462" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G462" s="2" t="s">
+      <c r="F462" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G462" s="5" t="s">
         <v>1385</v>
       </c>
     </row>
     <row r="463" spans="1:7">
-      <c r="A463" s="2" t="s">
+      <c r="A463" s="5" t="s">
         <v>1386</v>
       </c>
-      <c r="B463" s="2" t="s">
+      <c r="B463" s="5" t="s">
         <v>1387</v>
       </c>
-      <c r="C463" s="2" t="s">
+      <c r="C463" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="D463" s="2" t="s">
+      <c r="D463" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="E463" s="2" t="s">
+      <c r="E463" s="5" t="s">
         <v>1388</v>
       </c>
-      <c r="F463" s="2" t="s">
+      <c r="F463" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="G463" s="2" t="s">
+      <c r="G463" s="5" t="s">
         <v>1389</v>
       </c>
     </row>
     <row r="464" spans="1:7">
-      <c r="A464" s="2" t="s">
+      <c r="A464" s="5" t="s">
         <v>1390</v>
       </c>
-      <c r="B464" s="2" t="s">
+      <c r="B464" s="5" t="s">
         <v>1391</v>
       </c>
-      <c r="C464" s="2" t="s">
+      <c r="C464" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D464" s="2"/>
-      <c r="E464" s="2" t="s">
+      <c r="D464" s="5"/>
+      <c r="E464" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="F464" s="2" t="s">
+      <c r="F464" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="G464" s="2" t="s">
+      <c r="G464" s="5" t="s">
         <v>1392</v>
       </c>
     </row>
     <row r="465" spans="1:7">
-      <c r="A465" s="2" t="s">
+      <c r="A465" s="5" t="s">
         <v>1393</v>
       </c>
-      <c r="B465" s="2" t="s">
+      <c r="B465" s="5" t="s">
         <v>1394</v>
       </c>
-      <c r="C465" s="2" t="s">
+      <c r="C465" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="D465" s="2" t="s">
+      <c r="D465" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="E465" s="2" t="s">
+      <c r="E465" s="5" t="s">
         <v>579</v>
       </c>
-      <c r="F465" s="2" t="s">
+      <c r="F465" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="G465" s="2" t="s">
+      <c r="G465" s="5" t="s">
         <v>1395</v>
       </c>
     </row>
     <row r="466" spans="1:7">
-      <c r="A466" s="2" t="s">
+      <c r="A466" s="5" t="s">
         <v>1396</v>
       </c>
-      <c r="B466" s="2" t="s">
+      <c r="B466" s="5" t="s">
         <v>1397</v>
       </c>
-      <c r="C466" s="2" t="s">
+      <c r="C466" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="D466" s="2"/>
-      <c r="E466" s="2" t="s">
+      <c r="D466" s="5"/>
+      <c r="E466" s="5" t="s">
         <v>468</v>
       </c>
-      <c r="F466" s="2" t="s">
+      <c r="F466" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="G466" s="2" t="s">
+      <c r="G466" s="5" t="s">
         <v>1398</v>
       </c>
     </row>
     <row r="467" spans="1:7">
-      <c r="A467" s="2" t="s">
+      <c r="A467" s="5" t="s">
         <v>1399</v>
       </c>
-      <c r="B467" s="2" t="s">
+      <c r="B467" s="5" t="s">
         <v>1400</v>
       </c>
-      <c r="C467" s="2" t="s">
+      <c r="C467" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="D467" s="2"/>
-      <c r="E467" s="2" t="s">
+      <c r="D467" s="5"/>
+      <c r="E467" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="F467" s="2" t="s">
+      <c r="F467" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="G467" s="2" t="s">
+      <c r="G467" s="5" t="s">
         <v>1401</v>
       </c>
     </row>
     <row r="468" spans="1:7">
-      <c r="A468" s="2" t="s">
+      <c r="A468" s="5" t="s">
         <v>1402</v>
       </c>
-      <c r="B468" s="2" t="s">
+      <c r="B468" s="5" t="s">
         <v>1403</v>
       </c>
-      <c r="C468" s="2" t="s">
+      <c r="C468" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D468" s="2"/>
-      <c r="E468" s="2" t="s">
+      <c r="D468" s="5"/>
+      <c r="E468" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="F468" s="2" t="s">
+      <c r="F468" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="G468" s="2" t="s">
+      <c r="G468" s="5" t="s">
         <v>1404</v>
       </c>
     </row>
     <row r="469" spans="1:7">
-      <c r="A469" s="2" t="s">
+      <c r="A469" s="5" t="s">
         <v>1405</v>
       </c>
-      <c r="B469" s="2" t="s">
+      <c r="B469" s="5" t="s">
         <v>1406</v>
       </c>
-      <c r="C469" s="2" t="s">
+      <c r="C469" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="D469" s="2" t="s">
+      <c r="D469" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E469" s="2" t="s">
+      <c r="E469" s="5" t="s">
         <v>1407</v>
       </c>
-      <c r="F469" s="2" t="s">
+      <c r="F469" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="G469" s="2" t="s">
+      <c r="G469" s="5" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="470" spans="1:7">
-      <c r="A470" s="2" t="s">
+      <c r="A470" s="5" t="s">
         <v>1408</v>
       </c>
-      <c r="B470" s="2" t="s">
+      <c r="B470" s="5" t="s">
         <v>1409</v>
       </c>
-      <c r="C470" s="2" t="s">
+      <c r="C470" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D470" s="2" t="s">
+      <c r="D470" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E470" s="2" t="s">
+      <c r="E470" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="F470" s="2" t="s">
+      <c r="F470" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="G470" s="2" t="s">
+      <c r="G470" s="5" t="s">
         <v>1410</v>
       </c>
     </row>
     <row r="471" spans="1:7">
-      <c r="A471" s="2" t="s">
+      <c r="A471" s="5" t="s">
         <v>1411</v>
       </c>
-      <c r="B471" s="2" t="s">
+      <c r="B471" s="5" t="s">
         <v>1412</v>
       </c>
-      <c r="C471" s="2" t="s">
+      <c r="C471" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="D471" s="2"/>
-      <c r="E471" s="2" t="s">
+      <c r="D471" s="5"/>
+      <c r="E471" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="F471" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G471" s="2" t="s">
+      <c r="F471" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G471" s="5" t="s">
         <v>1233</v>
       </c>
     </row>
     <row r="472" spans="1:7">
-      <c r="A472" s="2" t="s">
+      <c r="A472" s="5" t="s">
         <v>1413</v>
       </c>
-      <c r="B472" s="2" t="s">
+      <c r="B472" s="5" t="s">
         <v>1414</v>
       </c>
-      <c r="C472" s="2" t="s">
+      <c r="C472" s="5" t="s">
         <v>1117</v>
       </c>
-      <c r="D472" s="2"/>
-      <c r="E472" s="2" t="s">
+      <c r="D472" s="5"/>
+      <c r="E472" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="F472" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G472" s="2" t="s">
+      <c r="F472" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G472" s="5" t="s">
         <v>1415</v>
       </c>
     </row>
     <row r="473" spans="1:7">
-      <c r="A473" s="2" t="s">
+      <c r="A473" s="5" t="s">
         <v>1416</v>
       </c>
-      <c r="B473" s="2" t="s">
+      <c r="B473" s="5" t="s">
         <v>1417</v>
       </c>
-      <c r="C473" s="2" t="s">
+      <c r="C473" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="D473" s="2" t="s">
+      <c r="D473" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E473" s="2" t="s">
+      <c r="E473" s="5" t="s">
         <v>697</v>
       </c>
-      <c r="F473" s="2" t="s">
+      <c r="F473" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="G473" s="2" t="s">
+      <c r="G473" s="5" t="s">
         <v>1418</v>
       </c>
     </row>
     <row r="474" spans="1:7">
-      <c r="A474" s="2" t="s">
+      <c r="A474" s="5" t="s">
         <v>1419</v>
       </c>
-      <c r="B474" s="2" t="s">
+      <c r="B474" s="5" t="s">
         <v>1420</v>
       </c>
-      <c r="C474" s="2" t="s">
+      <c r="C474" s="5" t="s">
         <v>1117</v>
       </c>
-      <c r="D474" s="2" t="s">
+      <c r="D474" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="E474" s="2" t="s">
+      <c r="E474" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F474" s="2" t="s">
+      <c r="F474" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="G474" s="2" t="s">
+      <c r="G474" s="5" t="s">
         <v>1421</v>
       </c>
     </row>
     <row r="475" spans="1:7">
-      <c r="A475" s="2" t="s">
+      <c r="A475" s="5" t="s">
         <v>1422</v>
       </c>
-      <c r="B475" s="2" t="s">
+      <c r="B475" s="5" t="s">
         <v>1423</v>
       </c>
-      <c r="C475" s="2" t="s">
+      <c r="C475" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D475" s="2"/>
-      <c r="E475" s="2" t="s">
+      <c r="D475" s="5"/>
+      <c r="E475" s="5" t="s">
         <v>579</v>
       </c>
-      <c r="F475" s="2" t="s">
+      <c r="F475" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="G475" s="2" t="s">
+      <c r="G475" s="5" t="s">
         <v>1385</v>
       </c>
     </row>
     <row r="476" spans="1:7">
-      <c r="A476" s="2" t="s">
+      <c r="A476" s="5" t="s">
         <v>1424</v>
       </c>
-      <c r="B476" s="2" t="s">
+      <c r="B476" s="5" t="s">
         <v>1425</v>
       </c>
-      <c r="C476" s="2" t="s">
+      <c r="C476" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="D476" s="2" t="s">
+      <c r="D476" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="E476" s="2" t="s">
+      <c r="E476" s="5" t="s">
         <v>896</v>
       </c>
-      <c r="F476" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G476" s="2" t="s">
+      <c r="F476" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G476" s="5" t="s">
         <v>829</v>
       </c>
     </row>
     <row r="477" spans="1:7">
-      <c r="A477" s="2" t="s">
+      <c r="A477" s="5" t="s">
         <v>1426</v>
       </c>
-      <c r="B477" s="2" t="s">
+      <c r="B477" s="5" t="s">
         <v>1427</v>
       </c>
-      <c r="C477" s="2" t="s">
+      <c r="C477" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="D477" s="2" t="s">
+      <c r="D477" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="E477" s="2" t="s">
+      <c r="E477" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="F477" s="2" t="s">
+      <c r="F477" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="G477" s="2" t="s">
+      <c r="G477" s="5" t="s">
         <v>1428</v>
       </c>
     </row>
     <row r="478" spans="1:7">
-      <c r="A478" s="2" t="s">
+      <c r="A478" s="5" t="s">
         <v>1429</v>
       </c>
-      <c r="B478" s="2" t="s">
+      <c r="B478" s="5" t="s">
         <v>1430</v>
       </c>
-      <c r="C478" s="2" t="s">
+      <c r="C478" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="D478" s="2"/>
-      <c r="E478" s="2" t="s">
+      <c r="D478" s="5"/>
+      <c r="E478" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F478" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G478" s="2" t="s">
+      <c r="F478" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G478" s="5" t="s">
         <v>1431</v>
       </c>
     </row>
     <row r="479" spans="1:7">
-      <c r="A479" s="2" t="s">
+      <c r="A479" s="5" t="s">
         <v>1432</v>
       </c>
-      <c r="B479" s="2" t="s">
+      <c r="B479" s="5" t="s">
         <v>1433</v>
       </c>
-      <c r="C479" s="2" t="s">
+      <c r="C479" s="5" t="s">
         <v>1117</v>
       </c>
-      <c r="D479" s="2" t="s">
+      <c r="D479" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="E479" s="2" t="s">
+      <c r="E479" s="5" t="s">
         <v>737</v>
       </c>
-      <c r="F479" s="2" t="s">
+      <c r="F479" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G479" s="2" t="s">
+      <c r="G479" s="5" t="s">
         <v>1434</v>
       </c>
     </row>
     <row r="480" spans="1:7">
-      <c r="A480" s="2" t="s">
+      <c r="A480" s="5" t="s">
         <v>1435</v>
       </c>
-      <c r="B480" s="2" t="s">
+      <c r="B480" s="5" t="s">
         <v>1436</v>
       </c>
-      <c r="C480" s="2" t="s">
+      <c r="C480" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="D480" s="2" t="s">
+      <c r="D480" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="E480" s="2" t="s">
+      <c r="E480" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="F480" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G480" s="2" t="s">
+      <c r="F480" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G480" s="5" t="s">
         <v>1437</v>
       </c>
     </row>
     <row r="481" spans="1:7">
-      <c r="A481" s="2" t="s">
+      <c r="A481" s="5" t="s">
         <v>1438</v>
       </c>
-      <c r="B481" s="2" t="s">
+      <c r="B481" s="5" t="s">
         <v>1439</v>
       </c>
-      <c r="C481" s="2" t="s">
+      <c r="C481" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="D481" s="2"/>
-      <c r="E481" s="2" t="s">
+      <c r="D481" s="5"/>
+      <c r="E481" s="5" t="s">
         <v>506</v>
       </c>
-      <c r="F481" s="2" t="s">
+      <c r="F481" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G481" s="2" t="s">
+      <c r="G481" s="5" t="s">
         <v>1437</v>
       </c>
     </row>
     <row r="482" spans="1:7">
-      <c r="A482" s="2" t="s">
+      <c r="A482" s="5" t="s">
         <v>1440</v>
       </c>
-      <c r="B482" s="2" t="s">
+      <c r="B482" s="5" t="s">
         <v>1441</v>
       </c>
-      <c r="C482" s="2" t="s">
+      <c r="C482" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="D482" s="2"/>
-      <c r="E482" s="2" t="s">
+      <c r="D482" s="5"/>
+      <c r="E482" s="5" t="s">
         <v>506</v>
       </c>
-      <c r="F482" s="2" t="s">
+      <c r="F482" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G482" s="2" t="s">
+      <c r="G482" s="5" t="s">
         <v>1437</v>
       </c>
     </row>
     <row r="483" spans="1:7">
-      <c r="A483" s="2" t="s">
+      <c r="A483" s="5" t="s">
         <v>1442</v>
       </c>
-      <c r="B483" s="2" t="s">
+      <c r="B483" s="5" t="s">
         <v>1443</v>
       </c>
-      <c r="C483" s="2" t="s">
+      <c r="C483" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="D483" s="2"/>
-      <c r="E483" s="2" t="s">
+      <c r="D483" s="5"/>
+      <c r="E483" s="5" t="s">
         <v>506</v>
       </c>
-      <c r="F483" s="2" t="s">
+      <c r="F483" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G483" s="2" t="s">
+      <c r="G483" s="5" t="s">
         <v>1437</v>
       </c>
     </row>
     <row r="484" spans="1:7">
-      <c r="A484" s="2" t="s">
+      <c r="A484" s="5" t="s">
         <v>1444</v>
       </c>
-      <c r="B484" s="2" t="s">
+      <c r="B484" s="5" t="s">
         <v>1445</v>
       </c>
-      <c r="C484" s="2" t="s">
+      <c r="C484" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="D484" s="2" t="s">
+      <c r="D484" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="E484" s="2" t="s">
+      <c r="E484" s="5" t="s">
         <v>527</v>
       </c>
-      <c r="F484" s="2" t="s">
+      <c r="F484" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G484" s="2" t="s">
+      <c r="G484" s="5" t="s">
         <v>1446</v>
       </c>
     </row>
     <row r="485" spans="1:7">
-      <c r="A485" s="2" t="s">
+      <c r="A485" s="5" t="s">
         <v>1447</v>
       </c>
-      <c r="B485" s="2" t="s">
+      <c r="B485" s="5" t="s">
         <v>1448</v>
       </c>
-      <c r="C485" s="2" t="s">
+      <c r="C485" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D485" s="2" t="s">
+      <c r="D485" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="E485" s="2" t="s">
+      <c r="E485" s="5" t="s">
         <v>527</v>
       </c>
-      <c r="F485" s="2" t="s">
+      <c r="F485" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G485" s="2" t="s">
+      <c r="G485" s="5" t="s">
         <v>1449</v>
       </c>
     </row>
     <row r="486" spans="1:7">
-      <c r="A486" s="2" t="s">
+      <c r="A486" s="5" t="s">
         <v>1450</v>
       </c>
-      <c r="B486" s="2" t="s">
+      <c r="B486" s="5" t="s">
         <v>1451</v>
       </c>
-      <c r="C486" s="2" t="s">
+      <c r="C486" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D486" s="2" t="s">
+      <c r="D486" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="E486" s="2" t="s">
+      <c r="E486" s="5" t="s">
         <v>524</v>
       </c>
-      <c r="F486" s="2" t="s">
+      <c r="F486" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G486" s="2" t="s">
+      <c r="G486" s="5" t="s">
         <v>1452</v>
       </c>
     </row>
     <row r="487" spans="1:7">
-      <c r="A487" s="2" t="s">
+      <c r="A487" s="5" t="s">
         <v>1453</v>
       </c>
-      <c r="B487" s="2" t="s">
+      <c r="B487" s="5" t="s">
         <v>1454</v>
       </c>
-      <c r="C487" s="2" t="s">
+      <c r="C487" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D487" s="2"/>
-      <c r="E487" s="2" t="s">
+      <c r="D487" s="5"/>
+      <c r="E487" s="5" t="s">
         <v>1455</v>
       </c>
-      <c r="F487" s="2" t="s">
+      <c r="F487" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G487" s="2" t="s">
+      <c r="G487" s="5" t="s">
         <v>1456</v>
       </c>
     </row>
     <row r="488" spans="1:7">
-      <c r="A488" s="2" t="s">
+      <c r="A488" s="5" t="s">
         <v>1457</v>
       </c>
-      <c r="B488" s="2" t="s">
+      <c r="B488" s="5" t="s">
         <v>1458</v>
       </c>
-      <c r="C488" s="2" t="s">
+      <c r="C488" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="D488" s="2" t="s">
+      <c r="D488" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="E488" s="2" t="s">
+      <c r="E488" s="5" t="s">
         <v>527</v>
       </c>
-      <c r="F488" s="2" t="s">
+      <c r="F488" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G488" s="2" t="s">
+      <c r="G488" s="5" t="s">
         <v>1459</v>
       </c>
     </row>
     <row r="489" spans="1:7">
-      <c r="A489" s="2" t="s">
+      <c r="A489" s="5" t="s">
         <v>1460</v>
       </c>
-      <c r="B489" s="2" t="s">
+      <c r="B489" s="5" t="s">
         <v>1461</v>
       </c>
-      <c r="C489" s="2" t="s">
+      <c r="C489" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="D489" s="2"/>
-      <c r="E489" s="2" t="s">
+      <c r="D489" s="5"/>
+      <c r="E489" s="5" t="s">
         <v>506</v>
       </c>
-      <c r="F489" s="2" t="s">
+      <c r="F489" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G489" s="2" t="s">
+      <c r="G489" s="5" t="s">
         <v>1462</v>
       </c>
     </row>
     <row r="490" spans="1:7">
-      <c r="A490" s="2" t="s">
+      <c r="A490" s="5" t="s">
         <v>1463</v>
       </c>
-      <c r="B490" s="2" t="s">
+      <c r="B490" s="5" t="s">
         <v>1464</v>
       </c>
-      <c r="C490" s="2" t="s">
+      <c r="C490" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D490" s="2"/>
-      <c r="E490" s="2" t="s">
+      <c r="D490" s="5"/>
+      <c r="E490" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="F490" s="2" t="s">
+      <c r="F490" s="5" t="s">
         <v>408</v>
       </c>
-      <c r="G490" s="2" t="s">
+      <c r="G490" s="5" t="s">
         <v>1465</v>
       </c>
     </row>
     <row r="491" spans="1:7">
-      <c r="A491" s="2" t="s">
+      <c r="A491" s="5" t="s">
         <v>1466</v>
       </c>
-      <c r="B491" s="2" t="s">
+      <c r="B491" s="5" t="s">
         <v>1467</v>
       </c>
-      <c r="C491" s="2" t="s">
+      <c r="C491" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D491" s="2"/>
-      <c r="E491" s="2" t="s">
+      <c r="D491" s="5"/>
+      <c r="E491" s="5" t="s">
         <v>814</v>
       </c>
-      <c r="F491" s="2" t="s">
+      <c r="F491" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G491" s="2" t="s">
+      <c r="G491" s="5" t="s">
         <v>1468</v>
       </c>
     </row>
     <row r="492" spans="1:7">
-      <c r="A492" s="2" t="s">
+      <c r="A492" s="5" t="s">
         <v>1469</v>
       </c>
-      <c r="B492" s="2" t="s">
+      <c r="B492" s="5" t="s">
         <v>1470</v>
       </c>
-      <c r="C492" s="2" t="s">
+      <c r="C492" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="D492" s="2"/>
-      <c r="E492" s="2" t="s">
+      <c r="D492" s="5"/>
+      <c r="E492" s="5" t="s">
         <v>814</v>
       </c>
-      <c r="F492" s="2" t="s">
+      <c r="F492" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G492" s="2" t="s">
+      <c r="G492" s="5" t="s">
         <v>746</v>
       </c>
     </row>
     <row r="493" spans="1:7">
-      <c r="A493" s="2" t="s">
+      <c r="A493" s="5" t="s">
         <v>1471</v>
       </c>
-      <c r="B493" s="2" t="s">
+      <c r="B493" s="5" t="s">
         <v>1472</v>
       </c>
-      <c r="C493" s="2" t="s">
+      <c r="C493" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="D493" s="2"/>
-      <c r="E493" s="2" t="s">
+      <c r="D493" s="5"/>
+      <c r="E493" s="5" t="s">
         <v>814</v>
       </c>
-      <c r="F493" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G493" s="2" t="s">
+      <c r="F493" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G493" s="5" t="s">
         <v>666</v>
       </c>
     </row>
     <row r="494" spans="1:7">
-      <c r="A494" s="2" t="s">
+      <c r="A494" s="5" t="s">
         <v>1473</v>
       </c>
-      <c r="B494" s="2" t="s">
+      <c r="B494" s="5" t="s">
         <v>1474</v>
       </c>
-      <c r="C494" s="2" t="s">
+      <c r="C494" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D494" s="2"/>
-      <c r="E494" s="2" t="s">
+      <c r="D494" s="5"/>
+      <c r="E494" s="5" t="s">
         <v>1475</v>
       </c>
-      <c r="F494" s="2" t="s">
+      <c r="F494" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G494" s="2" t="s">
+      <c r="G494" s="5" t="s">
         <v>1476</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adicionado 10 pokémon da 5ª geração e tambem um filtro no banco pra buscar pokémon pela habilidade
</commit_message>
<xml_diff>
--- a/pokemonv2/pokemons.xlsx
+++ b/pokemonv2/pokemons.xlsx
@@ -8364,7 +8364,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -8380,6 +8380,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8411,7 +8417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -8420,6 +8426,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8722,8 +8729,8 @@
   <dimension ref="A1:H1026"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A494" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B495" sqref="B495"/>
+      <pane ySplit="1" topLeftCell="A492" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B497" sqref="B497"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19800,3210 +19807,3210 @@
       </c>
     </row>
     <row r="505" spans="1:7">
-      <c r="A505" s="5" t="s">
+      <c r="A505" s="6" t="s">
         <v>1506</v>
       </c>
-      <c r="B505" s="5" t="s">
+      <c r="B505" s="6" t="s">
         <v>1507</v>
       </c>
-      <c r="C505" s="5" t="s">
+      <c r="C505" s="6" t="s">
         <v>389</v>
       </c>
-      <c r="D505" s="5"/>
-      <c r="E505" s="5" t="s">
+      <c r="D505" s="6"/>
+      <c r="E505" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F505" s="5" t="s">
+      <c r="F505" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G505" s="5" t="s">
+      <c r="G505" s="6" t="s">
         <v>1508</v>
       </c>
     </row>
     <row r="506" spans="1:7">
-      <c r="A506" s="5" t="s">
+      <c r="A506" s="6" t="s">
         <v>1509</v>
       </c>
-      <c r="B506" s="5" t="s">
+      <c r="B506" s="6" t="s">
         <v>1510</v>
       </c>
-      <c r="C506" s="5" t="s">
+      <c r="C506" s="6" t="s">
         <v>389</v>
       </c>
-      <c r="D506" s="5"/>
-      <c r="E506" s="5" t="s">
+      <c r="D506" s="6"/>
+      <c r="E506" s="6" t="s">
         <v>520</v>
       </c>
-      <c r="F506" s="5" t="s">
+      <c r="F506" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G506" s="5" t="s">
+      <c r="G506" s="6" t="s">
         <v>662</v>
       </c>
     </row>
     <row r="507" spans="1:7">
-      <c r="A507" s="5" t="s">
+      <c r="A507" s="6" t="s">
         <v>1511</v>
       </c>
-      <c r="B507" s="5" t="s">
+      <c r="B507" s="6" t="s">
         <v>1512</v>
       </c>
-      <c r="C507" s="5" t="s">
+      <c r="C507" s="6" t="s">
         <v>389</v>
       </c>
-      <c r="D507" s="5"/>
-      <c r="E507" s="5" t="s">
+      <c r="D507" s="6"/>
+      <c r="E507" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="F507" s="5" t="s">
+      <c r="F507" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G507" s="5" t="s">
+      <c r="G507" s="6" t="s">
         <v>1513</v>
       </c>
     </row>
     <row r="508" spans="1:7">
-      <c r="A508" s="5" t="s">
+      <c r="A508" s="6" t="s">
         <v>1514</v>
       </c>
-      <c r="B508" s="5" t="s">
+      <c r="B508" s="6" t="s">
         <v>1515</v>
       </c>
-      <c r="C508" s="5" t="s">
+      <c r="C508" s="6" t="s">
         <v>389</v>
       </c>
-      <c r="D508" s="5"/>
-      <c r="E508" s="5" t="s">
+      <c r="D508" s="6"/>
+      <c r="E508" s="6" t="s">
         <v>1516</v>
       </c>
-      <c r="F508" s="5" t="s">
+      <c r="F508" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G508" s="5" t="s">
+      <c r="G508" s="6" t="s">
         <v>1517</v>
       </c>
     </row>
     <row r="509" spans="1:7">
-      <c r="A509" s="5" t="s">
+      <c r="A509" s="6" t="s">
         <v>1518</v>
       </c>
-      <c r="B509" s="5" t="s">
+      <c r="B509" s="6" t="s">
         <v>1519</v>
       </c>
-      <c r="C509" s="5" t="s">
+      <c r="C509" s="6" t="s">
         <v>389</v>
       </c>
-      <c r="D509" s="5"/>
-      <c r="E509" s="5" t="s">
+      <c r="D509" s="6"/>
+      <c r="E509" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="F509" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G509" s="5" t="s">
+      <c r="F509" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G509" s="6" t="s">
         <v>1520</v>
       </c>
     </row>
     <row r="510" spans="1:7">
-      <c r="A510" s="5" t="s">
+      <c r="A510" s="6" t="s">
         <v>1521</v>
       </c>
-      <c r="B510" s="5" t="s">
+      <c r="B510" s="6" t="s">
         <v>1522</v>
       </c>
-      <c r="C510" s="5" t="s">
+      <c r="C510" s="6" t="s">
         <v>661</v>
       </c>
-      <c r="D510" s="5"/>
-      <c r="E510" s="5" t="s">
+      <c r="D510" s="6"/>
+      <c r="E510" s="6" t="s">
         <v>606</v>
       </c>
-      <c r="F510" s="5" t="s">
+      <c r="F510" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G510" s="5" t="s">
+      <c r="G510" s="6" t="s">
         <v>1523</v>
       </c>
     </row>
     <row r="511" spans="1:7">
-      <c r="A511" s="5" t="s">
+      <c r="A511" s="6" t="s">
         <v>1524</v>
       </c>
-      <c r="B511" s="5" t="s">
+      <c r="B511" s="6" t="s">
         <v>1525</v>
       </c>
-      <c r="C511" s="5" t="s">
+      <c r="C511" s="6" t="s">
         <v>661</v>
       </c>
-      <c r="D511" s="5"/>
-      <c r="E511" s="5" t="s">
+      <c r="D511" s="6"/>
+      <c r="E511" s="6" t="s">
         <v>1526</v>
       </c>
-      <c r="F511" s="5" t="s">
+      <c r="F511" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="G511" s="5" t="s">
+      <c r="G511" s="6" t="s">
         <v>1527</v>
       </c>
     </row>
     <row r="512" spans="1:7">
-      <c r="A512" s="5" t="s">
+      <c r="A512" s="6" t="s">
         <v>1528</v>
       </c>
-      <c r="B512" s="5" t="s">
+      <c r="B512" s="6" t="s">
         <v>1529</v>
       </c>
-      <c r="C512" s="5" t="s">
+      <c r="C512" s="6" t="s">
         <v>412</v>
       </c>
-      <c r="D512" s="5"/>
-      <c r="E512" s="5" t="s">
+      <c r="D512" s="6"/>
+      <c r="E512" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F512" s="5" t="s">
+      <c r="F512" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G512" s="5" t="s">
+      <c r="G512" s="6" t="s">
         <v>1530</v>
       </c>
     </row>
     <row r="513" spans="1:7">
-      <c r="A513" s="5" t="s">
+      <c r="A513" s="6" t="s">
         <v>1531</v>
       </c>
-      <c r="B513" s="5" t="s">
+      <c r="B513" s="6" t="s">
         <v>1532</v>
       </c>
-      <c r="C513" s="5" t="s">
+      <c r="C513" s="6" t="s">
         <v>412</v>
       </c>
-      <c r="D513" s="5"/>
-      <c r="E513" s="5" t="s">
+      <c r="D513" s="6"/>
+      <c r="E513" s="6" t="s">
         <v>1300</v>
       </c>
-      <c r="F513" s="5" t="s">
+      <c r="F513" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="G513" s="5" t="s">
+      <c r="G513" s="6" t="s">
         <v>1239</v>
       </c>
     </row>
     <row r="514" spans="1:7">
-      <c r="A514" s="5" t="s">
+      <c r="A514" s="6" t="s">
         <v>1533</v>
       </c>
-      <c r="B514" s="5" t="s">
+      <c r="B514" s="6" t="s">
         <v>1534</v>
       </c>
-      <c r="C514" s="5" t="s">
+      <c r="C514" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D514" s="5"/>
-      <c r="E514" s="5" t="s">
+      <c r="D514" s="6"/>
+      <c r="E514" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F514" s="5" t="s">
+      <c r="F514" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G514" s="5" t="s">
+      <c r="G514" s="6" t="s">
         <v>953</v>
       </c>
     </row>
     <row r="515" spans="1:7">
-      <c r="A515" s="5" t="s">
+      <c r="A515" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="B515" s="5" t="s">
+      <c r="B515" s="6" t="s">
         <v>1536</v>
       </c>
-      <c r="C515" s="5" t="s">
+      <c r="C515" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D515" s="5"/>
-      <c r="E515" s="5" t="s">
+      <c r="D515" s="6"/>
+      <c r="E515" s="6" t="s">
         <v>1300</v>
       </c>
-      <c r="F515" s="5" t="s">
+      <c r="F515" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="G515" s="5" t="s">
+      <c r="G515" s="6" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="516" spans="1:7">
-      <c r="A516" s="5" t="s">
+      <c r="A516" s="6" t="s">
         <v>1537</v>
       </c>
-      <c r="B516" s="5" t="s">
+      <c r="B516" s="6" t="s">
         <v>1538</v>
       </c>
-      <c r="C516" s="5" t="s">
+      <c r="C516" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D516" s="5"/>
-      <c r="E516" s="5" t="s">
+      <c r="D516" s="6"/>
+      <c r="E516" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F516" s="5" t="s">
+      <c r="F516" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G516" s="5" t="s">
+      <c r="G516" s="6" t="s">
         <v>1539</v>
       </c>
     </row>
     <row r="517" spans="1:7">
-      <c r="A517" s="5" t="s">
+      <c r="A517" s="6" t="s">
         <v>1540</v>
       </c>
-      <c r="B517" s="5" t="s">
+      <c r="B517" s="6" t="s">
         <v>1541</v>
       </c>
-      <c r="C517" s="5" t="s">
+      <c r="C517" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D517" s="5"/>
-      <c r="E517" s="5" t="s">
+      <c r="D517" s="6"/>
+      <c r="E517" s="6" t="s">
         <v>1300</v>
       </c>
-      <c r="F517" s="5" t="s">
+      <c r="F517" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="G517" s="5" t="s">
+      <c r="G517" s="6" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="518" spans="1:7">
-      <c r="A518" s="5" t="s">
+      <c r="A518" s="6" t="s">
         <v>1542</v>
       </c>
-      <c r="B518" s="5" t="s">
+      <c r="B518" s="6" t="s">
         <v>1543</v>
       </c>
-      <c r="C518" s="5" t="s">
+      <c r="C518" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="D518" s="5"/>
-      <c r="E518" s="5" t="s">
+      <c r="D518" s="6"/>
+      <c r="E518" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="F518" s="5" t="s">
+      <c r="F518" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G518" s="5" t="s">
+      <c r="G518" s="6" t="s">
         <v>1270</v>
       </c>
     </row>
     <row r="519" spans="1:7">
-      <c r="A519" s="5" t="s">
+      <c r="A519" s="6" t="s">
         <v>1544</v>
       </c>
-      <c r="B519" s="5" t="s">
+      <c r="B519" s="6" t="s">
         <v>1545</v>
       </c>
-      <c r="C519" s="5" t="s">
+      <c r="C519" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="D519" s="5"/>
-      <c r="E519" s="5" t="s">
+      <c r="D519" s="6"/>
+      <c r="E519" s="6" t="s">
         <v>404</v>
       </c>
-      <c r="F519" s="5" t="s">
+      <c r="F519" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="G519" s="5" t="s">
+      <c r="G519" s="6" t="s">
         <v>1326</v>
       </c>
     </row>
     <row r="520" spans="1:7">
-      <c r="A520" s="5" t="s">
+      <c r="A520" s="6" t="s">
         <v>1546</v>
       </c>
-      <c r="B520" s="5" t="s">
+      <c r="B520" s="6" t="s">
         <v>1547</v>
       </c>
-      <c r="C520" s="5" t="s">
+      <c r="C520" s="6" t="s">
         <v>389</v>
       </c>
-      <c r="D520" s="5" t="s">
+      <c r="D520" s="6" t="s">
         <v>2290</v>
       </c>
-      <c r="E520" s="5" t="s">
+      <c r="E520" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="F520" s="5" t="s">
+      <c r="F520" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G520" s="5" t="s">
+      <c r="G520" s="6" t="s">
         <v>666</v>
       </c>
     </row>
     <row r="521" spans="1:7">
-      <c r="A521" s="5" t="s">
+      <c r="A521" s="6" t="s">
         <v>1548</v>
       </c>
-      <c r="B521" s="5" t="s">
+      <c r="B521" s="6" t="s">
         <v>1549</v>
       </c>
-      <c r="C521" s="5" t="s">
+      <c r="C521" s="6" t="s">
         <v>389</v>
       </c>
-      <c r="D521" s="5" t="s">
+      <c r="D521" s="6" t="s">
         <v>2290</v>
       </c>
-      <c r="E521" s="5" t="s">
+      <c r="E521" s="6" t="s">
         <v>1550</v>
       </c>
-      <c r="F521" s="5" t="s">
+      <c r="F521" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G521" s="5" t="s">
+      <c r="G521" s="6" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="522" spans="1:7">
-      <c r="A522" s="5" t="s">
+      <c r="A522" s="6" t="s">
         <v>1551</v>
       </c>
-      <c r="B522" s="5" t="s">
+      <c r="B522" s="6" t="s">
         <v>1552</v>
       </c>
-      <c r="C522" s="5" t="s">
+      <c r="C522" s="6" t="s">
         <v>389</v>
       </c>
-      <c r="D522" s="5" t="s">
+      <c r="D522" s="6" t="s">
         <v>2290</v>
       </c>
-      <c r="E522" s="5" t="s">
+      <c r="E522" s="6" t="s">
         <v>1553</v>
       </c>
-      <c r="F522" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G522" s="5" t="s">
+      <c r="F522" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G522" s="6" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="523" spans="1:7">
-      <c r="A523" s="5" t="s">
+      <c r="A523" s="6" t="s">
         <v>1554</v>
       </c>
-      <c r="B523" s="5" t="s">
+      <c r="B523" s="6" t="s">
         <v>1555</v>
       </c>
-      <c r="C523" s="5" t="s">
+      <c r="C523" s="6" t="s">
         <v>449</v>
       </c>
-      <c r="D523" s="5"/>
-      <c r="E523" s="5" t="s">
+      <c r="D523" s="6"/>
+      <c r="E523" s="6" t="s">
         <v>420</v>
       </c>
-      <c r="F523" s="5" t="s">
+      <c r="F523" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G523" s="5" t="s">
+      <c r="G523" s="6" t="s">
         <v>1556</v>
       </c>
     </row>
     <row r="524" spans="1:7">
-      <c r="A524" s="5" t="s">
+      <c r="A524" s="6" t="s">
         <v>1557</v>
       </c>
-      <c r="B524" s="5" t="s">
+      <c r="B524" s="6" t="s">
         <v>1558</v>
       </c>
-      <c r="C524" s="5" t="s">
+      <c r="C524" s="6" t="s">
         <v>449</v>
       </c>
-      <c r="D524" s="5"/>
-      <c r="E524" s="5" t="s">
+      <c r="D524" s="6"/>
+      <c r="E524" s="6" t="s">
         <v>1300</v>
       </c>
-      <c r="F524" s="5" t="s">
+      <c r="F524" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="G524" s="5" t="s">
+      <c r="G524" s="6" t="s">
         <v>546</v>
       </c>
     </row>
     <row r="525" spans="1:7">
-      <c r="A525" s="5" t="s">
+      <c r="A525" s="6" t="s">
         <v>1559</v>
       </c>
-      <c r="B525" s="5" t="s">
+      <c r="B525" s="6" t="s">
         <v>1560</v>
       </c>
-      <c r="C525" s="5" t="s">
+      <c r="C525" s="6" t="s">
         <v>627</v>
       </c>
-      <c r="D525" s="5"/>
-      <c r="E525" s="5" t="s">
+      <c r="D525" s="6"/>
+      <c r="E525" s="6" t="s">
         <v>606</v>
       </c>
-      <c r="F525" s="5" t="s">
+      <c r="F525" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G525" s="5" t="s">
+      <c r="G525" s="6" t="s">
         <v>1561</v>
       </c>
     </row>
     <row r="526" spans="1:7">
-      <c r="A526" s="5" t="s">
+      <c r="A526" s="6" t="s">
         <v>1562</v>
       </c>
-      <c r="B526" s="5" t="s">
+      <c r="B526" s="6" t="s">
         <v>1563</v>
       </c>
-      <c r="C526" s="5" t="s">
+      <c r="C526" s="6" t="s">
         <v>627</v>
       </c>
-      <c r="D526" s="5"/>
-      <c r="E526" s="5" t="s">
+      <c r="D526" s="6"/>
+      <c r="E526" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="F526" s="5" t="s">
+      <c r="F526" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G526" s="5" t="s">
+      <c r="G526" s="6" t="s">
         <v>1564</v>
       </c>
     </row>
     <row r="527" spans="1:7">
-      <c r="A527" s="5" t="s">
+      <c r="A527" s="6" t="s">
         <v>1565</v>
       </c>
-      <c r="B527" s="5" t="s">
+      <c r="B527" s="6" t="s">
         <v>1566</v>
       </c>
-      <c r="C527" s="5" t="s">
+      <c r="C527" s="6" t="s">
         <v>627</v>
       </c>
-      <c r="D527" s="5"/>
-      <c r="E527" s="5" t="s">
+      <c r="D527" s="6"/>
+      <c r="E527" s="6" t="s">
         <v>1248</v>
       </c>
-      <c r="F527" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G527" s="5" t="s">
+      <c r="F527" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G527" s="6" t="s">
         <v>1567</v>
       </c>
     </row>
     <row r="528" spans="1:7">
-      <c r="A528" s="5" t="s">
+      <c r="A528" s="6" t="s">
         <v>1568</v>
       </c>
-      <c r="B528" s="5" t="s">
+      <c r="B528" s="6" t="s">
         <v>1569</v>
       </c>
-      <c r="C528" s="5" t="s">
+      <c r="C528" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="D528" s="5" t="s">
+      <c r="D528" s="6" t="s">
         <v>2290</v>
       </c>
-      <c r="E528" s="5" t="s">
+      <c r="E528" s="6" t="s">
         <v>304</v>
       </c>
-      <c r="F528" s="5" t="s">
+      <c r="F528" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G528" s="5" t="s">
+      <c r="G528" s="6" t="s">
         <v>666</v>
       </c>
     </row>
     <row r="529" spans="1:7">
-      <c r="A529" s="5" t="s">
+      <c r="A529" s="6" t="s">
         <v>1570</v>
       </c>
-      <c r="B529" s="5" t="s">
+      <c r="B529" s="6" t="s">
         <v>1571</v>
       </c>
-      <c r="C529" s="5" t="s">
+      <c r="C529" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="D529" s="5" t="s">
+      <c r="D529" s="6" t="s">
         <v>2290</v>
       </c>
-      <c r="E529" s="5" t="s">
+      <c r="E529" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="F529" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G529" s="5" t="s">
+      <c r="F529" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G529" s="6" t="s">
         <v>1530</v>
       </c>
     </row>
     <row r="530" spans="1:7">
-      <c r="A530" s="5" t="s">
+      <c r="A530" s="6" t="s">
         <v>1572</v>
       </c>
-      <c r="B530" s="5" t="s">
+      <c r="B530" s="6" t="s">
         <v>1573</v>
       </c>
-      <c r="C530" s="5" t="s">
+      <c r="C530" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D530" s="5"/>
-      <c r="E530" s="5" t="s">
+      <c r="D530" s="6"/>
+      <c r="E530" s="6" t="s">
         <v>351</v>
       </c>
-      <c r="F530" s="5" t="s">
+      <c r="F530" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G530" s="5" t="s">
+      <c r="G530" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="531" spans="1:7">
-      <c r="A531" s="5" t="s">
+      <c r="A531" s="6" t="s">
         <v>1574</v>
       </c>
-      <c r="B531" s="5" t="s">
+      <c r="B531" s="6" t="s">
         <v>1575</v>
       </c>
-      <c r="C531" s="5" t="s">
+      <c r="C531" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D531" s="5" t="s">
+      <c r="D531" s="6" t="s">
         <v>1169</v>
       </c>
-      <c r="E531" s="5" t="s">
+      <c r="E531" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F531" s="5" t="s">
+      <c r="F531" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="G531" s="5" t="s">
+      <c r="G531" s="6" t="s">
         <v>1576</v>
       </c>
     </row>
     <row r="532" spans="1:7">
-      <c r="A532" s="5" t="s">
+      <c r="A532" s="6" t="s">
         <v>1577</v>
       </c>
-      <c r="B532" s="5" t="s">
+      <c r="B532" s="6" t="s">
         <v>1578</v>
       </c>
-      <c r="C532" s="5" t="s">
+      <c r="C532" s="6" t="s">
         <v>389</v>
       </c>
-      <c r="D532" s="5"/>
-      <c r="E532" s="5" t="s">
+      <c r="D532" s="6"/>
+      <c r="E532" s="6" t="s">
         <v>1579</v>
       </c>
-      <c r="F532" s="5" t="s">
+      <c r="F532" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G532" s="5" t="s">
+      <c r="G532" s="6" t="s">
         <v>1580</v>
       </c>
     </row>
     <row r="533" spans="1:7">
-      <c r="A533" s="5" t="s">
+      <c r="A533" s="6" t="s">
         <v>1581</v>
       </c>
-      <c r="B533" s="5" t="s">
+      <c r="B533" s="6" t="s">
         <v>1582</v>
       </c>
-      <c r="C533" s="5" t="s">
+      <c r="C533" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="D533" s="5"/>
-      <c r="E533" s="5" t="s">
+      <c r="D533" s="6"/>
+      <c r="E533" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="F533" s="5" t="s">
+      <c r="F533" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="G533" s="5" t="s">
+      <c r="G533" s="6" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="534" spans="1:7">
-      <c r="A534" s="5" t="s">
+      <c r="A534" s="6" t="s">
         <v>1583</v>
       </c>
-      <c r="B534" s="5" t="s">
+      <c r="B534" s="6" t="s">
         <v>1584</v>
       </c>
-      <c r="C534" s="5" t="s">
+      <c r="C534" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="D534" s="5"/>
-      <c r="E534" s="5" t="s">
+      <c r="D534" s="6"/>
+      <c r="E534" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F534" s="5" t="s">
+      <c r="F534" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="G534" s="5" t="s">
+      <c r="G534" s="6" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="535" spans="1:7">
-      <c r="A535" s="5" t="s">
+      <c r="A535" s="6" t="s">
         <v>1585</v>
       </c>
-      <c r="B535" s="5" t="s">
+      <c r="B535" s="6" t="s">
         <v>1586</v>
       </c>
-      <c r="C535" s="5" t="s">
+      <c r="C535" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="D535" s="5"/>
-      <c r="E535" s="5" t="s">
+      <c r="D535" s="6"/>
+      <c r="E535" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="F535" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G535" s="5" t="s">
+      <c r="F535" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G535" s="6" t="s">
         <v>1587</v>
       </c>
     </row>
     <row r="536" spans="1:7">
-      <c r="A536" s="5" t="s">
+      <c r="A536" s="6" t="s">
         <v>1588</v>
       </c>
-      <c r="B536" s="5" t="s">
+      <c r="B536" s="6" t="s">
         <v>1589</v>
       </c>
-      <c r="C536" s="5" t="s">
+      <c r="C536" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D536" s="5"/>
-      <c r="E536" s="5" t="s">
+      <c r="D536" s="6"/>
+      <c r="E536" s="6" t="s">
         <v>420</v>
       </c>
-      <c r="F536" s="5" t="s">
+      <c r="F536" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G536" s="5" t="s">
+      <c r="G536" s="6" t="s">
         <v>905</v>
       </c>
     </row>
     <row r="537" spans="1:7">
-      <c r="A537" s="5" t="s">
+      <c r="A537" s="6" t="s">
         <v>1590</v>
       </c>
-      <c r="B537" s="5" t="s">
+      <c r="B537" s="6" t="s">
         <v>1591</v>
       </c>
-      <c r="C537" s="5" t="s">
+      <c r="C537" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D537" s="5" t="s">
+      <c r="D537" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="E537" s="5" t="s">
+      <c r="E537" s="6" t="s">
         <v>1232</v>
       </c>
-      <c r="F537" s="5" t="s">
+      <c r="F537" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G537" s="5" t="s">
+      <c r="G537" s="6" t="s">
         <v>1592</v>
       </c>
     </row>
     <row r="538" spans="1:7">
-      <c r="A538" s="5" t="s">
+      <c r="A538" s="6" t="s">
         <v>1593</v>
       </c>
-      <c r="B538" s="5" t="s">
+      <c r="B538" s="6" t="s">
         <v>1594</v>
       </c>
-      <c r="C538" s="5" t="s">
+      <c r="C538" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D538" s="5" t="s">
+      <c r="D538" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="E538" s="5" t="s">
+      <c r="E538" s="6" t="s">
         <v>1595</v>
       </c>
-      <c r="F538" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G538" s="5" t="s">
+      <c r="F538" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G538" s="6" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="539" spans="1:7">
-      <c r="A539" s="5" t="s">
+      <c r="A539" s="6" t="s">
         <v>1596</v>
       </c>
-      <c r="B539" s="5" t="s">
+      <c r="B539" s="6" t="s">
         <v>1597</v>
       </c>
-      <c r="C539" s="5" t="s">
+      <c r="C539" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="D539" s="5"/>
-      <c r="E539" s="5" t="s">
+      <c r="D539" s="6"/>
+      <c r="E539" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="F539" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G539" s="5" t="s">
+      <c r="F539" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G539" s="6" t="s">
         <v>1493</v>
       </c>
     </row>
     <row r="540" spans="1:7">
-      <c r="A540" s="5" t="s">
+      <c r="A540" s="6" t="s">
         <v>1598</v>
       </c>
-      <c r="B540" s="5" t="s">
+      <c r="B540" s="6" t="s">
         <v>1599</v>
       </c>
-      <c r="C540" s="5" t="s">
+      <c r="C540" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="D540" s="5"/>
-      <c r="E540" s="5" t="s">
+      <c r="D540" s="6"/>
+      <c r="E540" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="F540" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G540" s="5" t="s">
+      <c r="F540" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G540" s="6" t="s">
         <v>1600</v>
       </c>
     </row>
     <row r="541" spans="1:7">
-      <c r="A541" s="5" t="s">
+      <c r="A541" s="6" t="s">
         <v>1601</v>
       </c>
-      <c r="B541" s="5" t="s">
+      <c r="B541" s="6" t="s">
         <v>1602</v>
       </c>
-      <c r="C541" s="5" t="s">
+      <c r="C541" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D541" s="5" t="s">
+      <c r="D541" s="6" t="s">
         <v>412</v>
       </c>
-      <c r="E541" s="5" t="s">
+      <c r="E541" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F541" s="5" t="s">
+      <c r="F541" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G541" s="5" t="s">
+      <c r="G541" s="6" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="542" spans="1:7">
-      <c r="A542" s="5" t="s">
+      <c r="A542" s="6" t="s">
         <v>1603</v>
       </c>
-      <c r="B542" s="5" t="s">
+      <c r="B542" s="6" t="s">
         <v>1604</v>
       </c>
-      <c r="C542" s="5" t="s">
+      <c r="C542" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D542" s="5" t="s">
+      <c r="D542" s="6" t="s">
         <v>412</v>
       </c>
-      <c r="E542" s="5" t="s">
+      <c r="E542" s="6" t="s">
         <v>959</v>
       </c>
-      <c r="F542" s="5" t="s">
+      <c r="F542" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G542" s="5" t="s">
+      <c r="G542" s="6" t="s">
         <v>1605</v>
       </c>
     </row>
     <row r="543" spans="1:7">
-      <c r="A543" s="5" t="s">
+      <c r="A543" s="6" t="s">
         <v>1606</v>
       </c>
-      <c r="B543" s="5" t="s">
+      <c r="B543" s="6" t="s">
         <v>1607</v>
       </c>
-      <c r="C543" s="5" t="s">
+      <c r="C543" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D543" s="5" t="s">
+      <c r="D543" s="6" t="s">
         <v>412</v>
       </c>
-      <c r="E543" s="5" t="s">
+      <c r="E543" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="F543" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G543" s="5" t="s">
+      <c r="F543" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G543" s="6" t="s">
         <v>712</v>
       </c>
     </row>
     <row r="544" spans="1:7">
-      <c r="A544" s="5" t="s">
+      <c r="A544" s="6" t="s">
         <v>1608</v>
       </c>
-      <c r="B544" s="5" t="s">
+      <c r="B544" s="6" t="s">
         <v>1609</v>
       </c>
-      <c r="C544" s="5" t="s">
+      <c r="C544" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D544" s="5" t="s">
+      <c r="D544" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E544" s="5" t="s">
+      <c r="E544" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="F544" s="5" t="s">
+      <c r="F544" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G544" s="5" t="s">
+      <c r="G544" s="6" t="s">
         <v>1610</v>
       </c>
     </row>
     <row r="545" spans="1:7">
-      <c r="A545" s="5" t="s">
+      <c r="A545" s="6" t="s">
         <v>1611</v>
       </c>
-      <c r="B545" s="5" t="s">
+      <c r="B545" s="6" t="s">
         <v>1612</v>
       </c>
-      <c r="C545" s="5" t="s">
+      <c r="C545" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D545" s="5" t="s">
+      <c r="D545" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E545" s="5" t="s">
+      <c r="E545" s="6" t="s">
         <v>933</v>
       </c>
-      <c r="F545" s="5" t="s">
+      <c r="F545" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G545" s="5" t="s">
+      <c r="G545" s="6" t="s">
         <v>1613</v>
       </c>
     </row>
     <row r="546" spans="1:7">
-      <c r="A546" s="5" t="s">
+      <c r="A546" s="6" t="s">
         <v>1614</v>
       </c>
-      <c r="B546" s="5" t="s">
+      <c r="B546" s="6" t="s">
         <v>1615</v>
       </c>
-      <c r="C546" s="5" t="s">
+      <c r="C546" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D546" s="5" t="s">
+      <c r="D546" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E546" s="5" t="s">
+      <c r="E546" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="F546" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G546" s="5" t="s">
+      <c r="F546" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G546" s="6" t="s">
         <v>1616</v>
       </c>
     </row>
     <row r="547" spans="1:7">
-      <c r="A547" s="5" t="s">
+      <c r="A547" s="6" t="s">
         <v>1617</v>
       </c>
-      <c r="B547" s="5" t="s">
+      <c r="B547" s="6" t="s">
         <v>1618</v>
       </c>
-      <c r="C547" s="5" t="s">
+      <c r="C547" s="6" t="s">
         <v>412</v>
       </c>
-      <c r="D547" s="5" t="s">
+      <c r="D547" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="E547" s="5" t="s">
+      <c r="E547" s="6" t="s">
         <v>606</v>
       </c>
-      <c r="F547" s="5" t="s">
+      <c r="F547" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G547" s="5" t="s">
+      <c r="G547" s="6" t="s">
         <v>1318</v>
       </c>
     </row>
     <row r="548" spans="1:7">
-      <c r="A548" s="5" t="s">
+      <c r="A548" s="6" t="s">
         <v>1619</v>
       </c>
-      <c r="B548" s="5" t="s">
+      <c r="B548" s="6" t="s">
         <v>1620</v>
       </c>
-      <c r="C548" s="5" t="s">
+      <c r="C548" s="6" t="s">
         <v>412</v>
       </c>
-      <c r="D548" s="5" t="s">
+      <c r="D548" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="E548" s="5" t="s">
+      <c r="E548" s="6" t="s">
         <v>737</v>
       </c>
-      <c r="F548" s="5" t="s">
+      <c r="F548" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="G548" s="5" t="s">
+      <c r="G548" s="6" t="s">
         <v>889</v>
       </c>
     </row>
     <row r="549" spans="1:7">
-      <c r="A549" s="5" t="s">
+      <c r="A549" s="6" t="s">
         <v>1621</v>
       </c>
-      <c r="B549" s="5" t="s">
+      <c r="B549" s="6" t="s">
         <v>1622</v>
       </c>
-      <c r="C549" s="5" t="s">
+      <c r="C549" s="6" t="s">
         <v>412</v>
       </c>
-      <c r="D549" s="5"/>
-      <c r="E549" s="5" t="s">
+      <c r="D549" s="6"/>
+      <c r="E549" s="6" t="s">
         <v>606</v>
       </c>
-      <c r="F549" s="5" t="s">
+      <c r="F549" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G549" s="5" t="s">
+      <c r="G549" s="6" t="s">
         <v>889</v>
       </c>
     </row>
     <row r="550" spans="1:7">
-      <c r="A550" s="5" t="s">
+      <c r="A550" s="6" t="s">
         <v>1623</v>
       </c>
-      <c r="B550" s="5" t="s">
+      <c r="B550" s="6" t="s">
         <v>1624</v>
       </c>
-      <c r="C550" s="5" t="s">
+      <c r="C550" s="6" t="s">
         <v>412</v>
       </c>
-      <c r="D550" s="5"/>
-      <c r="E550" s="5" t="s">
+      <c r="D550" s="6"/>
+      <c r="E550" s="6" t="s">
         <v>737</v>
       </c>
-      <c r="F550" s="5" t="s">
+      <c r="F550" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="G550" s="5" t="s">
+      <c r="G550" s="6" t="s">
         <v>930</v>
       </c>
     </row>
     <row r="551" spans="1:7">
-      <c r="A551" s="5" t="s">
+      <c r="A551" s="6" t="s">
         <v>1625</v>
       </c>
-      <c r="B551" s="5" t="s">
+      <c r="B551" s="6" t="s">
         <v>1626</v>
       </c>
-      <c r="C551" s="5" t="s">
+      <c r="C551" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D551" s="5"/>
-      <c r="E551" s="5" t="s">
+      <c r="D551" s="6"/>
+      <c r="E551" s="6" t="s">
         <v>438</v>
       </c>
-      <c r="F551" s="5" t="s">
+      <c r="F551" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="G551" s="5" t="s">
+      <c r="G551" s="6" t="s">
         <v>1561</v>
       </c>
     </row>
     <row r="552" spans="1:7">
-      <c r="A552" s="5" t="s">
+      <c r="A552" s="6" t="s">
         <v>1627</v>
       </c>
-      <c r="B552" s="5" t="s">
+      <c r="B552" s="6" t="s">
         <v>1628</v>
       </c>
-      <c r="C552" s="5" t="s">
+      <c r="C552" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D552" s="5" t="s">
+      <c r="D552" s="6" t="s">
         <v>661</v>
       </c>
-      <c r="E552" s="5" t="s">
+      <c r="E552" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="F552" s="5" t="s">
+      <c r="F552" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="G552" s="5" t="s">
+      <c r="G552" s="6" t="s">
         <v>977</v>
       </c>
     </row>
     <row r="553" spans="1:7">
-      <c r="A553" s="5" t="s">
+      <c r="A553" s="6" t="s">
         <v>1629</v>
       </c>
-      <c r="B553" s="5" t="s">
+      <c r="B553" s="6" t="s">
         <v>1630</v>
       </c>
-      <c r="C553" s="5" t="s">
+      <c r="C553" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D553" s="5" t="s">
+      <c r="D553" s="6" t="s">
         <v>661</v>
       </c>
-      <c r="E553" s="5" t="s">
+      <c r="E553" s="6" t="s">
         <v>1631</v>
       </c>
-      <c r="F553" s="5" t="s">
+      <c r="F553" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="G553" s="5" t="s">
+      <c r="G553" s="6" t="s">
         <v>1632</v>
       </c>
     </row>
     <row r="554" spans="1:7">
-      <c r="A554" s="5" t="s">
+      <c r="A554" s="6" t="s">
         <v>1633</v>
       </c>
-      <c r="B554" s="5" t="s">
+      <c r="B554" s="6" t="s">
         <v>1634</v>
       </c>
-      <c r="C554" s="5" t="s">
+      <c r="C554" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D554" s="5" t="s">
+      <c r="D554" s="6" t="s">
         <v>661</v>
       </c>
-      <c r="E554" s="5" t="s">
+      <c r="E554" s="6" t="s">
         <v>1635</v>
       </c>
-      <c r="F554" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G554" s="5" t="s">
+      <c r="F554" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G554" s="6" t="s">
         <v>1636</v>
       </c>
     </row>
     <row r="555" spans="1:7">
-      <c r="A555" s="5" t="s">
+      <c r="A555" s="6" t="s">
         <v>1637</v>
       </c>
-      <c r="B555" s="5" t="s">
+      <c r="B555" s="6" t="s">
         <v>1638</v>
       </c>
-      <c r="C555" s="5" t="s">
+      <c r="C555" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D555" s="5"/>
-      <c r="E555" s="5" t="s">
+      <c r="D555" s="6"/>
+      <c r="E555" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F555" s="5" t="s">
+      <c r="F555" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G555" s="5" t="s">
+      <c r="G555" s="6" t="s">
         <v>1527</v>
       </c>
     </row>
     <row r="556" spans="1:7">
-      <c r="A556" s="5" t="s">
+      <c r="A556" s="6" t="s">
         <v>1639</v>
       </c>
-      <c r="B556" s="5" t="s">
+      <c r="B556" s="6" t="s">
         <v>1640</v>
       </c>
-      <c r="C556" s="5" t="s">
+      <c r="C556" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D556" s="5"/>
-      <c r="E556" s="5" t="s">
+      <c r="D556" s="6"/>
+      <c r="E556" s="6" t="s">
         <v>737</v>
       </c>
-      <c r="F556" s="5" t="s">
+      <c r="F556" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="G556" s="5" t="s">
+      <c r="G556" s="6" t="s">
         <v>1641</v>
       </c>
     </row>
     <row r="557" spans="1:7">
-      <c r="A557" s="5" t="s">
+      <c r="A557" s="6" t="s">
         <v>1642</v>
       </c>
-      <c r="B557" s="5" t="s">
+      <c r="B557" s="6" t="s">
         <v>1643</v>
       </c>
-      <c r="C557" s="5" t="s">
+      <c r="C557" s="6" t="s">
         <v>412</v>
       </c>
-      <c r="D557" s="5"/>
-      <c r="E557" s="5" t="s">
+      <c r="D557" s="6"/>
+      <c r="E557" s="6" t="s">
         <v>438</v>
       </c>
-      <c r="F557" s="5" t="s">
+      <c r="F557" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G557" s="5" t="s">
+      <c r="G557" s="6" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="558" spans="1:7">
-      <c r="A558" s="5" t="s">
+      <c r="A558" s="6" t="s">
         <v>1644</v>
       </c>
-      <c r="B558" s="5" t="s">
+      <c r="B558" s="6" t="s">
         <v>1645</v>
       </c>
-      <c r="C558" s="5" t="s">
+      <c r="C558" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D558" s="5" t="s">
+      <c r="D558" s="6" t="s">
         <v>627</v>
       </c>
-      <c r="E558" s="5" t="s">
+      <c r="E558" s="6" t="s">
         <v>304</v>
       </c>
-      <c r="F558" s="5" t="s">
+      <c r="F558" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G558" s="5" t="s">
+      <c r="G558" s="6" t="s">
         <v>1249</v>
       </c>
     </row>
     <row r="559" spans="1:7">
-      <c r="A559" s="5" t="s">
+      <c r="A559" s="6" t="s">
         <v>1646</v>
       </c>
-      <c r="B559" s="5" t="s">
+      <c r="B559" s="6" t="s">
         <v>1647</v>
       </c>
-      <c r="C559" s="5" t="s">
+      <c r="C559" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D559" s="5" t="s">
+      <c r="D559" s="6" t="s">
         <v>627</v>
       </c>
-      <c r="E559" s="5" t="s">
+      <c r="E559" s="6" t="s">
         <v>404</v>
       </c>
-      <c r="F559" s="5" t="s">
+      <c r="F559" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="G559" s="5" t="s">
+      <c r="G559" s="6" t="s">
         <v>1648</v>
       </c>
     </row>
     <row r="560" spans="1:7">
-      <c r="A560" s="5" t="s">
+      <c r="A560" s="6" t="s">
         <v>1649</v>
       </c>
-      <c r="B560" s="5" t="s">
+      <c r="B560" s="6" t="s">
         <v>1650</v>
       </c>
-      <c r="C560" s="5" t="s">
+      <c r="C560" s="6" t="s">
         <v>661</v>
       </c>
-      <c r="D560" s="5" t="s">
+      <c r="D560" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="E560" s="5" t="s">
+      <c r="E560" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="F560" s="5" t="s">
+      <c r="F560" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="G560" s="5" t="s">
+      <c r="G560" s="6" t="s">
         <v>1651</v>
       </c>
     </row>
     <row r="561" spans="1:7">
-      <c r="A561" s="5" t="s">
+      <c r="A561" s="6" t="s">
         <v>1652</v>
       </c>
-      <c r="B561" s="5" t="s">
+      <c r="B561" s="6" t="s">
         <v>1653</v>
       </c>
-      <c r="C561" s="5" t="s">
+      <c r="C561" s="6" t="s">
         <v>661</v>
       </c>
-      <c r="D561" s="5" t="s">
+      <c r="D561" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="E561" s="5" t="s">
+      <c r="E561" s="6" t="s">
         <v>1654</v>
       </c>
-      <c r="F561" s="5" t="s">
+      <c r="F561" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="G561" s="5" t="s">
+      <c r="G561" s="6" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="562" spans="1:7">
-      <c r="A562" s="5" t="s">
+      <c r="A562" s="6" t="s">
         <v>1655</v>
       </c>
-      <c r="B562" s="5" t="s">
+      <c r="B562" s="6" t="s">
         <v>1656</v>
       </c>
-      <c r="C562" s="5" t="s">
+      <c r="C562" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="D562" s="5" t="s">
+      <c r="D562" s="6" t="s">
         <v>2290</v>
       </c>
-      <c r="E562" s="5" t="s">
+      <c r="E562" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="F562" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G562" s="5" t="s">
+      <c r="F562" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G562" s="6" t="s">
         <v>690</v>
       </c>
     </row>
     <row r="563" spans="1:7">
-      <c r="A563" s="5" t="s">
+      <c r="A563" s="6" t="s">
         <v>1657</v>
       </c>
-      <c r="B563" s="5" t="s">
+      <c r="B563" s="6" t="s">
         <v>1658</v>
       </c>
-      <c r="C563" s="5" t="s">
+      <c r="C563" s="6" t="s">
         <v>672</v>
       </c>
-      <c r="D563" s="5"/>
-      <c r="E563" s="5" t="s">
+      <c r="D563" s="6"/>
+      <c r="E563" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="F563" s="5" t="s">
+      <c r="F563" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G563" s="5" t="s">
+      <c r="G563" s="6" t="s">
         <v>597</v>
       </c>
     </row>
     <row r="564" spans="1:7">
-      <c r="A564" s="5" t="s">
+      <c r="A564" s="6" t="s">
         <v>1659</v>
       </c>
-      <c r="B564" s="5" t="s">
+      <c r="B564" s="6" t="s">
         <v>1660</v>
       </c>
-      <c r="C564" s="5" t="s">
+      <c r="C564" s="6" t="s">
         <v>672</v>
       </c>
-      <c r="D564" s="5"/>
-      <c r="E564" s="5" t="s">
+      <c r="D564" s="6"/>
+      <c r="E564" s="6" t="s">
         <v>355</v>
       </c>
-      <c r="F564" s="5" t="s">
+      <c r="F564" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="G564" s="5" t="s">
+      <c r="G564" s="6" t="s">
         <v>1661</v>
       </c>
     </row>
     <row r="565" spans="1:7">
-      <c r="A565" s="5" t="s">
+      <c r="A565" s="6" t="s">
         <v>1662</v>
       </c>
-      <c r="B565" s="5" t="s">
+      <c r="B565" s="6" t="s">
         <v>1663</v>
       </c>
-      <c r="C565" s="5" t="s">
+      <c r="C565" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D565" s="5" t="s">
+      <c r="D565" s="6" t="s">
         <v>627</v>
       </c>
-      <c r="E565" s="5" t="s">
+      <c r="E565" s="6" t="s">
         <v>490</v>
       </c>
-      <c r="F565" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G565" s="5" t="s">
+      <c r="F565" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G565" s="6" t="s">
         <v>521</v>
       </c>
     </row>
     <row r="566" spans="1:7">
-      <c r="A566" s="5" t="s">
+      <c r="A566" s="6" t="s">
         <v>1664</v>
       </c>
-      <c r="B566" s="5" t="s">
+      <c r="B566" s="6" t="s">
         <v>1665</v>
       </c>
-      <c r="C566" s="5" t="s">
+      <c r="C566" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D566" s="5" t="s">
+      <c r="D566" s="6" t="s">
         <v>627</v>
       </c>
-      <c r="E566" s="5" t="s">
+      <c r="E566" s="6" t="s">
         <v>452</v>
       </c>
-      <c r="F566" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G566" s="5" t="s">
+      <c r="F566" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G566" s="6" t="s">
         <v>1666</v>
       </c>
     </row>
     <row r="567" spans="1:7">
-      <c r="A567" s="5" t="s">
+      <c r="A567" s="6" t="s">
         <v>1667</v>
       </c>
-      <c r="B567" s="5" t="s">
+      <c r="B567" s="6" t="s">
         <v>1668</v>
       </c>
-      <c r="C567" s="5" t="s">
+      <c r="C567" s="6" t="s">
         <v>627</v>
       </c>
-      <c r="D567" s="5" t="s">
+      <c r="D567" s="6" t="s">
         <v>2290</v>
       </c>
-      <c r="E567" s="5" t="s">
+      <c r="E567" s="6" t="s">
         <v>490</v>
       </c>
-      <c r="F567" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G567" s="5" t="s">
+      <c r="F567" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G567" s="6" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="568" spans="1:7">
-      <c r="A568" s="5" t="s">
+      <c r="A568" s="6" t="s">
         <v>1669</v>
       </c>
-      <c r="B568" s="5" t="s">
+      <c r="B568" s="6" t="s">
         <v>1670</v>
       </c>
-      <c r="C568" s="5" t="s">
+      <c r="C568" s="6" t="s">
         <v>627</v>
       </c>
-      <c r="D568" s="5" t="s">
+      <c r="D568" s="6" t="s">
         <v>2290</v>
       </c>
-      <c r="E568" s="5" t="s">
+      <c r="E568" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="F568" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G568" s="5" t="s">
+      <c r="F568" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G568" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="569" spans="1:7">
-      <c r="A569" s="5" t="s">
+      <c r="A569" s="6" t="s">
         <v>1671</v>
       </c>
-      <c r="B569" s="5" t="s">
+      <c r="B569" s="6" t="s">
         <v>1672</v>
       </c>
-      <c r="C569" s="5" t="s">
+      <c r="C569" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D569" s="5"/>
-      <c r="E569" s="5" t="s">
+      <c r="D569" s="6"/>
+      <c r="E569" s="6" t="s">
         <v>351</v>
       </c>
-      <c r="F569" s="5" t="s">
+      <c r="F569" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G569" s="5" t="s">
+      <c r="G569" s="6" t="s">
         <v>1580</v>
       </c>
     </row>
     <row r="570" spans="1:7">
-      <c r="A570" s="5" t="s">
+      <c r="A570" s="6" t="s">
         <v>1673</v>
       </c>
-      <c r="B570" s="5" t="s">
+      <c r="B570" s="6" t="s">
         <v>1674</v>
       </c>
-      <c r="C570" s="5" t="s">
+      <c r="C570" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D570" s="5"/>
-      <c r="E570" s="5" t="s">
+      <c r="D570" s="6"/>
+      <c r="E570" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="F570" s="5" t="s">
+      <c r="F570" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="G570" s="5" t="s">
+      <c r="G570" s="6" t="s">
         <v>1675</v>
       </c>
     </row>
     <row r="571" spans="1:7">
-      <c r="A571" s="5" t="s">
+      <c r="A571" s="6" t="s">
         <v>1676</v>
       </c>
-      <c r="B571" s="5" t="s">
+      <c r="B571" s="6" t="s">
         <v>1677</v>
       </c>
-      <c r="C571" s="5" t="s">
+      <c r="C571" s="6" t="s">
         <v>661</v>
       </c>
-      <c r="D571" s="5"/>
-      <c r="E571" s="5" t="s">
+      <c r="D571" s="6"/>
+      <c r="E571" s="6" t="s">
         <v>351</v>
       </c>
-      <c r="F571" s="5" t="s">
+      <c r="F571" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="G571" s="5" t="s">
+      <c r="G571" s="6" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="572" spans="1:7">
-      <c r="A572" s="5" t="s">
+      <c r="A572" s="6" t="s">
         <v>1678</v>
       </c>
-      <c r="B572" s="5" t="s">
+      <c r="B572" s="6" t="s">
         <v>1679</v>
       </c>
-      <c r="C572" s="5" t="s">
+      <c r="C572" s="6" t="s">
         <v>661</v>
       </c>
-      <c r="D572" s="5"/>
-      <c r="E572" s="5" t="s">
+      <c r="D572" s="6"/>
+      <c r="E572" s="6" t="s">
         <v>697</v>
       </c>
-      <c r="F572" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G572" s="5" t="s">
+      <c r="F572" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G572" s="6" t="s">
         <v>1680</v>
       </c>
     </row>
     <row r="573" spans="1:7">
-      <c r="A573" s="5" t="s">
+      <c r="A573" s="6" t="s">
         <v>1681</v>
       </c>
-      <c r="B573" s="5" t="s">
+      <c r="B573" s="6" t="s">
         <v>1682</v>
       </c>
-      <c r="C573" s="5" t="s">
+      <c r="C573" s="6" t="s">
         <v>389</v>
       </c>
-      <c r="D573" s="5"/>
-      <c r="E573" s="5" t="s">
+      <c r="D573" s="6"/>
+      <c r="E573" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="F573" s="5" t="s">
+      <c r="F573" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G573" s="5" t="s">
+      <c r="G573" s="6" t="s">
         <v>617</v>
       </c>
     </row>
     <row r="574" spans="1:7">
-      <c r="A574" s="5" t="s">
+      <c r="A574" s="6" t="s">
         <v>1683</v>
       </c>
-      <c r="B574" s="5" t="s">
+      <c r="B574" s="6" t="s">
         <v>1684</v>
       </c>
-      <c r="C574" s="5" t="s">
+      <c r="C574" s="6" t="s">
         <v>389</v>
       </c>
-      <c r="D574" s="5"/>
-      <c r="E574" s="5" t="s">
+      <c r="D574" s="6"/>
+      <c r="E574" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="F574" s="5" t="s">
+      <c r="F574" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="G574" s="5" t="s">
+      <c r="G574" s="6" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="575" spans="1:7">
-      <c r="A575" s="5" t="s">
+      <c r="A575" s="6" t="s">
         <v>1685</v>
       </c>
-      <c r="B575" s="5" t="s">
+      <c r="B575" s="6" t="s">
         <v>1686</v>
       </c>
-      <c r="C575" s="5" t="s">
+      <c r="C575" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="D575" s="5"/>
-      <c r="E575" s="5" t="s">
+      <c r="D575" s="6"/>
+      <c r="E575" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="F575" s="5" t="s">
+      <c r="F575" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="G575" s="5" t="s">
+      <c r="G575" s="6" t="s">
         <v>617</v>
       </c>
     </row>
     <row r="576" spans="1:7">
-      <c r="A576" s="5" t="s">
+      <c r="A576" s="6" t="s">
         <v>1687</v>
       </c>
-      <c r="B576" s="5" t="s">
+      <c r="B576" s="6" t="s">
         <v>1688</v>
       </c>
-      <c r="C576" s="5" t="s">
+      <c r="C576" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="D576" s="5"/>
-      <c r="E576" s="5" t="s">
+      <c r="D576" s="6"/>
+      <c r="E576" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="F576" s="5" t="s">
+      <c r="F576" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="G576" s="5" t="s">
+      <c r="G576" s="6" t="s">
         <v>1561</v>
       </c>
     </row>
     <row r="577" spans="1:7">
-      <c r="A577" s="5" t="s">
+      <c r="A577" s="6" t="s">
         <v>1689</v>
       </c>
-      <c r="B577" s="5" t="s">
+      <c r="B577" s="6" t="s">
         <v>1690</v>
       </c>
-      <c r="C577" s="5" t="s">
+      <c r="C577" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="D577" s="5"/>
-      <c r="E577" s="5" t="s">
+      <c r="D577" s="6"/>
+      <c r="E577" s="6" t="s">
         <v>1407</v>
       </c>
-      <c r="F577" s="5" t="s">
+      <c r="F577" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="G577" s="5" t="s">
+      <c r="G577" s="6" t="s">
         <v>1691</v>
       </c>
     </row>
     <row r="578" spans="1:7">
-      <c r="A578" s="5" t="s">
+      <c r="A578" s="6" t="s">
         <v>1692</v>
       </c>
-      <c r="B578" s="5" t="s">
+      <c r="B578" s="6" t="s">
         <v>1693</v>
       </c>
-      <c r="C578" s="5" t="s">
+      <c r="C578" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="D578" s="5"/>
-      <c r="E578" s="5" t="s">
+      <c r="D578" s="6"/>
+      <c r="E578" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="F578" s="5" t="s">
+      <c r="F578" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="G578" s="5" t="s">
+      <c r="G578" s="6" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="579" spans="1:7">
-      <c r="A579" s="5" t="s">
+      <c r="A579" s="6" t="s">
         <v>1694</v>
       </c>
-      <c r="B579" s="5" t="s">
+      <c r="B579" s="6" t="s">
         <v>1695</v>
       </c>
-      <c r="C579" s="5" t="s">
+      <c r="C579" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="D579" s="5"/>
-      <c r="E579" s="5" t="s">
+      <c r="D579" s="6"/>
+      <c r="E579" s="6" t="s">
         <v>1516</v>
       </c>
-      <c r="F579" s="5" t="s">
+      <c r="F579" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="G579" s="5" t="s">
+      <c r="G579" s="6" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="580" spans="1:7">
-      <c r="A580" s="5" t="s">
+      <c r="A580" s="6" t="s">
         <v>1696</v>
       </c>
-      <c r="B580" s="5" t="s">
+      <c r="B580" s="6" t="s">
         <v>1697</v>
       </c>
-      <c r="C580" s="5" t="s">
+      <c r="C580" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="D580" s="5"/>
-      <c r="E580" s="5" t="s">
+      <c r="D580" s="6"/>
+      <c r="E580" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="F580" s="5" t="s">
+      <c r="F580" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="G580" s="5" t="s">
+      <c r="G580" s="6" t="s">
         <v>1698</v>
       </c>
     </row>
     <row r="581" spans="1:7">
-      <c r="A581" s="5" t="s">
+      <c r="A581" s="6" t="s">
         <v>1699</v>
       </c>
-      <c r="B581" s="5" t="s">
+      <c r="B581" s="6" t="s">
         <v>1700</v>
       </c>
-      <c r="C581" s="5" t="s">
+      <c r="C581" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D581" s="5" t="s">
+      <c r="D581" s="6" t="s">
         <v>2290</v>
       </c>
-      <c r="E581" s="5" t="s">
+      <c r="E581" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="F581" s="5" t="s">
+      <c r="F581" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G581" s="5" t="s">
+      <c r="G581" s="6" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="582" spans="1:7">
-      <c r="A582" s="5" t="s">
+      <c r="A582" s="6" t="s">
         <v>1701</v>
       </c>
-      <c r="B582" s="5" t="s">
+      <c r="B582" s="6" t="s">
         <v>1702</v>
       </c>
-      <c r="C582" s="5" t="s">
+      <c r="C582" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D582" s="5" t="s">
+      <c r="D582" s="6" t="s">
         <v>2290</v>
       </c>
-      <c r="E582" s="5" t="s">
+      <c r="E582" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="F582" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G582" s="5" t="s">
+      <c r="F582" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G582" s="6" t="s">
         <v>1703</v>
       </c>
     </row>
     <row r="583" spans="1:7">
-      <c r="A583" s="5" t="s">
+      <c r="A583" s="6" t="s">
         <v>1704</v>
       </c>
-      <c r="B583" s="5" t="s">
+      <c r="B583" s="6" t="s">
         <v>1705</v>
       </c>
-      <c r="C583" s="5" t="s">
+      <c r="C583" s="6" t="s">
         <v>1117</v>
       </c>
-      <c r="D583" s="5"/>
-      <c r="E583" s="5" t="s">
+      <c r="D583" s="6"/>
+      <c r="E583" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="F583" s="5" t="s">
+      <c r="F583" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G583" s="5" t="s">
+      <c r="G583" s="6" t="s">
         <v>1706</v>
       </c>
     </row>
     <row r="584" spans="1:7">
-      <c r="A584" s="5" t="s">
+      <c r="A584" s="6" t="s">
         <v>1707</v>
       </c>
-      <c r="B584" s="5" t="s">
+      <c r="B584" s="6" t="s">
         <v>1708</v>
       </c>
-      <c r="C584" s="5" t="s">
+      <c r="C584" s="6" t="s">
         <v>1117</v>
       </c>
-      <c r="D584" s="5"/>
-      <c r="E584" s="5" t="s">
+      <c r="D584" s="6"/>
+      <c r="E584" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="F584" s="5" t="s">
+      <c r="F584" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G584" s="5" t="s">
+      <c r="G584" s="6" t="s">
         <v>1709</v>
       </c>
     </row>
     <row r="585" spans="1:7">
-      <c r="A585" s="5" t="s">
+      <c r="A585" s="6" t="s">
         <v>1710</v>
       </c>
-      <c r="B585" s="5" t="s">
+      <c r="B585" s="6" t="s">
         <v>1711</v>
       </c>
-      <c r="C585" s="5" t="s">
+      <c r="C585" s="6" t="s">
         <v>1117</v>
       </c>
-      <c r="D585" s="5"/>
-      <c r="E585" s="5" t="s">
+      <c r="D585" s="6"/>
+      <c r="E585" s="6" t="s">
         <v>579</v>
       </c>
-      <c r="F585" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G585" s="5" t="s">
+      <c r="F585" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G585" s="6" t="s">
         <v>1712</v>
       </c>
     </row>
     <row r="586" spans="1:7">
-      <c r="A586" s="5" t="s">
+      <c r="A586" s="6" t="s">
         <v>1713</v>
       </c>
-      <c r="B586" s="5" t="s">
+      <c r="B586" s="6" t="s">
         <v>1714</v>
       </c>
-      <c r="C586" s="5" t="s">
+      <c r="C586" s="6" t="s">
         <v>389</v>
       </c>
-      <c r="D586" s="5" t="s">
+      <c r="D586" s="6" t="s">
         <v>412</v>
       </c>
-      <c r="E586" s="5" t="s">
+      <c r="E586" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="F586" s="5" t="s">
+      <c r="F586" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G586" s="5" t="s">
+      <c r="G586" s="6" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="587" spans="1:7">
-      <c r="A587" s="5" t="s">
+      <c r="A587" s="6" t="s">
         <v>1715</v>
       </c>
-      <c r="B587" s="5" t="s">
+      <c r="B587" s="6" t="s">
         <v>1716</v>
       </c>
-      <c r="C587" s="5" t="s">
+      <c r="C587" s="6" t="s">
         <v>389</v>
       </c>
-      <c r="D587" s="5" t="s">
+      <c r="D587" s="6" t="s">
         <v>412</v>
       </c>
-      <c r="E587" s="5" t="s">
+      <c r="E587" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="F587" s="5" t="s">
+      <c r="F587" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="G587" s="5" t="s">
+      <c r="G587" s="6" t="s">
         <v>1717</v>
       </c>
     </row>
     <row r="588" spans="1:7">
-      <c r="A588" s="5" t="s">
+      <c r="A588" s="6" t="s">
         <v>1718</v>
       </c>
-      <c r="B588" s="5" t="s">
+      <c r="B588" s="6" t="s">
         <v>1719</v>
       </c>
-      <c r="C588" s="5" t="s">
+      <c r="C588" s="6" t="s">
         <v>449</v>
       </c>
-      <c r="D588" s="5" t="s">
+      <c r="D588" s="6" t="s">
         <v>2290</v>
       </c>
-      <c r="E588" s="5" t="s">
+      <c r="E588" s="6" t="s">
         <v>1720</v>
       </c>
-      <c r="F588" s="5" t="s">
+      <c r="F588" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="G588" s="5" t="s">
+      <c r="G588" s="6" t="s">
         <v>676</v>
       </c>
     </row>
     <row r="589" spans="1:7">
-      <c r="A589" s="5" t="s">
+      <c r="A589" s="6" t="s">
         <v>1721</v>
       </c>
-      <c r="B589" s="5" t="s">
+      <c r="B589" s="6" t="s">
         <v>1722</v>
       </c>
-      <c r="C589" s="5" t="s">
+      <c r="C589" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D589" s="5"/>
-      <c r="E589" s="5" t="s">
+      <c r="D589" s="6"/>
+      <c r="E589" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F589" s="5" t="s">
+      <c r="F589" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="G589" s="5" t="s">
+      <c r="G589" s="6" t="s">
         <v>1499</v>
       </c>
     </row>
     <row r="590" spans="1:7">
-      <c r="A590" s="5" t="s">
+      <c r="A590" s="6" t="s">
         <v>1723</v>
       </c>
-      <c r="B590" s="5" t="s">
+      <c r="B590" s="6" t="s">
         <v>1724</v>
       </c>
-      <c r="C590" s="5" t="s">
+      <c r="C590" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D590" s="5" t="s">
+      <c r="D590" s="6" t="s">
         <v>1169</v>
       </c>
-      <c r="E590" s="5" t="s">
+      <c r="E590" s="6" t="s">
         <v>452</v>
       </c>
-      <c r="F590" s="5" t="s">
+      <c r="F590" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="G590" s="5" t="s">
+      <c r="G590" s="6" t="s">
         <v>1725</v>
       </c>
     </row>
     <row r="591" spans="1:7">
-      <c r="A591" s="5" t="s">
+      <c r="A591" s="6" t="s">
         <v>1726</v>
       </c>
-      <c r="B591" s="5" t="s">
+      <c r="B591" s="6" t="s">
         <v>1727</v>
       </c>
-      <c r="C591" s="5" t="s">
+      <c r="C591" s="6" t="s">
         <v>412</v>
       </c>
-      <c r="D591" s="5" t="s">
+      <c r="D591" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E591" s="5" t="s">
+      <c r="E591" s="6" t="s">
         <v>420</v>
       </c>
-      <c r="F591" s="5" t="s">
+      <c r="F591" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G591" s="5" t="s">
+      <c r="G591" s="6" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="592" spans="1:7">
-      <c r="A592" s="5" t="s">
+      <c r="A592" s="6" t="s">
         <v>1728</v>
       </c>
-      <c r="B592" s="5" t="s">
+      <c r="B592" s="6" t="s">
         <v>1729</v>
       </c>
-      <c r="C592" s="5" t="s">
+      <c r="C592" s="6" t="s">
         <v>412</v>
       </c>
-      <c r="D592" s="5" t="s">
+      <c r="D592" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E592" s="5" t="s">
+      <c r="E592" s="6" t="s">
         <v>1730</v>
       </c>
-      <c r="F592" s="5" t="s">
+      <c r="F592" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="G592" s="5" t="s">
+      <c r="G592" s="6" t="s">
         <v>1530</v>
       </c>
     </row>
     <row r="593" spans="1:7">
-      <c r="A593" s="5" t="s">
+      <c r="A593" s="6" t="s">
         <v>1731</v>
       </c>
-      <c r="B593" s="5" t="s">
+      <c r="B593" s="6" t="s">
         <v>1732</v>
       </c>
-      <c r="C593" s="5" t="s">
+      <c r="C593" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D593" s="5" t="s">
+      <c r="D593" s="6" t="s">
         <v>672</v>
       </c>
-      <c r="E593" s="5" t="s">
+      <c r="E593" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="F593" s="5" t="s">
+      <c r="F593" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G593" s="5" t="s">
+      <c r="G593" s="6" t="s">
         <v>1725</v>
       </c>
     </row>
     <row r="594" spans="1:7">
-      <c r="A594" s="5" t="s">
+      <c r="A594" s="6" t="s">
         <v>1733</v>
       </c>
-      <c r="B594" s="5" t="s">
+      <c r="B594" s="6" t="s">
         <v>1734</v>
       </c>
-      <c r="C594" s="5" t="s">
+      <c r="C594" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D594" s="5" t="s">
+      <c r="D594" s="6" t="s">
         <v>672</v>
       </c>
-      <c r="E594" s="5" t="s">
+      <c r="E594" s="6" t="s">
         <v>737</v>
       </c>
-      <c r="F594" s="5" t="s">
+      <c r="F594" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="G594" s="5" t="s">
+      <c r="G594" s="6" t="s">
         <v>1735</v>
       </c>
     </row>
     <row r="595" spans="1:7">
-      <c r="A595" s="5" t="s">
+      <c r="A595" s="6" t="s">
         <v>1736</v>
       </c>
-      <c r="B595" s="5" t="s">
+      <c r="B595" s="6" t="s">
         <v>1737</v>
       </c>
-      <c r="C595" s="5" t="s">
+      <c r="C595" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D595" s="5"/>
-      <c r="E595" s="5" t="s">
+      <c r="D595" s="6"/>
+      <c r="E595" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="F595" s="5" t="s">
+      <c r="F595" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="G595" s="5" t="s">
+      <c r="G595" s="6" t="s">
         <v>861</v>
       </c>
     </row>
     <row r="596" spans="1:7">
-      <c r="A596" s="5" t="s">
+      <c r="A596" s="6" t="s">
         <v>1738</v>
       </c>
-      <c r="B596" s="5" t="s">
+      <c r="B596" s="6" t="s">
         <v>1739</v>
       </c>
-      <c r="C596" s="5" t="s">
+      <c r="C596" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D596" s="5" t="s">
+      <c r="D596" s="6" t="s">
         <v>449</v>
       </c>
-      <c r="E596" s="5" t="s">
+      <c r="E596" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F596" s="5" t="s">
+      <c r="F596" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G596" s="5" t="s">
+      <c r="G596" s="6" t="s">
         <v>1318</v>
       </c>
     </row>
     <row r="597" spans="1:7">
-      <c r="A597" s="5" t="s">
+      <c r="A597" s="6" t="s">
         <v>1740</v>
       </c>
-      <c r="B597" s="5" t="s">
+      <c r="B597" s="6" t="s">
         <v>1741</v>
       </c>
-      <c r="C597" s="5" t="s">
+      <c r="C597" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D597" s="5" t="s">
+      <c r="D597" s="6" t="s">
         <v>449</v>
       </c>
-      <c r="E597" s="5" t="s">
+      <c r="E597" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="F597" s="5" t="s">
+      <c r="F597" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="G597" s="5" t="s">
+      <c r="G597" s="6" t="s">
         <v>1742</v>
       </c>
     </row>
     <row r="598" spans="1:7">
-      <c r="A598" s="5" t="s">
+      <c r="A598" s="6" t="s">
         <v>1743</v>
       </c>
-      <c r="B598" s="5" t="s">
+      <c r="B598" s="6" t="s">
         <v>1744</v>
       </c>
-      <c r="C598" s="5" t="s">
+      <c r="C598" s="6" t="s">
         <v>412</v>
       </c>
-      <c r="D598" s="5" t="s">
+      <c r="D598" s="6" t="s">
         <v>1169</v>
       </c>
-      <c r="E598" s="5" t="s">
+      <c r="E598" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="F598" s="5" t="s">
+      <c r="F598" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G598" s="5" t="s">
+      <c r="G598" s="6" t="s">
         <v>1745</v>
       </c>
     </row>
     <row r="599" spans="1:7">
-      <c r="A599" s="5" t="s">
+      <c r="A599" s="6" t="s">
         <v>1746</v>
       </c>
-      <c r="B599" s="5" t="s">
+      <c r="B599" s="6" t="s">
         <v>1747</v>
       </c>
-      <c r="C599" s="5" t="s">
+      <c r="C599" s="6" t="s">
         <v>412</v>
       </c>
-      <c r="D599" s="5" t="s">
+      <c r="D599" s="6" t="s">
         <v>1169</v>
       </c>
-      <c r="E599" s="5" t="s">
+      <c r="E599" s="6" t="s">
         <v>1654</v>
       </c>
-      <c r="F599" s="5" t="s">
+      <c r="F599" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="G599" s="5" t="s">
+      <c r="G599" s="6" t="s">
         <v>1748</v>
       </c>
     </row>
     <row r="600" spans="1:7">
-      <c r="A600" s="5" t="s">
+      <c r="A600" s="6" t="s">
         <v>1749</v>
       </c>
-      <c r="B600" s="5" t="s">
+      <c r="B600" s="6" t="s">
         <v>1750</v>
       </c>
-      <c r="C600" s="5" t="s">
+      <c r="C600" s="6" t="s">
         <v>1169</v>
       </c>
-      <c r="D600" s="5"/>
-      <c r="E600" s="5" t="s">
+      <c r="D600" s="6"/>
+      <c r="E600" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="F600" s="5" t="s">
+      <c r="F600" s="6" t="s">
         <v>1337</v>
       </c>
-      <c r="G600" s="5" t="s">
+      <c r="G600" s="6" t="s">
         <v>768</v>
       </c>
     </row>
     <row r="601" spans="1:7">
-      <c r="A601" s="5" t="s">
+      <c r="A601" s="6" t="s">
         <v>1751</v>
       </c>
-      <c r="B601" s="5" t="s">
+      <c r="B601" s="6" t="s">
         <v>1752</v>
       </c>
-      <c r="C601" s="5" t="s">
+      <c r="C601" s="6" t="s">
         <v>1169</v>
       </c>
-      <c r="D601" s="5"/>
-      <c r="E601" s="5" t="s">
+      <c r="D601" s="6"/>
+      <c r="E601" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="F601" s="5" t="s">
+      <c r="F601" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="G601" s="5" t="s">
+      <c r="G601" s="6" t="s">
         <v>1600</v>
       </c>
     </row>
     <row r="602" spans="1:7">
-      <c r="A602" s="5" t="s">
+      <c r="A602" s="6" t="s">
         <v>1753</v>
       </c>
-      <c r="B602" s="5" t="s">
+      <c r="B602" s="6" t="s">
         <v>1754</v>
       </c>
-      <c r="C602" s="5" t="s">
+      <c r="C602" s="6" t="s">
         <v>1169</v>
       </c>
-      <c r="D602" s="5"/>
-      <c r="E602" s="5" t="s">
+      <c r="D602" s="6"/>
+      <c r="E602" s="6" t="s">
         <v>1031</v>
       </c>
-      <c r="F602" s="5" t="s">
+      <c r="F602" s="6" t="s">
         <v>408</v>
       </c>
-      <c r="G602" s="5" t="s">
+      <c r="G602" s="6" t="s">
         <v>1666</v>
       </c>
     </row>
     <row r="603" spans="1:7">
-      <c r="A603" s="5" t="s">
+      <c r="A603" s="6" t="s">
         <v>1755</v>
       </c>
-      <c r="B603" s="5" t="s">
+      <c r="B603" s="6" t="s">
         <v>1756</v>
       </c>
-      <c r="C603" s="5" t="s">
+      <c r="C603" s="6" t="s">
         <v>449</v>
       </c>
-      <c r="D603" s="5"/>
-      <c r="E603" s="5" t="s">
+      <c r="D603" s="6"/>
+      <c r="E603" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="F603" s="5" t="s">
+      <c r="F603" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G603" s="5" t="s">
+      <c r="G603" s="6" t="s">
         <v>1437</v>
       </c>
     </row>
     <row r="604" spans="1:7">
-      <c r="A604" s="5" t="s">
+      <c r="A604" s="6" t="s">
         <v>1757</v>
       </c>
-      <c r="B604" s="5" t="s">
+      <c r="B604" s="6" t="s">
         <v>1758</v>
       </c>
-      <c r="C604" s="5" t="s">
+      <c r="C604" s="6" t="s">
         <v>449</v>
       </c>
-      <c r="D604" s="5"/>
-      <c r="E604" s="5" t="s">
+      <c r="D604" s="6"/>
+      <c r="E604" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F604" s="5" t="s">
+      <c r="F604" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="G604" s="5" t="s">
+      <c r="G604" s="6" t="s">
         <v>1097</v>
       </c>
     </row>
     <row r="605" spans="1:7">
-      <c r="A605" s="5" t="s">
+      <c r="A605" s="6" t="s">
         <v>1759</v>
       </c>
-      <c r="B605" s="5" t="s">
+      <c r="B605" s="6" t="s">
         <v>1760</v>
       </c>
-      <c r="C605" s="5" t="s">
+      <c r="C605" s="6" t="s">
         <v>449</v>
       </c>
-      <c r="D605" s="5"/>
-      <c r="E605" s="5" t="s">
+      <c r="D605" s="6"/>
+      <c r="E605" s="6" t="s">
         <v>1761</v>
       </c>
-      <c r="F605" s="5" t="s">
+      <c r="F605" s="6" t="s">
         <v>408</v>
       </c>
-      <c r="G605" s="5" t="s">
+      <c r="G605" s="6" t="s">
         <v>1762</v>
       </c>
     </row>
     <row r="606" spans="1:7">
-      <c r="A606" s="5" t="s">
+      <c r="A606" s="6" t="s">
         <v>1763</v>
       </c>
-      <c r="B606" s="5" t="s">
+      <c r="B606" s="6" t="s">
         <v>1764</v>
       </c>
-      <c r="C606" s="5" t="s">
+      <c r="C606" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="D606" s="5"/>
-      <c r="E606" s="5" t="s">
+      <c r="D606" s="6"/>
+      <c r="E606" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="F606" s="5" t="s">
+      <c r="F606" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G606" s="5" t="s">
+      <c r="G606" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="607" spans="1:7">
-      <c r="A607" s="5" t="s">
+      <c r="A607" s="6" t="s">
         <v>1765</v>
       </c>
-      <c r="B607" s="5" t="s">
+      <c r="B607" s="6" t="s">
         <v>1766</v>
       </c>
-      <c r="C607" s="5" t="s">
+      <c r="C607" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="D607" s="5"/>
-      <c r="E607" s="5" t="s">
+      <c r="D607" s="6"/>
+      <c r="E607" s="6" t="s">
         <v>404</v>
       </c>
-      <c r="F607" s="5" t="s">
+      <c r="F607" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="G607" s="5" t="s">
+      <c r="G607" s="6" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="608" spans="1:7">
-      <c r="A608" s="5" t="s">
+      <c r="A608" s="6" t="s">
         <v>1767</v>
       </c>
-      <c r="B608" s="5" t="s">
+      <c r="B608" s="6" t="s">
         <v>1768</v>
       </c>
-      <c r="C608" s="5" t="s">
+      <c r="C608" s="6" t="s">
         <v>672</v>
       </c>
-      <c r="D608" s="5" t="s">
+      <c r="D608" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E608" s="5" t="s">
+      <c r="E608" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="F608" s="5" t="s">
+      <c r="F608" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G608" s="5" t="s">
+      <c r="G608" s="6" t="s">
         <v>1465</v>
       </c>
     </row>
     <row r="609" spans="1:7">
-      <c r="A609" s="5" t="s">
+      <c r="A609" s="6" t="s">
         <v>1769</v>
       </c>
-      <c r="B609" s="5" t="s">
+      <c r="B609" s="6" t="s">
         <v>1770</v>
       </c>
-      <c r="C609" s="5" t="s">
+      <c r="C609" s="6" t="s">
         <v>672</v>
       </c>
-      <c r="D609" s="5" t="s">
+      <c r="D609" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E609" s="5" t="s">
+      <c r="E609" s="6" t="s">
         <v>1516</v>
       </c>
-      <c r="F609" s="5" t="s">
+      <c r="F609" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="G609" s="5" t="s">
+      <c r="G609" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="610" spans="1:7">
-      <c r="A610" s="5" t="s">
+      <c r="A610" s="6" t="s">
         <v>1771</v>
       </c>
-      <c r="B610" s="5" t="s">
+      <c r="B610" s="6" t="s">
         <v>1772</v>
       </c>
-      <c r="C610" s="5" t="s">
+      <c r="C610" s="6" t="s">
         <v>672</v>
       </c>
-      <c r="D610" s="5" t="s">
+      <c r="D610" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E610" s="5" t="s">
+      <c r="E610" s="6" t="s">
         <v>1031</v>
       </c>
-      <c r="F610" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G610" s="5" t="s">
+      <c r="F610" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G610" s="6" t="s">
         <v>1773</v>
       </c>
     </row>
     <row r="611" spans="1:7">
-      <c r="A611" s="5" t="s">
+      <c r="A611" s="6" t="s">
         <v>1774</v>
       </c>
-      <c r="B611" s="5" t="s">
+      <c r="B611" s="6" t="s">
         <v>1775</v>
       </c>
-      <c r="C611" s="5" t="s">
+      <c r="C611" s="6" t="s">
         <v>516</v>
       </c>
-      <c r="D611" s="5"/>
-      <c r="E611" s="5" t="s">
+      <c r="D611" s="6"/>
+      <c r="E611" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F611" s="5" t="s">
+      <c r="F611" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="G611" s="5" t="s">
+      <c r="G611" s="6" t="s">
         <v>1561</v>
       </c>
     </row>
     <row r="612" spans="1:7">
-      <c r="A612" s="5" t="s">
+      <c r="A612" s="6" t="s">
         <v>1776</v>
       </c>
-      <c r="B612" s="5" t="s">
+      <c r="B612" s="6" t="s">
         <v>1777</v>
       </c>
-      <c r="C612" s="5" t="s">
+      <c r="C612" s="6" t="s">
         <v>516</v>
       </c>
-      <c r="D612" s="5"/>
-      <c r="E612" s="5" t="s">
+      <c r="D612" s="6"/>
+      <c r="E612" s="6" t="s">
         <v>628</v>
       </c>
-      <c r="F612" s="5" t="s">
+      <c r="F612" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="G612" s="5" t="s">
+      <c r="G612" s="6" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="613" spans="1:7">
-      <c r="A613" s="5" t="s">
+      <c r="A613" s="6" t="s">
         <v>1778</v>
       </c>
-      <c r="B613" s="5" t="s">
+      <c r="B613" s="6" t="s">
         <v>1779</v>
       </c>
-      <c r="C613" s="5" t="s">
+      <c r="C613" s="6" t="s">
         <v>516</v>
       </c>
-      <c r="D613" s="5"/>
-      <c r="E613" s="5" t="s">
+      <c r="D613" s="6"/>
+      <c r="E613" s="6" t="s">
         <v>814</v>
       </c>
-      <c r="F613" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G613" s="5" t="s">
+      <c r="F613" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G613" s="6" t="s">
         <v>1780</v>
       </c>
     </row>
     <row r="614" spans="1:7">
-      <c r="A614" s="5" t="s">
+      <c r="A614" s="6" t="s">
         <v>1781</v>
       </c>
-      <c r="B614" s="5" t="s">
+      <c r="B614" s="6" t="s">
         <v>1782</v>
       </c>
-      <c r="C614" s="5" t="s">
+      <c r="C614" s="6" t="s">
         <v>1117</v>
       </c>
-      <c r="D614" s="5"/>
-      <c r="E614" s="5" t="s">
+      <c r="D614" s="6"/>
+      <c r="E614" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="F614" s="5" t="s">
+      <c r="F614" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G614" s="5" t="s">
+      <c r="G614" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="615" spans="1:7">
-      <c r="A615" s="5" t="s">
+      <c r="A615" s="6" t="s">
         <v>1783</v>
       </c>
-      <c r="B615" s="5" t="s">
+      <c r="B615" s="6" t="s">
         <v>1784</v>
       </c>
-      <c r="C615" s="5" t="s">
+      <c r="C615" s="6" t="s">
         <v>1117</v>
       </c>
-      <c r="D615" s="5"/>
-      <c r="E615" s="5" t="s">
+      <c r="D615" s="6"/>
+      <c r="E615" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="F615" s="5" t="s">
+      <c r="F615" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="G615" s="5" t="s">
+      <c r="G615" s="6" t="s">
         <v>1567</v>
       </c>
     </row>
     <row r="616" spans="1:7">
-      <c r="A616" s="5" t="s">
+      <c r="A616" s="6" t="s">
         <v>1785</v>
       </c>
-      <c r="B616" s="5" t="s">
+      <c r="B616" s="6" t="s">
         <v>1786</v>
       </c>
-      <c r="C616" s="5" t="s">
+      <c r="C616" s="6" t="s">
         <v>1117</v>
       </c>
-      <c r="D616" s="5"/>
-      <c r="E616" s="5" t="s">
+      <c r="D616" s="6"/>
+      <c r="E616" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="F616" s="5" t="s">
+      <c r="F616" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="G616" s="5" t="s">
+      <c r="G616" s="6" t="s">
         <v>1787</v>
       </c>
     </row>
     <row r="617" spans="1:7">
-      <c r="A617" s="5" t="s">
+      <c r="A617" s="6" t="s">
         <v>1788</v>
       </c>
-      <c r="B617" s="5" t="s">
+      <c r="B617" s="6" t="s">
         <v>1789</v>
       </c>
-      <c r="C617" s="5" t="s">
+      <c r="C617" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D617" s="5"/>
-      <c r="E617" s="5" t="s">
+      <c r="D617" s="6"/>
+      <c r="E617" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="F617" s="5" t="s">
+      <c r="F617" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="G617" s="5" t="s">
+      <c r="G617" s="6" t="s">
         <v>1790</v>
       </c>
     </row>
     <row r="618" spans="1:7">
-      <c r="A618" s="5" t="s">
+      <c r="A618" s="6" t="s">
         <v>1791</v>
       </c>
-      <c r="B618" s="5" t="s">
+      <c r="B618" s="6" t="s">
         <v>1792</v>
       </c>
-      <c r="C618" s="5" t="s">
+      <c r="C618" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D618" s="5"/>
-      <c r="E618" s="5" t="s">
+      <c r="D618" s="6"/>
+      <c r="E618" s="6" t="s">
         <v>452</v>
       </c>
-      <c r="F618" s="5" t="s">
+      <c r="F618" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="G618" s="5" t="s">
+      <c r="G618" s="6" t="s">
         <v>1793</v>
       </c>
     </row>
     <row r="619" spans="1:7">
-      <c r="A619" s="5" t="s">
+      <c r="A619" s="6" t="s">
         <v>1794</v>
       </c>
-      <c r="B619" s="5" t="s">
+      <c r="B619" s="6" t="s">
         <v>1795</v>
       </c>
-      <c r="C619" s="5" t="s">
+      <c r="C619" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D619" s="5" t="s">
+      <c r="D619" s="6" t="s">
         <v>449</v>
       </c>
-      <c r="E619" s="5" t="s">
+      <c r="E619" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="F619" s="5" t="s">
+      <c r="F619" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="G619" s="5" t="s">
+      <c r="G619" s="6" t="s">
         <v>953</v>
       </c>
     </row>
     <row r="620" spans="1:7">
-      <c r="A620" s="5" t="s">
+      <c r="A620" s="6" t="s">
         <v>1796</v>
       </c>
-      <c r="B620" s="5" t="s">
+      <c r="B620" s="6" t="s">
         <v>1797</v>
       </c>
-      <c r="C620" s="5" t="s">
+      <c r="C620" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="D620" s="5"/>
-      <c r="E620" s="5" t="s">
+      <c r="D620" s="6"/>
+      <c r="E620" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="F620" s="5" t="s">
+      <c r="F620" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="G620" s="5" t="s">
+      <c r="G620" s="6" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="621" spans="1:7">
-      <c r="A621" s="5" t="s">
+      <c r="A621" s="6" t="s">
         <v>1798</v>
       </c>
-      <c r="B621" s="5" t="s">
+      <c r="B621" s="6" t="s">
         <v>1799</v>
       </c>
-      <c r="C621" s="5" t="s">
+      <c r="C621" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="D621" s="5"/>
-      <c r="E621" s="5" t="s">
+      <c r="D621" s="6"/>
+      <c r="E621" s="6" t="s">
         <v>697</v>
       </c>
-      <c r="F621" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G621" s="5" t="s">
+      <c r="F621" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G621" s="6" t="s">
         <v>1800</v>
       </c>
     </row>
     <row r="622" spans="1:7">
-      <c r="A622" s="5" t="s">
+      <c r="A622" s="6" t="s">
         <v>1801</v>
       </c>
-      <c r="B622" s="5" t="s">
+      <c r="B622" s="6" t="s">
         <v>1802</v>
       </c>
-      <c r="C622" s="5" t="s">
+      <c r="C622" s="6" t="s">
         <v>516</v>
       </c>
-      <c r="D622" s="5"/>
-      <c r="E622" s="5" t="s">
+      <c r="D622" s="6"/>
+      <c r="E622" s="6" t="s">
         <v>404</v>
       </c>
-      <c r="F622" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G622" s="5" t="s">
+      <c r="F622" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G622" s="6" t="s">
         <v>1803</v>
       </c>
     </row>
     <row r="623" spans="1:7">
-      <c r="A623" s="5" t="s">
+      <c r="A623" s="6" t="s">
         <v>1804</v>
       </c>
-      <c r="B623" s="5" t="s">
+      <c r="B623" s="6" t="s">
         <v>1805</v>
       </c>
-      <c r="C623" s="5" t="s">
+      <c r="C623" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D623" s="5" t="s">
+      <c r="D623" s="6" t="s">
         <v>672</v>
       </c>
-      <c r="E623" s="5" t="s">
+      <c r="E623" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="F623" s="5" t="s">
+      <c r="F623" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G623" s="5" t="s">
+      <c r="G623" s="6" t="s">
         <v>1806</v>
       </c>
     </row>
     <row r="624" spans="1:7">
-      <c r="A624" s="5" t="s">
+      <c r="A624" s="6" t="s">
         <v>1807</v>
       </c>
-      <c r="B624" s="5" t="s">
+      <c r="B624" s="6" t="s">
         <v>1808</v>
       </c>
-      <c r="C624" s="5" t="s">
+      <c r="C624" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D624" s="5" t="s">
+      <c r="D624" s="6" t="s">
         <v>672</v>
       </c>
-      <c r="E624" s="5" t="s">
+      <c r="E624" s="6" t="s">
         <v>355</v>
       </c>
-      <c r="F624" s="5" t="s">
+      <c r="F624" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="G624" s="5" t="s">
+      <c r="G624" s="6" t="s">
         <v>1809</v>
       </c>
     </row>
     <row r="625" spans="1:7">
-      <c r="A625" s="5" t="s">
+      <c r="A625" s="6" t="s">
         <v>1810</v>
       </c>
-      <c r="B625" s="5" t="s">
+      <c r="B625" s="6" t="s">
         <v>1811</v>
       </c>
-      <c r="C625" s="5" t="s">
+      <c r="C625" s="6" t="s">
         <v>661</v>
       </c>
-      <c r="D625" s="5" t="s">
+      <c r="D625" s="6" t="s">
         <v>1169</v>
       </c>
-      <c r="E625" s="5" t="s">
+      <c r="E625" s="6" t="s">
         <v>393</v>
       </c>
-      <c r="F625" s="5" t="s">
+      <c r="F625" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G625" s="5" t="s">
+      <c r="G625" s="6" t="s">
         <v>1193</v>
       </c>
     </row>
     <row r="626" spans="1:7">
-      <c r="A626" s="5" t="s">
+      <c r="A626" s="6" t="s">
         <v>1812</v>
       </c>
-      <c r="B626" s="5" t="s">
+      <c r="B626" s="6" t="s">
         <v>1813</v>
       </c>
-      <c r="C626" s="5" t="s">
+      <c r="C626" s="6" t="s">
         <v>661</v>
       </c>
-      <c r="D626" s="5" t="s">
+      <c r="D626" s="6" t="s">
         <v>1169</v>
       </c>
-      <c r="E626" s="5" t="s">
+      <c r="E626" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="F626" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G626" s="5" t="s">
+      <c r="F626" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G626" s="6" t="s">
         <v>1814</v>
       </c>
     </row>
     <row r="627" spans="1:7">
-      <c r="A627" s="5" t="s">
+      <c r="A627" s="6" t="s">
         <v>1815</v>
       </c>
-      <c r="B627" s="5" t="s">
+      <c r="B627" s="6" t="s">
         <v>1816</v>
       </c>
-      <c r="C627" s="5" t="s">
+      <c r="C627" s="6" t="s">
         <v>389</v>
       </c>
-      <c r="D627" s="5"/>
-      <c r="E627" s="5" t="s">
+      <c r="D627" s="6"/>
+      <c r="E627" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="F627" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G627" s="5" t="s">
+      <c r="F627" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G627" s="6" t="s">
         <v>1505</v>
       </c>
     </row>
     <row r="628" spans="1:7">
-      <c r="A628" s="5" t="s">
+      <c r="A628" s="6" t="s">
         <v>1817</v>
       </c>
-      <c r="B628" s="5" t="s">
+      <c r="B628" s="6" t="s">
         <v>1818</v>
       </c>
-      <c r="C628" s="5" t="s">
+      <c r="C628" s="6" t="s">
         <v>389</v>
       </c>
-      <c r="D628" s="5" t="s">
+      <c r="D628" s="6" t="s">
         <v>2290</v>
       </c>
-      <c r="E628" s="5" t="s">
+      <c r="E628" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="F628" s="5" t="s">
+      <c r="F628" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G628" s="5" t="s">
+      <c r="G628" s="6" t="s">
         <v>1530</v>
       </c>
     </row>
     <row r="629" spans="1:7">
-      <c r="A629" s="5" t="s">
+      <c r="A629" s="6" t="s">
         <v>1819</v>
       </c>
-      <c r="B629" s="5" t="s">
+      <c r="B629" s="6" t="s">
         <v>1820</v>
       </c>
-      <c r="C629" s="5" t="s">
+      <c r="C629" s="6" t="s">
         <v>389</v>
       </c>
-      <c r="D629" s="5" t="s">
+      <c r="D629" s="6" t="s">
         <v>2290</v>
       </c>
-      <c r="E629" s="5" t="s">
+      <c r="E629" s="6" t="s">
         <v>697</v>
       </c>
-      <c r="F629" s="5" t="s">
+      <c r="F629" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="G629" s="5" t="s">
+      <c r="G629" s="6" t="s">
         <v>1709</v>
       </c>
     </row>
     <row r="630" spans="1:7">
-      <c r="A630" s="5" t="s">
+      <c r="A630" s="6" t="s">
         <v>1821</v>
       </c>
-      <c r="B630" s="5" t="s">
+      <c r="B630" s="6" t="s">
         <v>1822</v>
       </c>
-      <c r="C630" s="5" t="s">
+      <c r="C630" s="6" t="s">
         <v>661</v>
       </c>
-      <c r="D630" s="5" t="s">
+      <c r="D630" s="6" t="s">
         <v>2290</v>
       </c>
-      <c r="E630" s="5" t="s">
+      <c r="E630" s="6" t="s">
         <v>1823</v>
       </c>
-      <c r="F630" s="5" t="s">
+      <c r="F630" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G630" s="5" t="s">
+      <c r="G630" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="631" spans="1:7">
-      <c r="A631" s="5" t="s">
+      <c r="A631" s="6" t="s">
         <v>1824</v>
       </c>
-      <c r="B631" s="5" t="s">
+      <c r="B631" s="6" t="s">
         <v>1825</v>
       </c>
-      <c r="C631" s="5" t="s">
+      <c r="C631" s="6" t="s">
         <v>661</v>
       </c>
-      <c r="D631" s="5" t="s">
+      <c r="D631" s="6" t="s">
         <v>2290</v>
       </c>
-      <c r="E631" s="5" t="s">
+      <c r="E631" s="6" t="s">
         <v>697</v>
       </c>
-      <c r="F631" s="5" t="s">
+      <c r="F631" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="G631" s="5" t="s">
+      <c r="G631" s="6" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="632" spans="1:7">
-      <c r="A632" s="5" t="s">
+      <c r="A632" s="6" t="s">
         <v>1826</v>
       </c>
-      <c r="B632" s="5" t="s">
+      <c r="B632" s="6" t="s">
         <v>1827</v>
       </c>
-      <c r="C632" s="5" t="s">
+      <c r="C632" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D632" s="5"/>
-      <c r="E632" s="5" t="s">
+      <c r="D632" s="6"/>
+      <c r="E632" s="6" t="s">
         <v>355</v>
       </c>
-      <c r="F632" s="5" t="s">
+      <c r="F632" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="G632" s="5" t="s">
+      <c r="G632" s="6" t="s">
         <v>765</v>
       </c>
     </row>
     <row r="633" spans="1:7">
-      <c r="A633" s="5" t="s">
+      <c r="A633" s="6" t="s">
         <v>1828</v>
       </c>
-      <c r="B633" s="5" t="s">
+      <c r="B633" s="6" t="s">
         <v>1829</v>
       </c>
-      <c r="C633" s="5" t="s">
+      <c r="C633" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D633" s="5" t="s">
+      <c r="D633" s="6" t="s">
         <v>1169</v>
       </c>
-      <c r="E633" s="5" t="s">
+      <c r="E633" s="6" t="s">
         <v>355</v>
       </c>
-      <c r="F633" s="5" t="s">
+      <c r="F633" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="G633" s="5" t="s">
+      <c r="G633" s="6" t="s">
         <v>1725</v>
       </c>
     </row>
     <row r="634" spans="1:7">
-      <c r="A634" s="5" t="s">
+      <c r="A634" s="6" t="s">
         <v>1830</v>
       </c>
-      <c r="B634" s="5" t="s">
+      <c r="B634" s="6" t="s">
         <v>1831</v>
       </c>
-      <c r="C634" s="5" t="s">
+      <c r="C634" s="6" t="s">
         <v>661</v>
       </c>
-      <c r="D634" s="5" t="s">
+      <c r="D634" s="6" t="s">
         <v>516</v>
       </c>
-      <c r="E634" s="5" t="s">
+      <c r="E634" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="F634" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G634" s="5" t="s">
+      <c r="F634" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G634" s="6" t="s">
         <v>1832</v>
       </c>
     </row>
     <row r="635" spans="1:7">
-      <c r="A635" s="5" t="s">
+      <c r="A635" s="6" t="s">
         <v>1833</v>
       </c>
-      <c r="B635" s="5" t="s">
+      <c r="B635" s="6" t="s">
         <v>1834</v>
       </c>
-      <c r="C635" s="5" t="s">
+      <c r="C635" s="6" t="s">
         <v>661</v>
       </c>
-      <c r="D635" s="5" t="s">
+      <c r="D635" s="6" t="s">
         <v>516</v>
       </c>
-      <c r="E635" s="5" t="s">
+      <c r="E635" s="6" t="s">
         <v>520</v>
       </c>
-      <c r="F635" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G635" s="5" t="s">
+      <c r="F635" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G635" s="6" t="s">
         <v>1835</v>
       </c>
     </row>
     <row r="636" spans="1:7">
-      <c r="A636" s="5" t="s">
+      <c r="A636" s="6" t="s">
         <v>1836</v>
       </c>
-      <c r="B636" s="5" t="s">
+      <c r="B636" s="6" t="s">
         <v>1837</v>
       </c>
-      <c r="C636" s="5" t="s">
+      <c r="C636" s="6" t="s">
         <v>661</v>
       </c>
-      <c r="D636" s="5" t="s">
+      <c r="D636" s="6" t="s">
         <v>516</v>
       </c>
-      <c r="E636" s="5" t="s">
+      <c r="E636" s="6" t="s">
         <v>524</v>
       </c>
-      <c r="F636" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G636" s="5" t="s">
+      <c r="F636" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G636" s="6" t="s">
         <v>1838</v>
       </c>
     </row>
     <row r="637" spans="1:7">
-      <c r="A637" s="5" t="s">
+      <c r="A637" s="6" t="s">
         <v>1839</v>
       </c>
-      <c r="B637" s="5" t="s">
+      <c r="B637" s="6" t="s">
         <v>1840</v>
       </c>
-      <c r="C637" s="5" t="s">
+      <c r="C637" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D637" s="5" t="s">
+      <c r="D637" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E637" s="5" t="s">
+      <c r="E637" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F637" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G637" s="5" t="s">
+      <c r="F637" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G637" s="6" t="s">
         <v>1841</v>
       </c>
     </row>
     <row r="638" spans="1:7">
-      <c r="A638" s="5" t="s">
+      <c r="A638" s="6" t="s">
         <v>1842</v>
       </c>
-      <c r="B638" s="5" t="s">
+      <c r="B638" s="6" t="s">
         <v>1843</v>
       </c>
-      <c r="C638" s="5" t="s">
+      <c r="C638" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D638" s="5" t="s">
+      <c r="D638" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E638" s="5" t="s">
+      <c r="E638" s="6" t="s">
         <v>1844</v>
       </c>
-      <c r="F638" s="5" t="s">
+      <c r="F638" s="6" t="s">
         <v>1845</v>
       </c>
-      <c r="G638" s="5" t="s">
+      <c r="G638" s="6" t="s">
         <v>1846</v>
       </c>
     </row>
     <row r="639" spans="1:7">
-      <c r="A639" s="5" t="s">
+      <c r="A639" s="6" t="s">
         <v>1847</v>
       </c>
-      <c r="B639" s="5" t="s">
+      <c r="B639" s="6" t="s">
         <v>1848</v>
       </c>
-      <c r="C639" s="5" t="s">
+      <c r="C639" s="6" t="s">
         <v>1169</v>
       </c>
-      <c r="D639" s="5" t="s">
+      <c r="D639" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="E639" s="5" t="s">
+      <c r="E639" s="6" t="s">
         <v>789</v>
       </c>
-      <c r="F639" s="5" t="s">
+      <c r="F639" s="6" t="s">
         <v>507</v>
       </c>
-      <c r="G639" s="5" t="s">
+      <c r="G639" s="6" t="s">
         <v>1849</v>
       </c>
     </row>
     <row r="640" spans="1:7">
-      <c r="A640" s="5" t="s">
+      <c r="A640" s="6" t="s">
         <v>1850</v>
       </c>
-      <c r="B640" s="5" t="s">
+      <c r="B640" s="6" t="s">
         <v>1851</v>
       </c>
-      <c r="C640" s="5" t="s">
+      <c r="C640" s="6" t="s">
         <v>627</v>
       </c>
-      <c r="D640" s="5" t="s">
+      <c r="D640" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="E640" s="5" t="s">
+      <c r="E640" s="6" t="s">
         <v>789</v>
       </c>
-      <c r="F640" s="5" t="s">
+      <c r="F640" s="6" t="s">
         <v>507</v>
       </c>
-      <c r="G640" s="5" t="s">
+      <c r="G640" s="6" t="s">
         <v>1567</v>
       </c>
     </row>
     <row r="641" spans="1:7">
-      <c r="A641" s="5" t="s">
+      <c r="A641" s="6" t="s">
         <v>1852</v>
       </c>
-      <c r="B641" s="5" t="s">
+      <c r="B641" s="6" t="s">
         <v>1853</v>
       </c>
-      <c r="C641" s="5" t="s">
+      <c r="C641" s="6" t="s">
         <v>412</v>
       </c>
-      <c r="D641" s="5" t="s">
+      <c r="D641" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="E641" s="5" t="s">
+      <c r="E641" s="6" t="s">
         <v>789</v>
       </c>
-      <c r="F641" s="5" t="s">
+      <c r="F641" s="6" t="s">
         <v>507</v>
       </c>
-      <c r="G641" s="5" t="s">
+      <c r="G641" s="6" t="s">
         <v>1648</v>
       </c>
     </row>
     <row r="642" spans="1:7">
-      <c r="A642" s="5" t="s">
+      <c r="A642" s="6" t="s">
         <v>1854</v>
       </c>
-      <c r="B642" s="5" t="s">
+      <c r="B642" s="6" t="s">
         <v>1855</v>
       </c>
-      <c r="C642" s="5" t="s">
+      <c r="C642" s="6" t="s">
         <v>2290</v>
       </c>
-      <c r="D642" s="5"/>
-      <c r="E642" s="5" t="s">
+      <c r="D642" s="6"/>
+      <c r="E642" s="6" t="s">
         <v>506</v>
       </c>
-      <c r="F642" s="5" t="s">
+      <c r="F642" s="6" t="s">
         <v>507</v>
       </c>
-      <c r="G642" s="5" t="s">
+      <c r="G642" s="6" t="s">
         <v>1487</v>
       </c>
     </row>
     <row r="643" spans="1:7">
-      <c r="A643" s="5" t="s">
+      <c r="A643" s="6" t="s">
         <v>1856</v>
       </c>
-      <c r="B643" s="5" t="s">
+      <c r="B643" s="6" t="s">
         <v>1857</v>
       </c>
-      <c r="C643" s="5" t="s">
+      <c r="C643" s="6" t="s">
         <v>449</v>
       </c>
-      <c r="D643" s="5" t="s">
+      <c r="D643" s="6" t="s">
         <v>2290</v>
       </c>
-      <c r="E643" s="5" t="s">
+      <c r="E643" s="6" t="s">
         <v>506</v>
       </c>
-      <c r="F643" s="5" t="s">
+      <c r="F643" s="6" t="s">
         <v>507</v>
       </c>
-      <c r="G643" s="5" t="s">
+      <c r="G643" s="6" t="s">
         <v>1520</v>
       </c>
     </row>
     <row r="644" spans="1:7">
-      <c r="A644" s="5" t="s">
+      <c r="A644" s="6" t="s">
         <v>1858</v>
       </c>
-      <c r="B644" s="5" t="s">
+      <c r="B644" s="6" t="s">
         <v>1859</v>
       </c>
-      <c r="C644" s="5" t="s">
+      <c r="C644" s="6" t="s">
         <v>516</v>
       </c>
-      <c r="D644" s="5" t="s">
+      <c r="D644" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E644" s="5" t="s">
+      <c r="E644" s="6" t="s">
         <v>807</v>
       </c>
-      <c r="F644" s="5" t="s">
+      <c r="F644" s="6" t="s">
         <v>507</v>
       </c>
-      <c r="G644" s="5" t="s">
+      <c r="G644" s="6" t="s">
         <v>1809</v>
       </c>
     </row>
     <row r="645" spans="1:7">
-      <c r="A645" s="5" t="s">
+      <c r="A645" s="6" t="s">
         <v>1860</v>
       </c>
-      <c r="B645" s="5" t="s">
+      <c r="B645" s="6" t="s">
         <v>1861</v>
       </c>
-      <c r="C645" s="5" t="s">
+      <c r="C645" s="6" t="s">
         <v>516</v>
       </c>
-      <c r="D645" s="5" t="s">
+      <c r="D645" s="6" t="s">
         <v>449</v>
       </c>
-      <c r="E645" s="5" t="s">
+      <c r="E645" s="6" t="s">
         <v>807</v>
       </c>
-      <c r="F645" s="5" t="s">
+      <c r="F645" s="6" t="s">
         <v>507</v>
       </c>
-      <c r="G645" s="5" t="s">
+      <c r="G645" s="6" t="s">
         <v>1862</v>
       </c>
     </row>
     <row r="646" spans="1:7">
-      <c r="A646" s="5" t="s">
+      <c r="A646" s="6" t="s">
         <v>1863</v>
       </c>
-      <c r="B646" s="5" t="s">
+      <c r="B646" s="6" t="s">
         <v>1864</v>
       </c>
-      <c r="C646" s="5" t="s">
+      <c r="C646" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D646" s="5" t="s">
+      <c r="D646" s="6" t="s">
         <v>2290</v>
       </c>
-      <c r="E646" s="5" t="s">
+      <c r="E646" s="6" t="s">
         <v>524</v>
       </c>
-      <c r="F646" s="5" t="s">
+      <c r="F646" s="6" t="s">
         <v>507</v>
       </c>
-      <c r="G646" s="5" t="s">
+      <c r="G646" s="6" t="s">
         <v>1404</v>
       </c>
     </row>
     <row r="647" spans="1:7">
-      <c r="A647" s="5" t="s">
+      <c r="A647" s="6" t="s">
         <v>1865</v>
       </c>
-      <c r="B647" s="5" t="s">
+      <c r="B647" s="6" t="s">
         <v>1866</v>
       </c>
-      <c r="C647" s="5" t="s">
+      <c r="C647" s="6" t="s">
         <v>516</v>
       </c>
-      <c r="D647" s="5" t="s">
+      <c r="D647" s="6" t="s">
         <v>1117</v>
       </c>
-      <c r="E647" s="5" t="s">
+      <c r="E647" s="6" t="s">
         <v>1867</v>
       </c>
-      <c r="F647" s="5" t="s">
+      <c r="F647" s="6" t="s">
         <v>507</v>
       </c>
-      <c r="G647" s="5" t="s">
+      <c r="G647" s="6" t="s">
         <v>1868</v>
       </c>
     </row>
     <row r="648" spans="1:7">
-      <c r="A648" s="5" t="s">
+      <c r="A648" s="6" t="s">
         <v>1869</v>
       </c>
-      <c r="B648" s="5" t="s">
+      <c r="B648" s="6" t="s">
         <v>1870</v>
       </c>
-      <c r="C648" s="5" t="s">
+      <c r="C648" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D648" s="5" t="s">
+      <c r="D648" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="E648" s="5" t="s">
+      <c r="E648" s="6" t="s">
         <v>789</v>
       </c>
-      <c r="F648" s="5" t="s">
+      <c r="F648" s="6" t="s">
         <v>507</v>
       </c>
-      <c r="G648" s="5" t="s">
+      <c r="G648" s="6" t="s">
         <v>1871</v>
       </c>
     </row>
     <row r="649" spans="1:7">
-      <c r="A649" s="5" t="s">
+      <c r="A649" s="6" t="s">
         <v>1872</v>
       </c>
-      <c r="B649" s="5" t="s">
+      <c r="B649" s="6" t="s">
         <v>1873</v>
       </c>
-      <c r="C649" s="5" t="s">
+      <c r="C649" s="6" t="s">
         <v>389</v>
       </c>
-      <c r="D649" s="5" t="s">
+      <c r="D649" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="E649" s="5" t="s">
+      <c r="E649" s="6" t="s">
         <v>524</v>
       </c>
-      <c r="F649" s="5" t="s">
+      <c r="F649" s="6" t="s">
         <v>507</v>
       </c>
-      <c r="G649" s="5" t="s">
+      <c r="G649" s="6" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="650" spans="1:7">
-      <c r="A650" s="5" t="s">
+      <c r="A650" s="6" t="s">
         <v>1874</v>
       </c>
-      <c r="B650" s="5" t="s">
+      <c r="B650" s="6" t="s">
         <v>1875</v>
       </c>
-      <c r="C650" s="5" t="s">
+      <c r="C650" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D650" s="5" t="s">
+      <c r="D650" s="6" t="s">
         <v>1169</v>
       </c>
-      <c r="E650" s="5" t="s">
+      <c r="E650" s="6" t="s">
         <v>814</v>
       </c>
-      <c r="F650" s="5" t="s">
+      <c r="F650" s="6" t="s">
         <v>507</v>
       </c>
-      <c r="G650" s="5" t="s">
+      <c r="G650" s="6" t="s">
         <v>1876</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adicionado +20 Pokémon da 5ª geração
</commit_message>
<xml_diff>
--- a/pokemonv2/pokemons.xlsx
+++ b/pokemonv2/pokemons.xlsx
@@ -8729,8 +8729,8 @@
   <dimension ref="A1:H1026"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A492" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B497" sqref="B497"/>
+      <pane ySplit="1" topLeftCell="A513" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B522" sqref="B522"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19807,428 +19807,428 @@
       </c>
     </row>
     <row r="505" spans="1:7">
-      <c r="A505" s="6" t="s">
+      <c r="A505" s="5" t="s">
         <v>1506</v>
       </c>
-      <c r="B505" s="6" t="s">
+      <c r="B505" s="5" t="s">
         <v>1507</v>
       </c>
-      <c r="C505" s="6" t="s">
+      <c r="C505" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D505" s="6"/>
-      <c r="E505" s="6" t="s">
+      <c r="D505" s="5"/>
+      <c r="E505" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="F505" s="6" t="s">
+      <c r="F505" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G505" s="6" t="s">
+      <c r="G505" s="5" t="s">
         <v>1508</v>
       </c>
     </row>
     <row r="506" spans="1:7">
-      <c r="A506" s="6" t="s">
+      <c r="A506" s="5" t="s">
         <v>1509</v>
       </c>
-      <c r="B506" s="6" t="s">
+      <c r="B506" s="5" t="s">
         <v>1510</v>
       </c>
-      <c r="C506" s="6" t="s">
+      <c r="C506" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D506" s="6"/>
-      <c r="E506" s="6" t="s">
+      <c r="D506" s="5"/>
+      <c r="E506" s="5" t="s">
         <v>520</v>
       </c>
-      <c r="F506" s="6" t="s">
+      <c r="F506" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G506" s="6" t="s">
+      <c r="G506" s="5" t="s">
         <v>662</v>
       </c>
     </row>
     <row r="507" spans="1:7">
-      <c r="A507" s="6" t="s">
+      <c r="A507" s="5" t="s">
         <v>1511</v>
       </c>
-      <c r="B507" s="6" t="s">
+      <c r="B507" s="5" t="s">
         <v>1512</v>
       </c>
-      <c r="C507" s="6" t="s">
+      <c r="C507" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D507" s="6"/>
-      <c r="E507" s="6" t="s">
+      <c r="D507" s="5"/>
+      <c r="E507" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F507" s="6" t="s">
+      <c r="F507" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G507" s="6" t="s">
+      <c r="G507" s="5" t="s">
         <v>1513</v>
       </c>
     </row>
     <row r="508" spans="1:7">
-      <c r="A508" s="6" t="s">
+      <c r="A508" s="5" t="s">
         <v>1514</v>
       </c>
-      <c r="B508" s="6" t="s">
+      <c r="B508" s="5" t="s">
         <v>1515</v>
       </c>
-      <c r="C508" s="6" t="s">
+      <c r="C508" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D508" s="6"/>
-      <c r="E508" s="6" t="s">
+      <c r="D508" s="5"/>
+      <c r="E508" s="5" t="s">
         <v>1516</v>
       </c>
-      <c r="F508" s="6" t="s">
+      <c r="F508" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G508" s="6" t="s">
+      <c r="G508" s="5" t="s">
         <v>1517</v>
       </c>
     </row>
     <row r="509" spans="1:7">
-      <c r="A509" s="6" t="s">
+      <c r="A509" s="5" t="s">
         <v>1518</v>
       </c>
-      <c r="B509" s="6" t="s">
+      <c r="B509" s="5" t="s">
         <v>1519</v>
       </c>
-      <c r="C509" s="6" t="s">
+      <c r="C509" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D509" s="6"/>
-      <c r="E509" s="6" t="s">
+      <c r="D509" s="5"/>
+      <c r="E509" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="F509" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G509" s="6" t="s">
+      <c r="F509" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G509" s="5" t="s">
         <v>1520</v>
       </c>
     </row>
     <row r="510" spans="1:7">
-      <c r="A510" s="6" t="s">
+      <c r="A510" s="5" t="s">
         <v>1521</v>
       </c>
-      <c r="B510" s="6" t="s">
+      <c r="B510" s="5" t="s">
         <v>1522</v>
       </c>
-      <c r="C510" s="6" t="s">
+      <c r="C510" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="D510" s="6"/>
-      <c r="E510" s="6" t="s">
+      <c r="D510" s="5"/>
+      <c r="E510" s="5" t="s">
         <v>606</v>
       </c>
-      <c r="F510" s="6" t="s">
+      <c r="F510" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G510" s="6" t="s">
+      <c r="G510" s="5" t="s">
         <v>1523</v>
       </c>
     </row>
     <row r="511" spans="1:7">
-      <c r="A511" s="6" t="s">
+      <c r="A511" s="5" t="s">
         <v>1524</v>
       </c>
-      <c r="B511" s="6" t="s">
+      <c r="B511" s="5" t="s">
         <v>1525</v>
       </c>
-      <c r="C511" s="6" t="s">
+      <c r="C511" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="D511" s="6"/>
-      <c r="E511" s="6" t="s">
+      <c r="D511" s="5"/>
+      <c r="E511" s="5" t="s">
         <v>1526</v>
       </c>
-      <c r="F511" s="6" t="s">
+      <c r="F511" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="G511" s="6" t="s">
+      <c r="G511" s="5" t="s">
         <v>1527</v>
       </c>
     </row>
     <row r="512" spans="1:7">
-      <c r="A512" s="6" t="s">
+      <c r="A512" s="5" t="s">
         <v>1528</v>
       </c>
-      <c r="B512" s="6" t="s">
+      <c r="B512" s="5" t="s">
         <v>1529</v>
       </c>
-      <c r="C512" s="6" t="s">
+      <c r="C512" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="D512" s="6"/>
-      <c r="E512" s="6" t="s">
+      <c r="D512" s="5"/>
+      <c r="E512" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F512" s="6" t="s">
+      <c r="F512" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G512" s="6" t="s">
+      <c r="G512" s="5" t="s">
         <v>1530</v>
       </c>
     </row>
     <row r="513" spans="1:7">
-      <c r="A513" s="6" t="s">
+      <c r="A513" s="5" t="s">
         <v>1531</v>
       </c>
-      <c r="B513" s="6" t="s">
+      <c r="B513" s="5" t="s">
         <v>1532</v>
       </c>
-      <c r="C513" s="6" t="s">
+      <c r="C513" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="D513" s="6"/>
-      <c r="E513" s="6" t="s">
+      <c r="D513" s="5"/>
+      <c r="E513" s="5" t="s">
         <v>1300</v>
       </c>
-      <c r="F513" s="6" t="s">
+      <c r="F513" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G513" s="6" t="s">
+      <c r="G513" s="5" t="s">
         <v>1239</v>
       </c>
     </row>
     <row r="514" spans="1:7">
-      <c r="A514" s="6" t="s">
+      <c r="A514" s="5" t="s">
         <v>1533</v>
       </c>
-      <c r="B514" s="6" t="s">
+      <c r="B514" s="5" t="s">
         <v>1534</v>
       </c>
-      <c r="C514" s="6" t="s">
+      <c r="C514" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D514" s="6"/>
-      <c r="E514" s="6" t="s">
+      <c r="D514" s="5"/>
+      <c r="E514" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F514" s="6" t="s">
+      <c r="F514" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G514" s="6" t="s">
+      <c r="G514" s="5" t="s">
         <v>953</v>
       </c>
     </row>
     <row r="515" spans="1:7">
-      <c r="A515" s="6" t="s">
+      <c r="A515" s="5" t="s">
         <v>1535</v>
       </c>
-      <c r="B515" s="6" t="s">
+      <c r="B515" s="5" t="s">
         <v>1536</v>
       </c>
-      <c r="C515" s="6" t="s">
+      <c r="C515" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D515" s="6"/>
-      <c r="E515" s="6" t="s">
+      <c r="D515" s="5"/>
+      <c r="E515" s="5" t="s">
         <v>1300</v>
       </c>
-      <c r="F515" s="6" t="s">
+      <c r="F515" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G515" s="6" t="s">
+      <c r="G515" s="5" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="516" spans="1:7">
-      <c r="A516" s="6" t="s">
+      <c r="A516" s="5" t="s">
         <v>1537</v>
       </c>
-      <c r="B516" s="6" t="s">
+      <c r="B516" s="5" t="s">
         <v>1538</v>
       </c>
-      <c r="C516" s="6" t="s">
+      <c r="C516" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D516" s="6"/>
-      <c r="E516" s="6" t="s">
+      <c r="D516" s="5"/>
+      <c r="E516" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F516" s="6" t="s">
+      <c r="F516" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G516" s="6" t="s">
+      <c r="G516" s="5" t="s">
         <v>1539</v>
       </c>
     </row>
     <row r="517" spans="1:7">
-      <c r="A517" s="6" t="s">
+      <c r="A517" s="5" t="s">
         <v>1540</v>
       </c>
-      <c r="B517" s="6" t="s">
+      <c r="B517" s="5" t="s">
         <v>1541</v>
       </c>
-      <c r="C517" s="6" t="s">
+      <c r="C517" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D517" s="6"/>
-      <c r="E517" s="6" t="s">
+      <c r="D517" s="5"/>
+      <c r="E517" s="5" t="s">
         <v>1300</v>
       </c>
-      <c r="F517" s="6" t="s">
+      <c r="F517" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G517" s="6" t="s">
+      <c r="G517" s="5" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="518" spans="1:7">
-      <c r="A518" s="6" t="s">
+      <c r="A518" s="5" t="s">
         <v>1542</v>
       </c>
-      <c r="B518" s="6" t="s">
+      <c r="B518" s="5" t="s">
         <v>1543</v>
       </c>
-      <c r="C518" s="6" t="s">
+      <c r="C518" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="D518" s="6"/>
-      <c r="E518" s="6" t="s">
+      <c r="D518" s="5"/>
+      <c r="E518" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="F518" s="6" t="s">
+      <c r="F518" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G518" s="6" t="s">
+      <c r="G518" s="5" t="s">
         <v>1270</v>
       </c>
     </row>
     <row r="519" spans="1:7">
-      <c r="A519" s="6" t="s">
+      <c r="A519" s="5" t="s">
         <v>1544</v>
       </c>
-      <c r="B519" s="6" t="s">
+      <c r="B519" s="5" t="s">
         <v>1545</v>
       </c>
-      <c r="C519" s="6" t="s">
+      <c r="C519" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="D519" s="6"/>
-      <c r="E519" s="6" t="s">
+      <c r="D519" s="5"/>
+      <c r="E519" s="5" t="s">
         <v>404</v>
       </c>
-      <c r="F519" s="6" t="s">
+      <c r="F519" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G519" s="6" t="s">
+      <c r="G519" s="5" t="s">
         <v>1326</v>
       </c>
     </row>
     <row r="520" spans="1:7">
-      <c r="A520" s="6" t="s">
+      <c r="A520" s="5" t="s">
         <v>1546</v>
       </c>
-      <c r="B520" s="6" t="s">
+      <c r="B520" s="5" t="s">
         <v>1547</v>
       </c>
-      <c r="C520" s="6" t="s">
+      <c r="C520" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D520" s="6" t="s">
+      <c r="D520" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E520" s="6" t="s">
+      <c r="E520" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="F520" s="6" t="s">
+      <c r="F520" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G520" s="6" t="s">
+      <c r="G520" s="5" t="s">
         <v>666</v>
       </c>
     </row>
     <row r="521" spans="1:7">
-      <c r="A521" s="6" t="s">
+      <c r="A521" s="5" t="s">
         <v>1548</v>
       </c>
-      <c r="B521" s="6" t="s">
+      <c r="B521" s="5" t="s">
         <v>1549</v>
       </c>
-      <c r="C521" s="6" t="s">
+      <c r="C521" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D521" s="6" t="s">
+      <c r="D521" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E521" s="6" t="s">
+      <c r="E521" s="5" t="s">
         <v>1550</v>
       </c>
-      <c r="F521" s="6" t="s">
+      <c r="F521" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G521" s="6" t="s">
+      <c r="G521" s="5" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="522" spans="1:7">
-      <c r="A522" s="6" t="s">
+      <c r="A522" s="5" t="s">
         <v>1551</v>
       </c>
-      <c r="B522" s="6" t="s">
+      <c r="B522" s="5" t="s">
         <v>1552</v>
       </c>
-      <c r="C522" s="6" t="s">
+      <c r="C522" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D522" s="6" t="s">
+      <c r="D522" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E522" s="6" t="s">
+      <c r="E522" s="5" t="s">
         <v>1553</v>
       </c>
-      <c r="F522" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G522" s="6" t="s">
+      <c r="F522" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G522" s="5" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="523" spans="1:7">
-      <c r="A523" s="6" t="s">
+      <c r="A523" s="5" t="s">
         <v>1554</v>
       </c>
-      <c r="B523" s="6" t="s">
+      <c r="B523" s="5" t="s">
         <v>1555</v>
       </c>
-      <c r="C523" s="6" t="s">
+      <c r="C523" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="D523" s="6"/>
-      <c r="E523" s="6" t="s">
+      <c r="D523" s="5"/>
+      <c r="E523" s="5" t="s">
         <v>420</v>
       </c>
-      <c r="F523" s="6" t="s">
+      <c r="F523" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G523" s="6" t="s">
+      <c r="G523" s="5" t="s">
         <v>1556</v>
       </c>
     </row>
     <row r="524" spans="1:7">
-      <c r="A524" s="6" t="s">
+      <c r="A524" s="5" t="s">
         <v>1557</v>
       </c>
-      <c r="B524" s="6" t="s">
+      <c r="B524" s="5" t="s">
         <v>1558</v>
       </c>
-      <c r="C524" s="6" t="s">
+      <c r="C524" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="D524" s="6"/>
-      <c r="E524" s="6" t="s">
+      <c r="D524" s="5"/>
+      <c r="E524" s="5" t="s">
         <v>1300</v>
       </c>
-      <c r="F524" s="6" t="s">
+      <c r="F524" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G524" s="6" t="s">
+      <c r="G524" s="5" t="s">
         <v>546</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adicionado +30 Pokemon da 5ª geracao
</commit_message>
<xml_diff>
--- a/pokemonv2/pokemons.xlsx
+++ b/pokemonv2/pokemons.xlsx
@@ -8729,8 +8729,8 @@
   <dimension ref="A1:H1026"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A513" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B522" sqref="B522"/>
+      <pane ySplit="1" topLeftCell="A493" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E544" sqref="E544"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20233,664 +20233,664 @@
       </c>
     </row>
     <row r="525" spans="1:7">
-      <c r="A525" s="6" t="s">
+      <c r="A525" s="5" t="s">
         <v>1559</v>
       </c>
-      <c r="B525" s="6" t="s">
+      <c r="B525" s="5" t="s">
         <v>1560</v>
       </c>
-      <c r="C525" s="6" t="s">
+      <c r="C525" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="D525" s="6"/>
-      <c r="E525" s="6" t="s">
+      <c r="D525" s="5"/>
+      <c r="E525" s="5" t="s">
         <v>606</v>
       </c>
-      <c r="F525" s="6" t="s">
+      <c r="F525" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G525" s="6" t="s">
+      <c r="G525" s="5" t="s">
         <v>1561</v>
       </c>
     </row>
     <row r="526" spans="1:7">
-      <c r="A526" s="6" t="s">
+      <c r="A526" s="5" t="s">
         <v>1562</v>
       </c>
-      <c r="B526" s="6" t="s">
+      <c r="B526" s="5" t="s">
         <v>1563</v>
       </c>
-      <c r="C526" s="6" t="s">
+      <c r="C526" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="D526" s="6"/>
-      <c r="E526" s="6" t="s">
+      <c r="D526" s="5"/>
+      <c r="E526" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="F526" s="6" t="s">
+      <c r="F526" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G526" s="6" t="s">
+      <c r="G526" s="5" t="s">
         <v>1564</v>
       </c>
     </row>
     <row r="527" spans="1:7">
-      <c r="A527" s="6" t="s">
+      <c r="A527" s="5" t="s">
         <v>1565</v>
       </c>
-      <c r="B527" s="6" t="s">
+      <c r="B527" s="5" t="s">
         <v>1566</v>
       </c>
-      <c r="C527" s="6" t="s">
+      <c r="C527" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="D527" s="6"/>
-      <c r="E527" s="6" t="s">
+      <c r="D527" s="5"/>
+      <c r="E527" s="5" t="s">
         <v>1248</v>
       </c>
-      <c r="F527" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G527" s="6" t="s">
+      <c r="F527" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G527" s="5" t="s">
         <v>1567</v>
       </c>
     </row>
     <row r="528" spans="1:7">
-      <c r="A528" s="6" t="s">
+      <c r="A528" s="5" t="s">
         <v>1568</v>
       </c>
-      <c r="B528" s="6" t="s">
+      <c r="B528" s="5" t="s">
         <v>1569</v>
       </c>
-      <c r="C528" s="6" t="s">
+      <c r="C528" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="D528" s="6" t="s">
+      <c r="D528" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E528" s="6" t="s">
+      <c r="E528" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="F528" s="6" t="s">
+      <c r="F528" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G528" s="6" t="s">
+      <c r="G528" s="5" t="s">
         <v>666</v>
       </c>
     </row>
     <row r="529" spans="1:7">
-      <c r="A529" s="6" t="s">
+      <c r="A529" s="5" t="s">
         <v>1570</v>
       </c>
-      <c r="B529" s="6" t="s">
+      <c r="B529" s="5" t="s">
         <v>1571</v>
       </c>
-      <c r="C529" s="6" t="s">
+      <c r="C529" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="D529" s="6" t="s">
+      <c r="D529" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E529" s="6" t="s">
+      <c r="E529" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="F529" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G529" s="6" t="s">
+      <c r="F529" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G529" s="5" t="s">
         <v>1530</v>
       </c>
     </row>
     <row r="530" spans="1:7">
-      <c r="A530" s="6" t="s">
+      <c r="A530" s="5" t="s">
         <v>1572</v>
       </c>
-      <c r="B530" s="6" t="s">
+      <c r="B530" s="5" t="s">
         <v>1573</v>
       </c>
-      <c r="C530" s="6" t="s">
+      <c r="C530" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="D530" s="6"/>
-      <c r="E530" s="6" t="s">
+      <c r="D530" s="5"/>
+      <c r="E530" s="5" t="s">
         <v>351</v>
       </c>
-      <c r="F530" s="6" t="s">
+      <c r="F530" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G530" s="6" t="s">
+      <c r="G530" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="531" spans="1:7">
-      <c r="A531" s="6" t="s">
+      <c r="A531" s="5" t="s">
         <v>1574</v>
       </c>
-      <c r="B531" s="6" t="s">
+      <c r="B531" s="5" t="s">
         <v>1575</v>
       </c>
-      <c r="C531" s="6" t="s">
+      <c r="C531" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="D531" s="6" t="s">
+      <c r="D531" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="E531" s="6" t="s">
+      <c r="E531" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="F531" s="6" t="s">
+      <c r="F531" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="G531" s="6" t="s">
+      <c r="G531" s="5" t="s">
         <v>1576</v>
       </c>
     </row>
     <row r="532" spans="1:7">
-      <c r="A532" s="6" t="s">
+      <c r="A532" s="5" t="s">
         <v>1577</v>
       </c>
-      <c r="B532" s="6" t="s">
+      <c r="B532" s="5" t="s">
         <v>1578</v>
       </c>
-      <c r="C532" s="6" t="s">
+      <c r="C532" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D532" s="6"/>
-      <c r="E532" s="6" t="s">
+      <c r="D532" s="5"/>
+      <c r="E532" s="5" t="s">
         <v>1579</v>
       </c>
-      <c r="F532" s="6" t="s">
+      <c r="F532" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G532" s="6" t="s">
+      <c r="G532" s="5" t="s">
         <v>1580</v>
       </c>
     </row>
     <row r="533" spans="1:7">
-      <c r="A533" s="6" t="s">
+      <c r="A533" s="5" t="s">
         <v>1581</v>
       </c>
-      <c r="B533" s="6" t="s">
+      <c r="B533" s="5" t="s">
         <v>1582</v>
       </c>
-      <c r="C533" s="6" t="s">
+      <c r="C533" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="D533" s="6"/>
-      <c r="E533" s="6" t="s">
+      <c r="D533" s="5"/>
+      <c r="E533" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="F533" s="6" t="s">
+      <c r="F533" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="G533" s="6" t="s">
+      <c r="G533" s="5" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="534" spans="1:7">
-      <c r="A534" s="6" t="s">
+      <c r="A534" s="5" t="s">
         <v>1583</v>
       </c>
-      <c r="B534" s="6" t="s">
+      <c r="B534" s="5" t="s">
         <v>1584</v>
       </c>
-      <c r="C534" s="6" t="s">
+      <c r="C534" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="D534" s="6"/>
-      <c r="E534" s="6" t="s">
+      <c r="D534" s="5"/>
+      <c r="E534" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F534" s="6" t="s">
+      <c r="F534" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="G534" s="6" t="s">
+      <c r="G534" s="5" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="535" spans="1:7">
-      <c r="A535" s="6" t="s">
+      <c r="A535" s="5" t="s">
         <v>1585</v>
       </c>
-      <c r="B535" s="6" t="s">
+      <c r="B535" s="5" t="s">
         <v>1586</v>
       </c>
-      <c r="C535" s="6" t="s">
+      <c r="C535" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="D535" s="6"/>
-      <c r="E535" s="6" t="s">
+      <c r="D535" s="5"/>
+      <c r="E535" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="F535" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G535" s="6" t="s">
+      <c r="F535" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G535" s="5" t="s">
         <v>1587</v>
       </c>
     </row>
     <row r="536" spans="1:7">
-      <c r="A536" s="6" t="s">
+      <c r="A536" s="5" t="s">
         <v>1588</v>
       </c>
-      <c r="B536" s="6" t="s">
+      <c r="B536" s="5" t="s">
         <v>1589</v>
       </c>
-      <c r="C536" s="6" t="s">
+      <c r="C536" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D536" s="6"/>
-      <c r="E536" s="6" t="s">
+      <c r="D536" s="5"/>
+      <c r="E536" s="5" t="s">
         <v>420</v>
       </c>
-      <c r="F536" s="6" t="s">
+      <c r="F536" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G536" s="6" t="s">
+      <c r="G536" s="5" t="s">
         <v>905</v>
       </c>
     </row>
     <row r="537" spans="1:7">
-      <c r="A537" s="6" t="s">
+      <c r="A537" s="5" t="s">
         <v>1590</v>
       </c>
-      <c r="B537" s="6" t="s">
+      <c r="B537" s="5" t="s">
         <v>1591</v>
       </c>
-      <c r="C537" s="6" t="s">
+      <c r="C537" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D537" s="6" t="s">
+      <c r="D537" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="E537" s="6" t="s">
+      <c r="E537" s="5" t="s">
         <v>1232</v>
       </c>
-      <c r="F537" s="6" t="s">
+      <c r="F537" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G537" s="6" t="s">
+      <c r="G537" s="5" t="s">
         <v>1592</v>
       </c>
     </row>
     <row r="538" spans="1:7">
-      <c r="A538" s="6" t="s">
+      <c r="A538" s="5" t="s">
         <v>1593</v>
       </c>
-      <c r="B538" s="6" t="s">
+      <c r="B538" s="5" t="s">
         <v>1594</v>
       </c>
-      <c r="C538" s="6" t="s">
+      <c r="C538" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D538" s="6" t="s">
+      <c r="D538" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="E538" s="6" t="s">
+      <c r="E538" s="5" t="s">
         <v>1595</v>
       </c>
-      <c r="F538" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G538" s="6" t="s">
+      <c r="F538" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G538" s="5" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="539" spans="1:7">
-      <c r="A539" s="6" t="s">
+      <c r="A539" s="5" t="s">
         <v>1596</v>
       </c>
-      <c r="B539" s="6" t="s">
+      <c r="B539" s="5" t="s">
         <v>1597</v>
       </c>
-      <c r="C539" s="6" t="s">
+      <c r="C539" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="D539" s="6"/>
-      <c r="E539" s="6" t="s">
+      <c r="D539" s="5"/>
+      <c r="E539" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="F539" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G539" s="6" t="s">
+      <c r="F539" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G539" s="5" t="s">
         <v>1493</v>
       </c>
     </row>
     <row r="540" spans="1:7">
-      <c r="A540" s="6" t="s">
+      <c r="A540" s="5" t="s">
         <v>1598</v>
       </c>
-      <c r="B540" s="6" t="s">
+      <c r="B540" s="5" t="s">
         <v>1599</v>
       </c>
-      <c r="C540" s="6" t="s">
+      <c r="C540" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="D540" s="6"/>
-      <c r="E540" s="6" t="s">
+      <c r="D540" s="5"/>
+      <c r="E540" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="F540" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G540" s="6" t="s">
+      <c r="F540" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G540" s="5" t="s">
         <v>1600</v>
       </c>
     </row>
     <row r="541" spans="1:7">
-      <c r="A541" s="6" t="s">
+      <c r="A541" s="5" t="s">
         <v>1601</v>
       </c>
-      <c r="B541" s="6" t="s">
+      <c r="B541" s="5" t="s">
         <v>1602</v>
       </c>
-      <c r="C541" s="6" t="s">
+      <c r="C541" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D541" s="6" t="s">
+      <c r="D541" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="E541" s="6" t="s">
+      <c r="E541" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F541" s="6" t="s">
+      <c r="F541" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G541" s="6" t="s">
+      <c r="G541" s="5" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="542" spans="1:7">
-      <c r="A542" s="6" t="s">
+      <c r="A542" s="5" t="s">
         <v>1603</v>
       </c>
-      <c r="B542" s="6" t="s">
+      <c r="B542" s="5" t="s">
         <v>1604</v>
       </c>
-      <c r="C542" s="6" t="s">
+      <c r="C542" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D542" s="6" t="s">
+      <c r="D542" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="E542" s="6" t="s">
+      <c r="E542" s="5" t="s">
         <v>959</v>
       </c>
-      <c r="F542" s="6" t="s">
+      <c r="F542" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G542" s="6" t="s">
+      <c r="G542" s="5" t="s">
         <v>1605</v>
       </c>
     </row>
     <row r="543" spans="1:7">
-      <c r="A543" s="6" t="s">
+      <c r="A543" s="5" t="s">
         <v>1606</v>
       </c>
-      <c r="B543" s="6" t="s">
+      <c r="B543" s="5" t="s">
         <v>1607</v>
       </c>
-      <c r="C543" s="6" t="s">
+      <c r="C543" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D543" s="6" t="s">
+      <c r="D543" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="E543" s="6" t="s">
+      <c r="E543" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="F543" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G543" s="6" t="s">
+      <c r="F543" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G543" s="5" t="s">
         <v>712</v>
       </c>
     </row>
     <row r="544" spans="1:7">
-      <c r="A544" s="6" t="s">
+      <c r="A544" s="5" t="s">
         <v>1608</v>
       </c>
-      <c r="B544" s="6" t="s">
+      <c r="B544" s="5" t="s">
         <v>1609</v>
       </c>
-      <c r="C544" s="6" t="s">
+      <c r="C544" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D544" s="6" t="s">
+      <c r="D544" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="E544" s="6" t="s">
+      <c r="E544" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="F544" s="6" t="s">
+      <c r="F544" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G544" s="6" t="s">
+      <c r="G544" s="5" t="s">
         <v>1610</v>
       </c>
     </row>
     <row r="545" spans="1:7">
-      <c r="A545" s="6" t="s">
+      <c r="A545" s="5" t="s">
         <v>1611</v>
       </c>
-      <c r="B545" s="6" t="s">
+      <c r="B545" s="5" t="s">
         <v>1612</v>
       </c>
-      <c r="C545" s="6" t="s">
+      <c r="C545" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D545" s="6" t="s">
+      <c r="D545" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="E545" s="6" t="s">
+      <c r="E545" s="5" t="s">
         <v>933</v>
       </c>
-      <c r="F545" s="6" t="s">
+      <c r="F545" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G545" s="6" t="s">
+      <c r="G545" s="5" t="s">
         <v>1613</v>
       </c>
     </row>
     <row r="546" spans="1:7">
-      <c r="A546" s="6" t="s">
+      <c r="A546" s="5" t="s">
         <v>1614</v>
       </c>
-      <c r="B546" s="6" t="s">
+      <c r="B546" s="5" t="s">
         <v>1615</v>
       </c>
-      <c r="C546" s="6" t="s">
+      <c r="C546" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D546" s="6" t="s">
+      <c r="D546" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="E546" s="6" t="s">
+      <c r="E546" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="F546" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G546" s="6" t="s">
+      <c r="F546" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G546" s="5" t="s">
         <v>1616</v>
       </c>
     </row>
     <row r="547" spans="1:7">
-      <c r="A547" s="6" t="s">
+      <c r="A547" s="5" t="s">
         <v>1617</v>
       </c>
-      <c r="B547" s="6" t="s">
+      <c r="B547" s="5" t="s">
         <v>1618</v>
       </c>
-      <c r="C547" s="6" t="s">
+      <c r="C547" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="D547" s="6" t="s">
+      <c r="D547" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E547" s="6" t="s">
+      <c r="E547" s="5" t="s">
         <v>606</v>
       </c>
-      <c r="F547" s="6" t="s">
+      <c r="F547" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G547" s="6" t="s">
+      <c r="G547" s="5" t="s">
         <v>1318</v>
       </c>
     </row>
     <row r="548" spans="1:7">
-      <c r="A548" s="6" t="s">
+      <c r="A548" s="5" t="s">
         <v>1619</v>
       </c>
-      <c r="B548" s="6" t="s">
+      <c r="B548" s="5" t="s">
         <v>1620</v>
       </c>
-      <c r="C548" s="6" t="s">
+      <c r="C548" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="D548" s="6" t="s">
+      <c r="D548" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E548" s="6" t="s">
+      <c r="E548" s="5" t="s">
         <v>737</v>
       </c>
-      <c r="F548" s="6" t="s">
+      <c r="F548" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G548" s="6" t="s">
+      <c r="G548" s="5" t="s">
         <v>889</v>
       </c>
     </row>
     <row r="549" spans="1:7">
-      <c r="A549" s="6" t="s">
+      <c r="A549" s="5" t="s">
         <v>1621</v>
       </c>
-      <c r="B549" s="6" t="s">
+      <c r="B549" s="5" t="s">
         <v>1622</v>
       </c>
-      <c r="C549" s="6" t="s">
+      <c r="C549" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="D549" s="6"/>
-      <c r="E549" s="6" t="s">
+      <c r="D549" s="5"/>
+      <c r="E549" s="5" t="s">
         <v>606</v>
       </c>
-      <c r="F549" s="6" t="s">
+      <c r="F549" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G549" s="6" t="s">
+      <c r="G549" s="5" t="s">
         <v>889</v>
       </c>
     </row>
     <row r="550" spans="1:7">
-      <c r="A550" s="6" t="s">
+      <c r="A550" s="5" t="s">
         <v>1623</v>
       </c>
-      <c r="B550" s="6" t="s">
+      <c r="B550" s="5" t="s">
         <v>1624</v>
       </c>
-      <c r="C550" s="6" t="s">
+      <c r="C550" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="D550" s="6"/>
-      <c r="E550" s="6" t="s">
+      <c r="D550" s="5"/>
+      <c r="E550" s="5" t="s">
         <v>737</v>
       </c>
-      <c r="F550" s="6" t="s">
+      <c r="F550" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G550" s="6" t="s">
+      <c r="G550" s="5" t="s">
         <v>930</v>
       </c>
     </row>
     <row r="551" spans="1:7">
-      <c r="A551" s="6" t="s">
+      <c r="A551" s="5" t="s">
         <v>1625</v>
       </c>
-      <c r="B551" s="6" t="s">
+      <c r="B551" s="5" t="s">
         <v>1626</v>
       </c>
-      <c r="C551" s="6" t="s">
+      <c r="C551" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D551" s="6"/>
-      <c r="E551" s="6" t="s">
+      <c r="D551" s="5"/>
+      <c r="E551" s="5" t="s">
         <v>438</v>
       </c>
-      <c r="F551" s="6" t="s">
+      <c r="F551" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="G551" s="6" t="s">
+      <c r="G551" s="5" t="s">
         <v>1561</v>
       </c>
     </row>
     <row r="552" spans="1:7">
-      <c r="A552" s="6" t="s">
+      <c r="A552" s="5" t="s">
         <v>1627</v>
       </c>
-      <c r="B552" s="6" t="s">
+      <c r="B552" s="5" t="s">
         <v>1628</v>
       </c>
-      <c r="C552" s="6" t="s">
+      <c r="C552" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="D552" s="6" t="s">
+      <c r="D552" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="E552" s="6" t="s">
+      <c r="E552" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="F552" s="6" t="s">
+      <c r="F552" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="G552" s="6" t="s">
+      <c r="G552" s="5" t="s">
         <v>977</v>
       </c>
     </row>
     <row r="553" spans="1:7">
-      <c r="A553" s="6" t="s">
+      <c r="A553" s="5" t="s">
         <v>1629</v>
       </c>
-      <c r="B553" s="6" t="s">
+      <c r="B553" s="5" t="s">
         <v>1630</v>
       </c>
-      <c r="C553" s="6" t="s">
+      <c r="C553" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="D553" s="6" t="s">
+      <c r="D553" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="E553" s="6" t="s">
+      <c r="E553" s="5" t="s">
         <v>1631</v>
       </c>
-      <c r="F553" s="6" t="s">
+      <c r="F553" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="G553" s="6" t="s">
+      <c r="G553" s="5" t="s">
         <v>1632</v>
       </c>
     </row>
     <row r="554" spans="1:7">
-      <c r="A554" s="6" t="s">
+      <c r="A554" s="5" t="s">
         <v>1633</v>
       </c>
-      <c r="B554" s="6" t="s">
+      <c r="B554" s="5" t="s">
         <v>1634</v>
       </c>
-      <c r="C554" s="6" t="s">
+      <c r="C554" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="D554" s="6" t="s">
+      <c r="D554" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="E554" s="6" t="s">
+      <c r="E554" s="5" t="s">
         <v>1635</v>
       </c>
-      <c r="F554" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G554" s="6" t="s">
+      <c r="F554" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G554" s="5" t="s">
         <v>1636</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adicionado os ultimos 66 pokemon da 5ª geração
</commit_message>
<xml_diff>
--- a/pokemonv2/pokemons.xlsx
+++ b/pokemonv2/pokemons.xlsx
@@ -8385,7 +8385,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8729,18 +8729,18 @@
   <dimension ref="A1:H1026"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A549" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D565" sqref="D565"/>
+      <pane ySplit="1" topLeftCell="A599" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B609" sqref="B609"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.140625" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.140625" customWidth="1"/>
+    <col min="6" max="6" width="4.42578125" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">

</xml_diff>

<commit_message>
dados dos pokemon atualizados no banco de dados
</commit_message>
<xml_diff>
--- a/pokemonv2/pokemons.xlsx
+++ b/pokemonv2/pokemons.xlsx
@@ -8364,7 +8364,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -8374,18 +8374,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8417,7 +8405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -8425,13 +8413,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00B050"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -8729,8 +8724,8 @@
   <dimension ref="A1:H1026"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A599" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B609" sqref="B609"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19591,3426 +19586,3426 @@
       </c>
     </row>
     <row r="495" spans="1:7">
-      <c r="A495" s="5" t="s">
+      <c r="A495" s="2" t="s">
         <v>1477</v>
       </c>
-      <c r="B495" s="5" t="s">
+      <c r="B495" s="2" t="s">
         <v>1478</v>
       </c>
-      <c r="C495" s="5" t="s">
+      <c r="C495" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D495" s="5" t="s">
+      <c r="D495" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E495" s="5" t="s">
+      <c r="E495" s="2" t="s">
         <v>814</v>
       </c>
-      <c r="F495" s="5" t="s">
+      <c r="F495" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="G495" s="5" t="s">
+      <c r="G495" s="2" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="496" spans="1:7">
-      <c r="A496" s="5" t="s">
+      <c r="A496" s="2" t="s">
         <v>1479</v>
       </c>
-      <c r="B496" s="5" t="s">
+      <c r="B496" s="2" t="s">
         <v>1480</v>
       </c>
-      <c r="C496" s="5" t="s">
+      <c r="C496" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D496" s="5"/>
-      <c r="E496" s="5" t="s">
+      <c r="D496" s="2"/>
+      <c r="E496" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F496" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G496" s="5" t="s">
+      <c r="F496" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G496" s="2" t="s">
         <v>1481</v>
       </c>
     </row>
     <row r="497" spans="1:7">
-      <c r="A497" s="5" t="s">
+      <c r="A497" s="2" t="s">
         <v>1482</v>
       </c>
-      <c r="B497" s="5" t="s">
+      <c r="B497" s="2" t="s">
         <v>1483</v>
       </c>
-      <c r="C497" s="5" t="s">
+      <c r="C497" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D497" s="5"/>
-      <c r="E497" s="5" t="s">
+      <c r="D497" s="2"/>
+      <c r="E497" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F497" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G497" s="5" t="s">
+      <c r="F497" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G497" s="2" t="s">
         <v>741</v>
       </c>
     </row>
     <row r="498" spans="1:7">
-      <c r="A498" s="5" t="s">
+      <c r="A498" s="2" t="s">
         <v>1484</v>
       </c>
-      <c r="B498" s="5" t="s">
+      <c r="B498" s="2" t="s">
         <v>1485</v>
       </c>
-      <c r="C498" s="5" t="s">
+      <c r="C498" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D498" s="5"/>
-      <c r="E498" s="5" t="s">
+      <c r="D498" s="2"/>
+      <c r="E498" s="2" t="s">
         <v>1486</v>
       </c>
-      <c r="F498" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G498" s="5" t="s">
+      <c r="F498" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G498" s="2" t="s">
         <v>1487</v>
       </c>
     </row>
     <row r="499" spans="1:7">
-      <c r="A499" s="5" t="s">
+      <c r="A499" s="2" t="s">
         <v>1488</v>
       </c>
-      <c r="B499" s="5" t="s">
+      <c r="B499" s="2" t="s">
         <v>1489</v>
       </c>
-      <c r="C499" s="5" t="s">
+      <c r="C499" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D499" s="5"/>
-      <c r="E499" s="5" t="s">
+      <c r="D499" s="2"/>
+      <c r="E499" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F499" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G499" s="5" t="s">
+      <c r="F499" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G499" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="500" spans="1:7">
-      <c r="A500" s="5" t="s">
+      <c r="A500" s="2" t="s">
         <v>1490</v>
       </c>
-      <c r="B500" s="5" t="s">
+      <c r="B500" s="2" t="s">
         <v>1491</v>
       </c>
-      <c r="C500" s="5" t="s">
+      <c r="C500" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D500" s="5" t="s">
+      <c r="D500" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="E500" s="5" t="s">
+      <c r="E500" s="2" t="s">
         <v>1492</v>
       </c>
-      <c r="F500" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G500" s="5" t="s">
+      <c r="F500" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G500" s="2" t="s">
         <v>1493</v>
       </c>
     </row>
     <row r="501" spans="1:7">
-      <c r="A501" s="5" t="s">
+      <c r="A501" s="2" t="s">
         <v>1494</v>
       </c>
-      <c r="B501" s="5" t="s">
+      <c r="B501" s="2" t="s">
         <v>1495</v>
       </c>
-      <c r="C501" s="5" t="s">
+      <c r="C501" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D501" s="5" t="s">
+      <c r="D501" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="E501" s="5" t="s">
+      <c r="E501" s="2" t="s">
         <v>1486</v>
       </c>
-      <c r="F501" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G501" s="5" t="s">
+      <c r="F501" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G501" s="2" t="s">
         <v>1496</v>
       </c>
     </row>
     <row r="502" spans="1:7">
-      <c r="A502" s="5" t="s">
+      <c r="A502" s="2" t="s">
         <v>1497</v>
       </c>
-      <c r="B502" s="5" t="s">
+      <c r="B502" s="2" t="s">
         <v>1498</v>
       </c>
-      <c r="C502" s="5" t="s">
+      <c r="C502" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D502" s="5"/>
-      <c r="E502" s="5" t="s">
+      <c r="D502" s="2"/>
+      <c r="E502" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F502" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G502" s="5" t="s">
+      <c r="F502" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G502" s="2" t="s">
         <v>1499</v>
       </c>
     </row>
     <row r="503" spans="1:7">
-      <c r="A503" s="5" t="s">
+      <c r="A503" s="2" t="s">
         <v>1500</v>
       </c>
-      <c r="B503" s="5" t="s">
+      <c r="B503" s="2" t="s">
         <v>1501</v>
       </c>
-      <c r="C503" s="5" t="s">
+      <c r="C503" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D503" s="5"/>
-      <c r="E503" s="5" t="s">
+      <c r="D503" s="2"/>
+      <c r="E503" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F503" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G503" s="5" t="s">
+      <c r="F503" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G503" s="2" t="s">
         <v>481</v>
       </c>
     </row>
     <row r="504" spans="1:7">
-      <c r="A504" s="5" t="s">
+      <c r="A504" s="2" t="s">
         <v>1502</v>
       </c>
-      <c r="B504" s="5" t="s">
+      <c r="B504" s="2" t="s">
         <v>1503</v>
       </c>
-      <c r="C504" s="5" t="s">
+      <c r="C504" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D504" s="5"/>
-      <c r="E504" s="5" t="s">
+      <c r="D504" s="2"/>
+      <c r="E504" s="2" t="s">
         <v>1504</v>
       </c>
-      <c r="F504" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G504" s="5" t="s">
+      <c r="F504" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G504" s="2" t="s">
         <v>1505</v>
       </c>
     </row>
     <row r="505" spans="1:7">
-      <c r="A505" s="5" t="s">
+      <c r="A505" s="2" t="s">
         <v>1506</v>
       </c>
-      <c r="B505" s="5" t="s">
+      <c r="B505" s="2" t="s">
         <v>1507</v>
       </c>
-      <c r="C505" s="5" t="s">
+      <c r="C505" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D505" s="5"/>
-      <c r="E505" s="5" t="s">
+      <c r="D505" s="2"/>
+      <c r="E505" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F505" s="5" t="s">
+      <c r="F505" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G505" s="5" t="s">
+      <c r="G505" s="2" t="s">
         <v>1508</v>
       </c>
     </row>
     <row r="506" spans="1:7">
-      <c r="A506" s="5" t="s">
+      <c r="A506" s="2" t="s">
         <v>1509</v>
       </c>
-      <c r="B506" s="5" t="s">
+      <c r="B506" s="2" t="s">
         <v>1510</v>
       </c>
-      <c r="C506" s="5" t="s">
+      <c r="C506" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D506" s="5"/>
-      <c r="E506" s="5" t="s">
+      <c r="D506" s="2"/>
+      <c r="E506" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="F506" s="5" t="s">
+      <c r="F506" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G506" s="5" t="s">
+      <c r="G506" s="2" t="s">
         <v>662</v>
       </c>
     </row>
     <row r="507" spans="1:7">
-      <c r="A507" s="5" t="s">
+      <c r="A507" s="2" t="s">
         <v>1511</v>
       </c>
-      <c r="B507" s="5" t="s">
+      <c r="B507" s="2" t="s">
         <v>1512</v>
       </c>
-      <c r="C507" s="5" t="s">
+      <c r="C507" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D507" s="5"/>
-      <c r="E507" s="5" t="s">
+      <c r="D507" s="2"/>
+      <c r="E507" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F507" s="5" t="s">
+      <c r="F507" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G507" s="5" t="s">
+      <c r="G507" s="2" t="s">
         <v>1513</v>
       </c>
     </row>
     <row r="508" spans="1:7">
-      <c r="A508" s="5" t="s">
+      <c r="A508" s="2" t="s">
         <v>1514</v>
       </c>
-      <c r="B508" s="5" t="s">
+      <c r="B508" s="2" t="s">
         <v>1515</v>
       </c>
-      <c r="C508" s="5" t="s">
+      <c r="C508" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D508" s="5"/>
-      <c r="E508" s="5" t="s">
+      <c r="D508" s="2"/>
+      <c r="E508" s="2" t="s">
         <v>1516</v>
       </c>
-      <c r="F508" s="5" t="s">
+      <c r="F508" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G508" s="5" t="s">
+      <c r="G508" s="2" t="s">
         <v>1517</v>
       </c>
     </row>
     <row r="509" spans="1:7">
-      <c r="A509" s="5" t="s">
+      <c r="A509" s="2" t="s">
         <v>1518</v>
       </c>
-      <c r="B509" s="5" t="s">
+      <c r="B509" s="2" t="s">
         <v>1519</v>
       </c>
-      <c r="C509" s="5" t="s">
+      <c r="C509" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D509" s="5"/>
-      <c r="E509" s="5" t="s">
+      <c r="D509" s="2"/>
+      <c r="E509" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="F509" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G509" s="5" t="s">
+      <c r="F509" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G509" s="2" t="s">
         <v>1520</v>
       </c>
     </row>
     <row r="510" spans="1:7">
-      <c r="A510" s="5" t="s">
+      <c r="A510" s="2" t="s">
         <v>1521</v>
       </c>
-      <c r="B510" s="5" t="s">
+      <c r="B510" s="2" t="s">
         <v>1522</v>
       </c>
-      <c r="C510" s="5" t="s">
+      <c r="C510" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="D510" s="5"/>
-      <c r="E510" s="5" t="s">
+      <c r="D510" s="2"/>
+      <c r="E510" s="2" t="s">
         <v>606</v>
       </c>
-      <c r="F510" s="5" t="s">
+      <c r="F510" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G510" s="5" t="s">
+      <c r="G510" s="2" t="s">
         <v>1523</v>
       </c>
     </row>
     <row r="511" spans="1:7">
-      <c r="A511" s="5" t="s">
+      <c r="A511" s="2" t="s">
         <v>1524</v>
       </c>
-      <c r="B511" s="5" t="s">
+      <c r="B511" s="2" t="s">
         <v>1525</v>
       </c>
-      <c r="C511" s="5" t="s">
+      <c r="C511" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="D511" s="5"/>
-      <c r="E511" s="5" t="s">
+      <c r="D511" s="2"/>
+      <c r="E511" s="2" t="s">
         <v>1526</v>
       </c>
-      <c r="F511" s="5" t="s">
+      <c r="F511" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G511" s="5" t="s">
+      <c r="G511" s="2" t="s">
         <v>1527</v>
       </c>
     </row>
     <row r="512" spans="1:7">
-      <c r="A512" s="5" t="s">
+      <c r="A512" s="2" t="s">
         <v>1528</v>
       </c>
-      <c r="B512" s="5" t="s">
+      <c r="B512" s="2" t="s">
         <v>1529</v>
       </c>
-      <c r="C512" s="5" t="s">
+      <c r="C512" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D512" s="5"/>
-      <c r="E512" s="5" t="s">
+      <c r="D512" s="2"/>
+      <c r="E512" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F512" s="5" t="s">
+      <c r="F512" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G512" s="5" t="s">
+      <c r="G512" s="2" t="s">
         <v>1530</v>
       </c>
     </row>
     <row r="513" spans="1:7">
-      <c r="A513" s="5" t="s">
+      <c r="A513" s="2" t="s">
         <v>1531</v>
       </c>
-      <c r="B513" s="5" t="s">
+      <c r="B513" s="2" t="s">
         <v>1532</v>
       </c>
-      <c r="C513" s="5" t="s">
+      <c r="C513" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D513" s="5"/>
-      <c r="E513" s="5" t="s">
+      <c r="D513" s="2"/>
+      <c r="E513" s="2" t="s">
         <v>1300</v>
       </c>
-      <c r="F513" s="5" t="s">
+      <c r="F513" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G513" s="5" t="s">
+      <c r="G513" s="2" t="s">
         <v>1239</v>
       </c>
     </row>
     <row r="514" spans="1:7">
-      <c r="A514" s="5" t="s">
+      <c r="A514" s="2" t="s">
         <v>1533</v>
       </c>
-      <c r="B514" s="5" t="s">
+      <c r="B514" s="2" t="s">
         <v>1534</v>
       </c>
-      <c r="C514" s="5" t="s">
+      <c r="C514" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D514" s="5"/>
-      <c r="E514" s="5" t="s">
+      <c r="D514" s="2"/>
+      <c r="E514" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F514" s="5" t="s">
+      <c r="F514" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G514" s="5" t="s">
+      <c r="G514" s="2" t="s">
         <v>953</v>
       </c>
     </row>
     <row r="515" spans="1:7">
-      <c r="A515" s="5" t="s">
+      <c r="A515" s="2" t="s">
         <v>1535</v>
       </c>
-      <c r="B515" s="5" t="s">
+      <c r="B515" s="2" t="s">
         <v>1536</v>
       </c>
-      <c r="C515" s="5" t="s">
+      <c r="C515" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D515" s="5"/>
-      <c r="E515" s="5" t="s">
+      <c r="D515" s="2"/>
+      <c r="E515" s="2" t="s">
         <v>1300</v>
       </c>
-      <c r="F515" s="5" t="s">
+      <c r="F515" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G515" s="5" t="s">
+      <c r="G515" s="2" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="516" spans="1:7">
-      <c r="A516" s="5" t="s">
+      <c r="A516" s="2" t="s">
         <v>1537</v>
       </c>
-      <c r="B516" s="5" t="s">
+      <c r="B516" s="2" t="s">
         <v>1538</v>
       </c>
-      <c r="C516" s="5" t="s">
+      <c r="C516" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D516" s="5"/>
-      <c r="E516" s="5" t="s">
+      <c r="D516" s="2"/>
+      <c r="E516" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F516" s="5" t="s">
+      <c r="F516" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G516" s="5" t="s">
+      <c r="G516" s="2" t="s">
         <v>1539</v>
       </c>
     </row>
     <row r="517" spans="1:7">
-      <c r="A517" s="5" t="s">
+      <c r="A517" s="2" t="s">
         <v>1540</v>
       </c>
-      <c r="B517" s="5" t="s">
+      <c r="B517" s="2" t="s">
         <v>1541</v>
       </c>
-      <c r="C517" s="5" t="s">
+      <c r="C517" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D517" s="5"/>
-      <c r="E517" s="5" t="s">
+      <c r="D517" s="2"/>
+      <c r="E517" s="2" t="s">
         <v>1300</v>
       </c>
-      <c r="F517" s="5" t="s">
+      <c r="F517" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G517" s="5" t="s">
+      <c r="G517" s="2" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="518" spans="1:7">
-      <c r="A518" s="5" t="s">
+      <c r="A518" s="2" t="s">
         <v>1542</v>
       </c>
-      <c r="B518" s="5" t="s">
+      <c r="B518" s="2" t="s">
         <v>1543</v>
       </c>
-      <c r="C518" s="5" t="s">
+      <c r="C518" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D518" s="5"/>
-      <c r="E518" s="5" t="s">
+      <c r="D518" s="2"/>
+      <c r="E518" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F518" s="5" t="s">
+      <c r="F518" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G518" s="5" t="s">
+      <c r="G518" s="2" t="s">
         <v>1270</v>
       </c>
     </row>
     <row r="519" spans="1:7">
-      <c r="A519" s="5" t="s">
+      <c r="A519" s="2" t="s">
         <v>1544</v>
       </c>
-      <c r="B519" s="5" t="s">
+      <c r="B519" s="2" t="s">
         <v>1545</v>
       </c>
-      <c r="C519" s="5" t="s">
+      <c r="C519" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D519" s="5"/>
-      <c r="E519" s="5" t="s">
+      <c r="D519" s="2"/>
+      <c r="E519" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="F519" s="5" t="s">
+      <c r="F519" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G519" s="5" t="s">
+      <c r="G519" s="2" t="s">
         <v>1326</v>
       </c>
     </row>
     <row r="520" spans="1:7">
-      <c r="A520" s="5" t="s">
+      <c r="A520" s="2" t="s">
         <v>1546</v>
       </c>
-      <c r="B520" s="5" t="s">
+      <c r="B520" s="2" t="s">
         <v>1547</v>
       </c>
-      <c r="C520" s="5" t="s">
+      <c r="C520" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D520" s="5" t="s">
+      <c r="D520" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E520" s="5" t="s">
+      <c r="E520" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="F520" s="5" t="s">
+      <c r="F520" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G520" s="5" t="s">
+      <c r="G520" s="2" t="s">
         <v>666</v>
       </c>
     </row>
     <row r="521" spans="1:7">
-      <c r="A521" s="5" t="s">
+      <c r="A521" s="2" t="s">
         <v>1548</v>
       </c>
-      <c r="B521" s="5" t="s">
+      <c r="B521" s="2" t="s">
         <v>1549</v>
       </c>
-      <c r="C521" s="5" t="s">
+      <c r="C521" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D521" s="5" t="s">
+      <c r="D521" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E521" s="5" t="s">
+      <c r="E521" s="2" t="s">
         <v>1550</v>
       </c>
-      <c r="F521" s="5" t="s">
+      <c r="F521" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G521" s="5" t="s">
+      <c r="G521" s="2" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="522" spans="1:7">
-      <c r="A522" s="5" t="s">
+      <c r="A522" s="2" t="s">
         <v>1551</v>
       </c>
-      <c r="B522" s="5" t="s">
+      <c r="B522" s="2" t="s">
         <v>1552</v>
       </c>
-      <c r="C522" s="5" t="s">
+      <c r="C522" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D522" s="5" t="s">
+      <c r="D522" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E522" s="5" t="s">
+      <c r="E522" s="2" t="s">
         <v>1553</v>
       </c>
-      <c r="F522" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G522" s="5" t="s">
+      <c r="F522" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G522" s="2" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="523" spans="1:7">
-      <c r="A523" s="5" t="s">
+      <c r="A523" s="2" t="s">
         <v>1554</v>
       </c>
-      <c r="B523" s="5" t="s">
+      <c r="B523" s="2" t="s">
         <v>1555</v>
       </c>
-      <c r="C523" s="5" t="s">
+      <c r="C523" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="D523" s="5"/>
-      <c r="E523" s="5" t="s">
+      <c r="D523" s="2"/>
+      <c r="E523" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="F523" s="5" t="s">
+      <c r="F523" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G523" s="5" t="s">
+      <c r="G523" s="2" t="s">
         <v>1556</v>
       </c>
     </row>
     <row r="524" spans="1:7">
-      <c r="A524" s="5" t="s">
+      <c r="A524" s="2" t="s">
         <v>1557</v>
       </c>
-      <c r="B524" s="5" t="s">
+      <c r="B524" s="2" t="s">
         <v>1558</v>
       </c>
-      <c r="C524" s="5" t="s">
+      <c r="C524" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="D524" s="5"/>
-      <c r="E524" s="5" t="s">
+      <c r="D524" s="2"/>
+      <c r="E524" s="2" t="s">
         <v>1300</v>
       </c>
-      <c r="F524" s="5" t="s">
+      <c r="F524" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G524" s="5" t="s">
+      <c r="G524" s="2" t="s">
         <v>546</v>
       </c>
     </row>
     <row r="525" spans="1:7">
-      <c r="A525" s="5" t="s">
+      <c r="A525" s="2" t="s">
         <v>1559</v>
       </c>
-      <c r="B525" s="5" t="s">
+      <c r="B525" s="2" t="s">
         <v>1560</v>
       </c>
-      <c r="C525" s="5" t="s">
+      <c r="C525" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="D525" s="5"/>
-      <c r="E525" s="5" t="s">
+      <c r="D525" s="2"/>
+      <c r="E525" s="2" t="s">
         <v>606</v>
       </c>
-      <c r="F525" s="5" t="s">
+      <c r="F525" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G525" s="5" t="s">
+      <c r="G525" s="2" t="s">
         <v>1561</v>
       </c>
     </row>
     <row r="526" spans="1:7">
-      <c r="A526" s="5" t="s">
+      <c r="A526" s="2" t="s">
         <v>1562</v>
       </c>
-      <c r="B526" s="5" t="s">
+      <c r="B526" s="2" t="s">
         <v>1563</v>
       </c>
-      <c r="C526" s="5" t="s">
+      <c r="C526" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="D526" s="5"/>
-      <c r="E526" s="5" t="s">
+      <c r="D526" s="2"/>
+      <c r="E526" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="F526" s="5" t="s">
+      <c r="F526" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G526" s="5" t="s">
+      <c r="G526" s="2" t="s">
         <v>1564</v>
       </c>
     </row>
     <row r="527" spans="1:7">
-      <c r="A527" s="5" t="s">
+      <c r="A527" s="2" t="s">
         <v>1565</v>
       </c>
-      <c r="B527" s="5" t="s">
+      <c r="B527" s="2" t="s">
         <v>1566</v>
       </c>
-      <c r="C527" s="5" t="s">
+      <c r="C527" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="D527" s="5"/>
-      <c r="E527" s="5" t="s">
+      <c r="D527" s="2"/>
+      <c r="E527" s="2" t="s">
         <v>1248</v>
       </c>
-      <c r="F527" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G527" s="5" t="s">
+      <c r="F527" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G527" s="2" t="s">
         <v>1567</v>
       </c>
     </row>
     <row r="528" spans="1:7">
-      <c r="A528" s="5" t="s">
+      <c r="A528" s="2" t="s">
         <v>1568</v>
       </c>
-      <c r="B528" s="5" t="s">
+      <c r="B528" s="2" t="s">
         <v>1569</v>
       </c>
-      <c r="C528" s="5" t="s">
+      <c r="C528" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D528" s="5" t="s">
+      <c r="D528" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E528" s="5" t="s">
+      <c r="E528" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="F528" s="5" t="s">
+      <c r="F528" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G528" s="5" t="s">
+      <c r="G528" s="2" t="s">
         <v>666</v>
       </c>
     </row>
     <row r="529" spans="1:7">
-      <c r="A529" s="5" t="s">
+      <c r="A529" s="2" t="s">
         <v>1570</v>
       </c>
-      <c r="B529" s="5" t="s">
+      <c r="B529" s="2" t="s">
         <v>1571</v>
       </c>
-      <c r="C529" s="5" t="s">
+      <c r="C529" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D529" s="5" t="s">
+      <c r="D529" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E529" s="5" t="s">
+      <c r="E529" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="F529" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G529" s="5" t="s">
+      <c r="F529" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G529" s="2" t="s">
         <v>1530</v>
       </c>
     </row>
     <row r="530" spans="1:7">
-      <c r="A530" s="5" t="s">
+      <c r="A530" s="2" t="s">
         <v>1572</v>
       </c>
-      <c r="B530" s="5" t="s">
+      <c r="B530" s="2" t="s">
         <v>1573</v>
       </c>
-      <c r="C530" s="5" t="s">
+      <c r="C530" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="D530" s="5"/>
-      <c r="E530" s="5" t="s">
+      <c r="D530" s="2"/>
+      <c r="E530" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="F530" s="5" t="s">
+      <c r="F530" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G530" s="5" t="s">
+      <c r="G530" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="531" spans="1:7">
-      <c r="A531" s="5" t="s">
+      <c r="A531" s="2" t="s">
         <v>1574</v>
       </c>
-      <c r="B531" s="5" t="s">
+      <c r="B531" s="2" t="s">
         <v>1575</v>
       </c>
-      <c r="C531" s="5" t="s">
+      <c r="C531" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="D531" s="5" t="s">
+      <c r="D531" s="2" t="s">
         <v>1169</v>
       </c>
-      <c r="E531" s="5" t="s">
+      <c r="E531" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F531" s="5" t="s">
+      <c r="F531" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="G531" s="5" t="s">
+      <c r="G531" s="2" t="s">
         <v>1576</v>
       </c>
     </row>
     <row r="532" spans="1:7">
-      <c r="A532" s="5" t="s">
+      <c r="A532" s="2" t="s">
         <v>1577</v>
       </c>
-      <c r="B532" s="5" t="s">
+      <c r="B532" s="2" t="s">
         <v>1578</v>
       </c>
-      <c r="C532" s="5" t="s">
+      <c r="C532" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D532" s="5"/>
-      <c r="E532" s="5" t="s">
+      <c r="D532" s="2"/>
+      <c r="E532" s="2" t="s">
         <v>1579</v>
       </c>
-      <c r="F532" s="5" t="s">
+      <c r="F532" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G532" s="5" t="s">
+      <c r="G532" s="2" t="s">
         <v>1580</v>
       </c>
     </row>
     <row r="533" spans="1:7">
-      <c r="A533" s="5" t="s">
+      <c r="A533" s="2" t="s">
         <v>1581</v>
       </c>
-      <c r="B533" s="5" t="s">
+      <c r="B533" s="2" t="s">
         <v>1582</v>
       </c>
-      <c r="C533" s="5" t="s">
+      <c r="C533" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="D533" s="5"/>
-      <c r="E533" s="5" t="s">
+      <c r="D533" s="2"/>
+      <c r="E533" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="F533" s="5" t="s">
+      <c r="F533" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="G533" s="5" t="s">
+      <c r="G533" s="2" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="534" spans="1:7">
-      <c r="A534" s="5" t="s">
+      <c r="A534" s="2" t="s">
         <v>1583</v>
       </c>
-      <c r="B534" s="5" t="s">
+      <c r="B534" s="2" t="s">
         <v>1584</v>
       </c>
-      <c r="C534" s="5" t="s">
+      <c r="C534" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="D534" s="5"/>
-      <c r="E534" s="5" t="s">
+      <c r="D534" s="2"/>
+      <c r="E534" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F534" s="5" t="s">
+      <c r="F534" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G534" s="5" t="s">
+      <c r="G534" s="2" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="535" spans="1:7">
-      <c r="A535" s="5" t="s">
+      <c r="A535" s="2" t="s">
         <v>1585</v>
       </c>
-      <c r="B535" s="5" t="s">
+      <c r="B535" s="2" t="s">
         <v>1586</v>
       </c>
-      <c r="C535" s="5" t="s">
+      <c r="C535" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="D535" s="5"/>
-      <c r="E535" s="5" t="s">
+      <c r="D535" s="2"/>
+      <c r="E535" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F535" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G535" s="5" t="s">
+      <c r="F535" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G535" s="2" t="s">
         <v>1587</v>
       </c>
     </row>
     <row r="536" spans="1:7">
-      <c r="A536" s="5" t="s">
+      <c r="A536" s="2" t="s">
         <v>1588</v>
       </c>
-      <c r="B536" s="5" t="s">
+      <c r="B536" s="2" t="s">
         <v>1589</v>
       </c>
-      <c r="C536" s="5" t="s">
+      <c r="C536" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D536" s="5"/>
-      <c r="E536" s="5" t="s">
+      <c r="D536" s="2"/>
+      <c r="E536" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="F536" s="5" t="s">
+      <c r="F536" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G536" s="5" t="s">
+      <c r="G536" s="2" t="s">
         <v>905</v>
       </c>
     </row>
     <row r="537" spans="1:7">
-      <c r="A537" s="5" t="s">
+      <c r="A537" s="2" t="s">
         <v>1590</v>
       </c>
-      <c r="B537" s="5" t="s">
+      <c r="B537" s="2" t="s">
         <v>1591</v>
       </c>
-      <c r="C537" s="5" t="s">
+      <c r="C537" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D537" s="5" t="s">
+      <c r="D537" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="E537" s="5" t="s">
+      <c r="E537" s="2" t="s">
         <v>1232</v>
       </c>
-      <c r="F537" s="5" t="s">
+      <c r="F537" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G537" s="5" t="s">
+      <c r="G537" s="2" t="s">
         <v>1592</v>
       </c>
     </row>
     <row r="538" spans="1:7">
-      <c r="A538" s="5" t="s">
+      <c r="A538" s="2" t="s">
         <v>1593</v>
       </c>
-      <c r="B538" s="5" t="s">
+      <c r="B538" s="2" t="s">
         <v>1594</v>
       </c>
-      <c r="C538" s="5" t="s">
+      <c r="C538" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D538" s="5" t="s">
+      <c r="D538" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="E538" s="5" t="s">
+      <c r="E538" s="2" t="s">
         <v>1595</v>
       </c>
-      <c r="F538" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G538" s="5" t="s">
+      <c r="F538" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G538" s="2" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="539" spans="1:7">
-      <c r="A539" s="5" t="s">
+      <c r="A539" s="2" t="s">
         <v>1596</v>
       </c>
-      <c r="B539" s="5" t="s">
+      <c r="B539" s="2" t="s">
         <v>1597</v>
       </c>
-      <c r="C539" s="5" t="s">
+      <c r="C539" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="D539" s="5"/>
-      <c r="E539" s="5" t="s">
+      <c r="D539" s="2"/>
+      <c r="E539" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="F539" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G539" s="5" t="s">
+      <c r="F539" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G539" s="2" t="s">
         <v>1493</v>
       </c>
     </row>
     <row r="540" spans="1:7">
-      <c r="A540" s="5" t="s">
+      <c r="A540" s="2" t="s">
         <v>1598</v>
       </c>
-      <c r="B540" s="5" t="s">
+      <c r="B540" s="2" t="s">
         <v>1599</v>
       </c>
-      <c r="C540" s="5" t="s">
+      <c r="C540" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="D540" s="5"/>
-      <c r="E540" s="5" t="s">
+      <c r="D540" s="2"/>
+      <c r="E540" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="F540" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G540" s="5" t="s">
+      <c r="F540" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G540" s="2" t="s">
         <v>1600</v>
       </c>
     </row>
     <row r="541" spans="1:7">
-      <c r="A541" s="5" t="s">
+      <c r="A541" s="2" t="s">
         <v>1601</v>
       </c>
-      <c r="B541" s="5" t="s">
+      <c r="B541" s="2" t="s">
         <v>1602</v>
       </c>
-      <c r="C541" s="5" t="s">
+      <c r="C541" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D541" s="5" t="s">
+      <c r="D541" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="E541" s="5" t="s">
+      <c r="E541" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F541" s="5" t="s">
+      <c r="F541" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G541" s="5" t="s">
+      <c r="G541" s="2" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="542" spans="1:7">
-      <c r="A542" s="5" t="s">
+      <c r="A542" s="2" t="s">
         <v>1603</v>
       </c>
-      <c r="B542" s="5" t="s">
+      <c r="B542" s="2" t="s">
         <v>1604</v>
       </c>
-      <c r="C542" s="5" t="s">
+      <c r="C542" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D542" s="5" t="s">
+      <c r="D542" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="E542" s="5" t="s">
+      <c r="E542" s="2" t="s">
         <v>959</v>
       </c>
-      <c r="F542" s="5" t="s">
+      <c r="F542" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G542" s="5" t="s">
+      <c r="G542" s="2" t="s">
         <v>1605</v>
       </c>
     </row>
     <row r="543" spans="1:7">
-      <c r="A543" s="5" t="s">
+      <c r="A543" s="2" t="s">
         <v>1606</v>
       </c>
-      <c r="B543" s="5" t="s">
+      <c r="B543" s="2" t="s">
         <v>1607</v>
       </c>
-      <c r="C543" s="5" t="s">
+      <c r="C543" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D543" s="5" t="s">
+      <c r="D543" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="E543" s="5" t="s">
+      <c r="E543" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="F543" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G543" s="5" t="s">
+      <c r="F543" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G543" s="2" t="s">
         <v>712</v>
       </c>
     </row>
     <row r="544" spans="1:7">
-      <c r="A544" s="5" t="s">
+      <c r="A544" s="2" t="s">
         <v>1608</v>
       </c>
-      <c r="B544" s="5" t="s">
+      <c r="B544" s="2" t="s">
         <v>1609</v>
       </c>
-      <c r="C544" s="5" t="s">
+      <c r="C544" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D544" s="5" t="s">
+      <c r="D544" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E544" s="5" t="s">
+      <c r="E544" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F544" s="5" t="s">
+      <c r="F544" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G544" s="5" t="s">
+      <c r="G544" s="2" t="s">
         <v>1610</v>
       </c>
     </row>
     <row r="545" spans="1:7">
-      <c r="A545" s="5" t="s">
+      <c r="A545" s="2" t="s">
         <v>1611</v>
       </c>
-      <c r="B545" s="5" t="s">
+      <c r="B545" s="2" t="s">
         <v>1612</v>
       </c>
-      <c r="C545" s="5" t="s">
+      <c r="C545" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D545" s="5" t="s">
+      <c r="D545" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E545" s="5" t="s">
+      <c r="E545" s="2" t="s">
         <v>933</v>
       </c>
-      <c r="F545" s="5" t="s">
+      <c r="F545" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G545" s="5" t="s">
+      <c r="G545" s="2" t="s">
         <v>1613</v>
       </c>
     </row>
     <row r="546" spans="1:7">
-      <c r="A546" s="5" t="s">
+      <c r="A546" s="2" t="s">
         <v>1614</v>
       </c>
-      <c r="B546" s="5" t="s">
+      <c r="B546" s="2" t="s">
         <v>1615</v>
       </c>
-      <c r="C546" s="5" t="s">
+      <c r="C546" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D546" s="5" t="s">
+      <c r="D546" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E546" s="5" t="s">
+      <c r="E546" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="F546" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G546" s="5" t="s">
+      <c r="F546" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G546" s="2" t="s">
         <v>1616</v>
       </c>
     </row>
     <row r="547" spans="1:7">
-      <c r="A547" s="5" t="s">
+      <c r="A547" s="2" t="s">
         <v>1617</v>
       </c>
-      <c r="B547" s="5" t="s">
+      <c r="B547" s="2" t="s">
         <v>1618</v>
       </c>
-      <c r="C547" s="5" t="s">
+      <c r="C547" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D547" s="5" t="s">
+      <c r="D547" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E547" s="5" t="s">
+      <c r="E547" s="2" t="s">
         <v>606</v>
       </c>
-      <c r="F547" s="5" t="s">
+      <c r="F547" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G547" s="5" t="s">
+      <c r="G547" s="2" t="s">
         <v>1318</v>
       </c>
     </row>
     <row r="548" spans="1:7">
-      <c r="A548" s="5" t="s">
+      <c r="A548" s="2" t="s">
         <v>1619</v>
       </c>
-      <c r="B548" s="5" t="s">
+      <c r="B548" s="2" t="s">
         <v>1620</v>
       </c>
-      <c r="C548" s="5" t="s">
+      <c r="C548" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D548" s="5" t="s">
+      <c r="D548" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E548" s="5" t="s">
+      <c r="E548" s="2" t="s">
         <v>737</v>
       </c>
-      <c r="F548" s="5" t="s">
+      <c r="F548" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G548" s="5" t="s">
+      <c r="G548" s="2" t="s">
         <v>889</v>
       </c>
     </row>
     <row r="549" spans="1:7">
-      <c r="A549" s="5" t="s">
+      <c r="A549" s="2" t="s">
         <v>1621</v>
       </c>
-      <c r="B549" s="5" t="s">
+      <c r="B549" s="2" t="s">
         <v>1622</v>
       </c>
-      <c r="C549" s="5" t="s">
+      <c r="C549" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D549" s="5"/>
-      <c r="E549" s="5" t="s">
+      <c r="D549" s="2"/>
+      <c r="E549" s="2" t="s">
         <v>606</v>
       </c>
-      <c r="F549" s="5" t="s">
+      <c r="F549" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G549" s="5" t="s">
+      <c r="G549" s="2" t="s">
         <v>889</v>
       </c>
     </row>
     <row r="550" spans="1:7">
-      <c r="A550" s="5" t="s">
+      <c r="A550" s="2" t="s">
         <v>1623</v>
       </c>
-      <c r="B550" s="5" t="s">
+      <c r="B550" s="2" t="s">
         <v>1624</v>
       </c>
-      <c r="C550" s="5" t="s">
+      <c r="C550" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D550" s="5"/>
-      <c r="E550" s="5" t="s">
+      <c r="D550" s="2"/>
+      <c r="E550" s="2" t="s">
         <v>737</v>
       </c>
-      <c r="F550" s="5" t="s">
+      <c r="F550" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G550" s="5" t="s">
+      <c r="G550" s="2" t="s">
         <v>930</v>
       </c>
     </row>
     <row r="551" spans="1:7">
-      <c r="A551" s="5" t="s">
+      <c r="A551" s="2" t="s">
         <v>1625</v>
       </c>
-      <c r="B551" s="5" t="s">
+      <c r="B551" s="2" t="s">
         <v>1626</v>
       </c>
-      <c r="C551" s="5" t="s">
+      <c r="C551" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D551" s="5"/>
-      <c r="E551" s="5" t="s">
+      <c r="D551" s="2"/>
+      <c r="E551" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="F551" s="5" t="s">
+      <c r="F551" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="G551" s="5" t="s">
+      <c r="G551" s="2" t="s">
         <v>1561</v>
       </c>
     </row>
     <row r="552" spans="1:7">
-      <c r="A552" s="5" t="s">
+      <c r="A552" s="2" t="s">
         <v>1627</v>
       </c>
-      <c r="B552" s="5" t="s">
+      <c r="B552" s="2" t="s">
         <v>1628</v>
       </c>
-      <c r="C552" s="5" t="s">
+      <c r="C552" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="D552" s="5" t="s">
+      <c r="D552" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="E552" s="5" t="s">
+      <c r="E552" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F552" s="5" t="s">
+      <c r="F552" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="G552" s="5" t="s">
+      <c r="G552" s="2" t="s">
         <v>977</v>
       </c>
     </row>
     <row r="553" spans="1:7">
-      <c r="A553" s="5" t="s">
+      <c r="A553" s="2" t="s">
         <v>1629</v>
       </c>
-      <c r="B553" s="5" t="s">
+      <c r="B553" s="2" t="s">
         <v>1630</v>
       </c>
-      <c r="C553" s="5" t="s">
+      <c r="C553" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="D553" s="5" t="s">
+      <c r="D553" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="E553" s="5" t="s">
+      <c r="E553" s="2" t="s">
         <v>1631</v>
       </c>
-      <c r="F553" s="5" t="s">
+      <c r="F553" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G553" s="5" t="s">
+      <c r="G553" s="2" t="s">
         <v>1632</v>
       </c>
     </row>
     <row r="554" spans="1:7">
-      <c r="A554" s="5" t="s">
+      <c r="A554" s="2" t="s">
         <v>1633</v>
       </c>
-      <c r="B554" s="5" t="s">
+      <c r="B554" s="2" t="s">
         <v>1634</v>
       </c>
-      <c r="C554" s="5" t="s">
+      <c r="C554" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="D554" s="5" t="s">
+      <c r="D554" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="E554" s="5" t="s">
+      <c r="E554" s="2" t="s">
         <v>1635</v>
       </c>
-      <c r="F554" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G554" s="5" t="s">
+      <c r="F554" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G554" s="2" t="s">
         <v>1636</v>
       </c>
     </row>
     <row r="555" spans="1:7">
-      <c r="A555" s="5" t="s">
+      <c r="A555" s="2" t="s">
         <v>1637</v>
       </c>
-      <c r="B555" s="5" t="s">
+      <c r="B555" s="2" t="s">
         <v>1638</v>
       </c>
-      <c r="C555" s="5" t="s">
+      <c r="C555" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D555" s="5"/>
-      <c r="E555" s="5" t="s">
+      <c r="D555" s="2"/>
+      <c r="E555" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F555" s="5" t="s">
+      <c r="F555" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G555" s="5" t="s">
+      <c r="G555" s="2" t="s">
         <v>1527</v>
       </c>
     </row>
     <row r="556" spans="1:7">
-      <c r="A556" s="5" t="s">
+      <c r="A556" s="2" t="s">
         <v>1639</v>
       </c>
-      <c r="B556" s="5" t="s">
+      <c r="B556" s="2" t="s">
         <v>1640</v>
       </c>
-      <c r="C556" s="5" t="s">
+      <c r="C556" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D556" s="5"/>
-      <c r="E556" s="5" t="s">
+      <c r="D556" s="2"/>
+      <c r="E556" s="2" t="s">
         <v>737</v>
       </c>
-      <c r="F556" s="5" t="s">
+      <c r="F556" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="G556" s="5" t="s">
+      <c r="G556" s="2" t="s">
         <v>1641</v>
       </c>
     </row>
     <row r="557" spans="1:7">
-      <c r="A557" s="5" t="s">
+      <c r="A557" s="2" t="s">
         <v>1642</v>
       </c>
-      <c r="B557" s="5" t="s">
+      <c r="B557" s="2" t="s">
         <v>1643</v>
       </c>
-      <c r="C557" s="5" t="s">
+      <c r="C557" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D557" s="5"/>
-      <c r="E557" s="5" t="s">
+      <c r="D557" s="2"/>
+      <c r="E557" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="F557" s="5" t="s">
+      <c r="F557" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G557" s="5" t="s">
+      <c r="G557" s="2" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="558" spans="1:7">
-      <c r="A558" s="5" t="s">
+      <c r="A558" s="2" t="s">
         <v>1644</v>
       </c>
-      <c r="B558" s="5" t="s">
+      <c r="B558" s="2" t="s">
         <v>1645</v>
       </c>
-      <c r="C558" s="5" t="s">
+      <c r="C558" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D558" s="5" t="s">
+      <c r="D558" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="E558" s="5" t="s">
+      <c r="E558" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="F558" s="5" t="s">
+      <c r="F558" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G558" s="5" t="s">
+      <c r="G558" s="2" t="s">
         <v>1249</v>
       </c>
     </row>
     <row r="559" spans="1:7">
-      <c r="A559" s="5" t="s">
+      <c r="A559" s="2" t="s">
         <v>1646</v>
       </c>
-      <c r="B559" s="5" t="s">
+      <c r="B559" s="2" t="s">
         <v>1647</v>
       </c>
-      <c r="C559" s="5" t="s">
+      <c r="C559" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D559" s="5" t="s">
+      <c r="D559" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="E559" s="5" t="s">
+      <c r="E559" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="F559" s="5" t="s">
+      <c r="F559" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G559" s="5" t="s">
+      <c r="G559" s="2" t="s">
         <v>1648</v>
       </c>
     </row>
     <row r="560" spans="1:7">
-      <c r="A560" s="5" t="s">
+      <c r="A560" s="2" t="s">
         <v>1649</v>
       </c>
-      <c r="B560" s="5" t="s">
+      <c r="B560" s="2" t="s">
         <v>1650</v>
       </c>
-      <c r="C560" s="5" t="s">
+      <c r="C560" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="D560" s="5" t="s">
+      <c r="D560" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="E560" s="5" t="s">
+      <c r="E560" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="F560" s="5" t="s">
+      <c r="F560" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="G560" s="5" t="s">
+      <c r="G560" s="2" t="s">
         <v>1651</v>
       </c>
     </row>
     <row r="561" spans="1:7">
-      <c r="A561" s="5" t="s">
+      <c r="A561" s="2" t="s">
         <v>1652</v>
       </c>
-      <c r="B561" s="5" t="s">
+      <c r="B561" s="2" t="s">
         <v>1653</v>
       </c>
-      <c r="C561" s="5" t="s">
+      <c r="C561" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="D561" s="5" t="s">
+      <c r="D561" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="E561" s="5" t="s">
+      <c r="E561" s="2" t="s">
         <v>1654</v>
       </c>
-      <c r="F561" s="5" t="s">
+      <c r="F561" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G561" s="5" t="s">
+      <c r="G561" s="2" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="562" spans="1:7">
-      <c r="A562" s="5" t="s">
+      <c r="A562" s="2" t="s">
         <v>1655</v>
       </c>
-      <c r="B562" s="5" t="s">
+      <c r="B562" s="2" t="s">
         <v>1656</v>
       </c>
-      <c r="C562" s="5" t="s">
+      <c r="C562" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D562" s="5" t="s">
+      <c r="D562" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E562" s="5" t="s">
+      <c r="E562" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="F562" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G562" s="5" t="s">
+      <c r="F562" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G562" s="2" t="s">
         <v>690</v>
       </c>
     </row>
     <row r="563" spans="1:7">
-      <c r="A563" s="5" t="s">
+      <c r="A563" s="2" t="s">
         <v>1657</v>
       </c>
-      <c r="B563" s="5" t="s">
+      <c r="B563" s="2" t="s">
         <v>1658</v>
       </c>
-      <c r="C563" s="5" t="s">
+      <c r="C563" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="D563" s="5"/>
-      <c r="E563" s="5" t="s">
+      <c r="D563" s="2"/>
+      <c r="E563" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="F563" s="5" t="s">
+      <c r="F563" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G563" s="5" t="s">
+      <c r="G563" s="2" t="s">
         <v>597</v>
       </c>
     </row>
     <row r="564" spans="1:7">
-      <c r="A564" s="5" t="s">
+      <c r="A564" s="2" t="s">
         <v>1659</v>
       </c>
-      <c r="B564" s="5" t="s">
+      <c r="B564" s="2" t="s">
         <v>1660</v>
       </c>
-      <c r="C564" s="5" t="s">
+      <c r="C564" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="D564" s="5"/>
-      <c r="E564" s="5" t="s">
+      <c r="D564" s="2"/>
+      <c r="E564" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="F564" s="5" t="s">
+      <c r="F564" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G564" s="5" t="s">
+      <c r="G564" s="2" t="s">
         <v>1661</v>
       </c>
     </row>
     <row r="565" spans="1:7">
-      <c r="A565" s="5" t="s">
+      <c r="A565" s="2" t="s">
         <v>1662</v>
       </c>
-      <c r="B565" s="5" t="s">
+      <c r="B565" s="2" t="s">
         <v>1663</v>
       </c>
-      <c r="C565" s="5" t="s">
+      <c r="C565" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D565" s="5" t="s">
+      <c r="D565" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="E565" s="5" t="s">
+      <c r="E565" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="F565" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G565" s="5" t="s">
+      <c r="F565" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G565" s="2" t="s">
         <v>521</v>
       </c>
     </row>
     <row r="566" spans="1:7">
-      <c r="A566" s="5" t="s">
+      <c r="A566" s="2" t="s">
         <v>1664</v>
       </c>
-      <c r="B566" s="5" t="s">
+      <c r="B566" s="2" t="s">
         <v>1665</v>
       </c>
-      <c r="C566" s="5" t="s">
+      <c r="C566" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D566" s="5" t="s">
+      <c r="D566" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="E566" s="5" t="s">
+      <c r="E566" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="F566" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G566" s="5" t="s">
+      <c r="F566" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G566" s="2" t="s">
         <v>1666</v>
       </c>
     </row>
     <row r="567" spans="1:7">
-      <c r="A567" s="5" t="s">
+      <c r="A567" s="2" t="s">
         <v>1667</v>
       </c>
-      <c r="B567" s="5" t="s">
+      <c r="B567" s="2" t="s">
         <v>1668</v>
       </c>
-      <c r="C567" s="5" t="s">
+      <c r="C567" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="D567" s="5" t="s">
+      <c r="D567" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E567" s="5" t="s">
+      <c r="E567" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="F567" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G567" s="5" t="s">
+      <c r="F567" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G567" s="2" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="568" spans="1:7">
-      <c r="A568" s="5" t="s">
+      <c r="A568" s="2" t="s">
         <v>1669</v>
       </c>
-      <c r="B568" s="5" t="s">
+      <c r="B568" s="2" t="s">
         <v>1670</v>
       </c>
-      <c r="C568" s="5" t="s">
+      <c r="C568" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="D568" s="5" t="s">
+      <c r="D568" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E568" s="5" t="s">
+      <c r="E568" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="F568" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G568" s="5" t="s">
+      <c r="F568" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G568" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="569" spans="1:7">
-      <c r="A569" s="5" t="s">
+      <c r="A569" s="2" t="s">
         <v>1671</v>
       </c>
-      <c r="B569" s="5" t="s">
+      <c r="B569" s="2" t="s">
         <v>1672</v>
       </c>
-      <c r="C569" s="5" t="s">
+      <c r="C569" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D569" s="5"/>
-      <c r="E569" s="5" t="s">
+      <c r="D569" s="2"/>
+      <c r="E569" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="F569" s="5" t="s">
+      <c r="F569" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G569" s="5" t="s">
+      <c r="G569" s="2" t="s">
         <v>1580</v>
       </c>
     </row>
     <row r="570" spans="1:7">
-      <c r="A570" s="5" t="s">
+      <c r="A570" s="2" t="s">
         <v>1673</v>
       </c>
-      <c r="B570" s="5" t="s">
+      <c r="B570" s="2" t="s">
         <v>1674</v>
       </c>
-      <c r="C570" s="5" t="s">
+      <c r="C570" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D570" s="5"/>
-      <c r="E570" s="5" t="s">
+      <c r="D570" s="2"/>
+      <c r="E570" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="F570" s="5" t="s">
+      <c r="F570" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="G570" s="5" t="s">
+      <c r="G570" s="2" t="s">
         <v>1675</v>
       </c>
     </row>
     <row r="571" spans="1:7">
-      <c r="A571" s="5" t="s">
+      <c r="A571" s="2" t="s">
         <v>1676</v>
       </c>
-      <c r="B571" s="5" t="s">
+      <c r="B571" s="2" t="s">
         <v>1677</v>
       </c>
-      <c r="C571" s="5" t="s">
+      <c r="C571" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="D571" s="5"/>
-      <c r="E571" s="5" t="s">
+      <c r="D571" s="2"/>
+      <c r="E571" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="F571" s="5" t="s">
+      <c r="F571" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G571" s="5" t="s">
+      <c r="G571" s="2" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="572" spans="1:7">
-      <c r="A572" s="5" t="s">
+      <c r="A572" s="2" t="s">
         <v>1678</v>
       </c>
-      <c r="B572" s="5" t="s">
+      <c r="B572" s="2" t="s">
         <v>1679</v>
       </c>
-      <c r="C572" s="5" t="s">
+      <c r="C572" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="D572" s="5"/>
-      <c r="E572" s="5" t="s">
+      <c r="D572" s="2"/>
+      <c r="E572" s="2" t="s">
         <v>697</v>
       </c>
-      <c r="F572" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G572" s="5" t="s">
+      <c r="F572" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G572" s="2" t="s">
         <v>1680</v>
       </c>
     </row>
     <row r="573" spans="1:7">
-      <c r="A573" s="5" t="s">
+      <c r="A573" s="2" t="s">
         <v>1681</v>
       </c>
-      <c r="B573" s="5" t="s">
+      <c r="B573" s="2" t="s">
         <v>1682</v>
       </c>
-      <c r="C573" s="5" t="s">
+      <c r="C573" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D573" s="5"/>
-      <c r="E573" s="5" t="s">
+      <c r="D573" s="2"/>
+      <c r="E573" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F573" s="5" t="s">
+      <c r="F573" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G573" s="5" t="s">
+      <c r="G573" s="2" t="s">
         <v>617</v>
       </c>
     </row>
     <row r="574" spans="1:7">
-      <c r="A574" s="5" t="s">
+      <c r="A574" s="2" t="s">
         <v>1683</v>
       </c>
-      <c r="B574" s="5" t="s">
+      <c r="B574" s="2" t="s">
         <v>1684</v>
       </c>
-      <c r="C574" s="5" t="s">
+      <c r="C574" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D574" s="5"/>
-      <c r="E574" s="5" t="s">
+      <c r="D574" s="2"/>
+      <c r="E574" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="F574" s="5" t="s">
+      <c r="F574" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="G574" s="5" t="s">
+      <c r="G574" s="2" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="575" spans="1:7">
-      <c r="A575" s="5" t="s">
+      <c r="A575" s="2" t="s">
         <v>1685</v>
       </c>
-      <c r="B575" s="5" t="s">
+      <c r="B575" s="2" t="s">
         <v>1686</v>
       </c>
-      <c r="C575" s="5" t="s">
+      <c r="C575" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D575" s="5"/>
-      <c r="E575" s="5" t="s">
+      <c r="D575" s="2"/>
+      <c r="E575" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F575" s="5" t="s">
+      <c r="F575" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="G575" s="5" t="s">
+      <c r="G575" s="2" t="s">
         <v>617</v>
       </c>
     </row>
     <row r="576" spans="1:7">
-      <c r="A576" s="5" t="s">
+      <c r="A576" s="2" t="s">
         <v>1687</v>
       </c>
-      <c r="B576" s="5" t="s">
+      <c r="B576" s="2" t="s">
         <v>1688</v>
       </c>
-      <c r="C576" s="5" t="s">
+      <c r="C576" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D576" s="5"/>
-      <c r="E576" s="5" t="s">
+      <c r="D576" s="2"/>
+      <c r="E576" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="F576" s="5" t="s">
+      <c r="F576" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="G576" s="5" t="s">
+      <c r="G576" s="2" t="s">
         <v>1561</v>
       </c>
     </row>
     <row r="577" spans="1:7">
-      <c r="A577" s="5" t="s">
+      <c r="A577" s="2" t="s">
         <v>1689</v>
       </c>
-      <c r="B577" s="5" t="s">
+      <c r="B577" s="2" t="s">
         <v>1690</v>
       </c>
-      <c r="C577" s="5" t="s">
+      <c r="C577" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D577" s="5"/>
-      <c r="E577" s="5" t="s">
+      <c r="D577" s="2"/>
+      <c r="E577" s="2" t="s">
         <v>1407</v>
       </c>
-      <c r="F577" s="5" t="s">
+      <c r="F577" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="G577" s="5" t="s">
+      <c r="G577" s="2" t="s">
         <v>1691</v>
       </c>
     </row>
     <row r="578" spans="1:7">
-      <c r="A578" s="5" t="s">
+      <c r="A578" s="2" t="s">
         <v>1692</v>
       </c>
-      <c r="B578" s="5" t="s">
+      <c r="B578" s="2" t="s">
         <v>1693</v>
       </c>
-      <c r="C578" s="5" t="s">
+      <c r="C578" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D578" s="5"/>
-      <c r="E578" s="5" t="s">
+      <c r="D578" s="2"/>
+      <c r="E578" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F578" s="5" t="s">
+      <c r="F578" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="G578" s="5" t="s">
+      <c r="G578" s="2" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="579" spans="1:7">
-      <c r="A579" s="5" t="s">
+      <c r="A579" s="2" t="s">
         <v>1694</v>
       </c>
-      <c r="B579" s="5" t="s">
+      <c r="B579" s="2" t="s">
         <v>1695</v>
       </c>
-      <c r="C579" s="5" t="s">
+      <c r="C579" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D579" s="5"/>
-      <c r="E579" s="5" t="s">
+      <c r="D579" s="2"/>
+      <c r="E579" s="2" t="s">
         <v>1516</v>
       </c>
-      <c r="F579" s="5" t="s">
+      <c r="F579" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="G579" s="5" t="s">
+      <c r="G579" s="2" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="580" spans="1:7">
-      <c r="A580" s="5" t="s">
+      <c r="A580" s="2" t="s">
         <v>1696</v>
       </c>
-      <c r="B580" s="5" t="s">
+      <c r="B580" s="2" t="s">
         <v>1697</v>
       </c>
-      <c r="C580" s="5" t="s">
+      <c r="C580" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D580" s="5"/>
-      <c r="E580" s="5" t="s">
+      <c r="D580" s="2"/>
+      <c r="E580" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="F580" s="5" t="s">
+      <c r="F580" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="G580" s="5" t="s">
+      <c r="G580" s="2" t="s">
         <v>1698</v>
       </c>
     </row>
     <row r="581" spans="1:7">
-      <c r="A581" s="5" t="s">
+      <c r="A581" s="2" t="s">
         <v>1699</v>
       </c>
-      <c r="B581" s="5" t="s">
+      <c r="B581" s="2" t="s">
         <v>1700</v>
       </c>
-      <c r="C581" s="5" t="s">
+      <c r="C581" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D581" s="5" t="s">
+      <c r="D581" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E581" s="5" t="s">
+      <c r="E581" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="F581" s="5" t="s">
+      <c r="F581" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G581" s="5" t="s">
+      <c r="G581" s="2" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="582" spans="1:7">
-      <c r="A582" s="5" t="s">
+      <c r="A582" s="2" t="s">
         <v>1701</v>
       </c>
-      <c r="B582" s="5" t="s">
+      <c r="B582" s="2" t="s">
         <v>1702</v>
       </c>
-      <c r="C582" s="5" t="s">
+      <c r="C582" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D582" s="5" t="s">
+      <c r="D582" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E582" s="5" t="s">
+      <c r="E582" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="F582" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G582" s="5" t="s">
+      <c r="F582" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G582" s="2" t="s">
         <v>1703</v>
       </c>
     </row>
     <row r="583" spans="1:7">
-      <c r="A583" s="5" t="s">
+      <c r="A583" s="2" t="s">
         <v>1704</v>
       </c>
-      <c r="B583" s="5" t="s">
+      <c r="B583" s="2" t="s">
         <v>1705</v>
       </c>
-      <c r="C583" s="5" t="s">
+      <c r="C583" s="2" t="s">
         <v>1117</v>
       </c>
-      <c r="D583" s="5"/>
-      <c r="E583" s="5" t="s">
+      <c r="D583" s="2"/>
+      <c r="E583" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="F583" s="5" t="s">
+      <c r="F583" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G583" s="5" t="s">
+      <c r="G583" s="2" t="s">
         <v>1706</v>
       </c>
     </row>
     <row r="584" spans="1:7">
-      <c r="A584" s="5" t="s">
+      <c r="A584" s="2" t="s">
         <v>1707</v>
       </c>
-      <c r="B584" s="5" t="s">
+      <c r="B584" s="2" t="s">
         <v>1708</v>
       </c>
-      <c r="C584" s="5" t="s">
+      <c r="C584" s="2" t="s">
         <v>1117</v>
       </c>
-      <c r="D584" s="5"/>
-      <c r="E584" s="5" t="s">
+      <c r="D584" s="2"/>
+      <c r="E584" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="F584" s="5" t="s">
+      <c r="F584" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G584" s="5" t="s">
+      <c r="G584" s="2" t="s">
         <v>1709</v>
       </c>
     </row>
     <row r="585" spans="1:7">
-      <c r="A585" s="6" t="s">
+      <c r="A585" s="2" t="s">
         <v>1710</v>
       </c>
-      <c r="B585" s="6" t="s">
+      <c r="B585" s="2" t="s">
         <v>1711</v>
       </c>
-      <c r="C585" s="6" t="s">
+      <c r="C585" s="2" t="s">
         <v>1117</v>
       </c>
-      <c r="D585" s="6"/>
-      <c r="E585" s="6" t="s">
+      <c r="D585" s="2"/>
+      <c r="E585" s="2" t="s">
         <v>579</v>
       </c>
-      <c r="F585" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G585" s="6" t="s">
+      <c r="F585" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G585" s="2" t="s">
         <v>1712</v>
       </c>
     </row>
     <row r="586" spans="1:7">
-      <c r="A586" s="6" t="s">
+      <c r="A586" s="2" t="s">
         <v>1713</v>
       </c>
-      <c r="B586" s="6" t="s">
+      <c r="B586" s="2" t="s">
         <v>1714</v>
       </c>
-      <c r="C586" s="6" t="s">
+      <c r="C586" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D586" s="6" t="s">
+      <c r="D586" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="E586" s="6" t="s">
+      <c r="E586" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="F586" s="6" t="s">
+      <c r="F586" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G586" s="6" t="s">
+      <c r="G586" s="2" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="587" spans="1:7">
-      <c r="A587" s="6" t="s">
+      <c r="A587" s="2" t="s">
         <v>1715</v>
       </c>
-      <c r="B587" s="6" t="s">
+      <c r="B587" s="2" t="s">
         <v>1716</v>
       </c>
-      <c r="C587" s="6" t="s">
+      <c r="C587" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D587" s="6" t="s">
+      <c r="D587" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="E587" s="6" t="s">
+      <c r="E587" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="F587" s="6" t="s">
+      <c r="F587" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G587" s="6" t="s">
+      <c r="G587" s="2" t="s">
         <v>1717</v>
       </c>
     </row>
     <row r="588" spans="1:7">
-      <c r="A588" s="6" t="s">
+      <c r="A588" s="2" t="s">
         <v>1718</v>
       </c>
-      <c r="B588" s="6" t="s">
+      <c r="B588" s="2" t="s">
         <v>1719</v>
       </c>
-      <c r="C588" s="6" t="s">
+      <c r="C588" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="D588" s="6" t="s">
+      <c r="D588" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E588" s="6" t="s">
+      <c r="E588" s="2" t="s">
         <v>1720</v>
       </c>
-      <c r="F588" s="6" t="s">
+      <c r="F588" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="G588" s="6" t="s">
+      <c r="G588" s="2" t="s">
         <v>676</v>
       </c>
     </row>
     <row r="589" spans="1:7">
-      <c r="A589" s="6" t="s">
+      <c r="A589" s="2" t="s">
         <v>1721</v>
       </c>
-      <c r="B589" s="6" t="s">
+      <c r="B589" s="2" t="s">
         <v>1722</v>
       </c>
-      <c r="C589" s="6" t="s">
+      <c r="C589" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D589" s="6"/>
-      <c r="E589" s="6" t="s">
+      <c r="D589" s="2"/>
+      <c r="E589" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F589" s="6" t="s">
+      <c r="F589" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="G589" s="6" t="s">
+      <c r="G589" s="2" t="s">
         <v>1499</v>
       </c>
     </row>
     <row r="590" spans="1:7">
-      <c r="A590" s="6" t="s">
+      <c r="A590" s="2" t="s">
         <v>1723</v>
       </c>
-      <c r="B590" s="6" t="s">
+      <c r="B590" s="2" t="s">
         <v>1724</v>
       </c>
-      <c r="C590" s="6" t="s">
+      <c r="C590" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D590" s="6" t="s">
+      <c r="D590" s="2" t="s">
         <v>1169</v>
       </c>
-      <c r="E590" s="6" t="s">
+      <c r="E590" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="F590" s="6" t="s">
+      <c r="F590" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G590" s="6" t="s">
+      <c r="G590" s="2" t="s">
         <v>1725</v>
       </c>
     </row>
     <row r="591" spans="1:7">
-      <c r="A591" s="6" t="s">
+      <c r="A591" s="2" t="s">
         <v>1726</v>
       </c>
-      <c r="B591" s="6" t="s">
+      <c r="B591" s="2" t="s">
         <v>1727</v>
       </c>
-      <c r="C591" s="6" t="s">
+      <c r="C591" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D591" s="6" t="s">
+      <c r="D591" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E591" s="6" t="s">
+      <c r="E591" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="F591" s="6" t="s">
+      <c r="F591" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G591" s="6" t="s">
+      <c r="G591" s="2" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="592" spans="1:7">
-      <c r="A592" s="6" t="s">
+      <c r="A592" s="2" t="s">
         <v>1728</v>
       </c>
-      <c r="B592" s="6" t="s">
+      <c r="B592" s="2" t="s">
         <v>1729</v>
       </c>
-      <c r="C592" s="6" t="s">
+      <c r="C592" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D592" s="6" t="s">
+      <c r="D592" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E592" s="6" t="s">
+      <c r="E592" s="2" t="s">
         <v>1730</v>
       </c>
-      <c r="F592" s="6" t="s">
+      <c r="F592" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G592" s="6" t="s">
+      <c r="G592" s="2" t="s">
         <v>1530</v>
       </c>
     </row>
     <row r="593" spans="1:7">
-      <c r="A593" s="6" t="s">
+      <c r="A593" s="2" t="s">
         <v>1731</v>
       </c>
-      <c r="B593" s="6" t="s">
+      <c r="B593" s="2" t="s">
         <v>1732</v>
       </c>
-      <c r="C593" s="6" t="s">
+      <c r="C593" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D593" s="6" t="s">
+      <c r="D593" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="E593" s="6" t="s">
+      <c r="E593" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="F593" s="6" t="s">
+      <c r="F593" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G593" s="6" t="s">
+      <c r="G593" s="2" t="s">
         <v>1725</v>
       </c>
     </row>
     <row r="594" spans="1:7">
-      <c r="A594" s="6" t="s">
+      <c r="A594" s="2" t="s">
         <v>1733</v>
       </c>
-      <c r="B594" s="6" t="s">
+      <c r="B594" s="2" t="s">
         <v>1734</v>
       </c>
-      <c r="C594" s="6" t="s">
+      <c r="C594" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D594" s="6" t="s">
+      <c r="D594" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="E594" s="6" t="s">
+      <c r="E594" s="2" t="s">
         <v>737</v>
       </c>
-      <c r="F594" s="6" t="s">
+      <c r="F594" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="G594" s="6" t="s">
+      <c r="G594" s="2" t="s">
         <v>1735</v>
       </c>
     </row>
     <row r="595" spans="1:7">
-      <c r="A595" s="6" t="s">
+      <c r="A595" s="2" t="s">
         <v>1736</v>
       </c>
-      <c r="B595" s="6" t="s">
+      <c r="B595" s="2" t="s">
         <v>1737</v>
       </c>
-      <c r="C595" s="6" t="s">
+      <c r="C595" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D595" s="6"/>
-      <c r="E595" s="6" t="s">
+      <c r="D595" s="2"/>
+      <c r="E595" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="F595" s="6" t="s">
+      <c r="F595" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G595" s="6" t="s">
+      <c r="G595" s="2" t="s">
         <v>861</v>
       </c>
     </row>
     <row r="596" spans="1:7">
-      <c r="A596" s="6" t="s">
+      <c r="A596" s="2" t="s">
         <v>1738</v>
       </c>
-      <c r="B596" s="6" t="s">
+      <c r="B596" s="2" t="s">
         <v>1739</v>
       </c>
-      <c r="C596" s="6" t="s">
+      <c r="C596" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D596" s="6" t="s">
+      <c r="D596" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="E596" s="6" t="s">
+      <c r="E596" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F596" s="6" t="s">
+      <c r="F596" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G596" s="6" t="s">
+      <c r="G596" s="2" t="s">
         <v>1318</v>
       </c>
     </row>
     <row r="597" spans="1:7">
-      <c r="A597" s="6" t="s">
+      <c r="A597" s="2" t="s">
         <v>1740</v>
       </c>
-      <c r="B597" s="6" t="s">
+      <c r="B597" s="2" t="s">
         <v>1741</v>
       </c>
-      <c r="C597" s="6" t="s">
+      <c r="C597" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D597" s="6" t="s">
+      <c r="D597" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="E597" s="6" t="s">
+      <c r="E597" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="F597" s="6" t="s">
+      <c r="F597" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G597" s="6" t="s">
+      <c r="G597" s="2" t="s">
         <v>1742</v>
       </c>
     </row>
     <row r="598" spans="1:7">
-      <c r="A598" s="6" t="s">
+      <c r="A598" s="2" t="s">
         <v>1743</v>
       </c>
-      <c r="B598" s="6" t="s">
+      <c r="B598" s="2" t="s">
         <v>1744</v>
       </c>
-      <c r="C598" s="6" t="s">
+      <c r="C598" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D598" s="6" t="s">
+      <c r="D598" s="2" t="s">
         <v>1169</v>
       </c>
-      <c r="E598" s="6" t="s">
+      <c r="E598" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="F598" s="6" t="s">
+      <c r="F598" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G598" s="6" t="s">
+      <c r="G598" s="2" t="s">
         <v>1745</v>
       </c>
     </row>
     <row r="599" spans="1:7">
-      <c r="A599" s="6" t="s">
+      <c r="A599" s="2" t="s">
         <v>1746</v>
       </c>
-      <c r="B599" s="6" t="s">
+      <c r="B599" s="2" t="s">
         <v>1747</v>
       </c>
-      <c r="C599" s="6" t="s">
+      <c r="C599" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D599" s="6" t="s">
+      <c r="D599" s="2" t="s">
         <v>1169</v>
       </c>
-      <c r="E599" s="6" t="s">
+      <c r="E599" s="2" t="s">
         <v>1654</v>
       </c>
-      <c r="F599" s="6" t="s">
+      <c r="F599" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G599" s="6" t="s">
+      <c r="G599" s="2" t="s">
         <v>1748</v>
       </c>
     </row>
     <row r="600" spans="1:7">
-      <c r="A600" s="6" t="s">
+      <c r="A600" s="2" t="s">
         <v>1749</v>
       </c>
-      <c r="B600" s="6" t="s">
+      <c r="B600" s="2" t="s">
         <v>1750</v>
       </c>
-      <c r="C600" s="6" t="s">
+      <c r="C600" s="2" t="s">
         <v>1169</v>
       </c>
-      <c r="D600" s="6"/>
-      <c r="E600" s="6" t="s">
+      <c r="D600" s="2"/>
+      <c r="E600" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F600" s="6" t="s">
+      <c r="F600" s="2" t="s">
         <v>1337</v>
       </c>
-      <c r="G600" s="6" t="s">
+      <c r="G600" s="2" t="s">
         <v>768</v>
       </c>
     </row>
     <row r="601" spans="1:7">
-      <c r="A601" s="6" t="s">
+      <c r="A601" s="2" t="s">
         <v>1751</v>
       </c>
-      <c r="B601" s="6" t="s">
+      <c r="B601" s="2" t="s">
         <v>1752</v>
       </c>
-      <c r="C601" s="6" t="s">
+      <c r="C601" s="2" t="s">
         <v>1169</v>
       </c>
-      <c r="D601" s="6"/>
-      <c r="E601" s="6" t="s">
+      <c r="D601" s="2"/>
+      <c r="E601" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="F601" s="6" t="s">
+      <c r="F601" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="G601" s="6" t="s">
+      <c r="G601" s="2" t="s">
         <v>1600</v>
       </c>
     </row>
     <row r="602" spans="1:7">
-      <c r="A602" s="6" t="s">
+      <c r="A602" s="2" t="s">
         <v>1753</v>
       </c>
-      <c r="B602" s="6" t="s">
+      <c r="B602" s="2" t="s">
         <v>1754</v>
       </c>
-      <c r="C602" s="6" t="s">
+      <c r="C602" s="2" t="s">
         <v>1169</v>
       </c>
-      <c r="D602" s="6"/>
-      <c r="E602" s="6" t="s">
+      <c r="D602" s="2"/>
+      <c r="E602" s="2" t="s">
         <v>1031</v>
       </c>
-      <c r="F602" s="6" t="s">
+      <c r="F602" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="G602" s="6" t="s">
+      <c r="G602" s="2" t="s">
         <v>1666</v>
       </c>
     </row>
     <row r="603" spans="1:7">
-      <c r="A603" s="6" t="s">
+      <c r="A603" s="2" t="s">
         <v>1755</v>
       </c>
-      <c r="B603" s="6" t="s">
+      <c r="B603" s="2" t="s">
         <v>1756</v>
       </c>
-      <c r="C603" s="6" t="s">
+      <c r="C603" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="D603" s="6"/>
-      <c r="E603" s="6" t="s">
+      <c r="D603" s="2"/>
+      <c r="E603" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F603" s="6" t="s">
+      <c r="F603" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G603" s="6" t="s">
+      <c r="G603" s="2" t="s">
         <v>1437</v>
       </c>
     </row>
     <row r="604" spans="1:7">
-      <c r="A604" s="6" t="s">
+      <c r="A604" s="2" t="s">
         <v>1757</v>
       </c>
-      <c r="B604" s="6" t="s">
+      <c r="B604" s="2" t="s">
         <v>1758</v>
       </c>
-      <c r="C604" s="6" t="s">
+      <c r="C604" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="D604" s="6"/>
-      <c r="E604" s="6" t="s">
+      <c r="D604" s="2"/>
+      <c r="E604" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F604" s="6" t="s">
+      <c r="F604" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="G604" s="6" t="s">
+      <c r="G604" s="2" t="s">
         <v>1097</v>
       </c>
     </row>
     <row r="605" spans="1:7">
-      <c r="A605" s="6" t="s">
+      <c r="A605" s="2" t="s">
         <v>1759</v>
       </c>
-      <c r="B605" s="6" t="s">
+      <c r="B605" s="2" t="s">
         <v>1760</v>
       </c>
-      <c r="C605" s="6" t="s">
+      <c r="C605" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="D605" s="6"/>
-      <c r="E605" s="6" t="s">
+      <c r="D605" s="2"/>
+      <c r="E605" s="2" t="s">
         <v>1761</v>
       </c>
-      <c r="F605" s="6" t="s">
+      <c r="F605" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="G605" s="6" t="s">
+      <c r="G605" s="2" t="s">
         <v>1762</v>
       </c>
     </row>
     <row r="606" spans="1:7">
-      <c r="A606" s="6" t="s">
+      <c r="A606" s="2" t="s">
         <v>1763</v>
       </c>
-      <c r="B606" s="6" t="s">
+      <c r="B606" s="2" t="s">
         <v>1764</v>
       </c>
-      <c r="C606" s="6" t="s">
+      <c r="C606" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D606" s="6"/>
-      <c r="E606" s="6" t="s">
+      <c r="D606" s="2"/>
+      <c r="E606" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="F606" s="6" t="s">
+      <c r="F606" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G606" s="6" t="s">
+      <c r="G606" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="607" spans="1:7">
-      <c r="A607" s="6" t="s">
+      <c r="A607" s="2" t="s">
         <v>1765</v>
       </c>
-      <c r="B607" s="6" t="s">
+      <c r="B607" s="2" t="s">
         <v>1766</v>
       </c>
-      <c r="C607" s="6" t="s">
+      <c r="C607" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D607" s="6"/>
-      <c r="E607" s="6" t="s">
+      <c r="D607" s="2"/>
+      <c r="E607" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="F607" s="6" t="s">
+      <c r="F607" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G607" s="6" t="s">
+      <c r="G607" s="2" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="608" spans="1:7">
-      <c r="A608" s="6" t="s">
+      <c r="A608" s="2" t="s">
         <v>1767</v>
       </c>
-      <c r="B608" s="6" t="s">
+      <c r="B608" s="2" t="s">
         <v>1768</v>
       </c>
-      <c r="C608" s="6" t="s">
+      <c r="C608" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="D608" s="6" t="s">
+      <c r="D608" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E608" s="6" t="s">
+      <c r="E608" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F608" s="6" t="s">
+      <c r="F608" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G608" s="6" t="s">
+      <c r="G608" s="2" t="s">
         <v>1465</v>
       </c>
     </row>
     <row r="609" spans="1:7">
-      <c r="A609" s="6" t="s">
+      <c r="A609" s="2" t="s">
         <v>1769</v>
       </c>
-      <c r="B609" s="6" t="s">
+      <c r="B609" s="2" t="s">
         <v>1770</v>
       </c>
-      <c r="C609" s="6" t="s">
+      <c r="C609" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="D609" s="6" t="s">
+      <c r="D609" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E609" s="6" t="s">
+      <c r="E609" s="2" t="s">
         <v>1516</v>
       </c>
-      <c r="F609" s="6" t="s">
+      <c r="F609" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G609" s="6" t="s">
+      <c r="G609" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="610" spans="1:7">
-      <c r="A610" s="6" t="s">
+      <c r="A610" s="2" t="s">
         <v>1771</v>
       </c>
-      <c r="B610" s="6" t="s">
+      <c r="B610" s="2" t="s">
         <v>1772</v>
       </c>
-      <c r="C610" s="6" t="s">
+      <c r="C610" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="D610" s="6" t="s">
+      <c r="D610" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E610" s="6" t="s">
+      <c r="E610" s="2" t="s">
         <v>1031</v>
       </c>
-      <c r="F610" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G610" s="6" t="s">
+      <c r="F610" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G610" s="2" t="s">
         <v>1773</v>
       </c>
     </row>
     <row r="611" spans="1:7">
-      <c r="A611" s="6" t="s">
+      <c r="A611" s="2" t="s">
         <v>1774</v>
       </c>
-      <c r="B611" s="6" t="s">
+      <c r="B611" s="2" t="s">
         <v>1775</v>
       </c>
-      <c r="C611" s="6" t="s">
+      <c r="C611" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="D611" s="6"/>
-      <c r="E611" s="6" t="s">
+      <c r="D611" s="2"/>
+      <c r="E611" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F611" s="6" t="s">
+      <c r="F611" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G611" s="6" t="s">
+      <c r="G611" s="2" t="s">
         <v>1561</v>
       </c>
     </row>
     <row r="612" spans="1:7">
-      <c r="A612" s="6" t="s">
+      <c r="A612" s="2" t="s">
         <v>1776</v>
       </c>
-      <c r="B612" s="6" t="s">
+      <c r="B612" s="2" t="s">
         <v>1777</v>
       </c>
-      <c r="C612" s="6" t="s">
+      <c r="C612" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="D612" s="6"/>
-      <c r="E612" s="6" t="s">
+      <c r="D612" s="2"/>
+      <c r="E612" s="2" t="s">
         <v>628</v>
       </c>
-      <c r="F612" s="6" t="s">
+      <c r="F612" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="G612" s="6" t="s">
+      <c r="G612" s="2" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="613" spans="1:7">
-      <c r="A613" s="6" t="s">
+      <c r="A613" s="2" t="s">
         <v>1778</v>
       </c>
-      <c r="B613" s="6" t="s">
+      <c r="B613" s="2" t="s">
         <v>1779</v>
       </c>
-      <c r="C613" s="6" t="s">
+      <c r="C613" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="D613" s="6"/>
-      <c r="E613" s="6" t="s">
+      <c r="D613" s="2"/>
+      <c r="E613" s="2" t="s">
         <v>814</v>
       </c>
-      <c r="F613" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G613" s="6" t="s">
+      <c r="F613" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G613" s="2" t="s">
         <v>1780</v>
       </c>
     </row>
     <row r="614" spans="1:7">
-      <c r="A614" s="6" t="s">
+      <c r="A614" s="2" t="s">
         <v>1781</v>
       </c>
-      <c r="B614" s="6" t="s">
+      <c r="B614" s="2" t="s">
         <v>1782</v>
       </c>
-      <c r="C614" s="6" t="s">
+      <c r="C614" s="2" t="s">
         <v>1117</v>
       </c>
-      <c r="D614" s="6"/>
-      <c r="E614" s="6" t="s">
+      <c r="D614" s="2"/>
+      <c r="E614" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="F614" s="6" t="s">
+      <c r="F614" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G614" s="6" t="s">
+      <c r="G614" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="615" spans="1:7">
-      <c r="A615" s="6" t="s">
+      <c r="A615" s="2" t="s">
         <v>1783</v>
       </c>
-      <c r="B615" s="6" t="s">
+      <c r="B615" s="2" t="s">
         <v>1784</v>
       </c>
-      <c r="C615" s="6" t="s">
+      <c r="C615" s="2" t="s">
         <v>1117</v>
       </c>
-      <c r="D615" s="6"/>
-      <c r="E615" s="6" t="s">
+      <c r="D615" s="2"/>
+      <c r="E615" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="F615" s="6" t="s">
+      <c r="F615" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="G615" s="6" t="s">
+      <c r="G615" s="2" t="s">
         <v>1567</v>
       </c>
     </row>
     <row r="616" spans="1:7">
-      <c r="A616" s="6" t="s">
+      <c r="A616" s="2" t="s">
         <v>1785</v>
       </c>
-      <c r="B616" s="6" t="s">
+      <c r="B616" s="2" t="s">
         <v>1786</v>
       </c>
-      <c r="C616" s="6" t="s">
+      <c r="C616" s="2" t="s">
         <v>1117</v>
       </c>
-      <c r="D616" s="6"/>
-      <c r="E616" s="6" t="s">
+      <c r="D616" s="2"/>
+      <c r="E616" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="F616" s="6" t="s">
+      <c r="F616" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="G616" s="6" t="s">
+      <c r="G616" s="2" t="s">
         <v>1787</v>
       </c>
     </row>
     <row r="617" spans="1:7">
-      <c r="A617" s="6" t="s">
+      <c r="A617" s="2" t="s">
         <v>1788</v>
       </c>
-      <c r="B617" s="6" t="s">
+      <c r="B617" s="2" t="s">
         <v>1789</v>
       </c>
-      <c r="C617" s="6" t="s">
+      <c r="C617" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D617" s="6"/>
-      <c r="E617" s="6" t="s">
+      <c r="D617" s="2"/>
+      <c r="E617" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="F617" s="6" t="s">
+      <c r="F617" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="G617" s="6" t="s">
+      <c r="G617" s="2" t="s">
         <v>1790</v>
       </c>
     </row>
     <row r="618" spans="1:7">
-      <c r="A618" s="6" t="s">
+      <c r="A618" s="2" t="s">
         <v>1791</v>
       </c>
-      <c r="B618" s="6" t="s">
+      <c r="B618" s="2" t="s">
         <v>1792</v>
       </c>
-      <c r="C618" s="6" t="s">
+      <c r="C618" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D618" s="6"/>
-      <c r="E618" s="6" t="s">
+      <c r="D618" s="2"/>
+      <c r="E618" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="F618" s="6" t="s">
+      <c r="F618" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G618" s="6" t="s">
+      <c r="G618" s="2" t="s">
         <v>1793</v>
       </c>
     </row>
     <row r="619" spans="1:7">
-      <c r="A619" s="6" t="s">
+      <c r="A619" s="2" t="s">
         <v>1794</v>
       </c>
-      <c r="B619" s="6" t="s">
+      <c r="B619" s="2" t="s">
         <v>1795</v>
       </c>
-      <c r="C619" s="6" t="s">
+      <c r="C619" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="D619" s="6" t="s">
+      <c r="D619" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="E619" s="6" t="s">
+      <c r="E619" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="F619" s="6" t="s">
+      <c r="F619" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G619" s="6" t="s">
+      <c r="G619" s="2" t="s">
         <v>953</v>
       </c>
     </row>
     <row r="620" spans="1:7">
-      <c r="A620" s="6" t="s">
+      <c r="A620" s="2" t="s">
         <v>1796</v>
       </c>
-      <c r="B620" s="6" t="s">
+      <c r="B620" s="2" t="s">
         <v>1797</v>
       </c>
-      <c r="C620" s="6" t="s">
+      <c r="C620" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="D620" s="6"/>
-      <c r="E620" s="6" t="s">
+      <c r="D620" s="2"/>
+      <c r="E620" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="F620" s="6" t="s">
+      <c r="F620" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="G620" s="6" t="s">
+      <c r="G620" s="2" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="621" spans="1:7">
-      <c r="A621" s="6" t="s">
+      <c r="A621" s="2" t="s">
         <v>1798</v>
       </c>
-      <c r="B621" s="6" t="s">
+      <c r="B621" s="2" t="s">
         <v>1799</v>
       </c>
-      <c r="C621" s="6" t="s">
+      <c r="C621" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="D621" s="6"/>
-      <c r="E621" s="6" t="s">
+      <c r="D621" s="2"/>
+      <c r="E621" s="2" t="s">
         <v>697</v>
       </c>
-      <c r="F621" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G621" s="6" t="s">
+      <c r="F621" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G621" s="2" t="s">
         <v>1800</v>
       </c>
     </row>
     <row r="622" spans="1:7">
-      <c r="A622" s="6" t="s">
+      <c r="A622" s="2" t="s">
         <v>1801</v>
       </c>
-      <c r="B622" s="6" t="s">
+      <c r="B622" s="2" t="s">
         <v>1802</v>
       </c>
-      <c r="C622" s="6" t="s">
+      <c r="C622" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="D622" s="6"/>
-      <c r="E622" s="6" t="s">
+      <c r="D622" s="2"/>
+      <c r="E622" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="F622" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G622" s="6" t="s">
+      <c r="F622" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G622" s="2" t="s">
         <v>1803</v>
       </c>
     </row>
     <row r="623" spans="1:7">
-      <c r="A623" s="6" t="s">
+      <c r="A623" s="2" t="s">
         <v>1804</v>
       </c>
-      <c r="B623" s="6" t="s">
+      <c r="B623" s="2" t="s">
         <v>1805</v>
       </c>
-      <c r="C623" s="6" t="s">
+      <c r="C623" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="D623" s="6" t="s">
+      <c r="D623" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="E623" s="6" t="s">
+      <c r="E623" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="F623" s="6" t="s">
+      <c r="F623" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G623" s="6" t="s">
+      <c r="G623" s="2" t="s">
         <v>1806</v>
       </c>
     </row>
     <row r="624" spans="1:7">
-      <c r="A624" s="6" t="s">
+      <c r="A624" s="2" t="s">
         <v>1807</v>
       </c>
-      <c r="B624" s="6" t="s">
+      <c r="B624" s="2" t="s">
         <v>1808</v>
       </c>
-      <c r="C624" s="6" t="s">
+      <c r="C624" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="D624" s="6" t="s">
+      <c r="D624" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="E624" s="6" t="s">
+      <c r="E624" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="F624" s="6" t="s">
+      <c r="F624" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G624" s="6" t="s">
+      <c r="G624" s="2" t="s">
         <v>1809</v>
       </c>
     </row>
     <row r="625" spans="1:7">
-      <c r="A625" s="6" t="s">
+      <c r="A625" s="2" t="s">
         <v>1810</v>
       </c>
-      <c r="B625" s="6" t="s">
+      <c r="B625" s="2" t="s">
         <v>1811</v>
       </c>
-      <c r="C625" s="6" t="s">
+      <c r="C625" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="D625" s="6" t="s">
+      <c r="D625" s="2" t="s">
         <v>1169</v>
       </c>
-      <c r="E625" s="6" t="s">
+      <c r="E625" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="F625" s="6" t="s">
+      <c r="F625" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G625" s="6" t="s">
+      <c r="G625" s="2" t="s">
         <v>1193</v>
       </c>
     </row>
     <row r="626" spans="1:7">
-      <c r="A626" s="6" t="s">
+      <c r="A626" s="2" t="s">
         <v>1812</v>
       </c>
-      <c r="B626" s="6" t="s">
+      <c r="B626" s="2" t="s">
         <v>1813</v>
       </c>
-      <c r="C626" s="6" t="s">
+      <c r="C626" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="D626" s="6" t="s">
+      <c r="D626" s="2" t="s">
         <v>1169</v>
       </c>
-      <c r="E626" s="6" t="s">
+      <c r="E626" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="F626" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G626" s="6" t="s">
+      <c r="F626" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G626" s="2" t="s">
         <v>1814</v>
       </c>
     </row>
     <row r="627" spans="1:7">
-      <c r="A627" s="6" t="s">
+      <c r="A627" s="2" t="s">
         <v>1815</v>
       </c>
-      <c r="B627" s="6" t="s">
+      <c r="B627" s="2" t="s">
         <v>1816</v>
       </c>
-      <c r="C627" s="6" t="s">
+      <c r="C627" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D627" s="6"/>
-      <c r="E627" s="6" t="s">
+      <c r="D627" s="2"/>
+      <c r="E627" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="F627" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G627" s="6" t="s">
+      <c r="F627" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G627" s="2" t="s">
         <v>1505</v>
       </c>
     </row>
     <row r="628" spans="1:7">
-      <c r="A628" s="6" t="s">
+      <c r="A628" s="2" t="s">
         <v>1817</v>
       </c>
-      <c r="B628" s="6" t="s">
+      <c r="B628" s="2" t="s">
         <v>1818</v>
       </c>
-      <c r="C628" s="6" t="s">
+      <c r="C628" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D628" s="6" t="s">
+      <c r="D628" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E628" s="6" t="s">
+      <c r="E628" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="F628" s="6" t="s">
+      <c r="F628" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G628" s="6" t="s">
+      <c r="G628" s="2" t="s">
         <v>1530</v>
       </c>
     </row>
     <row r="629" spans="1:7">
-      <c r="A629" s="6" t="s">
+      <c r="A629" s="2" t="s">
         <v>1819</v>
       </c>
-      <c r="B629" s="6" t="s">
+      <c r="B629" s="2" t="s">
         <v>1820</v>
       </c>
-      <c r="C629" s="6" t="s">
+      <c r="C629" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D629" s="6" t="s">
+      <c r="D629" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E629" s="6" t="s">
+      <c r="E629" s="2" t="s">
         <v>697</v>
       </c>
-      <c r="F629" s="6" t="s">
+      <c r="F629" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="G629" s="6" t="s">
+      <c r="G629" s="2" t="s">
         <v>1709</v>
       </c>
     </row>
     <row r="630" spans="1:7">
-      <c r="A630" s="6" t="s">
+      <c r="A630" s="2" t="s">
         <v>1821</v>
       </c>
-      <c r="B630" s="6" t="s">
+      <c r="B630" s="2" t="s">
         <v>1822</v>
       </c>
-      <c r="C630" s="6" t="s">
+      <c r="C630" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="D630" s="6" t="s">
+      <c r="D630" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E630" s="6" t="s">
+      <c r="E630" s="2" t="s">
         <v>1823</v>
       </c>
-      <c r="F630" s="6" t="s">
+      <c r="F630" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G630" s="6" t="s">
+      <c r="G630" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="631" spans="1:7">
-      <c r="A631" s="6" t="s">
+      <c r="A631" s="2" t="s">
         <v>1824</v>
       </c>
-      <c r="B631" s="6" t="s">
+      <c r="B631" s="2" t="s">
         <v>1825</v>
       </c>
-      <c r="C631" s="6" t="s">
+      <c r="C631" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="D631" s="6" t="s">
+      <c r="D631" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E631" s="6" t="s">
+      <c r="E631" s="2" t="s">
         <v>697</v>
       </c>
-      <c r="F631" s="6" t="s">
+      <c r="F631" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="G631" s="6" t="s">
+      <c r="G631" s="2" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="632" spans="1:7">
-      <c r="A632" s="6" t="s">
+      <c r="A632" s="2" t="s">
         <v>1826</v>
       </c>
-      <c r="B632" s="6" t="s">
+      <c r="B632" s="2" t="s">
         <v>1827</v>
       </c>
-      <c r="C632" s="6" t="s">
+      <c r="C632" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D632" s="6"/>
-      <c r="E632" s="6" t="s">
+      <c r="D632" s="2"/>
+      <c r="E632" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="F632" s="6" t="s">
+      <c r="F632" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G632" s="6" t="s">
+      <c r="G632" s="2" t="s">
         <v>765</v>
       </c>
     </row>
     <row r="633" spans="1:7">
-      <c r="A633" s="6" t="s">
+      <c r="A633" s="2" t="s">
         <v>1828</v>
       </c>
-      <c r="B633" s="6" t="s">
+      <c r="B633" s="2" t="s">
         <v>1829</v>
       </c>
-      <c r="C633" s="6" t="s">
+      <c r="C633" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D633" s="6" t="s">
+      <c r="D633" s="2" t="s">
         <v>1169</v>
       </c>
-      <c r="E633" s="6" t="s">
+      <c r="E633" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="F633" s="6" t="s">
+      <c r="F633" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G633" s="6" t="s">
+      <c r="G633" s="2" t="s">
         <v>1725</v>
       </c>
     </row>
     <row r="634" spans="1:7">
-      <c r="A634" s="6" t="s">
+      <c r="A634" s="2" t="s">
         <v>1830</v>
       </c>
-      <c r="B634" s="6" t="s">
+      <c r="B634" s="2" t="s">
         <v>1831</v>
       </c>
-      <c r="C634" s="6" t="s">
+      <c r="C634" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="D634" s="6" t="s">
+      <c r="D634" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="E634" s="6" t="s">
+      <c r="E634" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F634" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G634" s="6" t="s">
+      <c r="F634" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G634" s="2" t="s">
         <v>1832</v>
       </c>
     </row>
     <row r="635" spans="1:7">
-      <c r="A635" s="6" t="s">
+      <c r="A635" s="2" t="s">
         <v>1833</v>
       </c>
-      <c r="B635" s="6" t="s">
+      <c r="B635" s="2" t="s">
         <v>1834</v>
       </c>
-      <c r="C635" s="6" t="s">
+      <c r="C635" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="D635" s="6" t="s">
+      <c r="D635" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="E635" s="6" t="s">
+      <c r="E635" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="F635" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G635" s="6" t="s">
+      <c r="F635" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G635" s="2" t="s">
         <v>1835</v>
       </c>
     </row>
     <row r="636" spans="1:7">
-      <c r="A636" s="6" t="s">
+      <c r="A636" s="2" t="s">
         <v>1836</v>
       </c>
-      <c r="B636" s="6" t="s">
+      <c r="B636" s="2" t="s">
         <v>1837</v>
       </c>
-      <c r="C636" s="6" t="s">
+      <c r="C636" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="D636" s="6" t="s">
+      <c r="D636" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="E636" s="6" t="s">
+      <c r="E636" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="F636" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G636" s="6" t="s">
+      <c r="F636" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G636" s="2" t="s">
         <v>1838</v>
       </c>
     </row>
     <row r="637" spans="1:7">
-      <c r="A637" s="6" t="s">
+      <c r="A637" s="2" t="s">
         <v>1839</v>
       </c>
-      <c r="B637" s="6" t="s">
+      <c r="B637" s="2" t="s">
         <v>1840</v>
       </c>
-      <c r="C637" s="6" t="s">
+      <c r="C637" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D637" s="6" t="s">
+      <c r="D637" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E637" s="6" t="s">
+      <c r="E637" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F637" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G637" s="6" t="s">
+      <c r="F637" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G637" s="2" t="s">
         <v>1841</v>
       </c>
     </row>
     <row r="638" spans="1:7">
-      <c r="A638" s="6" t="s">
+      <c r="A638" s="2" t="s">
         <v>1842</v>
       </c>
-      <c r="B638" s="6" t="s">
+      <c r="B638" s="2" t="s">
         <v>1843</v>
       </c>
-      <c r="C638" s="6" t="s">
+      <c r="C638" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D638" s="6" t="s">
+      <c r="D638" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E638" s="6" t="s">
+      <c r="E638" s="2" t="s">
         <v>1844</v>
       </c>
-      <c r="F638" s="6" t="s">
+      <c r="F638" s="2" t="s">
         <v>1845</v>
       </c>
-      <c r="G638" s="6" t="s">
+      <c r="G638" s="2" t="s">
         <v>1846</v>
       </c>
     </row>
     <row r="639" spans="1:7">
-      <c r="A639" s="6" t="s">
+      <c r="A639" s="2" t="s">
         <v>1847</v>
       </c>
-      <c r="B639" s="6" t="s">
+      <c r="B639" s="2" t="s">
         <v>1848</v>
       </c>
-      <c r="C639" s="6" t="s">
+      <c r="C639" s="2" t="s">
         <v>1169</v>
       </c>
-      <c r="D639" s="6" t="s">
+      <c r="D639" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="E639" s="6" t="s">
+      <c r="E639" s="2" t="s">
         <v>789</v>
       </c>
-      <c r="F639" s="6" t="s">
+      <c r="F639" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="G639" s="6" t="s">
+      <c r="G639" s="2" t="s">
         <v>1849</v>
       </c>
     </row>
     <row r="640" spans="1:7">
-      <c r="A640" s="6" t="s">
+      <c r="A640" s="2" t="s">
         <v>1850</v>
       </c>
-      <c r="B640" s="6" t="s">
+      <c r="B640" s="2" t="s">
         <v>1851</v>
       </c>
-      <c r="C640" s="6" t="s">
+      <c r="C640" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="D640" s="6" t="s">
+      <c r="D640" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="E640" s="6" t="s">
+      <c r="E640" s="2" t="s">
         <v>789</v>
       </c>
-      <c r="F640" s="6" t="s">
+      <c r="F640" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="G640" s="6" t="s">
+      <c r="G640" s="2" t="s">
         <v>1567</v>
       </c>
     </row>
     <row r="641" spans="1:7">
-      <c r="A641" s="6" t="s">
+      <c r="A641" s="2" t="s">
         <v>1852</v>
       </c>
-      <c r="B641" s="6" t="s">
+      <c r="B641" s="2" t="s">
         <v>1853</v>
       </c>
-      <c r="C641" s="6" t="s">
+      <c r="C641" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D641" s="6" t="s">
+      <c r="D641" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="E641" s="6" t="s">
+      <c r="E641" s="2" t="s">
         <v>789</v>
       </c>
-      <c r="F641" s="6" t="s">
+      <c r="F641" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="G641" s="6" t="s">
+      <c r="G641" s="2" t="s">
         <v>1648</v>
       </c>
     </row>
     <row r="642" spans="1:7">
-      <c r="A642" s="6" t="s">
+      <c r="A642" s="2" t="s">
         <v>1854</v>
       </c>
-      <c r="B642" s="6" t="s">
+      <c r="B642" s="2" t="s">
         <v>1855</v>
       </c>
-      <c r="C642" s="6" t="s">
+      <c r="C642" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="D642" s="6"/>
-      <c r="E642" s="6" t="s">
+      <c r="D642" s="2"/>
+      <c r="E642" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="F642" s="6" t="s">
+      <c r="F642" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="G642" s="6" t="s">
+      <c r="G642" s="2" t="s">
         <v>1487</v>
       </c>
     </row>
     <row r="643" spans="1:7">
-      <c r="A643" s="6" t="s">
+      <c r="A643" s="2" t="s">
         <v>1856</v>
       </c>
-      <c r="B643" s="6" t="s">
+      <c r="B643" s="2" t="s">
         <v>1857</v>
       </c>
-      <c r="C643" s="6" t="s">
+      <c r="C643" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="D643" s="6" t="s">
+      <c r="D643" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E643" s="6" t="s">
+      <c r="E643" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="F643" s="6" t="s">
+      <c r="F643" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="G643" s="6" t="s">
+      <c r="G643" s="2" t="s">
         <v>1520</v>
       </c>
     </row>
     <row r="644" spans="1:7">
-      <c r="A644" s="6" t="s">
+      <c r="A644" s="2" t="s">
         <v>1858</v>
       </c>
-      <c r="B644" s="6" t="s">
+      <c r="B644" s="2" t="s">
         <v>1859</v>
       </c>
-      <c r="C644" s="6" t="s">
+      <c r="C644" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="D644" s="6" t="s">
+      <c r="D644" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E644" s="6" t="s">
+      <c r="E644" s="2" t="s">
         <v>807</v>
       </c>
-      <c r="F644" s="6" t="s">
+      <c r="F644" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="G644" s="6" t="s">
+      <c r="G644" s="2" t="s">
         <v>1809</v>
       </c>
     </row>
     <row r="645" spans="1:7">
-      <c r="A645" s="6" t="s">
+      <c r="A645" s="2" t="s">
         <v>1860</v>
       </c>
-      <c r="B645" s="6" t="s">
+      <c r="B645" s="2" t="s">
         <v>1861</v>
       </c>
-      <c r="C645" s="6" t="s">
+      <c r="C645" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="D645" s="6" t="s">
+      <c r="D645" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="E645" s="6" t="s">
+      <c r="E645" s="2" t="s">
         <v>807</v>
       </c>
-      <c r="F645" s="6" t="s">
+      <c r="F645" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="G645" s="6" t="s">
+      <c r="G645" s="2" t="s">
         <v>1862</v>
       </c>
     </row>
     <row r="646" spans="1:7">
-      <c r="A646" s="6" t="s">
+      <c r="A646" s="2" t="s">
         <v>1863</v>
       </c>
-      <c r="B646" s="6" t="s">
+      <c r="B646" s="2" t="s">
         <v>1864</v>
       </c>
-      <c r="C646" s="6" t="s">
+      <c r="C646" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="D646" s="6" t="s">
+      <c r="D646" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="E646" s="6" t="s">
+      <c r="E646" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="F646" s="6" t="s">
+      <c r="F646" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="G646" s="6" t="s">
+      <c r="G646" s="2" t="s">
         <v>1404</v>
       </c>
     </row>
     <row r="647" spans="1:7">
-      <c r="A647" s="6" t="s">
+      <c r="A647" s="2" t="s">
         <v>1865</v>
       </c>
-      <c r="B647" s="6" t="s">
+      <c r="B647" s="2" t="s">
         <v>1866</v>
       </c>
-      <c r="C647" s="6" t="s">
+      <c r="C647" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="D647" s="6" t="s">
+      <c r="D647" s="2" t="s">
         <v>1117</v>
       </c>
-      <c r="E647" s="6" t="s">
+      <c r="E647" s="2" t="s">
         <v>1867</v>
       </c>
-      <c r="F647" s="6" t="s">
+      <c r="F647" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="G647" s="6" t="s">
+      <c r="G647" s="2" t="s">
         <v>1868</v>
       </c>
     </row>
     <row r="648" spans="1:7">
-      <c r="A648" s="6" t="s">
+      <c r="A648" s="2" t="s">
         <v>1869</v>
       </c>
-      <c r="B648" s="6" t="s">
+      <c r="B648" s="2" t="s">
         <v>1870</v>
       </c>
-      <c r="C648" s="6" t="s">
+      <c r="C648" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D648" s="6" t="s">
+      <c r="D648" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="E648" s="6" t="s">
+      <c r="E648" s="2" t="s">
         <v>789</v>
       </c>
-      <c r="F648" s="6" t="s">
+      <c r="F648" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="G648" s="6" t="s">
+      <c r="G648" s="2" t="s">
         <v>1871</v>
       </c>
     </row>
     <row r="649" spans="1:7">
-      <c r="A649" s="6" t="s">
+      <c r="A649" s="2" t="s">
         <v>1872</v>
       </c>
-      <c r="B649" s="6" t="s">
+      <c r="B649" s="2" t="s">
         <v>1873</v>
       </c>
-      <c r="C649" s="6" t="s">
+      <c r="C649" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D649" s="6" t="s">
+      <c r="D649" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="E649" s="6" t="s">
+      <c r="E649" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="F649" s="6" t="s">
+      <c r="F649" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="G649" s="6" t="s">
+      <c r="G649" s="2" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="650" spans="1:7">
-      <c r="A650" s="6" t="s">
+      <c r="A650" s="2" t="s">
         <v>1874</v>
       </c>
-      <c r="B650" s="6" t="s">
+      <c r="B650" s="2" t="s">
         <v>1875</v>
       </c>
-      <c r="C650" s="6" t="s">
+      <c r="C650" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D650" s="6" t="s">
+      <c r="D650" s="2" t="s">
         <v>1169</v>
       </c>
-      <c r="E650" s="6" t="s">
+      <c r="E650" s="2" t="s">
         <v>814</v>
       </c>
-      <c r="F650" s="6" t="s">
+      <c r="F650" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="G650" s="6" t="s">
+      <c r="G650" s="2" t="s">
         <v>1876</v>
       </c>
     </row>
@@ -31188,7 +31183,7 @@
   </sheetData>
   <autoFilter ref="A1:G1026">
     <sortState ref="A2:G1026">
-      <sortCondition ref="A1:A1026"/>
+      <sortCondition sortBy="cellColor" ref="C1:C1026" dxfId="0"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
adicionado os 72 pokemon da 6ª geração! (finalizado), falta apenas a descricao da dex no banco de dados
</commit_message>
<xml_diff>
--- a/pokemonv2/pokemons.xlsx
+++ b/pokemonv2/pokemons.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6683" uniqueCount="2773">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6683" uniqueCount="2774">
   <si>
     <t>ID</t>
   </si>
@@ -8336,6 +8336,9 @@
   </si>
   <si>
     <t>Type 2</t>
+  </si>
+  <si>
+    <t>g</t>
   </si>
 </sst>
 </file>
@@ -8364,7 +8367,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -8374,6 +8377,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8405,7 +8414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -8413,6 +8422,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8724,8 +8734,8 @@
   <dimension ref="A1:H1026"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <pane ySplit="1" topLeftCell="A702" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B711" sqref="B711"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22948,7 +22958,7 @@
         <v>1870</v>
       </c>
       <c r="C648" s="2" t="s">
-        <v>32</v>
+        <v>2773</v>
       </c>
       <c r="D648" s="2" t="s">
         <v>219</v>
@@ -23010,1565 +23020,1596 @@
       </c>
     </row>
     <row r="651" spans="1:7">
-      <c r="A651" t="s">
+      <c r="A651" s="5" t="s">
         <v>1877</v>
       </c>
-      <c r="B651" t="s">
+      <c r="B651" s="5" t="s">
         <v>1878</v>
       </c>
-      <c r="C651" t="s">
+      <c r="C651" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="E651" t="s">
+      <c r="D651" s="5"/>
+      <c r="E651" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F651" t="s">
-        <v>8</v>
-      </c>
-      <c r="G651" t="s">
+      <c r="F651" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G651" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="652" spans="1:7">
-      <c r="A652" t="s">
+      <c r="A652" s="5" t="s">
         <v>1879</v>
       </c>
-      <c r="B652" t="s">
+      <c r="B652" s="5" t="s">
         <v>1880</v>
       </c>
-      <c r="C652" t="s">
+      <c r="C652" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="E652" t="s">
+      <c r="D652" s="5"/>
+      <c r="E652" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F652" t="s">
-        <v>8</v>
-      </c>
-      <c r="G652" t="s">
+      <c r="F652" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G652" s="5" t="s">
         <v>478</v>
       </c>
     </row>
     <row r="653" spans="1:7">
-      <c r="A653" t="s">
+      <c r="A653" s="5" t="s">
         <v>1881</v>
       </c>
-      <c r="B653" t="s">
+      <c r="B653" s="5" t="s">
         <v>1882</v>
       </c>
-      <c r="C653" t="s">
+      <c r="C653" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="D653" t="s">
+      <c r="D653" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="E653" t="s">
+      <c r="E653" s="5" t="s">
         <v>1883</v>
       </c>
-      <c r="F653" t="s">
-        <v>8</v>
-      </c>
-      <c r="G653" t="s">
+      <c r="F653" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G653" s="5" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="654" spans="1:7">
-      <c r="A654" t="s">
+      <c r="A654" s="5" t="s">
         <v>1884</v>
       </c>
-      <c r="B654" t="s">
+      <c r="B654" s="5" t="s">
         <v>1885</v>
       </c>
-      <c r="C654" t="s">
+      <c r="C654" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E654" t="s">
+      <c r="D654" s="5"/>
+      <c r="E654" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="F654" t="s">
-        <v>8</v>
-      </c>
-      <c r="G654" t="s">
+      <c r="F654" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G654" s="5" t="s">
         <v>1886</v>
       </c>
     </row>
     <row r="655" spans="1:7">
-      <c r="A655" t="s">
+      <c r="A655" s="5" t="s">
         <v>1887</v>
       </c>
-      <c r="B655" t="s">
+      <c r="B655" s="5" t="s">
         <v>1888</v>
       </c>
-      <c r="C655" t="s">
+      <c r="C655" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E655" t="s">
+      <c r="D655" s="5"/>
+      <c r="E655" s="5" t="s">
         <v>1889</v>
       </c>
-      <c r="F655" t="s">
-        <v>8</v>
-      </c>
-      <c r="G655" t="s">
+      <c r="F655" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G655" s="5" t="s">
         <v>1249</v>
       </c>
     </row>
     <row r="656" spans="1:7">
-      <c r="A656" t="s">
+      <c r="A656" s="5" t="s">
         <v>1890</v>
       </c>
-      <c r="B656" t="s">
+      <c r="B656" s="5" t="s">
         <v>1891</v>
       </c>
-      <c r="C656" t="s">
+      <c r="C656" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D656" t="s">
+      <c r="D656" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E656" t="s">
+      <c r="E656" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F656" t="s">
-        <v>8</v>
-      </c>
-      <c r="G656" t="s">
+      <c r="F656" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G656" s="5" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="657" spans="1:7">
-      <c r="A657" t="s">
+      <c r="A657" s="5" t="s">
         <v>1892</v>
       </c>
-      <c r="B657" t="s">
+      <c r="B657" s="5" t="s">
         <v>1893</v>
       </c>
-      <c r="C657" t="s">
+      <c r="C657" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E657" t="s">
+      <c r="D657" s="5"/>
+      <c r="E657" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F657" t="s">
-        <v>8</v>
-      </c>
-      <c r="G657" t="s">
+      <c r="F657" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G657" s="5" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="658" spans="1:7">
-      <c r="A658" t="s">
+      <c r="A658" s="5" t="s">
         <v>1894</v>
       </c>
-      <c r="B658" t="s">
+      <c r="B658" s="5" t="s">
         <v>1895</v>
       </c>
-      <c r="C658" t="s">
+      <c r="C658" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E658" t="s">
+      <c r="D658" s="5"/>
+      <c r="E658" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F658" t="s">
-        <v>8</v>
-      </c>
-      <c r="G658" t="s">
+      <c r="F658" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G658" s="5" t="s">
         <v>1896</v>
       </c>
     </row>
     <row r="659" spans="1:7">
-      <c r="A659" t="s">
+      <c r="A659" s="5" t="s">
         <v>1897</v>
       </c>
-      <c r="B659" t="s">
+      <c r="B659" s="5" t="s">
         <v>1898</v>
       </c>
-      <c r="C659" t="s">
+      <c r="C659" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D659" t="s">
+      <c r="D659" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="E659" t="s">
+      <c r="E659" s="5" t="s">
         <v>1883</v>
       </c>
-      <c r="F659" t="s">
-        <v>8</v>
-      </c>
-      <c r="G659" t="s">
+      <c r="F659" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G659" s="5" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="660" spans="1:7">
-      <c r="A660" t="s">
+      <c r="A660" s="5" t="s">
         <v>1899</v>
       </c>
-      <c r="B660" t="s">
+      <c r="B660" s="5" t="s">
         <v>1900</v>
       </c>
-      <c r="C660" t="s">
+      <c r="C660" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="E660" t="s">
+      <c r="D660" s="5"/>
+      <c r="E660" s="5" t="s">
         <v>939</v>
       </c>
-      <c r="F660" t="s">
+      <c r="F660" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G660" t="s">
+      <c r="G660" s="5" t="s">
         <v>676</v>
       </c>
     </row>
     <row r="661" spans="1:7">
-      <c r="A661" t="s">
+      <c r="A661" s="5" t="s">
         <v>1901</v>
       </c>
-      <c r="B661" t="s">
+      <c r="B661" s="5" t="s">
         <v>1902</v>
       </c>
-      <c r="C661" t="s">
+      <c r="C661" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D661" t="s">
+      <c r="D661" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="E661" t="s">
+      <c r="E661" s="5" t="s">
         <v>1267</v>
       </c>
-      <c r="F661" t="s">
+      <c r="F661" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="G661" t="s">
+      <c r="G661" s="5" t="s">
         <v>1903</v>
       </c>
     </row>
     <row r="662" spans="1:7">
-      <c r="A662" t="s">
+      <c r="A662" s="5" t="s">
         <v>1904</v>
       </c>
-      <c r="B662" t="s">
+      <c r="B662" s="5" t="s">
         <v>1905</v>
       </c>
-      <c r="C662" t="s">
+      <c r="C662" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="D662" t="s">
+      <c r="D662" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E662" t="s">
+      <c r="E662" s="5" t="s">
         <v>606</v>
       </c>
-      <c r="F662" t="s">
+      <c r="F662" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G662" t="s">
+      <c r="G662" s="5" t="s">
         <v>900</v>
       </c>
     </row>
     <row r="663" spans="1:7">
-      <c r="A663" t="s">
+      <c r="A663" s="5" t="s">
         <v>1906</v>
       </c>
-      <c r="B663" t="s">
+      <c r="B663" s="5" t="s">
         <v>1907</v>
       </c>
-      <c r="C663" t="s">
+      <c r="C663" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D663" t="s">
+      <c r="D663" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E663" t="s">
+      <c r="E663" s="5" t="s">
         <v>1232</v>
       </c>
-      <c r="F663" t="s">
+      <c r="F663" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G663" t="s">
+      <c r="G663" s="5" t="s">
         <v>741</v>
       </c>
     </row>
     <row r="664" spans="1:7">
-      <c r="A664" t="s">
+      <c r="A664" s="5" t="s">
         <v>1908</v>
       </c>
-      <c r="B664" t="s">
+      <c r="B664" s="5" t="s">
         <v>1909</v>
       </c>
-      <c r="C664" t="s">
+      <c r="C664" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D664" t="s">
+      <c r="D664" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E664" t="s">
+      <c r="E664" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F664" t="s">
-        <v>8</v>
-      </c>
-      <c r="G664" t="s">
+      <c r="F664" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G664" s="5" t="s">
         <v>481</v>
       </c>
     </row>
     <row r="665" spans="1:7">
-      <c r="A665" t="s">
+      <c r="A665" s="5" t="s">
         <v>1910</v>
       </c>
-      <c r="B665" t="s">
+      <c r="B665" s="5" t="s">
         <v>1911</v>
       </c>
-      <c r="C665" t="s">
+      <c r="C665" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E665" t="s">
+      <c r="D665" s="5"/>
+      <c r="E665" s="5" t="s">
         <v>461</v>
       </c>
-      <c r="F665" t="s">
+      <c r="F665" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G665" t="s">
+      <c r="G665" s="5" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="666" spans="1:7">
-      <c r="A666" t="s">
+      <c r="A666" s="5" t="s">
         <v>1912</v>
       </c>
-      <c r="B666" t="s">
+      <c r="B666" s="5" t="s">
         <v>1913</v>
       </c>
-      <c r="C666" t="s">
+      <c r="C666" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E666" t="s">
+      <c r="D666" s="5"/>
+      <c r="E666" s="5" t="s">
         <v>949</v>
       </c>
-      <c r="F666" t="s">
+      <c r="F666" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G666" t="s">
+      <c r="G666" s="5" t="s">
         <v>1914</v>
       </c>
     </row>
     <row r="667" spans="1:7">
-      <c r="A667" t="s">
+      <c r="A667" s="5" t="s">
         <v>1915</v>
       </c>
-      <c r="B667" t="s">
+      <c r="B667" s="5" t="s">
         <v>1916</v>
       </c>
-      <c r="C667" t="s">
+      <c r="C667" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D667" t="s">
+      <c r="D667" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E667" t="s">
+      <c r="E667" s="5" t="s">
         <v>1917</v>
       </c>
-      <c r="F667" t="s">
-        <v>8</v>
-      </c>
-      <c r="G667" t="s">
+      <c r="F667" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G667" s="5" t="s">
         <v>1592</v>
       </c>
     </row>
     <row r="668" spans="1:7">
-      <c r="A668" t="s">
+      <c r="A668" s="5" t="s">
         <v>1918</v>
       </c>
-      <c r="B668" t="s">
+      <c r="B668" s="5" t="s">
         <v>1919</v>
       </c>
-      <c r="C668" t="s">
+      <c r="C668" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D668" t="s">
+      <c r="D668" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="E668" t="s">
+      <c r="E668" s="5" t="s">
         <v>1823</v>
       </c>
-      <c r="F668" t="s">
+      <c r="F668" s="5" t="s">
         <v>1920</v>
       </c>
-      <c r="G668" t="s">
+      <c r="G668" s="5" t="s">
         <v>1539</v>
       </c>
     </row>
     <row r="669" spans="1:7">
-      <c r="A669" t="s">
+      <c r="A669" s="5" t="s">
         <v>1921</v>
       </c>
-      <c r="B669" t="s">
+      <c r="B669" s="5" t="s">
         <v>1922</v>
       </c>
-      <c r="C669" t="s">
+      <c r="C669" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D669" t="s">
+      <c r="D669" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="E669" t="s">
+      <c r="E669" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="F669" t="s">
+      <c r="F669" s="5" t="s">
         <v>629</v>
       </c>
-      <c r="G669" t="s">
+      <c r="G669" s="5" t="s">
         <v>1923</v>
       </c>
     </row>
     <row r="670" spans="1:7">
-      <c r="A670" t="s">
+      <c r="A670" s="5" t="s">
         <v>1924</v>
       </c>
-      <c r="B670" t="s">
+      <c r="B670" s="5" t="s">
         <v>1925</v>
       </c>
-      <c r="C670" t="s">
+      <c r="C670" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E670" t="s">
+      <c r="D670" s="5"/>
+      <c r="E670" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="F670" t="s">
+      <c r="F670" s="5" t="s">
         <v>359</v>
       </c>
-      <c r="G670" t="s">
+      <c r="G670" s="5" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="671" spans="1:7">
-      <c r="A671" t="s">
+      <c r="A671" s="5" t="s">
         <v>1926</v>
       </c>
-      <c r="B671" t="s">
+      <c r="B671" s="5" t="s">
         <v>1927</v>
       </c>
-      <c r="C671" t="s">
+      <c r="C671" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E671" t="s">
+      <c r="D671" s="5"/>
+      <c r="E671" s="5" t="s">
         <v>1516</v>
       </c>
-      <c r="F671" t="s">
+      <c r="F671" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G671" t="s">
+      <c r="G671" s="5" t="s">
         <v>1928</v>
       </c>
     </row>
     <row r="672" spans="1:7">
-      <c r="A672" t="s">
+      <c r="A672" s="5" t="s">
         <v>1929</v>
       </c>
-      <c r="B672" t="s">
+      <c r="B672" s="5" t="s">
         <v>1930</v>
       </c>
-      <c r="C672" t="s">
+      <c r="C672" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E672" t="s">
+      <c r="D672" s="5"/>
+      <c r="E672" s="5" t="s">
         <v>1931</v>
       </c>
-      <c r="F672" t="s">
-        <v>8</v>
-      </c>
-      <c r="G672" t="s">
+      <c r="F672" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G672" s="5" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="673" spans="1:7">
-      <c r="A673" t="s">
+      <c r="A673" s="5" t="s">
         <v>1932</v>
       </c>
-      <c r="B673" t="s">
+      <c r="B673" s="5" t="s">
         <v>1933</v>
       </c>
-      <c r="C673" t="s">
+      <c r="C673" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="E673" t="s">
+      <c r="D673" s="5"/>
+      <c r="E673" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="F673" t="s">
+      <c r="F673" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="G673" t="s">
+      <c r="G673" s="5" t="s">
         <v>1580</v>
       </c>
     </row>
     <row r="674" spans="1:7">
-      <c r="A674" t="s">
+      <c r="A674" s="5" t="s">
         <v>1934</v>
       </c>
-      <c r="B674" t="s">
+      <c r="B674" s="5" t="s">
         <v>1935</v>
       </c>
-      <c r="C674" t="s">
+      <c r="C674" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="E674" t="s">
+      <c r="D674" s="5"/>
+      <c r="E674" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="F674" t="s">
-        <v>8</v>
-      </c>
-      <c r="G674" t="s">
+      <c r="F674" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G674" s="5" t="s">
         <v>1936</v>
       </c>
     </row>
     <row r="675" spans="1:7">
-      <c r="A675" t="s">
+      <c r="A675" s="5" t="s">
         <v>1937</v>
       </c>
-      <c r="B675" t="s">
+      <c r="B675" s="5" t="s">
         <v>1938</v>
       </c>
-      <c r="C675" t="s">
+      <c r="C675" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="E675" t="s">
+      <c r="D675" s="5"/>
+      <c r="E675" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="F675" t="s">
+      <c r="F675" s="5" t="s">
         <v>1920</v>
       </c>
-      <c r="G675" t="s">
+      <c r="G675" s="5" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="676" spans="1:7">
-      <c r="A676" t="s">
+      <c r="A676" s="5" t="s">
         <v>1939</v>
       </c>
-      <c r="B676" t="s">
+      <c r="B676" s="5" t="s">
         <v>1940</v>
       </c>
-      <c r="C676" t="s">
+      <c r="C676" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="D676" t="s">
+      <c r="D676" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="E676" t="s">
+      <c r="E676" s="5" t="s">
         <v>452</v>
       </c>
-      <c r="F676" t="s">
+      <c r="F676" s="5" t="s">
         <v>629</v>
       </c>
-      <c r="G676" t="s">
+      <c r="G676" s="5" t="s">
         <v>1941</v>
       </c>
     </row>
     <row r="677" spans="1:7">
-      <c r="A677" t="s">
+      <c r="A677" s="5" t="s">
         <v>1942</v>
       </c>
-      <c r="B677" t="s">
+      <c r="B677" s="5" t="s">
         <v>1943</v>
       </c>
-      <c r="C677" t="s">
+      <c r="C677" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="E677" t="s">
+      <c r="D677" s="5"/>
+      <c r="E677" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="F677" t="s">
+      <c r="F677" s="5" t="s">
         <v>1944</v>
       </c>
-      <c r="G677" t="s">
+      <c r="G677" s="5" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="678" spans="1:7">
-      <c r="A678" t="s">
+      <c r="A678" s="5" t="s">
         <v>1945</v>
       </c>
-      <c r="B678" t="s">
+      <c r="B678" s="5" t="s">
         <v>1946</v>
       </c>
-      <c r="C678" t="s">
+      <c r="C678" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E678" t="s">
+      <c r="D678" s="5"/>
+      <c r="E678" s="5" t="s">
         <v>490</v>
       </c>
-      <c r="F678" t="s">
+      <c r="F678" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G678" t="s">
+      <c r="G678" s="5" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="679" spans="1:7">
-      <c r="A679" t="s">
+      <c r="A679" s="5" t="s">
         <v>1947</v>
       </c>
-      <c r="B679" t="s">
+      <c r="B679" s="5" t="s">
         <v>1948</v>
       </c>
-      <c r="C679" t="s">
+      <c r="C679" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E679" t="s">
+      <c r="D679" s="5"/>
+      <c r="E679" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="F679" t="s">
+      <c r="F679" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G679" t="s">
+      <c r="G679" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="680" spans="1:7">
-      <c r="A680" t="s">
+      <c r="A680" s="5" t="s">
         <v>1949</v>
       </c>
-      <c r="B680" t="s">
+      <c r="B680" s="5" t="s">
         <v>1950</v>
       </c>
-      <c r="C680" t="s">
+      <c r="C680" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="D680" t="s">
+      <c r="D680" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="E680" t="s">
+      <c r="E680" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="F680" t="s">
+      <c r="F680" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="G680" t="s">
+      <c r="G680" s="5" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="681" spans="1:7">
-      <c r="A681" t="s">
+      <c r="A681" s="5" t="s">
         <v>1951</v>
       </c>
-      <c r="B681" t="s">
+      <c r="B681" s="5" t="s">
         <v>1952</v>
       </c>
-      <c r="C681" t="s">
+      <c r="C681" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="D681" t="s">
+      <c r="D681" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="E681" t="s">
+      <c r="E681" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="F681" t="s">
+      <c r="F681" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="G681" t="s">
+      <c r="G681" s="5" t="s">
         <v>905</v>
       </c>
     </row>
     <row r="682" spans="1:7">
-      <c r="A682" t="s">
+      <c r="A682" s="5" t="s">
         <v>1953</v>
       </c>
-      <c r="B682" t="s">
+      <c r="B682" s="5" t="s">
         <v>1954</v>
       </c>
-      <c r="C682" t="s">
+      <c r="C682" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="D682" t="s">
+      <c r="D682" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="E682" t="s">
+      <c r="E682" s="5" t="s">
         <v>1031</v>
       </c>
-      <c r="F682" t="s">
-        <v>8</v>
-      </c>
-      <c r="G682" t="s">
+      <c r="F682" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G682" s="5" t="s">
         <v>1955</v>
       </c>
     </row>
     <row r="683" spans="1:7">
-      <c r="A683" t="s">
+      <c r="A683" s="5" t="s">
         <v>1956</v>
       </c>
-      <c r="B683" t="s">
+      <c r="B683" s="5" t="s">
         <v>1957</v>
       </c>
-      <c r="C683" t="s">
+      <c r="C683" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E683" t="s">
+      <c r="D683" s="5"/>
+      <c r="E683" s="5" t="s">
         <v>393</v>
       </c>
-      <c r="F683" t="s">
+      <c r="F683" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="G683" t="s">
+      <c r="G683" s="5" t="s">
         <v>635</v>
       </c>
     </row>
     <row r="684" spans="1:7">
-      <c r="A684" t="s">
+      <c r="A684" s="5" t="s">
         <v>1958</v>
       </c>
-      <c r="B684" t="s">
+      <c r="B684" s="5" t="s">
         <v>1959</v>
       </c>
-      <c r="C684" t="s">
+      <c r="C684" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E684" t="s">
+      <c r="D684" s="5"/>
+      <c r="E684" s="5" t="s">
         <v>1730</v>
       </c>
-      <c r="F684" t="s">
+      <c r="F684" s="5" t="s">
         <v>1357</v>
       </c>
-      <c r="G684" t="s">
+      <c r="G684" s="5" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="685" spans="1:7">
-      <c r="A685" t="s">
+      <c r="A685" s="5" t="s">
         <v>1960</v>
       </c>
-      <c r="B685" t="s">
+      <c r="B685" s="5" t="s">
         <v>1961</v>
       </c>
-      <c r="C685" t="s">
+      <c r="C685" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E685" t="s">
+      <c r="D685" s="5"/>
+      <c r="E685" s="5" t="s">
         <v>393</v>
       </c>
-      <c r="F685" t="s">
+      <c r="F685" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="G685" t="s">
+      <c r="G685" s="5" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="686" spans="1:7">
-      <c r="A686" t="s">
+      <c r="A686" s="5" t="s">
         <v>1962</v>
       </c>
-      <c r="B686" t="s">
+      <c r="B686" s="5" t="s">
         <v>1963</v>
       </c>
-      <c r="C686" t="s">
+      <c r="C686" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E686" t="s">
+      <c r="D686" s="5"/>
+      <c r="E686" s="5" t="s">
         <v>737</v>
       </c>
-      <c r="F686" t="s">
+      <c r="F686" s="5" t="s">
         <v>1357</v>
       </c>
-      <c r="G686" t="s">
+      <c r="G686" s="5" t="s">
         <v>676</v>
       </c>
     </row>
     <row r="687" spans="1:7">
-      <c r="A687" t="s">
+      <c r="A687" s="5" t="s">
         <v>1964</v>
       </c>
-      <c r="B687" t="s">
+      <c r="B687" s="5" t="s">
         <v>1965</v>
       </c>
-      <c r="C687" t="s">
+      <c r="C687" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="D687" t="s">
+      <c r="D687" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E687" t="s">
+      <c r="E687" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="F687" t="s">
+      <c r="F687" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G687" t="s">
+      <c r="G687" s="5" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="688" spans="1:7">
-      <c r="A688" t="s">
+      <c r="A688" s="5" t="s">
         <v>1966</v>
       </c>
-      <c r="B688" t="s">
+      <c r="B688" s="5" t="s">
         <v>1967</v>
       </c>
-      <c r="C688" t="s">
+      <c r="C688" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="D688" t="s">
+      <c r="D688" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E688" t="s">
+      <c r="E688" s="5" t="s">
         <v>355</v>
       </c>
-      <c r="F688" t="s">
+      <c r="F688" s="5" t="s">
         <v>1968</v>
       </c>
-      <c r="G688" t="s">
+      <c r="G688" s="5" t="s">
         <v>1112</v>
       </c>
     </row>
     <row r="689" spans="1:7">
-      <c r="A689" t="s">
+      <c r="A689" s="5" t="s">
         <v>1969</v>
       </c>
-      <c r="B689" t="s">
+      <c r="B689" s="5" t="s">
         <v>1970</v>
       </c>
-      <c r="C689" t="s">
+      <c r="C689" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="D689" t="s">
+      <c r="D689" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E689" t="s">
+      <c r="E689" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="F689" t="s">
+      <c r="F689" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G689" t="s">
+      <c r="G689" s="5" t="s">
         <v>1580</v>
       </c>
     </row>
     <row r="690" spans="1:7">
-      <c r="A690" t="s">
+      <c r="A690" s="5" t="s">
         <v>1971</v>
       </c>
-      <c r="B690" t="s">
+      <c r="B690" s="5" t="s">
         <v>1972</v>
       </c>
-      <c r="C690" t="s">
+      <c r="C690" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="D690" t="s">
+      <c r="D690" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E690" t="s">
+      <c r="E690" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F690" t="s">
-        <v>8</v>
-      </c>
-      <c r="G690" t="s">
+      <c r="F690" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G690" s="5" t="s">
         <v>1973</v>
       </c>
     </row>
     <row r="691" spans="1:7">
-      <c r="A691" t="s">
+      <c r="A691" s="5" t="s">
         <v>1974</v>
       </c>
-      <c r="B691" t="s">
+      <c r="B691" s="5" t="s">
         <v>1975</v>
       </c>
-      <c r="C691" t="s">
+      <c r="C691" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D691" t="s">
+      <c r="D691" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E691" t="s">
+      <c r="E691" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F691" t="s">
+      <c r="F691" s="5" t="s">
         <v>359</v>
       </c>
-      <c r="G691" t="s">
+      <c r="G691" s="5" t="s">
         <v>1605</v>
       </c>
     </row>
     <row r="692" spans="1:7">
-      <c r="A692" t="s">
+      <c r="A692" s="5" t="s">
         <v>1976</v>
       </c>
-      <c r="B692" t="s">
+      <c r="B692" s="5" t="s">
         <v>1977</v>
       </c>
-      <c r="C692" t="s">
+      <c r="C692" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D692" t="s">
+      <c r="D692" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="E692" t="s">
+      <c r="E692" s="5" t="s">
         <v>452</v>
       </c>
-      <c r="F692" t="s">
+      <c r="F692" s="5" t="s">
         <v>1978</v>
       </c>
-      <c r="G692" t="s">
+      <c r="G692" s="5" t="s">
         <v>1923</v>
       </c>
     </row>
     <row r="693" spans="1:7">
-      <c r="A693" t="s">
+      <c r="A693" s="5" t="s">
         <v>1979</v>
       </c>
-      <c r="B693" t="s">
+      <c r="B693" s="5" t="s">
         <v>1980</v>
       </c>
-      <c r="C693" t="s">
+      <c r="C693" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E693" t="s">
+      <c r="D693" s="5"/>
+      <c r="E693" s="5" t="s">
         <v>351</v>
       </c>
-      <c r="F693" t="s">
+      <c r="F693" s="5" t="s">
         <v>359</v>
       </c>
-      <c r="G693" t="s">
+      <c r="G693" s="5" t="s">
         <v>1981</v>
       </c>
     </row>
     <row r="694" spans="1:7">
-      <c r="A694" t="s">
+      <c r="A694" s="5" t="s">
         <v>1982</v>
       </c>
-      <c r="B694" t="s">
+      <c r="B694" s="5" t="s">
         <v>1983</v>
       </c>
-      <c r="C694" t="s">
+      <c r="C694" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E694" t="s">
+      <c r="D694" s="5"/>
+      <c r="E694" s="5" t="s">
         <v>442</v>
       </c>
-      <c r="F694" t="s">
+      <c r="F694" s="5" t="s">
         <v>1978</v>
       </c>
-      <c r="G694" t="s">
+      <c r="G694" s="5" t="s">
         <v>1984</v>
       </c>
     </row>
     <row r="695" spans="1:7">
-      <c r="A695" t="s">
+      <c r="A695" s="5" t="s">
         <v>1985</v>
       </c>
-      <c r="B695" t="s">
+      <c r="B695" s="5" t="s">
         <v>1986</v>
       </c>
-      <c r="C695" t="s">
+      <c r="C695" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="D695" t="s">
+      <c r="D695" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="E695" t="s">
+      <c r="E695" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="F695" t="s">
+      <c r="F695" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G695" t="s">
+      <c r="G695" s="5" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="696" spans="1:7">
-      <c r="A696" t="s">
+      <c r="A696" s="5" t="s">
         <v>1987</v>
       </c>
-      <c r="B696" t="s">
+      <c r="B696" s="5" t="s">
         <v>1988</v>
       </c>
-      <c r="C696" t="s">
+      <c r="C696" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="D696" t="s">
+      <c r="D696" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="E696" t="s">
+      <c r="E696" s="5" t="s">
         <v>737</v>
       </c>
-      <c r="F696" t="s">
+      <c r="F696" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G696" t="s">
+      <c r="G696" s="5" t="s">
         <v>768</v>
       </c>
     </row>
     <row r="697" spans="1:7">
-      <c r="A697" t="s">
+      <c r="A697" s="5" t="s">
         <v>1989</v>
       </c>
-      <c r="B697" t="s">
+      <c r="B697" s="5" t="s">
         <v>1990</v>
       </c>
-      <c r="C697" t="s">
+      <c r="C697" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="D697" t="s">
+      <c r="D697" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="E697" t="s">
+      <c r="E697" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F697" t="s">
-        <v>8</v>
-      </c>
-      <c r="G697" t="s">
+      <c r="F697" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G697" s="5" t="s">
         <v>1991</v>
       </c>
     </row>
     <row r="698" spans="1:7">
-      <c r="A698" t="s">
+      <c r="A698" s="5" t="s">
         <v>1992</v>
       </c>
-      <c r="B698" t="s">
+      <c r="B698" s="5" t="s">
         <v>1993</v>
       </c>
-      <c r="C698" t="s">
+      <c r="C698" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="D698" t="s">
+      <c r="D698" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="E698" t="s">
+      <c r="E698" s="5" t="s">
         <v>435</v>
       </c>
-      <c r="F698" t="s">
-        <v>8</v>
-      </c>
-      <c r="G698" t="s">
+      <c r="F698" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G698" s="5" t="s">
         <v>1994</v>
       </c>
     </row>
     <row r="699" spans="1:7">
-      <c r="A699" t="s">
+      <c r="A699" s="5" t="s">
         <v>1995</v>
       </c>
-      <c r="B699" t="s">
+      <c r="B699" s="5" t="s">
         <v>1996</v>
       </c>
-      <c r="C699" t="s">
+      <c r="C699" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="D699" t="s">
+      <c r="D699" s="5" t="s">
         <v>1117</v>
       </c>
-      <c r="E699" t="s">
+      <c r="E699" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F699" t="s">
-        <v>8</v>
-      </c>
-      <c r="G699" t="s">
+      <c r="F699" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G699" s="5" t="s">
         <v>1997</v>
       </c>
     </row>
     <row r="700" spans="1:7">
-      <c r="A700" t="s">
+      <c r="A700" s="5" t="s">
         <v>1998</v>
       </c>
-      <c r="B700" t="s">
+      <c r="B700" s="5" t="s">
         <v>1999</v>
       </c>
-      <c r="C700" t="s">
+      <c r="C700" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="D700" t="s">
+      <c r="D700" s="5" t="s">
         <v>1117</v>
       </c>
-      <c r="E700" t="s">
+      <c r="E700" s="5" t="s">
         <v>2000</v>
       </c>
-      <c r="F700" t="s">
-        <v>8</v>
-      </c>
-      <c r="G700" t="s">
+      <c r="F700" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G700" s="5" t="s">
         <v>2001</v>
       </c>
     </row>
     <row r="701" spans="1:7">
-      <c r="A701" t="s">
+      <c r="A701" s="5" t="s">
         <v>2002</v>
       </c>
-      <c r="B701" t="s">
+      <c r="B701" s="5" t="s">
         <v>2003</v>
       </c>
-      <c r="C701" t="s">
+      <c r="C701" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E701" t="s">
+      <c r="D701" s="5"/>
+      <c r="E701" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="F701" t="s">
-        <v>8</v>
-      </c>
-      <c r="G701" t="s">
+      <c r="F701" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G701" s="5" t="s">
         <v>775</v>
       </c>
     </row>
     <row r="702" spans="1:7">
-      <c r="A702" t="s">
+      <c r="A702" s="5" t="s">
         <v>2004</v>
       </c>
-      <c r="B702" t="s">
+      <c r="B702" s="5" t="s">
         <v>2005</v>
       </c>
-      <c r="C702" t="s">
+      <c r="C702" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="D702" t="s">
+      <c r="D702" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E702" t="s">
+      <c r="E702" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="F702" t="s">
+      <c r="F702" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="G702" t="s">
+      <c r="G702" s="5" t="s">
         <v>1072</v>
       </c>
     </row>
     <row r="703" spans="1:7">
-      <c r="A703" t="s">
+      <c r="A703" s="5" t="s">
         <v>2006</v>
       </c>
-      <c r="B703" t="s">
+      <c r="B703" s="5" t="s">
         <v>2007</v>
       </c>
-      <c r="C703" t="s">
+      <c r="C703" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="D703" t="s">
+      <c r="D703" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E703" t="s">
+      <c r="E703" s="5" t="s">
         <v>655</v>
       </c>
-      <c r="F703" t="s">
+      <c r="F703" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="G703" t="s">
+      <c r="G703" s="5" t="s">
         <v>1229</v>
       </c>
     </row>
     <row r="704" spans="1:7">
-      <c r="A704" t="s">
+      <c r="A704" s="5" t="s">
         <v>2008</v>
       </c>
-      <c r="B704" t="s">
+      <c r="B704" s="5" t="s">
         <v>2009</v>
       </c>
-      <c r="C704" t="s">
+      <c r="C704" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="D704" t="s">
+      <c r="D704" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E704" t="s">
+      <c r="E704" s="5" t="s">
         <v>442</v>
       </c>
-      <c r="F704" t="s">
+      <c r="F704" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="G704" t="s">
+      <c r="G704" s="5" t="s">
         <v>1706</v>
       </c>
     </row>
     <row r="705" spans="1:7">
-      <c r="A705" t="s">
+      <c r="A705" s="5" t="s">
         <v>2010</v>
       </c>
-      <c r="B705" t="s">
+      <c r="B705" s="5" t="s">
         <v>2011</v>
       </c>
-      <c r="C705" t="s">
+      <c r="C705" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="E705" t="s">
+      <c r="D705" s="5"/>
+      <c r="E705" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="F705" t="s">
-        <v>8</v>
-      </c>
-      <c r="G705" t="s">
+      <c r="F705" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G705" s="5" t="s">
         <v>2012</v>
       </c>
     </row>
     <row r="706" spans="1:7">
-      <c r="A706" t="s">
+      <c r="A706" s="5" t="s">
         <v>2013</v>
       </c>
-      <c r="B706" t="s">
+      <c r="B706" s="5" t="s">
         <v>2014</v>
       </c>
-      <c r="C706" t="s">
+      <c r="C706" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="E706" t="s">
+      <c r="D706" s="5"/>
+      <c r="E706" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="F706" t="s">
-        <v>8</v>
-      </c>
-      <c r="G706" t="s">
+      <c r="F706" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G706" s="5" t="s">
         <v>846</v>
       </c>
     </row>
     <row r="707" spans="1:7">
-      <c r="A707" t="s">
+      <c r="A707" s="5" t="s">
         <v>2015</v>
       </c>
-      <c r="B707" t="s">
+      <c r="B707" s="5" t="s">
         <v>2016</v>
       </c>
-      <c r="C707" t="s">
+      <c r="C707" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="E707" t="s">
+      <c r="D707" s="5"/>
+      <c r="E707" s="5" t="s">
         <v>524</v>
       </c>
-      <c r="F707" t="s">
-        <v>8</v>
-      </c>
-      <c r="G707" t="s">
+      <c r="F707" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G707" s="5" t="s">
         <v>2017</v>
       </c>
     </row>
     <row r="708" spans="1:7">
-      <c r="A708" t="s">
+      <c r="A708" s="5" t="s">
         <v>2018</v>
       </c>
-      <c r="B708" t="s">
+      <c r="B708" s="5" t="s">
         <v>2019</v>
       </c>
-      <c r="C708" t="s">
+      <c r="C708" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="D708" t="s">
+      <c r="D708" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E708" t="s">
+      <c r="E708" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="F708" t="s">
+      <c r="F708" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="G708" t="s">
+      <c r="G708" s="5" t="s">
         <v>591</v>
       </c>
     </row>
     <row r="709" spans="1:7">
-      <c r="A709" t="s">
+      <c r="A709" s="5" t="s">
         <v>2020</v>
       </c>
-      <c r="B709" t="s">
+      <c r="B709" s="5" t="s">
         <v>2021</v>
       </c>
-      <c r="C709" t="s">
+      <c r="C709" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="D709" t="s">
+      <c r="D709" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="E709" t="s">
+      <c r="E709" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F709" t="s">
+      <c r="F709" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G709" t="s">
+      <c r="G709" s="5" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="710" spans="1:7">
-      <c r="A710" t="s">
+      <c r="A710" s="5" t="s">
         <v>2022</v>
       </c>
-      <c r="B710" t="s">
+      <c r="B710" s="5" t="s">
         <v>2023</v>
       </c>
-      <c r="C710" t="s">
+      <c r="C710" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="D710" t="s">
+      <c r="D710" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="E710" t="s">
+      <c r="E710" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="F710" t="s">
+      <c r="F710" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="G710" t="s">
+      <c r="G710" s="5" t="s">
         <v>2024</v>
       </c>
     </row>
     <row r="711" spans="1:7">
-      <c r="A711" t="s">
+      <c r="A711" s="5" t="s">
         <v>2025</v>
       </c>
-      <c r="B711" t="s">
+      <c r="B711" s="5" t="s">
         <v>2026</v>
       </c>
-      <c r="C711" t="s">
+      <c r="C711" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="D711" t="s">
+      <c r="D711" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="E711" t="s">
+      <c r="E711" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="F711" t="s">
+      <c r="F711" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G711" t="s">
+      <c r="G711" s="5" t="s">
         <v>676</v>
       </c>
     </row>
     <row r="712" spans="1:7">
-      <c r="A712" t="s">
+      <c r="A712" s="5" t="s">
         <v>2027</v>
       </c>
-      <c r="B712" t="s">
+      <c r="B712" s="5" t="s">
         <v>2028</v>
       </c>
-      <c r="C712" t="s">
+      <c r="C712" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="D712" t="s">
+      <c r="D712" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="E712" t="s">
+      <c r="E712" s="5" t="s">
         <v>452</v>
       </c>
-      <c r="F712" t="s">
+      <c r="F712" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="G712" t="s">
+      <c r="G712" s="5" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="713" spans="1:7">
-      <c r="A713" t="s">
+      <c r="A713" s="5" t="s">
         <v>2029</v>
       </c>
-      <c r="B713" t="s">
+      <c r="B713" s="5" t="s">
         <v>2030</v>
       </c>
-      <c r="C713" t="s">
+      <c r="C713" s="5" t="s">
         <v>1117</v>
       </c>
-      <c r="E713" t="s">
+      <c r="D713" s="5"/>
+      <c r="E713" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="F713" t="s">
+      <c r="F713" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G713" t="s">
+      <c r="G713" s="5" t="s">
         <v>2031</v>
       </c>
     </row>
     <row r="714" spans="1:7">
-      <c r="A714" t="s">
+      <c r="A714" s="5" t="s">
         <v>2032</v>
       </c>
-      <c r="B714" t="s">
+      <c r="B714" s="5" t="s">
         <v>2033</v>
       </c>
-      <c r="C714" t="s">
+      <c r="C714" s="5" t="s">
         <v>1117</v>
       </c>
-      <c r="E714" t="s">
+      <c r="D714" s="5"/>
+      <c r="E714" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="F714" t="s">
+      <c r="F714" s="5" t="s">
         <v>1978</v>
       </c>
-      <c r="G714" t="s">
+      <c r="G714" s="5" t="s">
         <v>2034</v>
       </c>
     </row>
     <row r="715" spans="1:7">
-      <c r="A715" t="s">
+      <c r="A715" s="5" t="s">
         <v>2035</v>
       </c>
-      <c r="B715" t="s">
+      <c r="B715" s="5" t="s">
         <v>2036</v>
       </c>
-      <c r="C715" t="s">
+      <c r="C715" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="D715" t="s">
+      <c r="D715" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="E715" t="s">
+      <c r="E715" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="F715" t="s">
+      <c r="F715" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="G715" t="s">
+      <c r="G715" s="5" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="716" spans="1:7">
-      <c r="A716" t="s">
+      <c r="A716" s="5" t="s">
         <v>2037</v>
       </c>
-      <c r="B716" t="s">
+      <c r="B716" s="5" t="s">
         <v>2038</v>
       </c>
-      <c r="C716" t="s">
+      <c r="C716" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="D716" t="s">
+      <c r="D716" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="E716" t="s">
+      <c r="E716" s="5" t="s">
         <v>468</v>
       </c>
-      <c r="F716" t="s">
-        <v>8</v>
-      </c>
-      <c r="G716" t="s">
+      <c r="F716" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G716" s="5" t="s">
         <v>2039</v>
       </c>
     </row>
     <row r="717" spans="1:7">
-      <c r="A717" t="s">
+      <c r="A717" s="5" t="s">
         <v>2040</v>
       </c>
-      <c r="B717" t="s">
+      <c r="B717" s="5" t="s">
         <v>2041</v>
       </c>
-      <c r="C717" t="s">
+      <c r="C717" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E717" t="s">
+      <c r="D717" s="5"/>
+      <c r="E717" s="5" t="s">
         <v>807</v>
       </c>
-      <c r="F717" t="s">
-        <v>8</v>
-      </c>
-      <c r="G717" t="s">
+      <c r="F717" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G717" s="5" t="s">
         <v>2042</v>
       </c>
     </row>
     <row r="718" spans="1:7">
-      <c r="A718" t="s">
+      <c r="A718" s="5" t="s">
         <v>2043</v>
       </c>
-      <c r="B718" t="s">
+      <c r="B718" s="5" t="s">
         <v>2044</v>
       </c>
-      <c r="C718" t="s">
+      <c r="C718" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="D718" t="s">
+      <c r="D718" s="5" t="s">
         <v>2290</v>
       </c>
-      <c r="E718" t="s">
+      <c r="E718" s="5" t="s">
         <v>807</v>
       </c>
-      <c r="F718" t="s">
-        <v>8</v>
-      </c>
-      <c r="G718" t="s">
+      <c r="F718" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G718" s="5" t="s">
         <v>2045</v>
       </c>
     </row>
     <row r="719" spans="1:7">
-      <c r="A719" t="s">
+      <c r="A719" s="5" t="s">
         <v>2046</v>
       </c>
-      <c r="B719" t="s">
+      <c r="B719" s="5" t="s">
         <v>2047</v>
       </c>
-      <c r="C719" t="s">
+      <c r="C719" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="D719" t="s">
+      <c r="D719" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="E719" t="s">
+      <c r="E719" s="5" t="s">
         <v>814</v>
       </c>
-      <c r="F719" t="s">
+      <c r="F719" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G719" t="s">
+      <c r="G719" s="5" t="s">
         <v>2048</v>
       </c>
     </row>
     <row r="720" spans="1:7">
-      <c r="A720" t="s">
+      <c r="A720" s="5" t="s">
         <v>2049</v>
       </c>
-      <c r="B720" t="s">
+      <c r="B720" s="5" t="s">
         <v>2050</v>
       </c>
-      <c r="C720" t="s">
+      <c r="C720" s="5" t="s">
         <v>627</v>
       </c>
-      <c r="D720" t="s">
+      <c r="D720" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E720" t="s">
+      <c r="E720" s="5" t="s">
         <v>524</v>
       </c>
-      <c r="F720" t="s">
+      <c r="F720" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G720" t="s">
+      <c r="G720" s="5" t="s">
         <v>719</v>
       </c>
     </row>
     <row r="721" spans="1:7">
-      <c r="A721" t="s">
+      <c r="A721" s="5" t="s">
         <v>2051</v>
       </c>
-      <c r="B721" t="s">
+      <c r="B721" s="5" t="s">
         <v>2052</v>
       </c>
-      <c r="C721" t="s">
+      <c r="C721" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="D721" t="s">
+      <c r="D721" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="E721" t="s">
+      <c r="E721" s="5" t="s">
         <v>524</v>
       </c>
-      <c r="F721" t="s">
+      <c r="F721" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G721" t="s">
+      <c r="G721" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="722" spans="1:7">
-      <c r="A722" t="s">
+      <c r="A722" s="5" t="s">
         <v>2053</v>
       </c>
-      <c r="B722" t="s">
+      <c r="B722" s="5" t="s">
         <v>2054</v>
       </c>
-      <c r="C722" t="s">
+      <c r="C722" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D722" t="s">
+      <c r="D722" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E722" t="s">
+      <c r="E722" s="5" t="s">
         <v>524</v>
       </c>
-      <c r="F722" t="s">
+      <c r="F722" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="G722" t="s">
+      <c r="G722" s="5" t="s">
         <v>2055</v>
       </c>
     </row>

</xml_diff>